<commit_message>
major reorganization of the feeds and gndsub into a single cell. Added the ild sub box and the ild via to ground.
</commit_message>
<xml_diff>
--- a/masks/code/ResonatorArray.xlsx
+++ b/masks/code/ResonatorArray.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -786,7 +786,7 @@
         <v>20</v>
       </c>
       <c r="D15" t="n">
-        <v>0.75</v>
+        <v>0.95</v>
       </c>
       <c r="E15" t="n">
         <v>0.4</v>
@@ -798,10 +798,10 @@
         <v>0.5</v>
       </c>
       <c r="H15" t="n">
-        <v>0.4</v>
+        <v>0.6</v>
       </c>
       <c r="I15" t="n">
-        <v>1.1</v>
+        <v>1.3</v>
       </c>
       <c r="J15" t="n">
         <v>0.65</v>
@@ -810,13 +810,13 @@
         <v>0.15</v>
       </c>
       <c r="M15" t="n">
-        <v>-42.158</v>
+        <v>-41.758</v>
       </c>
       <c r="N15" t="n">
         <v>-44.1</v>
       </c>
       <c r="O15" t="n">
-        <v>42.908</v>
+        <v>42.70800000000001</v>
       </c>
       <c r="P15" t="n">
         <v>44.5</v>
@@ -828,7 +828,7 @@
         <v>8</v>
       </c>
       <c r="V15" t="n">
-        <v>-42.158</v>
+        <v>-41.758</v>
       </c>
       <c r="W15" t="n">
         <v>-44.1</v>
@@ -1034,7 +1034,7 @@
         <v>23</v>
       </c>
       <c r="D19" t="n">
-        <v>2.1</v>
+        <v>2.3</v>
       </c>
       <c r="E19" t="n">
         <v>0.45</v>
@@ -1046,10 +1046,10 @@
         <v>0.4</v>
       </c>
       <c r="H19" t="n">
-        <v>1.9</v>
+        <v>2.1</v>
       </c>
       <c r="I19" t="n">
-        <v>2.3</v>
+        <v>2.5</v>
       </c>
       <c r="J19" t="n">
         <v>0.65</v>
@@ -1064,7 +1064,7 @@
         <v>-24.241</v>
       </c>
       <c r="O19" t="n">
-        <v>49.35</v>
+        <v>49.55</v>
       </c>
       <c r="P19" t="n">
         <v>24.691</v>
@@ -1096,7 +1096,7 @@
         <v>23</v>
       </c>
       <c r="D20" t="n">
-        <v>2.1</v>
+        <v>2.3</v>
       </c>
       <c r="E20" t="n">
         <v>0.45</v>
@@ -1108,10 +1108,10 @@
         <v>0.4</v>
       </c>
       <c r="H20" t="n">
-        <v>1.9</v>
+        <v>2.1</v>
       </c>
       <c r="I20" t="n">
-        <v>2.3</v>
+        <v>2.5</v>
       </c>
       <c r="J20" t="n">
         <v>0.65</v>
@@ -1126,7 +1126,7 @@
         <v>-49.441</v>
       </c>
       <c r="O20" t="n">
-        <v>49.35</v>
+        <v>49.55</v>
       </c>
       <c r="P20" t="n">
         <v>49.89100000000001</v>
@@ -1158,7 +1158,7 @@
         <v>23</v>
       </c>
       <c r="D21" t="n">
-        <v>2.1</v>
+        <v>2.3</v>
       </c>
       <c r="E21" t="n">
         <v>0.45</v>
@@ -1170,10 +1170,10 @@
         <v>0.4</v>
       </c>
       <c r="H21" t="n">
-        <v>1.9</v>
+        <v>2.1</v>
       </c>
       <c r="I21" t="n">
-        <v>2.3</v>
+        <v>2.5</v>
       </c>
       <c r="J21" t="n">
         <v>0.65</v>
@@ -1188,7 +1188,7 @@
         <v>-11.641</v>
       </c>
       <c r="O21" t="n">
-        <v>-45.15</v>
+        <v>-44.95</v>
       </c>
       <c r="P21" t="n">
         <v>12.091</v>
@@ -1220,7 +1220,7 @@
         <v>23</v>
       </c>
       <c r="D22" t="n">
-        <v>2.1</v>
+        <v>2.3</v>
       </c>
       <c r="E22" t="n">
         <v>0.45</v>
@@ -1232,10 +1232,10 @@
         <v>0.4</v>
       </c>
       <c r="H22" t="n">
-        <v>1.9</v>
+        <v>2.1</v>
       </c>
       <c r="I22" t="n">
-        <v>2.3</v>
+        <v>2.5</v>
       </c>
       <c r="J22" t="n">
         <v>0.65</v>
@@ -1250,7 +1250,7 @@
         <v>-36.841</v>
       </c>
       <c r="O22" t="n">
-        <v>-45.15</v>
+        <v>-44.95</v>
       </c>
       <c r="P22" t="n">
         <v>37.291</v>
@@ -1282,7 +1282,7 @@
         <v>23</v>
       </c>
       <c r="D23" t="n">
-        <v>2.1</v>
+        <v>2.3</v>
       </c>
       <c r="E23" t="n">
         <v>0.45</v>
@@ -1294,10 +1294,10 @@
         <v>0.4</v>
       </c>
       <c r="H23" t="n">
-        <v>1.9</v>
+        <v>2.1</v>
       </c>
       <c r="I23" t="n">
-        <v>2.3</v>
+        <v>2.5</v>
       </c>
       <c r="J23" t="n">
         <v>0.65</v>
@@ -1312,7 +1312,7 @@
         <v>45.059</v>
       </c>
       <c r="O23" t="n">
-        <v>-49.09999999999999</v>
+        <v>-48.9</v>
       </c>
       <c r="P23" t="n">
         <v>-44.60899999999999</v>
@@ -1326,7 +1326,7 @@
         <v>23</v>
       </c>
       <c r="D24" t="n">
-        <v>2.1</v>
+        <v>2.3</v>
       </c>
       <c r="E24" t="n">
         <v>0.45</v>
@@ -1338,10 +1338,10 @@
         <v>0.4</v>
       </c>
       <c r="H24" t="n">
-        <v>1.9</v>
+        <v>2.1</v>
       </c>
       <c r="I24" t="n">
-        <v>2.3</v>
+        <v>2.5</v>
       </c>
       <c r="J24" t="n">
         <v>0.65</v>
@@ -1356,7 +1356,7 @@
         <v>-43.141</v>
       </c>
       <c r="O24" t="n">
-        <v>-49.09999999999999</v>
+        <v>-48.9</v>
       </c>
       <c r="P24" t="n">
         <v>43.591</v>
@@ -1376,16 +1376,16 @@
         <v>1.7</v>
       </c>
       <c r="F25" t="n">
-        <v>4</v>
+        <v>4.4</v>
       </c>
       <c r="G25" t="n">
         <v>2.1</v>
       </c>
       <c r="H25" t="n">
-        <v>-2</v>
+        <v>-2.2</v>
       </c>
       <c r="I25" t="n">
-        <v>2</v>
+        <v>2.2</v>
       </c>
       <c r="J25" t="n">
         <v>2.75</v>
@@ -1432,7 +1432,7 @@
         <v>25</v>
       </c>
       <c r="D26" t="n">
-        <v>4.3</v>
+        <v>4.5</v>
       </c>
       <c r="E26" t="n">
         <v>1.75</v>
@@ -1444,10 +1444,10 @@
         <v>0.4</v>
       </c>
       <c r="H26" t="n">
-        <v>4.05</v>
+        <v>4.25</v>
       </c>
       <c r="I26" t="n">
-        <v>4.55</v>
+        <v>4.75</v>
       </c>
       <c r="J26" t="n">
         <v>1.95</v>
@@ -1462,7 +1462,7 @@
         <v>45.059</v>
       </c>
       <c r="O26" t="n">
-        <v>-43</v>
+        <v>-42.8</v>
       </c>
       <c r="P26" t="n">
         <v>-43.309</v>
@@ -1494,7 +1494,7 @@
         <v>25</v>
       </c>
       <c r="D27" t="n">
-        <v>4.3</v>
+        <v>4.5</v>
       </c>
       <c r="E27" t="n">
         <v>1.75</v>
@@ -1506,10 +1506,10 @@
         <v>0.4</v>
       </c>
       <c r="H27" t="n">
-        <v>4.05</v>
+        <v>4.25</v>
       </c>
       <c r="I27" t="n">
-        <v>4.55</v>
+        <v>4.75</v>
       </c>
       <c r="J27" t="n">
         <v>1.95</v>
@@ -1524,7 +1524,7 @@
         <v>-43.141</v>
       </c>
       <c r="O27" t="n">
-        <v>-43</v>
+        <v>-42.8</v>
       </c>
       <c r="P27" t="n">
         <v>44.891</v>
@@ -1704,13 +1704,13 @@
         <v>11.5</v>
       </c>
       <c r="M30" t="n">
-        <v>-44.883</v>
+        <v>-45.083</v>
       </c>
       <c r="N30" t="n">
         <v>-44.1</v>
       </c>
       <c r="O30" t="n">
-        <v>34.783</v>
+        <v>34.983</v>
       </c>
       <c r="P30" t="n">
         <v>56.35</v>
@@ -1748,13 +1748,13 @@
         <v>11.5</v>
       </c>
       <c r="M31" t="n">
-        <v>-44.883</v>
+        <v>-45.083</v>
       </c>
       <c r="N31" t="n">
         <v>-31.5</v>
       </c>
       <c r="O31" t="n">
-        <v>36.583</v>
+        <v>36.783</v>
       </c>
       <c r="P31" t="n">
         <v>43.75</v>
@@ -1792,13 +1792,13 @@
         <v>11.5</v>
       </c>
       <c r="M32" t="n">
-        <v>-32.283</v>
+        <v>-32.483</v>
       </c>
       <c r="N32" t="n">
         <v>-31.5</v>
       </c>
       <c r="O32" t="n">
-        <v>25.783</v>
+        <v>25.983</v>
       </c>
       <c r="P32" t="n">
         <v>43.75</v>
@@ -1836,13 +1836,13 @@
         <v>11.5</v>
       </c>
       <c r="M33" t="n">
-        <v>-32.283</v>
+        <v>-32.483</v>
       </c>
       <c r="N33" t="n">
         <v>-44.1</v>
       </c>
       <c r="O33" t="n">
-        <v>27.583</v>
+        <v>27.783</v>
       </c>
       <c r="P33" t="n">
         <v>56.35</v>
@@ -1880,13 +1880,13 @@
         <v>11.5</v>
       </c>
       <c r="M34" t="n">
-        <v>-19.683</v>
+        <v>-19.883</v>
       </c>
       <c r="N34" t="n">
         <v>-44.1</v>
       </c>
       <c r="O34" t="n">
-        <v>16.783</v>
+        <v>16.983</v>
       </c>
       <c r="P34" t="n">
         <v>56.35</v>
@@ -1924,13 +1924,13 @@
         <v>10</v>
       </c>
       <c r="M35" t="n">
-        <v>-7.083</v>
+        <v>-7.283</v>
       </c>
       <c r="N35" t="n">
         <v>-44.1</v>
       </c>
       <c r="O35" t="n">
-        <v>-3.016999999999999</v>
+        <v>-2.816999999999999</v>
       </c>
       <c r="P35" t="n">
         <v>54.85</v>
@@ -1968,13 +1968,13 @@
         <v>10</v>
       </c>
       <c r="M36" t="n">
-        <v>-7.083</v>
+        <v>-7.283</v>
       </c>
       <c r="N36" t="n">
         <v>-31.5</v>
       </c>
       <c r="O36" t="n">
-        <v>-1.217000000000001</v>
+        <v>-1.017</v>
       </c>
       <c r="P36" t="n">
         <v>42.25</v>
@@ -2012,13 +2012,13 @@
         <v>10</v>
       </c>
       <c r="M37" t="n">
-        <v>-19.683</v>
+        <v>-19.883</v>
       </c>
       <c r="N37" t="n">
         <v>-31.5</v>
       </c>
       <c r="O37" t="n">
-        <v>13.183</v>
+        <v>13.383</v>
       </c>
       <c r="P37" t="n">
         <v>42.25</v>
@@ -2056,13 +2056,13 @@
         <v>10</v>
       </c>
       <c r="M38" t="n">
-        <v>-19.683</v>
+        <v>-19.883</v>
       </c>
       <c r="N38" t="n">
         <v>-18.9</v>
       </c>
       <c r="O38" t="n">
-        <v>14.983</v>
+        <v>15.183</v>
       </c>
       <c r="P38" t="n">
         <v>29.65</v>
@@ -2100,13 +2100,13 @@
         <v>10</v>
       </c>
       <c r="M39" t="n">
-        <v>-7.083</v>
+        <v>-7.283</v>
       </c>
       <c r="N39" t="n">
         <v>-18.9</v>
       </c>
       <c r="O39" t="n">
-        <v>4.183</v>
+        <v>4.383000000000001</v>
       </c>
       <c r="P39" t="n">
         <v>29.65</v>
@@ -2144,13 +2144,13 @@
         <v>8.5</v>
       </c>
       <c r="M40" t="n">
-        <v>-7.083</v>
+        <v>-7.283</v>
       </c>
       <c r="N40" t="n">
         <v>-6.3</v>
       </c>
       <c r="O40" t="n">
-        <v>-3.016999999999999</v>
+        <v>-2.816999999999999</v>
       </c>
       <c r="P40" t="n">
         <v>15.55</v>
@@ -2188,13 +2188,13 @@
         <v>8.5</v>
       </c>
       <c r="M41" t="n">
-        <v>-19.683</v>
+        <v>-19.883</v>
       </c>
       <c r="N41" t="n">
         <v>-6.3</v>
       </c>
       <c r="O41" t="n">
-        <v>11.383</v>
+        <v>11.583</v>
       </c>
       <c r="P41" t="n">
         <v>15.55</v>
@@ -2232,13 +2232,13 @@
         <v>8.5</v>
       </c>
       <c r="M42" t="n">
-        <v>-32.283</v>
+        <v>-32.483</v>
       </c>
       <c r="N42" t="n">
         <v>-6.3</v>
       </c>
       <c r="O42" t="n">
-        <v>25.783</v>
+        <v>25.983</v>
       </c>
       <c r="P42" t="n">
         <v>15.55</v>
@@ -2276,13 +2276,13 @@
         <v>8.5</v>
       </c>
       <c r="M43" t="n">
-        <v>-32.283</v>
+        <v>-32.483</v>
       </c>
       <c r="N43" t="n">
         <v>-18.9</v>
       </c>
       <c r="O43" t="n">
-        <v>27.583</v>
+        <v>27.783</v>
       </c>
       <c r="P43" t="n">
         <v>28.15</v>
@@ -2320,13 +2320,13 @@
         <v>8.5</v>
       </c>
       <c r="M44" t="n">
-        <v>-44.883</v>
+        <v>-45.083</v>
       </c>
       <c r="N44" t="n">
         <v>-18.9</v>
       </c>
       <c r="O44" t="n">
-        <v>41.983</v>
+        <v>42.183</v>
       </c>
       <c r="P44" t="n">
         <v>28.15</v>
@@ -2364,13 +2364,13 @@
         <v>7</v>
       </c>
       <c r="M45" t="n">
-        <v>-44.883</v>
+        <v>-45.083</v>
       </c>
       <c r="N45" t="n">
         <v>-6.3</v>
       </c>
       <c r="O45" t="n">
-        <v>34.783</v>
+        <v>34.983</v>
       </c>
       <c r="P45" t="n">
         <v>14.05</v>
@@ -2408,13 +2408,13 @@
         <v>7</v>
       </c>
       <c r="M46" t="n">
-        <v>-44.883</v>
+        <v>-45.083</v>
       </c>
       <c r="N46" t="n">
         <v>6.3</v>
       </c>
       <c r="O46" t="n">
-        <v>36.583</v>
+        <v>36.783</v>
       </c>
       <c r="P46" t="n">
         <v>1.45</v>
@@ -2452,13 +2452,13 @@
         <v>7</v>
       </c>
       <c r="M47" t="n">
-        <v>-32.283</v>
+        <v>-32.483</v>
       </c>
       <c r="N47" t="n">
         <v>6.3</v>
       </c>
       <c r="O47" t="n">
-        <v>25.783</v>
+        <v>25.983</v>
       </c>
       <c r="P47" t="n">
         <v>1.45</v>
@@ -2496,13 +2496,13 @@
         <v>7</v>
       </c>
       <c r="M48" t="n">
-        <v>-32.283</v>
+        <v>-32.483</v>
       </c>
       <c r="N48" t="n">
         <v>18.9</v>
       </c>
       <c r="O48" t="n">
-        <v>27.583</v>
+        <v>27.783</v>
       </c>
       <c r="P48" t="n">
         <v>-11.15</v>
@@ -2540,13 +2540,13 @@
         <v>7</v>
       </c>
       <c r="M49" t="n">
-        <v>-44.883</v>
+        <v>-45.083</v>
       </c>
       <c r="N49" t="n">
         <v>18.9</v>
       </c>
       <c r="O49" t="n">
-        <v>41.983</v>
+        <v>42.183</v>
       </c>
       <c r="P49" t="n">
         <v>-11.15</v>
@@ -2584,13 +2584,13 @@
         <v>5.5</v>
       </c>
       <c r="M50" t="n">
-        <v>-44.883</v>
+        <v>-45.083</v>
       </c>
       <c r="N50" t="n">
         <v>31.5</v>
       </c>
       <c r="O50" t="n">
-        <v>34.783</v>
+        <v>34.983</v>
       </c>
       <c r="P50" t="n">
         <v>-25.25</v>
@@ -2628,13 +2628,13 @@
         <v>5.5</v>
       </c>
       <c r="M51" t="n">
-        <v>-44.883</v>
+        <v>-45.083</v>
       </c>
       <c r="N51" t="n">
         <v>44.1</v>
       </c>
       <c r="O51" t="n">
-        <v>36.583</v>
+        <v>36.783</v>
       </c>
       <c r="P51" t="n">
         <v>-37.85</v>
@@ -2672,13 +2672,13 @@
         <v>5.5</v>
       </c>
       <c r="M52" t="n">
-        <v>-32.283</v>
+        <v>-32.483</v>
       </c>
       <c r="N52" t="n">
         <v>44.1</v>
       </c>
       <c r="O52" t="n">
-        <v>25.783</v>
+        <v>25.983</v>
       </c>
       <c r="P52" t="n">
         <v>-37.85</v>
@@ -2716,13 +2716,13 @@
         <v>5.5</v>
       </c>
       <c r="M53" t="n">
-        <v>-32.283</v>
+        <v>-32.483</v>
       </c>
       <c r="N53" t="n">
         <v>31.5</v>
       </c>
       <c r="O53" t="n">
-        <v>27.583</v>
+        <v>27.783</v>
       </c>
       <c r="P53" t="n">
         <v>-25.25</v>
@@ -2760,13 +2760,13 @@
         <v>5.5</v>
       </c>
       <c r="M54" t="n">
-        <v>-19.683</v>
+        <v>-19.883</v>
       </c>
       <c r="N54" t="n">
         <v>31.5</v>
       </c>
       <c r="O54" t="n">
-        <v>16.783</v>
+        <v>16.983</v>
       </c>
       <c r="P54" t="n">
         <v>-25.25</v>
@@ -2804,13 +2804,13 @@
         <v>4</v>
       </c>
       <c r="M55" t="n">
-        <v>-19.683</v>
+        <v>-19.883</v>
       </c>
       <c r="N55" t="n">
         <v>44.1</v>
       </c>
       <c r="O55" t="n">
-        <v>9.583</v>
+        <v>9.782999999999999</v>
       </c>
       <c r="P55" t="n">
         <v>-39.35</v>
@@ -2848,13 +2848,13 @@
         <v>4</v>
       </c>
       <c r="M56" t="n">
-        <v>-7.083</v>
+        <v>-7.283</v>
       </c>
       <c r="N56" t="n">
         <v>44.1</v>
       </c>
       <c r="O56" t="n">
-        <v>-1.217000000000001</v>
+        <v>-1.017</v>
       </c>
       <c r="P56" t="n">
         <v>-39.35</v>
@@ -2892,13 +2892,13 @@
         <v>4</v>
       </c>
       <c r="M57" t="n">
-        <v>-7.083</v>
+        <v>-7.283</v>
       </c>
       <c r="N57" t="n">
         <v>31.5</v>
       </c>
       <c r="O57" t="n">
-        <v>0.5830000000000002</v>
+        <v>0.7830000000000004</v>
       </c>
       <c r="P57" t="n">
         <v>-26.75</v>
@@ -2936,13 +2936,13 @@
         <v>4</v>
       </c>
       <c r="M58" t="n">
-        <v>-7.083</v>
+        <v>-7.283</v>
       </c>
       <c r="N58" t="n">
         <v>18.9</v>
       </c>
       <c r="O58" t="n">
-        <v>2.383</v>
+        <v>2.583</v>
       </c>
       <c r="P58" t="n">
         <v>-14.15</v>
@@ -2980,13 +2980,13 @@
         <v>4</v>
       </c>
       <c r="M59" t="n">
-        <v>-19.683</v>
+        <v>-19.883</v>
       </c>
       <c r="N59" t="n">
         <v>18.9</v>
       </c>
       <c r="O59" t="n">
-        <v>16.783</v>
+        <v>16.983</v>
       </c>
       <c r="P59" t="n">
         <v>-14.15</v>
@@ -3024,13 +3024,13 @@
         <v>2.5</v>
       </c>
       <c r="M60" t="n">
-        <v>-19.683</v>
+        <v>-19.883</v>
       </c>
       <c r="N60" t="n">
         <v>6.3</v>
       </c>
       <c r="O60" t="n">
-        <v>9.583</v>
+        <v>9.782999999999999</v>
       </c>
       <c r="P60" t="n">
         <v>-3.05</v>
@@ -3068,13 +3068,13 @@
         <v>2.5</v>
       </c>
       <c r="M61" t="n">
-        <v>-7.083</v>
+        <v>-7.283</v>
       </c>
       <c r="N61" t="n">
         <v>6.3</v>
       </c>
       <c r="O61" t="n">
-        <v>-1.217000000000001</v>
+        <v>-1.017</v>
       </c>
       <c r="P61" t="n">
         <v>-3.05</v>
@@ -3112,13 +3112,13 @@
         <v>2.5</v>
       </c>
       <c r="M62" t="n">
-        <v>5.517</v>
+        <v>5.317</v>
       </c>
       <c r="N62" t="n">
         <v>6.3</v>
       </c>
       <c r="O62" t="n">
-        <v>-12.017</v>
+        <v>-11.817</v>
       </c>
       <c r="P62" t="n">
         <v>-3.05</v>
@@ -3156,13 +3156,13 @@
         <v>2.5</v>
       </c>
       <c r="M63" t="n">
-        <v>18.117</v>
+        <v>17.917</v>
       </c>
       <c r="N63" t="n">
         <v>6.3</v>
       </c>
       <c r="O63" t="n">
-        <v>-22.817</v>
+        <v>-22.617</v>
       </c>
       <c r="P63" t="n">
         <v>-3.05</v>
@@ -3200,13 +3200,13 @@
         <v>2.5</v>
       </c>
       <c r="M64" t="n">
-        <v>18.117</v>
+        <v>17.917</v>
       </c>
       <c r="N64" t="n">
         <v>18.9</v>
       </c>
       <c r="O64" t="n">
-        <v>-21.017</v>
+        <v>-20.817</v>
       </c>
       <c r="P64" t="n">
         <v>-15.65</v>
@@ -3244,13 +3244,13 @@
         <v>1</v>
       </c>
       <c r="M65" t="n">
-        <v>5.517</v>
+        <v>5.317</v>
       </c>
       <c r="N65" t="n">
         <v>18.9</v>
       </c>
       <c r="O65" t="n">
-        <v>-15.617</v>
+        <v>-15.417</v>
       </c>
       <c r="P65" t="n">
         <v>-17.15</v>
@@ -3288,13 +3288,13 @@
         <v>1</v>
       </c>
       <c r="M66" t="n">
-        <v>5.517</v>
+        <v>5.317</v>
       </c>
       <c r="N66" t="n">
         <v>31.5</v>
       </c>
       <c r="O66" t="n">
-        <v>-13.817</v>
+        <v>-13.617</v>
       </c>
       <c r="P66" t="n">
         <v>-29.75</v>
@@ -3332,13 +3332,13 @@
         <v>1</v>
       </c>
       <c r="M67" t="n">
-        <v>5.517</v>
+        <v>5.317</v>
       </c>
       <c r="N67" t="n">
         <v>44.1</v>
       </c>
       <c r="O67" t="n">
-        <v>-12.017</v>
+        <v>-11.817</v>
       </c>
       <c r="P67" t="n">
         <v>-42.35</v>
@@ -3376,13 +3376,13 @@
         <v>1</v>
       </c>
       <c r="M68" t="n">
-        <v>18.117</v>
+        <v>17.917</v>
       </c>
       <c r="N68" t="n">
         <v>44.1</v>
       </c>
       <c r="O68" t="n">
-        <v>-22.817</v>
+        <v>-22.617</v>
       </c>
       <c r="P68" t="n">
         <v>-42.35</v>
@@ -3420,13 +3420,13 @@
         <v>1</v>
       </c>
       <c r="M69" t="n">
-        <v>18.117</v>
+        <v>17.917</v>
       </c>
       <c r="N69" t="n">
         <v>31.5</v>
       </c>
       <c r="O69" t="n">
-        <v>-21.017</v>
+        <v>-20.817</v>
       </c>
       <c r="P69" t="n">
         <v>-29.75</v>
@@ -3464,13 +3464,13 @@
         <v>-0.5</v>
       </c>
       <c r="M70" t="n">
-        <v>30.717</v>
+        <v>30.517</v>
       </c>
       <c r="N70" t="n">
         <v>31.5</v>
       </c>
       <c r="O70" t="n">
-        <v>-40.817</v>
+        <v>-40.617</v>
       </c>
       <c r="P70" t="n">
         <v>-31.25</v>
@@ -3508,13 +3508,13 @@
         <v>-0.5</v>
       </c>
       <c r="M71" t="n">
-        <v>30.717</v>
+        <v>30.517</v>
       </c>
       <c r="N71" t="n">
         <v>44.1</v>
       </c>
       <c r="O71" t="n">
-        <v>-39.017</v>
+        <v>-38.817</v>
       </c>
       <c r="P71" t="n">
         <v>-43.85</v>
@@ -3552,13 +3552,13 @@
         <v>-0.5</v>
       </c>
       <c r="M72" t="n">
-        <v>43.317</v>
+        <v>43.117</v>
       </c>
       <c r="N72" t="n">
         <v>44.1</v>
       </c>
       <c r="O72" t="n">
-        <v>-49.817</v>
+        <v>-49.617</v>
       </c>
       <c r="P72" t="n">
         <v>-43.85</v>
@@ -3596,13 +3596,13 @@
         <v>-0.5</v>
       </c>
       <c r="M73" t="n">
-        <v>43.317</v>
+        <v>43.117</v>
       </c>
       <c r="N73" t="n">
         <v>31.5</v>
       </c>
       <c r="O73" t="n">
-        <v>-48.017</v>
+        <v>-47.817</v>
       </c>
       <c r="P73" t="n">
         <v>-31.25</v>
@@ -3640,13 +3640,13 @@
         <v>-0.5</v>
       </c>
       <c r="M74" t="n">
-        <v>43.317</v>
+        <v>43.117</v>
       </c>
       <c r="N74" t="n">
         <v>18.9</v>
       </c>
       <c r="O74" t="n">
-        <v>-46.217</v>
+        <v>-46.017</v>
       </c>
       <c r="P74" t="n">
         <v>-18.65</v>
@@ -3684,13 +3684,13 @@
         <v>-2</v>
       </c>
       <c r="M75" t="n">
-        <v>30.717</v>
+        <v>30.517</v>
       </c>
       <c r="N75" t="n">
         <v>18.9</v>
       </c>
       <c r="O75" t="n">
-        <v>-40.817</v>
+        <v>-40.617</v>
       </c>
       <c r="P75" t="n">
         <v>-20.15</v>
@@ -3728,13 +3728,13 @@
         <v>-2</v>
       </c>
       <c r="M76" t="n">
-        <v>30.717</v>
+        <v>30.517</v>
       </c>
       <c r="N76" t="n">
         <v>6.3</v>
       </c>
       <c r="O76" t="n">
-        <v>-39.017</v>
+        <v>-38.817</v>
       </c>
       <c r="P76" t="n">
         <v>-7.55</v>
@@ -3772,13 +3772,13 @@
         <v>-2</v>
       </c>
       <c r="M77" t="n">
-        <v>43.317</v>
+        <v>43.117</v>
       </c>
       <c r="N77" t="n">
         <v>6.3</v>
       </c>
       <c r="O77" t="n">
-        <v>-49.817</v>
+        <v>-49.617</v>
       </c>
       <c r="P77" t="n">
         <v>-7.55</v>
@@ -3816,13 +3816,13 @@
         <v>-2</v>
       </c>
       <c r="M78" t="n">
-        <v>43.317</v>
+        <v>43.117</v>
       </c>
       <c r="N78" t="n">
         <v>-6.3</v>
       </c>
       <c r="O78" t="n">
-        <v>-48.017</v>
+        <v>-47.817</v>
       </c>
       <c r="P78" t="n">
         <v>5.05</v>
@@ -3860,13 +3860,13 @@
         <v>-2</v>
       </c>
       <c r="M79" t="n">
-        <v>43.317</v>
+        <v>43.117</v>
       </c>
       <c r="N79" t="n">
         <v>-18.9</v>
       </c>
       <c r="O79" t="n">
-        <v>-46.217</v>
+        <v>-46.017</v>
       </c>
       <c r="P79" t="n">
         <v>17.65</v>
@@ -3904,13 +3904,13 @@
         <v>-3.5</v>
       </c>
       <c r="M80" t="n">
-        <v>30.717</v>
+        <v>30.517</v>
       </c>
       <c r="N80" t="n">
         <v>-18.9</v>
       </c>
       <c r="O80" t="n">
-        <v>-40.817</v>
+        <v>-40.617</v>
       </c>
       <c r="P80" t="n">
         <v>16.15</v>
@@ -3948,13 +3948,13 @@
         <v>-3.5</v>
       </c>
       <c r="M81" t="n">
-        <v>30.717</v>
+        <v>30.517</v>
       </c>
       <c r="N81" t="n">
         <v>-6.3</v>
       </c>
       <c r="O81" t="n">
-        <v>-39.017</v>
+        <v>-38.817</v>
       </c>
       <c r="P81" t="n">
         <v>3.55</v>
@@ -3992,13 +3992,13 @@
         <v>-3.5</v>
       </c>
       <c r="M82" t="n">
-        <v>18.117</v>
+        <v>17.917</v>
       </c>
       <c r="N82" t="n">
         <v>-6.3</v>
       </c>
       <c r="O82" t="n">
-        <v>-24.617</v>
+        <v>-24.417</v>
       </c>
       <c r="P82" t="n">
         <v>3.55</v>
@@ -4036,13 +4036,13 @@
         <v>-3.5</v>
       </c>
       <c r="M83" t="n">
-        <v>5.517</v>
+        <v>5.317</v>
       </c>
       <c r="N83" t="n">
         <v>-6.3</v>
       </c>
       <c r="O83" t="n">
-        <v>-10.217</v>
+        <v>-10.017</v>
       </c>
       <c r="P83" t="n">
         <v>3.55</v>
@@ -4080,13 +4080,13 @@
         <v>-3.5</v>
       </c>
       <c r="M84" t="n">
-        <v>5.517</v>
+        <v>5.317</v>
       </c>
       <c r="N84" t="n">
         <v>-18.9</v>
       </c>
       <c r="O84" t="n">
-        <v>-8.417</v>
+        <v>-8.217000000000001</v>
       </c>
       <c r="P84" t="n">
         <v>16.15</v>
@@ -4124,13 +4124,13 @@
         <v>-5</v>
       </c>
       <c r="M85" t="n">
-        <v>18.117</v>
+        <v>17.917</v>
       </c>
       <c r="N85" t="n">
         <v>-18.9</v>
       </c>
       <c r="O85" t="n">
-        <v>-28.217</v>
+        <v>-28.017</v>
       </c>
       <c r="P85" t="n">
         <v>14.65</v>
@@ -4168,13 +4168,13 @@
         <v>-5</v>
       </c>
       <c r="M86" t="n">
-        <v>18.117</v>
+        <v>17.917</v>
       </c>
       <c r="N86" t="n">
         <v>-31.5</v>
       </c>
       <c r="O86" t="n">
-        <v>-26.417</v>
+        <v>-26.217</v>
       </c>
       <c r="P86" t="n">
         <v>27.25</v>
@@ -4212,13 +4212,13 @@
         <v>-5</v>
       </c>
       <c r="M87" t="n">
-        <v>5.517</v>
+        <v>5.317</v>
       </c>
       <c r="N87" t="n">
         <v>-31.5</v>
       </c>
       <c r="O87" t="n">
-        <v>-12.017</v>
+        <v>-11.817</v>
       </c>
       <c r="P87" t="n">
         <v>27.25</v>
@@ -4256,13 +4256,13 @@
         <v>-5</v>
       </c>
       <c r="M88" t="n">
-        <v>5.517</v>
+        <v>5.317</v>
       </c>
       <c r="N88" t="n">
         <v>-44.1</v>
       </c>
       <c r="O88" t="n">
-        <v>-10.217</v>
+        <v>-10.017</v>
       </c>
       <c r="P88" t="n">
         <v>39.85</v>
@@ -4300,13 +4300,13 @@
         <v>-5</v>
       </c>
       <c r="M89" t="n">
-        <v>18.117</v>
+        <v>17.917</v>
       </c>
       <c r="N89" t="n">
         <v>-44.1</v>
       </c>
       <c r="O89" t="n">
-        <v>-21.017</v>
+        <v>-20.817</v>
       </c>
       <c r="P89" t="n">
         <v>39.85</v>
@@ -4344,13 +4344,13 @@
         <v>-6.5</v>
       </c>
       <c r="M90" t="n">
-        <v>30.717</v>
+        <v>30.517</v>
       </c>
       <c r="N90" t="n">
         <v>-44.1</v>
       </c>
       <c r="O90" t="n">
-        <v>-40.817</v>
+        <v>-40.617</v>
       </c>
       <c r="P90" t="n">
         <v>38.35</v>
@@ -4388,13 +4388,13 @@
         <v>-6.5</v>
       </c>
       <c r="M91" t="n">
-        <v>30.717</v>
+        <v>30.517</v>
       </c>
       <c r="N91" t="n">
         <v>-31.5</v>
       </c>
       <c r="O91" t="n">
-        <v>-39.017</v>
+        <v>-38.817</v>
       </c>
       <c r="P91" t="n">
         <v>25.75</v>
@@ -4432,13 +4432,13 @@
         <v>-6.5</v>
       </c>
       <c r="M92" t="n">
-        <v>43.317</v>
+        <v>43.117</v>
       </c>
       <c r="N92" t="n">
         <v>-31.5</v>
       </c>
       <c r="O92" t="n">
-        <v>-49.817</v>
+        <v>-49.617</v>
       </c>
       <c r="P92" t="n">
         <v>25.75</v>
@@ -4476,13 +4476,13 @@
         <v>-6.5</v>
       </c>
       <c r="M93" t="n">
-        <v>43.317</v>
+        <v>43.117</v>
       </c>
       <c r="N93" t="n">
         <v>-44.1</v>
       </c>
       <c r="O93" t="n">
-        <v>-48.017</v>
+        <v>-47.817</v>
       </c>
       <c r="P93" t="n">
         <v>38.35</v>
@@ -4496,7 +4496,7 @@
         <v>92</v>
       </c>
       <c r="D94" t="n">
-        <v>-1.05</v>
+        <v>-1.25</v>
       </c>
       <c r="E94" t="n">
         <v>0.05</v>
@@ -4508,10 +4508,10 @@
         <v>1.2</v>
       </c>
       <c r="H94" t="n">
-        <v>-1.7</v>
+        <v>-1.9</v>
       </c>
       <c r="I94" t="n">
-        <v>-0.4</v>
+        <v>-0.6</v>
       </c>
       <c r="J94" t="n">
         <v>0.65</v>
@@ -4520,13 +4520,13 @@
         <v>-0.5499999999999999</v>
       </c>
       <c r="M94" t="n">
-        <v>-44.125</v>
+        <v>-44.52500000000001</v>
       </c>
       <c r="N94" t="n">
         <v>-44.1</v>
       </c>
       <c r="O94" t="n">
-        <v>43.075</v>
+        <v>43.27500000000001</v>
       </c>
       <c r="P94" t="n">
         <v>44.15</v>
@@ -4538,7 +4538,7 @@
         <v>8</v>
       </c>
       <c r="V94" t="n">
-        <v>-44.125</v>
+        <v>-44.52500000000001</v>
       </c>
       <c r="W94" t="n">
         <v>-44.1</v>
@@ -4558,7 +4558,7 @@
         <v>93</v>
       </c>
       <c r="D95" t="n">
-        <v>4.3</v>
+        <v>4.5</v>
       </c>
       <c r="E95" t="n">
         <v>2.35</v>
@@ -4570,10 +4570,10 @@
         <v>0.8</v>
       </c>
       <c r="H95" t="n">
-        <v>3.9</v>
+        <v>4.1</v>
       </c>
       <c r="I95" t="n">
-        <v>4.7</v>
+        <v>4.9</v>
       </c>
       <c r="J95" t="n">
         <v>2.75</v>
@@ -4588,7 +4588,7 @@
         <v>7.059</v>
       </c>
       <c r="O95" t="n">
-        <v>-44.95</v>
+        <v>-44.75</v>
       </c>
       <c r="P95" t="n">
         <v>-4.709</v>
@@ -4602,7 +4602,7 @@
         <v>93</v>
       </c>
       <c r="D96" t="n">
-        <v>4.3</v>
+        <v>4.5</v>
       </c>
       <c r="E96" t="n">
         <v>2.35</v>
@@ -4614,10 +4614,10 @@
         <v>0.8</v>
       </c>
       <c r="H96" t="n">
-        <v>3.9</v>
+        <v>4.1</v>
       </c>
       <c r="I96" t="n">
-        <v>4.7</v>
+        <v>4.9</v>
       </c>
       <c r="J96" t="n">
         <v>2.75</v>
@@ -4632,7 +4632,7 @@
         <v>-5.141</v>
       </c>
       <c r="O96" t="n">
-        <v>-44.95</v>
+        <v>-44.75</v>
       </c>
       <c r="P96" t="n">
         <v>7.491</v>
@@ -4652,16 +4652,16 @@
         <v>0</v>
       </c>
       <c r="F97" t="n">
-        <v>0.8</v>
+        <v>1.2</v>
       </c>
       <c r="G97" t="n">
         <v>1.3</v>
       </c>
       <c r="H97" t="n">
-        <v>-0.4</v>
+        <v>-0.6</v>
       </c>
       <c r="I97" t="n">
-        <v>0.4</v>
+        <v>0.6</v>
       </c>
       <c r="J97" t="n">
         <v>0.65</v>
@@ -4708,7 +4708,7 @@
         <v>96</v>
       </c>
       <c r="D98" t="n">
-        <v>2.5</v>
+        <v>2.7</v>
       </c>
       <c r="E98" t="n">
         <v>2.35</v>
@@ -4720,10 +4720,10 @@
         <v>0.8</v>
       </c>
       <c r="H98" t="n">
-        <v>2.1</v>
+        <v>2.3</v>
       </c>
       <c r="I98" t="n">
-        <v>2.9</v>
+        <v>3.1</v>
       </c>
       <c r="J98" t="n">
         <v>2.75</v>
@@ -4738,7 +4738,7 @@
         <v>7.059</v>
       </c>
       <c r="O98" t="n">
-        <v>-46.75</v>
+        <v>-46.55</v>
       </c>
       <c r="P98" t="n">
         <v>-4.709</v>
@@ -4752,7 +4752,7 @@
         <v>96</v>
       </c>
       <c r="D99" t="n">
-        <v>2.5</v>
+        <v>2.7</v>
       </c>
       <c r="E99" t="n">
         <v>2.35</v>
@@ -4764,10 +4764,10 @@
         <v>0.8</v>
       </c>
       <c r="H99" t="n">
-        <v>2.1</v>
+        <v>2.3</v>
       </c>
       <c r="I99" t="n">
-        <v>2.9</v>
+        <v>3.1</v>
       </c>
       <c r="J99" t="n">
         <v>2.75</v>
@@ -4782,7 +4782,7 @@
         <v>-5.141</v>
       </c>
       <c r="O99" t="n">
-        <v>-46.75</v>
+        <v>-46.55</v>
       </c>
       <c r="P99" t="n">
         <v>7.491</v>
@@ -4796,7 +4796,7 @@
         <v>97</v>
       </c>
       <c r="D100" t="n">
-        <v>0.6</v>
+        <v>0.8</v>
       </c>
       <c r="E100" t="n">
         <v>-0.25</v>
@@ -4808,10 +4808,10 @@
         <v>0.8</v>
       </c>
       <c r="H100" t="n">
-        <v>0.4</v>
+        <v>0.6000000000000001</v>
       </c>
       <c r="I100" t="n">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="J100" t="n">
         <v>0.15</v>
@@ -4820,13 +4820,13 @@
         <v>-0.65</v>
       </c>
       <c r="M100" t="n">
-        <v>-44.25</v>
+        <v>-44.45</v>
       </c>
       <c r="N100" t="n">
         <v>-43.344</v>
       </c>
       <c r="O100" t="n">
-        <v>44.85</v>
+        <v>45.25</v>
       </c>
       <c r="P100" t="n">
         <v>43.094</v>
@@ -4838,7 +4838,7 @@
         <v>8</v>
       </c>
       <c r="V100" t="n">
-        <v>-44.25</v>
+        <v>-44.45</v>
       </c>
       <c r="W100" t="n">
         <v>-43.344</v>
@@ -4858,7 +4858,7 @@
         <v>98</v>
       </c>
       <c r="D101" t="n">
-        <v>1</v>
+        <v>1.2</v>
       </c>
       <c r="E101" t="n">
         <v>-0.15</v>
@@ -4870,10 +4870,10 @@
         <v>0.6</v>
       </c>
       <c r="H101" t="n">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="I101" t="n">
-        <v>1.2</v>
+        <v>1.4</v>
       </c>
       <c r="J101" t="n">
         <v>0.15</v>
@@ -4882,13 +4882,13 @@
         <v>-0.45</v>
       </c>
       <c r="M101" t="n">
-        <v>-44.25</v>
+        <v>-44.45</v>
       </c>
       <c r="N101" t="n">
         <v>-44.754</v>
       </c>
       <c r="O101" t="n">
-        <v>45.25</v>
+        <v>45.65000000000001</v>
       </c>
       <c r="P101" t="n">
         <v>44.604</v>
@@ -4900,7 +4900,7 @@
         <v>8</v>
       </c>
       <c r="V101" t="n">
-        <v>-44.25</v>
+        <v>-44.45</v>
       </c>
       <c r="W101" t="n">
         <v>-44.754</v>
@@ -4920,7 +4920,7 @@
         <v>99</v>
       </c>
       <c r="D102" t="n">
-        <v>1.3</v>
+        <v>1.5</v>
       </c>
       <c r="E102" t="n">
         <v>0.45</v>
@@ -4932,10 +4932,10 @@
         <v>0.4</v>
       </c>
       <c r="H102" t="n">
-        <v>1.1</v>
+        <v>1.3</v>
       </c>
       <c r="I102" t="n">
-        <v>1.5</v>
+        <v>1.7</v>
       </c>
       <c r="J102" t="n">
         <v>0.65</v>
@@ -4950,7 +4950,7 @@
         <v>-24.241</v>
       </c>
       <c r="O102" t="n">
-        <v>48.55</v>
+        <v>48.75</v>
       </c>
       <c r="P102" t="n">
         <v>24.691</v>
@@ -4982,7 +4982,7 @@
         <v>99</v>
       </c>
       <c r="D103" t="n">
-        <v>1.3</v>
+        <v>1.5</v>
       </c>
       <c r="E103" t="n">
         <v>0.45</v>
@@ -4994,10 +4994,10 @@
         <v>0.4</v>
       </c>
       <c r="H103" t="n">
-        <v>1.1</v>
+        <v>1.3</v>
       </c>
       <c r="I103" t="n">
-        <v>1.5</v>
+        <v>1.7</v>
       </c>
       <c r="J103" t="n">
         <v>0.65</v>
@@ -5012,7 +5012,7 @@
         <v>-49.441</v>
       </c>
       <c r="O103" t="n">
-        <v>48.55</v>
+        <v>48.75</v>
       </c>
       <c r="P103" t="n">
         <v>49.89100000000001</v>
@@ -5044,7 +5044,7 @@
         <v>99</v>
       </c>
       <c r="D104" t="n">
-        <v>1.3</v>
+        <v>1.5</v>
       </c>
       <c r="E104" t="n">
         <v>0.45</v>
@@ -5056,10 +5056,10 @@
         <v>0.4</v>
       </c>
       <c r="H104" t="n">
-        <v>1.1</v>
+        <v>1.3</v>
       </c>
       <c r="I104" t="n">
-        <v>1.5</v>
+        <v>1.7</v>
       </c>
       <c r="J104" t="n">
         <v>0.65</v>
@@ -5074,7 +5074,7 @@
         <v>-11.641</v>
       </c>
       <c r="O104" t="n">
-        <v>-45.95</v>
+        <v>-45.75</v>
       </c>
       <c r="P104" t="n">
         <v>12.091</v>
@@ -5106,7 +5106,7 @@
         <v>99</v>
       </c>
       <c r="D105" t="n">
-        <v>1.3</v>
+        <v>1.5</v>
       </c>
       <c r="E105" t="n">
         <v>0.45</v>
@@ -5118,10 +5118,10 @@
         <v>0.4</v>
       </c>
       <c r="H105" t="n">
-        <v>1.1</v>
+        <v>1.3</v>
       </c>
       <c r="I105" t="n">
-        <v>1.5</v>
+        <v>1.7</v>
       </c>
       <c r="J105" t="n">
         <v>0.65</v>
@@ -5136,7 +5136,7 @@
         <v>-36.841</v>
       </c>
       <c r="O105" t="n">
-        <v>-45.95</v>
+        <v>-45.75</v>
       </c>
       <c r="P105" t="n">
         <v>37.291</v>
@@ -5168,7 +5168,7 @@
         <v>99</v>
       </c>
       <c r="D106" t="n">
-        <v>1.3</v>
+        <v>1.5</v>
       </c>
       <c r="E106" t="n">
         <v>0.45</v>
@@ -5180,10 +5180,10 @@
         <v>0.4</v>
       </c>
       <c r="H106" t="n">
-        <v>1.1</v>
+        <v>1.3</v>
       </c>
       <c r="I106" t="n">
-        <v>1.5</v>
+        <v>1.7</v>
       </c>
       <c r="J106" t="n">
         <v>0.65</v>
@@ -5198,7 +5198,7 @@
         <v>45.059</v>
       </c>
       <c r="O106" t="n">
-        <v>-49.9</v>
+        <v>-49.7</v>
       </c>
       <c r="P106" t="n">
         <v>-44.60899999999999</v>
@@ -5212,7 +5212,7 @@
         <v>99</v>
       </c>
       <c r="D107" t="n">
-        <v>1.3</v>
+        <v>1.5</v>
       </c>
       <c r="E107" t="n">
         <v>0.45</v>
@@ -5224,10 +5224,10 @@
         <v>0.4</v>
       </c>
       <c r="H107" t="n">
-        <v>1.1</v>
+        <v>1.3</v>
       </c>
       <c r="I107" t="n">
-        <v>1.5</v>
+        <v>1.7</v>
       </c>
       <c r="J107" t="n">
         <v>0.65</v>
@@ -5242,7 +5242,7 @@
         <v>-43.141</v>
       </c>
       <c r="O107" t="n">
-        <v>-49.9</v>
+        <v>-49.7</v>
       </c>
       <c r="P107" t="n">
         <v>43.591</v>
@@ -5442,7 +5442,7 @@
         <v>101</v>
       </c>
       <c r="D111" t="n">
-        <v>2.5</v>
+        <v>2.7</v>
       </c>
       <c r="E111" t="n">
         <v>1.75</v>
@@ -5454,10 +5454,10 @@
         <v>0.4</v>
       </c>
       <c r="H111" t="n">
-        <v>2.25</v>
+        <v>2.45</v>
       </c>
       <c r="I111" t="n">
-        <v>2.75</v>
+        <v>2.95</v>
       </c>
       <c r="J111" t="n">
         <v>1.95</v>
@@ -5472,7 +5472,7 @@
         <v>45.059</v>
       </c>
       <c r="O111" t="n">
-        <v>-44.8</v>
+        <v>-44.59999999999999</v>
       </c>
       <c r="P111" t="n">
         <v>-43.309</v>
@@ -5504,7 +5504,7 @@
         <v>101</v>
       </c>
       <c r="D112" t="n">
-        <v>2.5</v>
+        <v>2.7</v>
       </c>
       <c r="E112" t="n">
         <v>1.75</v>
@@ -5516,10 +5516,10 @@
         <v>0.4</v>
       </c>
       <c r="H112" t="n">
-        <v>2.25</v>
+        <v>2.45</v>
       </c>
       <c r="I112" t="n">
-        <v>2.75</v>
+        <v>2.95</v>
       </c>
       <c r="J112" t="n">
         <v>1.95</v>
@@ -5534,7 +5534,7 @@
         <v>-43.141</v>
       </c>
       <c r="O112" t="n">
-        <v>-44.8</v>
+        <v>-44.59999999999999</v>
       </c>
       <c r="P112" t="n">
         <v>44.891</v>
@@ -5690,7 +5690,7 @@
         <v>104</v>
       </c>
       <c r="D115" t="n">
-        <v>1.7</v>
+        <v>1.9</v>
       </c>
       <c r="E115" t="n">
         <v>0.45</v>
@@ -5702,10 +5702,10 @@
         <v>0.4</v>
       </c>
       <c r="H115" t="n">
-        <v>1.5</v>
+        <v>1.7</v>
       </c>
       <c r="I115" t="n">
-        <v>1.9</v>
+        <v>2.1</v>
       </c>
       <c r="J115" t="n">
         <v>0.65</v>
@@ -5720,7 +5720,7 @@
         <v>-24.241</v>
       </c>
       <c r="O115" t="n">
-        <v>48.95</v>
+        <v>49.15</v>
       </c>
       <c r="P115" t="n">
         <v>24.691</v>
@@ -5752,7 +5752,7 @@
         <v>104</v>
       </c>
       <c r="D116" t="n">
-        <v>1.7</v>
+        <v>1.9</v>
       </c>
       <c r="E116" t="n">
         <v>0.45</v>
@@ -5764,10 +5764,10 @@
         <v>0.4</v>
       </c>
       <c r="H116" t="n">
-        <v>1.5</v>
+        <v>1.7</v>
       </c>
       <c r="I116" t="n">
-        <v>1.9</v>
+        <v>2.1</v>
       </c>
       <c r="J116" t="n">
         <v>0.65</v>
@@ -5782,7 +5782,7 @@
         <v>-49.441</v>
       </c>
       <c r="O116" t="n">
-        <v>48.95</v>
+        <v>49.15</v>
       </c>
       <c r="P116" t="n">
         <v>49.89100000000001</v>
@@ -5814,7 +5814,7 @@
         <v>104</v>
       </c>
       <c r="D117" t="n">
-        <v>1.7</v>
+        <v>1.9</v>
       </c>
       <c r="E117" t="n">
         <v>0.45</v>
@@ -5826,10 +5826,10 @@
         <v>0.4</v>
       </c>
       <c r="H117" t="n">
-        <v>1.5</v>
+        <v>1.7</v>
       </c>
       <c r="I117" t="n">
-        <v>1.9</v>
+        <v>2.1</v>
       </c>
       <c r="J117" t="n">
         <v>0.65</v>
@@ -5844,7 +5844,7 @@
         <v>-11.641</v>
       </c>
       <c r="O117" t="n">
-        <v>-45.55</v>
+        <v>-45.35</v>
       </c>
       <c r="P117" t="n">
         <v>12.091</v>
@@ -5876,7 +5876,7 @@
         <v>104</v>
       </c>
       <c r="D118" t="n">
-        <v>1.7</v>
+        <v>1.9</v>
       </c>
       <c r="E118" t="n">
         <v>0.45</v>
@@ -5888,10 +5888,10 @@
         <v>0.4</v>
       </c>
       <c r="H118" t="n">
-        <v>1.5</v>
+        <v>1.7</v>
       </c>
       <c r="I118" t="n">
-        <v>1.9</v>
+        <v>2.1</v>
       </c>
       <c r="J118" t="n">
         <v>0.65</v>
@@ -5906,7 +5906,7 @@
         <v>-36.841</v>
       </c>
       <c r="O118" t="n">
-        <v>-45.55</v>
+        <v>-45.35</v>
       </c>
       <c r="P118" t="n">
         <v>37.291</v>
@@ -5938,7 +5938,7 @@
         <v>104</v>
       </c>
       <c r="D119" t="n">
-        <v>1.7</v>
+        <v>1.9</v>
       </c>
       <c r="E119" t="n">
         <v>0.45</v>
@@ -5950,10 +5950,10 @@
         <v>0.4</v>
       </c>
       <c r="H119" t="n">
-        <v>1.5</v>
+        <v>1.7</v>
       </c>
       <c r="I119" t="n">
-        <v>1.9</v>
+        <v>2.1</v>
       </c>
       <c r="J119" t="n">
         <v>0.65</v>
@@ -5968,7 +5968,7 @@
         <v>45.059</v>
       </c>
       <c r="O119" t="n">
-        <v>-49.49999999999999</v>
+        <v>-49.3</v>
       </c>
       <c r="P119" t="n">
         <v>-44.60899999999999</v>
@@ -5982,7 +5982,7 @@
         <v>104</v>
       </c>
       <c r="D120" t="n">
-        <v>1.7</v>
+        <v>1.9</v>
       </c>
       <c r="E120" t="n">
         <v>0.45</v>
@@ -5994,10 +5994,10 @@
         <v>0.4</v>
       </c>
       <c r="H120" t="n">
-        <v>1.5</v>
+        <v>1.7</v>
       </c>
       <c r="I120" t="n">
-        <v>1.9</v>
+        <v>2.1</v>
       </c>
       <c r="J120" t="n">
         <v>0.65</v>
@@ -6012,7 +6012,7 @@
         <v>-43.141</v>
       </c>
       <c r="O120" t="n">
-        <v>-49.49999999999999</v>
+        <v>-49.3</v>
       </c>
       <c r="P120" t="n">
         <v>43.591</v>
@@ -6026,7 +6026,7 @@
         <v>105</v>
       </c>
       <c r="D121" t="n">
-        <v>3.4</v>
+        <v>3.6</v>
       </c>
       <c r="E121" t="n">
         <v>2.35</v>
@@ -6038,10 +6038,10 @@
         <v>0.8</v>
       </c>
       <c r="H121" t="n">
-        <v>3</v>
+        <v>3.2</v>
       </c>
       <c r="I121" t="n">
-        <v>3.8</v>
+        <v>4</v>
       </c>
       <c r="J121" t="n">
         <v>2.75</v>
@@ -6056,7 +6056,7 @@
         <v>7.059</v>
       </c>
       <c r="O121" t="n">
-        <v>-45.85</v>
+        <v>-45.65</v>
       </c>
       <c r="P121" t="n">
         <v>-4.709</v>
@@ -6070,7 +6070,7 @@
         <v>105</v>
       </c>
       <c r="D122" t="n">
-        <v>3.4</v>
+        <v>3.6</v>
       </c>
       <c r="E122" t="n">
         <v>2.35</v>
@@ -6082,10 +6082,10 @@
         <v>0.8</v>
       </c>
       <c r="H122" t="n">
-        <v>3</v>
+        <v>3.2</v>
       </c>
       <c r="I122" t="n">
-        <v>3.8</v>
+        <v>4</v>
       </c>
       <c r="J122" t="n">
         <v>2.75</v>
@@ -6100,7 +6100,7 @@
         <v>-5.141</v>
       </c>
       <c r="O122" t="n">
-        <v>-45.85</v>
+        <v>-45.65</v>
       </c>
       <c r="P122" t="n">
         <v>7.491</v>
@@ -6300,7 +6300,7 @@
         <v>107</v>
       </c>
       <c r="D126" t="n">
-        <v>3.4</v>
+        <v>3.6</v>
       </c>
       <c r="E126" t="n">
         <v>1.75</v>
@@ -6312,10 +6312,10 @@
         <v>0.4</v>
       </c>
       <c r="H126" t="n">
-        <v>3.15</v>
+        <v>3.35</v>
       </c>
       <c r="I126" t="n">
-        <v>3.65</v>
+        <v>3.85</v>
       </c>
       <c r="J126" t="n">
         <v>1.95</v>
@@ -6330,7 +6330,7 @@
         <v>45.059</v>
       </c>
       <c r="O126" t="n">
-        <v>-43.9</v>
+        <v>-43.7</v>
       </c>
       <c r="P126" t="n">
         <v>-43.309</v>
@@ -6362,7 +6362,7 @@
         <v>107</v>
       </c>
       <c r="D127" t="n">
-        <v>3.4</v>
+        <v>3.6</v>
       </c>
       <c r="E127" t="n">
         <v>1.75</v>
@@ -6374,10 +6374,10 @@
         <v>0.4</v>
       </c>
       <c r="H127" t="n">
-        <v>3.15</v>
+        <v>3.35</v>
       </c>
       <c r="I127" t="n">
-        <v>3.65</v>
+        <v>3.85</v>
       </c>
       <c r="J127" t="n">
         <v>1.95</v>
@@ -6392,7 +6392,7 @@
         <v>-43.141</v>
       </c>
       <c r="O127" t="n">
-        <v>-43.9</v>
+        <v>-43.7</v>
       </c>
       <c r="P127" t="n">
         <v>44.891</v>

</xml_diff>

<commit_message>
restructuring the line to the bondpads
</commit_message>
<xml_diff>
--- a/masks/code/ResonatorArray.xlsx
+++ b/masks/code/ResonatorArray.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="111">
   <si>
     <t>Alternate Array Layout</t>
   </si>
@@ -308,6 +308,12 @@
     <t>Cap_to_Ind_lines</t>
   </si>
   <si>
+    <t>GP_edge_filler_hor</t>
+  </si>
+  <si>
+    <t>GP_edge_filler_vert</t>
+  </si>
+  <si>
     <t>MSfeed_bondpad</t>
   </si>
   <si>
@@ -332,10 +338,10 @@
     <t>ILD</t>
   </si>
   <si>
-    <t>GP_edge_opening_hor</t>
-  </si>
-  <si>
-    <t>GP_edge_opening_vert</t>
+    <t>GP_edge_opening_hor_r</t>
+  </si>
+  <si>
+    <t>GP_edge_opening_vert_r</t>
   </si>
   <si>
     <t>Via_to_Ground</t>
@@ -677,7 +683,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A12:Y103"/>
+  <dimension ref="A12:Y105"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -848,7 +854,7 @@
         <v>21</v>
       </c>
       <c r="D16" t="n">
-        <v>-3.05</v>
+        <v>-11.05</v>
       </c>
       <c r="E16" t="n">
         <v>-10.4</v>
@@ -860,10 +866,10 @@
         <v>0.5</v>
       </c>
       <c r="H16" t="n">
-        <v>-3.5</v>
+        <v>-11.5</v>
       </c>
       <c r="I16" t="n">
-        <v>-2.6</v>
+        <v>-10.6</v>
       </c>
       <c r="J16" t="n">
         <v>-10.15</v>
@@ -878,7 +884,7 @@
         <v>0</v>
       </c>
       <c r="O16" t="n">
-        <v>-0.395</v>
+        <v>-8.395000000000001</v>
       </c>
       <c r="P16" t="n">
         <v>-10.4</v>
@@ -972,22 +978,22 @@
         <v>24</v>
       </c>
       <c r="D18" t="n">
-        <v>-7.4</v>
+        <v>-1.4</v>
       </c>
       <c r="E18" t="n">
         <v>-0.9</v>
       </c>
       <c r="F18" t="n">
-        <v>2.4</v>
+        <v>6.4</v>
       </c>
       <c r="G18" t="n">
         <v>22.4</v>
       </c>
       <c r="H18" t="n">
-        <v>-8.6</v>
+        <v>-4.6</v>
       </c>
       <c r="I18" t="n">
-        <v>-6.2</v>
+        <v>1.8</v>
       </c>
       <c r="J18" t="n">
         <v>10.3</v>
@@ -1002,7 +1008,7 @@
         <v>0</v>
       </c>
       <c r="O18" t="n">
-        <v>-7.4</v>
+        <v>-1.4</v>
       </c>
       <c r="P18" t="n">
         <v>-0.9</v>
@@ -1016,7 +1022,7 @@
         <v>25</v>
       </c>
       <c r="D19" t="n">
-        <v>3.1</v>
+        <v>-4.9</v>
       </c>
       <c r="E19" t="n">
         <v>-11.05</v>
@@ -1028,10 +1034,10 @@
         <v>2.1</v>
       </c>
       <c r="H19" t="n">
-        <v>0.8999999999999999</v>
+        <v>-7.100000000000001</v>
       </c>
       <c r="I19" t="n">
-        <v>5.300000000000001</v>
+        <v>-2.7</v>
       </c>
       <c r="J19" t="n">
         <v>-10</v>
@@ -1046,7 +1052,7 @@
         <v>0</v>
       </c>
       <c r="O19" t="n">
-        <v>3.1</v>
+        <v>-4.9</v>
       </c>
       <c r="P19" t="n">
         <v>-11.05</v>
@@ -1078,22 +1084,22 @@
         <v>26</v>
       </c>
       <c r="D20" t="n">
-        <v>7.4</v>
+        <v>1.4</v>
       </c>
       <c r="E20" t="n">
         <v>-0.9</v>
       </c>
       <c r="F20" t="n">
-        <v>2.4</v>
+        <v>6.4</v>
       </c>
       <c r="G20" t="n">
         <v>22.4</v>
       </c>
       <c r="H20" t="n">
-        <v>6.2</v>
+        <v>-1.8</v>
       </c>
       <c r="I20" t="n">
-        <v>8.6</v>
+        <v>4.6</v>
       </c>
       <c r="J20" t="n">
         <v>10.3</v>
@@ -1108,7 +1114,7 @@
         <v>0</v>
       </c>
       <c r="O20" t="n">
-        <v>7.4</v>
+        <v>1.4</v>
       </c>
       <c r="P20" t="n">
         <v>-0.9</v>
@@ -1122,7 +1128,7 @@
         <v>27</v>
       </c>
       <c r="D21" t="n">
-        <v>-5.6</v>
+        <v>2.4</v>
       </c>
       <c r="E21" t="n">
         <v>-6.4</v>
@@ -1134,10 +1140,10 @@
         <v>11.4</v>
       </c>
       <c r="H21" t="n">
-        <v>-5.8</v>
+        <v>2.2</v>
       </c>
       <c r="I21" t="n">
-        <v>-5.399999999999999</v>
+        <v>2.6</v>
       </c>
       <c r="J21" t="n">
         <v>-0.7000000000000002</v>
@@ -1152,7 +1158,7 @@
         <v>0</v>
       </c>
       <c r="O21" t="n">
-        <v>-5.6</v>
+        <v>2.4</v>
       </c>
       <c r="P21" t="n">
         <v>-6.4</v>
@@ -1184,7 +1190,7 @@
         <v>27</v>
       </c>
       <c r="D22" t="n">
-        <v>-5.6</v>
+        <v>2.4</v>
       </c>
       <c r="E22" t="n">
         <v>-6.4</v>
@@ -1196,10 +1202,10 @@
         <v>11.4</v>
       </c>
       <c r="H22" t="n">
-        <v>-5.8</v>
+        <v>2.2</v>
       </c>
       <c r="I22" t="n">
-        <v>-5.399999999999999</v>
+        <v>2.6</v>
       </c>
       <c r="J22" t="n">
         <v>-0.7000000000000002</v>
@@ -1214,7 +1220,7 @@
         <v>0</v>
       </c>
       <c r="O22" t="n">
-        <v>-5.6</v>
+        <v>2.4</v>
       </c>
       <c r="P22" t="n">
         <v>-6.4</v>
@@ -4124,7 +4130,7 @@
         <v>94</v>
       </c>
       <c r="D88" t="n">
-        <v>-3</v>
+        <v>-11</v>
       </c>
       <c r="E88" t="n">
         <v>-11.45</v>
@@ -4136,10 +4142,10 @@
         <v>0.8</v>
       </c>
       <c r="H88" t="n">
-        <v>-3.4</v>
+        <v>-11.4</v>
       </c>
       <c r="I88" t="n">
-        <v>-2.6</v>
+        <v>-10.6</v>
       </c>
       <c r="J88" t="n">
         <v>-11.05</v>
@@ -4154,7 +4160,7 @@
         <v>0</v>
       </c>
       <c r="O88" t="n">
-        <v>-3</v>
+        <v>-11</v>
       </c>
       <c r="P88" t="n">
         <v>-11.45</v>
@@ -4168,7 +4174,7 @@
         <v>94</v>
       </c>
       <c r="D89" t="n">
-        <v>-3</v>
+        <v>-11</v>
       </c>
       <c r="E89" t="n">
         <v>-11.45</v>
@@ -4180,10 +4186,10 @@
         <v>0.8</v>
       </c>
       <c r="H89" t="n">
-        <v>-3.4</v>
+        <v>-11.4</v>
       </c>
       <c r="I89" t="n">
-        <v>-2.6</v>
+        <v>-10.6</v>
       </c>
       <c r="J89" t="n">
         <v>-11.05</v>
@@ -4198,7 +4204,7 @@
         <v>0</v>
       </c>
       <c r="O89" t="n">
-        <v>-3</v>
+        <v>-11</v>
       </c>
       <c r="P89" t="n">
         <v>-11.45</v>
@@ -4274,28 +4280,28 @@
         <v>97</v>
       </c>
       <c r="D91" t="n">
-        <v>-3.8</v>
+        <v>0</v>
       </c>
       <c r="E91" t="n">
-        <v>-11.45</v>
+        <v>11.55</v>
       </c>
       <c r="F91" t="n">
-        <v>0.8</v>
+        <v>16.9</v>
       </c>
       <c r="G91" t="n">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
       <c r="H91" t="n">
-        <v>-4.2</v>
+        <v>-8.449999999999999</v>
       </c>
       <c r="I91" t="n">
-        <v>-3.4</v>
+        <v>8.449999999999999</v>
       </c>
       <c r="J91" t="n">
-        <v>-11.05</v>
+        <v>12</v>
       </c>
       <c r="K91" t="n">
-        <v>-11.85</v>
+        <v>11.1</v>
       </c>
       <c r="M91" t="n">
         <v>0</v>
@@ -4304,10 +4310,28 @@
         <v>0</v>
       </c>
       <c r="O91" t="n">
-        <v>-3.8</v>
+        <v>0</v>
       </c>
       <c r="P91" t="n">
-        <v>-11.45</v>
+        <v>11.55</v>
+      </c>
+      <c r="T91" t="n">
+        <v>2</v>
+      </c>
+      <c r="U91" t="n">
+        <v>2</v>
+      </c>
+      <c r="V91" t="n">
+        <v>-0</v>
+      </c>
+      <c r="W91" t="n">
+        <v>0</v>
+      </c>
+      <c r="X91" t="n">
+        <v>38.9</v>
+      </c>
+      <c r="Y91" t="n">
+        <v>99.88</v>
       </c>
     </row>
     <row r="92" spans="1:25">
@@ -4315,31 +4339,31 @@
         <v>95</v>
       </c>
       <c r="C92" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D92" t="n">
-        <v>-3.8</v>
+        <v>3.05</v>
       </c>
       <c r="E92" t="n">
-        <v>-11.45</v>
+        <v>-3.65</v>
       </c>
       <c r="F92" t="n">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
       <c r="G92" t="n">
-        <v>0.8</v>
+        <v>16.9</v>
       </c>
       <c r="H92" t="n">
-        <v>-4.2</v>
+        <v>2.6</v>
       </c>
       <c r="I92" t="n">
-        <v>-3.4</v>
+        <v>3.5</v>
       </c>
       <c r="J92" t="n">
-        <v>-11.05</v>
+        <v>4.799999999999999</v>
       </c>
       <c r="K92" t="n">
-        <v>-11.85</v>
+        <v>-12.1</v>
       </c>
       <c r="M92" t="n">
         <v>0</v>
@@ -4348,10 +4372,28 @@
         <v>0</v>
       </c>
       <c r="O92" t="n">
-        <v>-3.8</v>
+        <v>3.05</v>
       </c>
       <c r="P92" t="n">
-        <v>-11.45</v>
+        <v>-3.65</v>
+      </c>
+      <c r="T92" t="n">
+        <v>2</v>
+      </c>
+      <c r="U92" t="n">
+        <v>2</v>
+      </c>
+      <c r="V92" t="n">
+        <v>-0</v>
+      </c>
+      <c r="W92" t="n">
+        <v>0</v>
+      </c>
+      <c r="X92" t="n">
+        <v>99.88</v>
+      </c>
+      <c r="Y92" t="n">
+        <v>38.9</v>
       </c>
     </row>
     <row r="93" spans="1:25">
@@ -4359,61 +4401,43 @@
         <v>95</v>
       </c>
       <c r="C93" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D93" t="n">
-        <v>-2.4</v>
+        <v>-11.8</v>
       </c>
       <c r="E93" t="n">
-        <v>-10.55</v>
+        <v>-11.45</v>
       </c>
       <c r="F93" t="n">
-        <v>0.4</v>
+        <v>0.8</v>
       </c>
       <c r="G93" t="n">
         <v>0.8</v>
       </c>
       <c r="H93" t="n">
-        <v>-2.6</v>
+        <v>-12.2</v>
       </c>
       <c r="I93" t="n">
-        <v>-2.2</v>
+        <v>-11.4</v>
       </c>
       <c r="J93" t="n">
-        <v>-10.15</v>
+        <v>-11.05</v>
       </c>
       <c r="K93" t="n">
-        <v>-10.95</v>
+        <v>-11.85</v>
       </c>
       <c r="M93" t="n">
-        <v>-0.3</v>
+        <v>0</v>
       </c>
       <c r="N93" t="n">
-        <v>0.756</v>
+        <v>0</v>
       </c>
       <c r="O93" t="n">
-        <v>-2.1</v>
+        <v>-11.8</v>
       </c>
       <c r="P93" t="n">
-        <v>-11.306</v>
-      </c>
-      <c r="T93" t="n">
-        <v>8</v>
-      </c>
-      <c r="U93" t="n">
-        <v>8</v>
-      </c>
-      <c r="V93" t="n">
-        <v>-0</v>
-      </c>
-      <c r="W93" t="n">
-        <v>0.099</v>
-      </c>
-      <c r="X93" t="n">
-        <v>11</v>
-      </c>
-      <c r="Y93" t="n">
-        <v>11</v>
+        <v>-11.45</v>
       </c>
     </row>
     <row r="94" spans="1:25">
@@ -4424,58 +4448,40 @@
         <v>99</v>
       </c>
       <c r="D94" t="n">
-        <v>-2.4</v>
+        <v>-11.8</v>
       </c>
       <c r="E94" t="n">
-        <v>-11.25</v>
+        <v>-11.45</v>
       </c>
       <c r="F94" t="n">
-        <v>0.4</v>
+        <v>0.8</v>
       </c>
       <c r="G94" t="n">
-        <v>0.6</v>
+        <v>0.8</v>
       </c>
       <c r="H94" t="n">
-        <v>-2.6</v>
+        <v>-12.2</v>
       </c>
       <c r="I94" t="n">
-        <v>-2.2</v>
+        <v>-11.4</v>
       </c>
       <c r="J94" t="n">
-        <v>-10.95</v>
+        <v>-11.05</v>
       </c>
       <c r="K94" t="n">
-        <v>-11.55</v>
+        <v>-11.85</v>
       </c>
       <c r="M94" t="n">
-        <v>-0.3</v>
+        <v>0</v>
       </c>
       <c r="N94" t="n">
-        <v>-0.662</v>
+        <v>0</v>
       </c>
       <c r="O94" t="n">
-        <v>-2.1</v>
+        <v>-11.8</v>
       </c>
       <c r="P94" t="n">
-        <v>-10.588</v>
-      </c>
-      <c r="T94" t="n">
-        <v>8</v>
-      </c>
-      <c r="U94" t="n">
-        <v>8</v>
-      </c>
-      <c r="V94" t="n">
-        <v>-0</v>
-      </c>
-      <c r="W94" t="n">
-        <v>0.099</v>
-      </c>
-      <c r="X94" t="n">
-        <v>11</v>
-      </c>
-      <c r="Y94" t="n">
-        <v>11</v>
+        <v>-11.45</v>
       </c>
     </row>
     <row r="95" spans="1:25">
@@ -4486,40 +4492,40 @@
         <v>100</v>
       </c>
       <c r="D95" t="n">
-        <v>0</v>
+        <v>-10.4</v>
       </c>
       <c r="E95" t="n">
-        <v>10.9</v>
+        <v>-10.55</v>
       </c>
       <c r="F95" t="n">
-        <v>11.4</v>
+        <v>0.4</v>
       </c>
       <c r="G95" t="n">
-        <v>0.4</v>
+        <v>0.8</v>
       </c>
       <c r="H95" t="n">
-        <v>-5.7</v>
+        <v>-10.6</v>
       </c>
       <c r="I95" t="n">
-        <v>5.7</v>
+        <v>-10.2</v>
       </c>
       <c r="J95" t="n">
-        <v>11.1</v>
+        <v>-10.15</v>
       </c>
       <c r="K95" t="n">
-        <v>10.7</v>
+        <v>-10.95</v>
       </c>
       <c r="M95" t="n">
-        <v>0</v>
+        <v>-0.3</v>
       </c>
       <c r="N95" t="n">
-        <v>0</v>
+        <v>0.756</v>
       </c>
       <c r="O95" t="n">
-        <v>0</v>
+        <v>-10.1</v>
       </c>
       <c r="P95" t="n">
-        <v>10.9</v>
+        <v>-11.306</v>
       </c>
       <c r="T95" t="n">
         <v>8</v>
@@ -4548,40 +4554,58 @@
         <v>101</v>
       </c>
       <c r="D96" t="n">
-        <v>-9.800000000000001</v>
+        <v>-10.4</v>
       </c>
       <c r="E96" t="n">
-        <v>-0.9</v>
+        <v>-11.25</v>
       </c>
       <c r="F96" t="n">
-        <v>2.4</v>
+        <v>0.4</v>
       </c>
       <c r="G96" t="n">
-        <v>22.4</v>
+        <v>0.6</v>
       </c>
       <c r="H96" t="n">
-        <v>-11</v>
+        <v>-10.6</v>
       </c>
       <c r="I96" t="n">
-        <v>-8.600000000000001</v>
+        <v>-10.2</v>
       </c>
       <c r="J96" t="n">
-        <v>10.3</v>
+        <v>-10.95</v>
       </c>
       <c r="K96" t="n">
-        <v>-12.1</v>
+        <v>-11.55</v>
       </c>
       <c r="M96" t="n">
-        <v>0</v>
+        <v>-0.3</v>
       </c>
       <c r="N96" t="n">
-        <v>0</v>
+        <v>-0.662</v>
       </c>
       <c r="O96" t="n">
-        <v>-9.800000000000001</v>
+        <v>-10.1</v>
       </c>
       <c r="P96" t="n">
-        <v>-0.9</v>
+        <v>-10.588</v>
+      </c>
+      <c r="T96" t="n">
+        <v>8</v>
+      </c>
+      <c r="U96" t="n">
+        <v>8</v>
+      </c>
+      <c r="V96" t="n">
+        <v>-0</v>
+      </c>
+      <c r="W96" t="n">
+        <v>0.099</v>
+      </c>
+      <c r="X96" t="n">
+        <v>11</v>
+      </c>
+      <c r="Y96" t="n">
+        <v>11</v>
       </c>
     </row>
     <row r="97" spans="1:25">
@@ -4592,40 +4616,58 @@
         <v>102</v>
       </c>
       <c r="D97" t="n">
-        <v>9.800000000000001</v>
+        <v>0</v>
       </c>
       <c r="E97" t="n">
-        <v>-0.9</v>
+        <v>10.9</v>
       </c>
       <c r="F97" t="n">
-        <v>2.4</v>
+        <v>11.4</v>
       </c>
       <c r="G97" t="n">
-        <v>22.4</v>
+        <v>0.4</v>
       </c>
       <c r="H97" t="n">
-        <v>8.600000000000001</v>
+        <v>-5.7</v>
       </c>
       <c r="I97" t="n">
+        <v>5.7</v>
+      </c>
+      <c r="J97" t="n">
+        <v>11.1</v>
+      </c>
+      <c r="K97" t="n">
+        <v>10.7</v>
+      </c>
+      <c r="M97" t="n">
+        <v>0</v>
+      </c>
+      <c r="N97" t="n">
+        <v>0</v>
+      </c>
+      <c r="O97" t="n">
+        <v>0</v>
+      </c>
+      <c r="P97" t="n">
+        <v>10.9</v>
+      </c>
+      <c r="T97" t="n">
+        <v>8</v>
+      </c>
+      <c r="U97" t="n">
+        <v>8</v>
+      </c>
+      <c r="V97" t="n">
+        <v>-0</v>
+      </c>
+      <c r="W97" t="n">
+        <v>0.099</v>
+      </c>
+      <c r="X97" t="n">
         <v>11</v>
       </c>
-      <c r="J97" t="n">
-        <v>10.3</v>
-      </c>
-      <c r="K97" t="n">
-        <v>-12.1</v>
-      </c>
-      <c r="M97" t="n">
-        <v>0</v>
-      </c>
-      <c r="N97" t="n">
-        <v>0</v>
-      </c>
-      <c r="O97" t="n">
-        <v>9.800000000000001</v>
-      </c>
-      <c r="P97" t="n">
-        <v>-0.9</v>
+      <c r="Y97" t="n">
+        <v>11</v>
       </c>
     </row>
     <row r="98" spans="1:25">
@@ -4636,25 +4678,25 @@
         <v>103</v>
       </c>
       <c r="D98" t="n">
-        <v>-6</v>
+        <v>-7.8</v>
       </c>
       <c r="E98" t="n">
-        <v>-6.4</v>
+        <v>-0.9</v>
       </c>
       <c r="F98" t="n">
-        <v>0.4</v>
+        <v>6.4</v>
       </c>
       <c r="G98" t="n">
-        <v>11.4</v>
+        <v>22.4</v>
       </c>
       <c r="H98" t="n">
-        <v>-6.2</v>
+        <v>-11</v>
       </c>
       <c r="I98" t="n">
-        <v>-5.8</v>
+        <v>-4.6</v>
       </c>
       <c r="J98" t="n">
-        <v>-0.7000000000000002</v>
+        <v>10.3</v>
       </c>
       <c r="K98" t="n">
         <v>-12.1</v>
@@ -4666,28 +4708,10 @@
         <v>0</v>
       </c>
       <c r="O98" t="n">
-        <v>-6</v>
+        <v>-7.8</v>
       </c>
       <c r="P98" t="n">
-        <v>-6.4</v>
-      </c>
-      <c r="T98" t="n">
-        <v>1</v>
-      </c>
-      <c r="U98" t="n">
-        <v>4</v>
-      </c>
-      <c r="V98" t="n">
-        <v>-44</v>
-      </c>
-      <c r="W98" t="n">
-        <v>0.959</v>
-      </c>
-      <c r="X98" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y98" t="n">
-        <v>22</v>
+        <v>-0.9</v>
       </c>
     </row>
     <row r="99" spans="1:25">
@@ -4695,28 +4719,28 @@
         <v>95</v>
       </c>
       <c r="C99" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D99" t="n">
-        <v>-6</v>
+        <v>7.8</v>
       </c>
       <c r="E99" t="n">
-        <v>-6.4</v>
+        <v>-0.9</v>
       </c>
       <c r="F99" t="n">
-        <v>0.4</v>
+        <v>6.4</v>
       </c>
       <c r="G99" t="n">
-        <v>11.4</v>
+        <v>22.4</v>
       </c>
       <c r="H99" t="n">
-        <v>-6.2</v>
+        <v>4.6</v>
       </c>
       <c r="I99" t="n">
-        <v>-5.8</v>
+        <v>11</v>
       </c>
       <c r="J99" t="n">
-        <v>-0.7000000000000002</v>
+        <v>10.3</v>
       </c>
       <c r="K99" t="n">
         <v>-12.1</v>
@@ -4728,275 +4752,381 @@
         <v>0</v>
       </c>
       <c r="O99" t="n">
-        <v>-6</v>
+        <v>7.8</v>
       </c>
       <c r="P99" t="n">
-        <v>-6.4</v>
-      </c>
-      <c r="T99" t="n">
-        <v>1</v>
-      </c>
-      <c r="U99" t="n">
-        <v>3</v>
-      </c>
-      <c r="V99" t="n">
-        <v>44</v>
-      </c>
-      <c r="W99" t="n">
-        <v>0.959</v>
-      </c>
-      <c r="X99" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y99" t="n">
-        <v>22</v>
+        <v>-0.9</v>
       </c>
     </row>
     <row r="100" spans="1:25">
       <c r="A100" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="C100" t="s">
         <v>105</v>
       </c>
       <c r="D100" t="n">
-        <v>5.75</v>
+        <v>2</v>
       </c>
       <c r="E100" t="n">
-        <v>-3.65</v>
+        <v>-6.4</v>
       </c>
       <c r="F100" t="n">
-        <v>0.9</v>
+        <v>0.4</v>
       </c>
       <c r="G100" t="n">
-        <v>16.9</v>
+        <v>11.4</v>
       </c>
       <c r="H100" t="n">
-        <v>5.3</v>
+        <v>1.8</v>
       </c>
       <c r="I100" t="n">
-        <v>6.2</v>
+        <v>2.2</v>
       </c>
       <c r="J100" t="n">
-        <v>4.799999999999999</v>
+        <v>-0.7000000000000002</v>
       </c>
       <c r="K100" t="n">
         <v>-12.1</v>
       </c>
       <c r="M100" t="n">
-        <v>-48.125</v>
+        <v>0</v>
       </c>
       <c r="N100" t="n">
-        <v>-19.25</v>
+        <v>0</v>
       </c>
       <c r="O100" t="n">
-        <v>53.875</v>
+        <v>2</v>
       </c>
       <c r="P100" t="n">
-        <v>15.6</v>
+        <v>-6.4</v>
       </c>
       <c r="T100" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U100" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="V100" t="n">
-        <v>-0</v>
+        <v>-44</v>
       </c>
       <c r="W100" t="n">
-        <v>0</v>
+        <v>0.959</v>
       </c>
       <c r="X100" t="n">
-        <v>96.25</v>
+        <v>0</v>
       </c>
       <c r="Y100" t="n">
-        <v>38.5</v>
+        <v>22</v>
       </c>
     </row>
     <row r="101" spans="1:25">
       <c r="A101" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="C101" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D101" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E101" t="n">
-        <v>-12.55</v>
+        <v>-6.4</v>
       </c>
       <c r="F101" t="n">
-        <v>16.9</v>
+        <v>0.4</v>
       </c>
       <c r="G101" t="n">
-        <v>0.9</v>
+        <v>11.4</v>
       </c>
       <c r="H101" t="n">
-        <v>-8.449999999999999</v>
+        <v>1.8</v>
       </c>
       <c r="I101" t="n">
-        <v>8.449999999999999</v>
+        <v>2.2</v>
       </c>
       <c r="J101" t="n">
+        <v>-0.7000000000000002</v>
+      </c>
+      <c r="K101" t="n">
         <v>-12.1</v>
       </c>
-      <c r="K101" t="n">
-        <v>-13</v>
-      </c>
       <c r="M101" t="n">
-        <v>-19.25</v>
+        <v>0</v>
       </c>
       <c r="N101" t="n">
-        <v>-48.125</v>
+        <v>0</v>
       </c>
       <c r="O101" t="n">
-        <v>19.25</v>
+        <v>2</v>
       </c>
       <c r="P101" t="n">
-        <v>35.575</v>
+        <v>-6.4</v>
       </c>
       <c r="T101" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U101" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="V101" t="n">
-        <v>-0</v>
+        <v>44</v>
       </c>
       <c r="W101" t="n">
-        <v>0</v>
+        <v>0.959</v>
       </c>
       <c r="X101" t="n">
-        <v>38.5</v>
+        <v>0</v>
       </c>
       <c r="Y101" t="n">
-        <v>96.25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="102" spans="1:25">
       <c r="A102" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C102" t="s">
         <v>107</v>
       </c>
       <c r="D102" t="n">
-        <v>-2.8</v>
+        <v>0</v>
       </c>
       <c r="E102" t="n">
-        <v>-10.85</v>
+        <v>-12.55</v>
       </c>
       <c r="F102" t="n">
-        <v>0.4</v>
+        <v>16.9</v>
       </c>
       <c r="G102" t="n">
-        <v>0.4</v>
+        <v>0.9</v>
       </c>
       <c r="H102" t="n">
-        <v>-3</v>
+        <v>-8.449999999999999</v>
       </c>
       <c r="I102" t="n">
-        <v>-2.6</v>
+        <v>8.449999999999999</v>
       </c>
       <c r="J102" t="n">
-        <v>-10.65</v>
+        <v>-12.1</v>
       </c>
       <c r="K102" t="n">
-        <v>-11.05</v>
+        <v>-13</v>
       </c>
       <c r="M102" t="n">
-        <v>-0.3</v>
+        <v>0</v>
       </c>
       <c r="N102" t="n">
-        <v>-0.767</v>
+        <v>0</v>
       </c>
       <c r="O102" t="n">
-        <v>-2.5</v>
+        <v>0</v>
       </c>
       <c r="P102" t="n">
-        <v>-10.083</v>
+        <v>-12.55</v>
       </c>
       <c r="T102" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="U102" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="V102" t="n">
         <v>-0</v>
       </c>
       <c r="W102" t="n">
-        <v>0.099</v>
+        <v>0</v>
       </c>
       <c r="X102" t="n">
-        <v>11</v>
+        <v>38.9</v>
       </c>
       <c r="Y102" t="n">
-        <v>11</v>
+        <v>99.88</v>
       </c>
     </row>
     <row r="103" spans="1:25">
       <c r="A103" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C103" t="s">
         <v>108</v>
       </c>
       <c r="D103" t="n">
-        <v>-0.65</v>
+        <v>-2.25</v>
       </c>
       <c r="E103" t="n">
-        <v>-11.05</v>
+        <v>-3.65</v>
       </c>
       <c r="F103" t="n">
-        <v>3.1</v>
+        <v>0.9</v>
       </c>
       <c r="G103" t="n">
-        <v>1.8</v>
+        <v>16.9</v>
       </c>
       <c r="H103" t="n">
-        <v>-2.2</v>
+        <v>-2.7</v>
       </c>
       <c r="I103" t="n">
-        <v>0.9</v>
+        <v>-1.8</v>
       </c>
       <c r="J103" t="n">
-        <v>-10.15</v>
+        <v>4.799999999999999</v>
       </c>
       <c r="K103" t="n">
-        <v>-11.95</v>
+        <v>-12.1</v>
       </c>
       <c r="M103" t="n">
-        <v>-0.5629999999999999</v>
+        <v>0</v>
       </c>
       <c r="N103" t="n">
         <v>0</v>
       </c>
       <c r="O103" t="n">
-        <v>-0.08700000000000008</v>
+        <v>-2.25</v>
       </c>
       <c r="P103" t="n">
-        <v>-11.05</v>
+        <v>-3.65</v>
       </c>
       <c r="T103" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="U103" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="V103" t="n">
         <v>-0</v>
       </c>
       <c r="W103" t="n">
+        <v>0</v>
+      </c>
+      <c r="X103" t="n">
+        <v>99.88</v>
+      </c>
+      <c r="Y103" t="n">
+        <v>38.9</v>
+      </c>
+    </row>
+    <row r="104" spans="1:25">
+      <c r="A104" t="s">
+        <v>106</v>
+      </c>
+      <c r="C104" t="s">
+        <v>109</v>
+      </c>
+      <c r="D104" t="n">
+        <v>-10.8</v>
+      </c>
+      <c r="E104" t="n">
+        <v>-10.85</v>
+      </c>
+      <c r="F104" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="G104" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="H104" t="n">
+        <v>-11</v>
+      </c>
+      <c r="I104" t="n">
+        <v>-10.6</v>
+      </c>
+      <c r="J104" t="n">
+        <v>-10.65</v>
+      </c>
+      <c r="K104" t="n">
+        <v>-11.05</v>
+      </c>
+      <c r="M104" t="n">
+        <v>-0.3</v>
+      </c>
+      <c r="N104" t="n">
+        <v>-0.767</v>
+      </c>
+      <c r="O104" t="n">
+        <v>-10.5</v>
+      </c>
+      <c r="P104" t="n">
+        <v>-10.083</v>
+      </c>
+      <c r="T104" t="n">
+        <v>8</v>
+      </c>
+      <c r="U104" t="n">
+        <v>8</v>
+      </c>
+      <c r="V104" t="n">
+        <v>-0</v>
+      </c>
+      <c r="W104" t="n">
         <v>0.099</v>
       </c>
-      <c r="X103" t="n">
+      <c r="X104" t="n">
         <v>11</v>
       </c>
-      <c r="Y103" t="n">
+      <c r="Y104" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="105" spans="1:25">
+      <c r="A105" t="s">
+        <v>106</v>
+      </c>
+      <c r="C105" t="s">
+        <v>110</v>
+      </c>
+      <c r="D105" t="n">
+        <v>-8.65</v>
+      </c>
+      <c r="E105" t="n">
+        <v>-11.05</v>
+      </c>
+      <c r="F105" t="n">
+        <v>3.1</v>
+      </c>
+      <c r="G105" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="H105" t="n">
+        <v>-10.2</v>
+      </c>
+      <c r="I105" t="n">
+        <v>-7.100000000000001</v>
+      </c>
+      <c r="J105" t="n">
+        <v>-10.15</v>
+      </c>
+      <c r="K105" t="n">
+        <v>-11.95</v>
+      </c>
+      <c r="M105" t="n">
+        <v>-0.5629999999999999</v>
+      </c>
+      <c r="N105" t="n">
+        <v>0</v>
+      </c>
+      <c r="O105" t="n">
+        <v>-8.087</v>
+      </c>
+      <c r="P105" t="n">
+        <v>-11.05</v>
+      </c>
+      <c r="T105" t="n">
+        <v>8</v>
+      </c>
+      <c r="U105" t="n">
+        <v>8</v>
+      </c>
+      <c r="V105" t="n">
+        <v>-0</v>
+      </c>
+      <c r="W105" t="n">
+        <v>0.099</v>
+      </c>
+      <c r="X105" t="n">
+        <v>11</v>
+      </c>
+      <c r="Y105" t="n">
         <v>11</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fixed line to bond pad corner
</commit_message>
<xml_diff>
--- a/masks/code/ResonatorArray.xlsx
+++ b/masks/code/ResonatorArray.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>

<commit_message>
tiny chnges to spreadsheet generator
</commit_message>
<xml_diff>
--- a/masks/code/ResonatorArray.xlsx
+++ b/masks/code/ResonatorArray.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="114">
   <si>
     <t>Alternate Array Layout</t>
   </si>
@@ -305,55 +305,58 @@
     <t>Capacitor_common</t>
   </si>
   <si>
+    <t>400nm_NbWiring</t>
+  </si>
+  <si>
+    <t>Cap_to_Ind_lines</t>
+  </si>
+  <si>
+    <t>GP_edge_filler_hor</t>
+  </si>
+  <si>
+    <t>GP_edge_filler_vert</t>
+  </si>
+  <si>
+    <t>MSfeed_bondpad</t>
+  </si>
+  <si>
+    <t>cap_to_feed</t>
+  </si>
+  <si>
+    <t>cap_to_gnd</t>
+  </si>
+  <si>
+    <t>feedline_main</t>
+  </si>
+  <si>
+    <t>main_hor_feedline_to_pad</t>
+  </si>
+  <si>
+    <t>main_vert_feedline_to_pad</t>
+  </si>
+  <si>
+    <t>vert_main_with_corners</t>
+  </si>
+  <si>
+    <t>ILD</t>
+  </si>
+  <si>
+    <t>GP_edge_opening_hor_r</t>
+  </si>
+  <si>
+    <t>GP_edge_opening_vert_r</t>
+  </si>
+  <si>
+    <t>Via_to_Ground</t>
+  </si>
+  <si>
+    <t>reso_ILD_sub</t>
+  </si>
+  <si>
+    <t>GP</t>
+  </si>
+  <si>
     <t>GNDfeed_bondpad</t>
-  </si>
-  <si>
-    <t>400nm_NbWiring</t>
-  </si>
-  <si>
-    <t>Cap_to_Ind_lines</t>
-  </si>
-  <si>
-    <t>GP_edge_filler_hor</t>
-  </si>
-  <si>
-    <t>GP_edge_filler_vert</t>
-  </si>
-  <si>
-    <t>MSfeed_bondpad</t>
-  </si>
-  <si>
-    <t>cap_to_feed</t>
-  </si>
-  <si>
-    <t>cap_to_gnd</t>
-  </si>
-  <si>
-    <t>feedline_main</t>
-  </si>
-  <si>
-    <t>main_hor_feedline_to_pad</t>
-  </si>
-  <si>
-    <t>main_vert_feedline_to_pad</t>
-  </si>
-  <si>
-    <t>vert_main_with_corners</t>
-  </si>
-  <si>
-    <t>ILD</t>
-  </si>
-  <si>
-    <t>GP_edge_opening_hor_r</t>
-  </si>
-  <si>
-    <t>GP_edge_opening_vert_r</t>
-  </si>
-  <si>
-    <t>Via_to_Ground</t>
-  </si>
-  <si>
-    <t>reso_ILD_sub</t>
   </si>
 </sst>
 </file>
@@ -840,7 +843,7 @@
         <v>8</v>
       </c>
       <c r="V15" t="n">
-        <v>0.699</v>
+        <v>0.7</v>
       </c>
       <c r="W15" t="n">
         <v>0</v>
@@ -4258,13 +4261,13 @@
         <v>-0.6</v>
       </c>
       <c r="M89" t="n">
-        <v>-0.5620000000000001</v>
+        <v>-0.5629999999999999</v>
       </c>
       <c r="N89" t="n">
         <v>0</v>
       </c>
       <c r="O89" t="n">
-        <v>-0.738</v>
+        <v>-0.7370000000000001</v>
       </c>
       <c r="P89" t="n">
         <v>0</v>
@@ -4276,7 +4279,7 @@
         <v>8</v>
       </c>
       <c r="V89" t="n">
-        <v>0.699</v>
+        <v>0.7</v>
       </c>
       <c r="W89" t="n">
         <v>0</v>
@@ -4290,69 +4293,69 @@
     </row>
     <row r="90" spans="1:25">
       <c r="A90" t="s">
-        <v>28</v>
+        <v>96</v>
       </c>
       <c r="C90" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D90" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E90" t="n">
+        <v>0</v>
+      </c>
+      <c r="F90" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="G90" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="H90" t="n">
+        <v>-0.6</v>
+      </c>
+      <c r="I90" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="J90" t="n">
         <v>0.65</v>
       </c>
-      <c r="F90" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="G90" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="H90" t="n">
-        <v>2.6</v>
-      </c>
-      <c r="I90" t="n">
-        <v>3.4</v>
-      </c>
-      <c r="J90" t="n">
-        <v>1.05</v>
-      </c>
       <c r="K90" t="n">
-        <v>0.25</v>
+        <v>-0.65</v>
       </c>
       <c r="M90" t="n">
-        <v>0</v>
+        <v>0.2585</v>
       </c>
       <c r="N90" t="n">
         <v>0</v>
       </c>
       <c r="O90" t="n">
-        <v>3</v>
+        <v>-0.2585</v>
       </c>
       <c r="P90" t="n">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="T90" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="U90" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="V90" t="n">
-        <v>2.996</v>
+        <v>0.7</v>
       </c>
       <c r="W90" t="n">
         <v>0</v>
       </c>
       <c r="X90" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="Y90" t="n">
-        <v>32.604</v>
+        <v>11</v>
       </c>
     </row>
     <row r="91" spans="1:25">
       <c r="A91" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C91" t="s">
         <v>98</v>
@@ -4361,88 +4364,88 @@
         <v>0</v>
       </c>
       <c r="E91" t="n">
-        <v>0</v>
+        <v>-11.25</v>
       </c>
       <c r="F91" t="n">
-        <v>1.2</v>
+        <v>16.9</v>
       </c>
       <c r="G91" t="n">
-        <v>1.3</v>
+        <v>0.9</v>
       </c>
       <c r="H91" t="n">
-        <v>-0.6</v>
+        <v>-8.449999999999999</v>
       </c>
       <c r="I91" t="n">
-        <v>0.6</v>
+        <v>8.449999999999999</v>
       </c>
       <c r="J91" t="n">
-        <v>0.65</v>
+        <v>-10.8</v>
       </c>
       <c r="K91" t="n">
-        <v>-0.65</v>
+        <v>-11.7</v>
       </c>
       <c r="M91" t="n">
-        <v>0.259</v>
+        <v>0</v>
       </c>
       <c r="N91" t="n">
         <v>0</v>
       </c>
       <c r="O91" t="n">
-        <v>-0.259</v>
+        <v>0</v>
       </c>
       <c r="P91" t="n">
-        <v>0</v>
+        <v>-11.25</v>
       </c>
       <c r="T91" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="U91" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="V91" t="n">
-        <v>0.699</v>
+        <v>-0</v>
       </c>
       <c r="W91" t="n">
         <v>0</v>
       </c>
       <c r="X91" t="n">
-        <v>11</v>
+        <v>38.9</v>
       </c>
       <c r="Y91" t="n">
-        <v>11</v>
+        <v>99.88</v>
       </c>
     </row>
     <row r="92" spans="1:25">
       <c r="A92" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C92" t="s">
         <v>99</v>
       </c>
       <c r="D92" t="n">
-        <v>0</v>
+        <v>9.75</v>
       </c>
       <c r="E92" t="n">
-        <v>-11.25</v>
+        <v>0</v>
       </c>
       <c r="F92" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="G92" t="n">
         <v>16.9</v>
       </c>
-      <c r="G92" t="n">
-        <v>0.9</v>
-      </c>
       <c r="H92" t="n">
+        <v>9.300000000000001</v>
+      </c>
+      <c r="I92" t="n">
+        <v>10.2</v>
+      </c>
+      <c r="J92" t="n">
+        <v>8.449999999999999</v>
+      </c>
+      <c r="K92" t="n">
         <v>-8.449999999999999</v>
       </c>
-      <c r="I92" t="n">
-        <v>8.449999999999999</v>
-      </c>
-      <c r="J92" t="n">
-        <v>-10.8</v>
-      </c>
-      <c r="K92" t="n">
-        <v>-11.7</v>
-      </c>
       <c r="M92" t="n">
         <v>0</v>
       </c>
@@ -4450,60 +4453,60 @@
         <v>0</v>
       </c>
       <c r="O92" t="n">
-        <v>0</v>
+        <v>9.75</v>
       </c>
       <c r="P92" t="n">
-        <v>-11.25</v>
+        <v>0</v>
       </c>
       <c r="T92" t="n">
+        <v>1</v>
+      </c>
+      <c r="U92" t="n">
         <v>3</v>
       </c>
-      <c r="U92" t="n">
-        <v>2</v>
-      </c>
       <c r="V92" t="n">
-        <v>-0</v>
+        <v>-49.95</v>
       </c>
       <c r="W92" t="n">
         <v>0</v>
       </c>
       <c r="X92" t="n">
+        <v>99.88</v>
+      </c>
+      <c r="Y92" t="n">
         <v>38.9</v>
-      </c>
-      <c r="Y92" t="n">
-        <v>99.88</v>
       </c>
     </row>
     <row r="93" spans="1:25">
       <c r="A93" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C93" t="s">
         <v>100</v>
       </c>
       <c r="D93" t="n">
-        <v>9.75</v>
+        <v>3</v>
       </c>
       <c r="E93" t="n">
-        <v>0</v>
+        <v>-0.35</v>
       </c>
       <c r="F93" t="n">
-        <v>0.9</v>
+        <v>0.8</v>
       </c>
       <c r="G93" t="n">
-        <v>16.9</v>
+        <v>0.8</v>
       </c>
       <c r="H93" t="n">
-        <v>9.300000000000001</v>
+        <v>2.6</v>
       </c>
       <c r="I93" t="n">
-        <v>10.2</v>
+        <v>3.4</v>
       </c>
       <c r="J93" t="n">
-        <v>8.449999999999999</v>
+        <v>0.05000000000000004</v>
       </c>
       <c r="K93" t="n">
-        <v>-8.449999999999999</v>
+        <v>-0.75</v>
       </c>
       <c r="M93" t="n">
         <v>0</v>
@@ -4512,95 +4515,95 @@
         <v>0</v>
       </c>
       <c r="O93" t="n">
-        <v>9.75</v>
+        <v>3</v>
       </c>
       <c r="P93" t="n">
-        <v>0</v>
+        <v>-0.35</v>
       </c>
       <c r="T93" t="n">
         <v>1</v>
       </c>
       <c r="U93" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="V93" t="n">
-        <v>-49.95</v>
+        <v>2.996</v>
       </c>
       <c r="W93" t="n">
         <v>0</v>
       </c>
       <c r="X93" t="n">
-        <v>99.88</v>
+        <v>0</v>
       </c>
       <c r="Y93" t="n">
-        <v>38.9</v>
+        <v>32.604</v>
       </c>
     </row>
     <row r="94" spans="1:25">
       <c r="A94" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C94" t="s">
         <v>101</v>
       </c>
       <c r="D94" t="n">
-        <v>3</v>
+        <v>2.2</v>
       </c>
       <c r="E94" t="n">
-        <v>-0.35</v>
+        <v>0.65</v>
       </c>
       <c r="F94" t="n">
-        <v>0.8</v>
+        <v>0.4</v>
       </c>
       <c r="G94" t="n">
         <v>0.8</v>
       </c>
       <c r="H94" t="n">
-        <v>2.6</v>
+        <v>2</v>
       </c>
       <c r="I94" t="n">
-        <v>3.4</v>
+        <v>2.4</v>
       </c>
       <c r="J94" t="n">
-        <v>0.05000000000000004</v>
+        <v>1.05</v>
       </c>
       <c r="K94" t="n">
-        <v>-0.75</v>
+        <v>0.25</v>
       </c>
       <c r="M94" t="n">
-        <v>0</v>
+        <v>-0.3</v>
       </c>
       <c r="N94" t="n">
-        <v>0</v>
+        <v>0.756</v>
       </c>
       <c r="O94" t="n">
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="P94" t="n">
-        <v>-0.35</v>
+        <v>-0.106</v>
       </c>
       <c r="T94" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="U94" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="V94" t="n">
-        <v>2.996</v>
+        <v>-0</v>
       </c>
       <c r="W94" t="n">
-        <v>0</v>
+        <v>0.099</v>
       </c>
       <c r="X94" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="Y94" t="n">
-        <v>32.604</v>
+        <v>11</v>
       </c>
     </row>
     <row r="95" spans="1:25">
       <c r="A95" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C95" t="s">
         <v>102</v>
@@ -4609,13 +4612,13 @@
         <v>2.2</v>
       </c>
       <c r="E95" t="n">
-        <v>0.65</v>
+        <v>-0.25</v>
       </c>
       <c r="F95" t="n">
         <v>0.4</v>
       </c>
       <c r="G95" t="n">
-        <v>0.8</v>
+        <v>0.6</v>
       </c>
       <c r="H95" t="n">
         <v>2</v>
@@ -4624,22 +4627,22 @@
         <v>2.4</v>
       </c>
       <c r="J95" t="n">
-        <v>1.05</v>
+        <v>0.04999999999999999</v>
       </c>
       <c r="K95" t="n">
-        <v>0.25</v>
+        <v>-0.55</v>
       </c>
       <c r="M95" t="n">
         <v>-0.3</v>
       </c>
       <c r="N95" t="n">
-        <v>0.756</v>
+        <v>-0.662</v>
       </c>
       <c r="O95" t="n">
         <v>2.5</v>
       </c>
       <c r="P95" t="n">
-        <v>-0.106</v>
+        <v>0.412</v>
       </c>
       <c r="T95" t="n">
         <v>8</v>
@@ -4662,46 +4665,46 @@
     </row>
     <row r="96" spans="1:25">
       <c r="A96" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C96" t="s">
         <v>103</v>
       </c>
       <c r="D96" t="n">
-        <v>2.2</v>
+        <v>0</v>
       </c>
       <c r="E96" t="n">
-        <v>-0.25</v>
+        <v>12</v>
       </c>
       <c r="F96" t="n">
+        <v>11.4</v>
+      </c>
+      <c r="G96" t="n">
         <v>0.4</v>
       </c>
-      <c r="G96" t="n">
-        <v>0.6</v>
-      </c>
       <c r="H96" t="n">
-        <v>2</v>
+        <v>-5.7</v>
       </c>
       <c r="I96" t="n">
-        <v>2.4</v>
+        <v>5.7</v>
       </c>
       <c r="J96" t="n">
-        <v>0.04999999999999999</v>
+        <v>12.2</v>
       </c>
       <c r="K96" t="n">
-        <v>-0.55</v>
+        <v>11.8</v>
       </c>
       <c r="M96" t="n">
-        <v>-0.3</v>
+        <v>0</v>
       </c>
       <c r="N96" t="n">
-        <v>-0.662</v>
+        <v>0</v>
       </c>
       <c r="O96" t="n">
-        <v>2.5</v>
+        <v>0</v>
       </c>
       <c r="P96" t="n">
-        <v>0.412</v>
+        <v>12</v>
       </c>
       <c r="T96" t="n">
         <v>8</v>
@@ -4724,7 +4727,7 @@
     </row>
     <row r="97" spans="1:25">
       <c r="A97" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C97" t="s">
         <v>104</v>
@@ -4733,99 +4736,99 @@
         <v>0</v>
       </c>
       <c r="E97" t="n">
-        <v>12</v>
+        <v>10.8</v>
       </c>
       <c r="F97" t="n">
-        <v>11.4</v>
+        <v>6.4</v>
       </c>
       <c r="G97" t="n">
         <v>0.4</v>
       </c>
       <c r="H97" t="n">
-        <v>-5.7</v>
+        <v>-3.2</v>
       </c>
       <c r="I97" t="n">
-        <v>5.7</v>
+        <v>3.2</v>
       </c>
       <c r="J97" t="n">
-        <v>12.2</v>
+        <v>11</v>
       </c>
       <c r="K97" t="n">
-        <v>11.8</v>
+        <v>10.6</v>
       </c>
       <c r="M97" t="n">
         <v>0</v>
       </c>
       <c r="N97" t="n">
-        <v>0</v>
+        <v>-38.5</v>
       </c>
       <c r="O97" t="n">
         <v>0</v>
       </c>
       <c r="P97" t="n">
-        <v>12</v>
+        <v>49.3</v>
       </c>
       <c r="T97" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="U97" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="V97" t="n">
         <v>-0</v>
       </c>
       <c r="W97" t="n">
-        <v>0.099</v>
+        <v>0</v>
       </c>
       <c r="X97" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="Y97" t="n">
-        <v>11</v>
+        <v>77</v>
       </c>
     </row>
     <row r="98" spans="1:25">
       <c r="A98" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C98" t="s">
         <v>105</v>
       </c>
       <c r="D98" t="n">
-        <v>0</v>
+        <v>10.6</v>
       </c>
       <c r="E98" t="n">
+        <v>0</v>
+      </c>
+      <c r="F98" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="G98" t="n">
+        <v>22.4</v>
+      </c>
+      <c r="H98" t="n">
+        <v>10.4</v>
+      </c>
+      <c r="I98" t="n">
         <v>10.8</v>
       </c>
-      <c r="F98" t="n">
-        <v>6.4</v>
-      </c>
-      <c r="G98" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="H98" t="n">
-        <v>-3.2</v>
-      </c>
-      <c r="I98" t="n">
-        <v>3.2</v>
-      </c>
       <c r="J98" t="n">
-        <v>11</v>
+        <v>11.2</v>
       </c>
       <c r="K98" t="n">
-        <v>10.6</v>
+        <v>-11.2</v>
       </c>
       <c r="M98" t="n">
-        <v>0</v>
+        <v>2.996</v>
       </c>
       <c r="N98" t="n">
-        <v>-38.5</v>
+        <v>-27.496</v>
       </c>
       <c r="O98" t="n">
-        <v>0</v>
+        <v>7.603999999999999</v>
       </c>
       <c r="P98" t="n">
-        <v>49.3</v>
+        <v>27.496</v>
       </c>
       <c r="T98" t="n">
         <v>1</v>
@@ -4834,7 +4837,7 @@
         <v>2</v>
       </c>
       <c r="V98" t="n">
-        <v>-0</v>
+        <v>2.996</v>
       </c>
       <c r="W98" t="n">
         <v>0</v>
@@ -4843,18 +4846,18 @@
         <v>0</v>
       </c>
       <c r="Y98" t="n">
-        <v>77</v>
+        <v>54.992</v>
       </c>
     </row>
     <row r="99" spans="1:25">
       <c r="A99" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C99" t="s">
         <v>106</v>
       </c>
       <c r="D99" t="n">
-        <v>10.6</v>
+        <v>-9.4</v>
       </c>
       <c r="E99" t="n">
         <v>0</v>
@@ -4863,57 +4866,57 @@
         <v>0.4</v>
       </c>
       <c r="G99" t="n">
-        <v>22.4</v>
+        <v>11.4</v>
       </c>
       <c r="H99" t="n">
-        <v>10.4</v>
+        <v>-9.6</v>
       </c>
       <c r="I99" t="n">
-        <v>10.8</v>
+        <v>-9.200000000000001</v>
       </c>
       <c r="J99" t="n">
-        <v>11.2</v>
+        <v>5.7</v>
       </c>
       <c r="K99" t="n">
-        <v>-11.2</v>
+        <v>-5.7</v>
       </c>
       <c r="M99" t="n">
-        <v>2.996</v>
+        <v>0</v>
       </c>
       <c r="N99" t="n">
-        <v>-27.496</v>
+        <v>0</v>
       </c>
       <c r="O99" t="n">
-        <v>7.603999999999999</v>
+        <v>-9.4</v>
       </c>
       <c r="P99" t="n">
-        <v>27.496</v>
+        <v>0</v>
       </c>
       <c r="T99" t="n">
         <v>1</v>
       </c>
       <c r="U99" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="V99" t="n">
-        <v>2.996</v>
+        <v>-44</v>
       </c>
       <c r="W99" t="n">
-        <v>0</v>
+        <v>0.959</v>
       </c>
       <c r="X99" t="n">
         <v>0</v>
       </c>
       <c r="Y99" t="n">
-        <v>54.992</v>
+        <v>22</v>
       </c>
     </row>
     <row r="100" spans="1:25">
       <c r="A100" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C100" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D100" t="n">
         <v>-9.4</v>
@@ -4955,10 +4958,10 @@
         <v>1</v>
       </c>
       <c r="U100" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="V100" t="n">
-        <v>-44</v>
+        <v>44</v>
       </c>
       <c r="W100" t="n">
         <v>0.959</v>
@@ -4972,34 +4975,34 @@
     </row>
     <row r="101" spans="1:25">
       <c r="A101" t="s">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="C101" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D101" t="n">
-        <v>-9.4</v>
+        <v>0</v>
       </c>
       <c r="E101" t="n">
-        <v>0</v>
+        <v>-12.35</v>
       </c>
       <c r="F101" t="n">
-        <v>0.4</v>
+        <v>16.9</v>
       </c>
       <c r="G101" t="n">
-        <v>11.4</v>
+        <v>0.9</v>
       </c>
       <c r="H101" t="n">
-        <v>-9.6</v>
+        <v>-8.449999999999999</v>
       </c>
       <c r="I101" t="n">
-        <v>-9.200000000000001</v>
+        <v>8.449999999999999</v>
       </c>
       <c r="J101" t="n">
-        <v>5.7</v>
+        <v>-11.9</v>
       </c>
       <c r="K101" t="n">
-        <v>-5.7</v>
+        <v>-12.8</v>
       </c>
       <c r="M101" t="n">
         <v>0</v>
@@ -5008,61 +5011,61 @@
         <v>0</v>
       </c>
       <c r="O101" t="n">
-        <v>-9.4</v>
+        <v>0</v>
       </c>
       <c r="P101" t="n">
-        <v>0</v>
+        <v>-12.35</v>
       </c>
       <c r="T101" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="U101" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="V101" t="n">
-        <v>44</v>
+        <v>-0</v>
       </c>
       <c r="W101" t="n">
-        <v>0.959</v>
+        <v>0</v>
       </c>
       <c r="X101" t="n">
-        <v>0</v>
+        <v>38.9</v>
       </c>
       <c r="Y101" t="n">
-        <v>22</v>
+        <v>99.88</v>
       </c>
     </row>
     <row r="102" spans="1:25">
       <c r="A102" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C102" t="s">
         <v>109</v>
       </c>
       <c r="D102" t="n">
-        <v>0</v>
+        <v>8.65</v>
       </c>
       <c r="E102" t="n">
-        <v>-12.35</v>
+        <v>0</v>
       </c>
       <c r="F102" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="G102" t="n">
         <v>16.9</v>
       </c>
-      <c r="G102" t="n">
-        <v>0.9</v>
-      </c>
       <c r="H102" t="n">
+        <v>8.200000000000001</v>
+      </c>
+      <c r="I102" t="n">
+        <v>9.1</v>
+      </c>
+      <c r="J102" t="n">
+        <v>8.449999999999999</v>
+      </c>
+      <c r="K102" t="n">
         <v>-8.449999999999999</v>
       </c>
-      <c r="I102" t="n">
-        <v>8.449999999999999</v>
-      </c>
-      <c r="J102" t="n">
-        <v>-11.9</v>
-      </c>
-      <c r="K102" t="n">
-        <v>-12.8</v>
-      </c>
       <c r="M102" t="n">
         <v>0</v>
       </c>
@@ -5070,134 +5073,134 @@
         <v>0</v>
       </c>
       <c r="O102" t="n">
-        <v>0</v>
+        <v>8.65</v>
       </c>
       <c r="P102" t="n">
-        <v>-12.35</v>
+        <v>0</v>
       </c>
       <c r="T102" t="n">
+        <v>1</v>
+      </c>
+      <c r="U102" t="n">
         <v>3</v>
       </c>
-      <c r="U102" t="n">
-        <v>2</v>
-      </c>
       <c r="V102" t="n">
-        <v>-0</v>
+        <v>-49.95</v>
       </c>
       <c r="W102" t="n">
         <v>0</v>
       </c>
       <c r="X102" t="n">
+        <v>99.88</v>
+      </c>
+      <c r="Y102" t="n">
         <v>38.9</v>
-      </c>
-      <c r="Y102" t="n">
-        <v>99.88</v>
       </c>
     </row>
     <row r="103" spans="1:25">
       <c r="A103" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C103" t="s">
         <v>110</v>
       </c>
       <c r="D103" t="n">
-        <v>8.65</v>
+        <v>1.75</v>
       </c>
       <c r="E103" t="n">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="F103" t="n">
-        <v>0.9</v>
+        <v>0.4</v>
       </c>
       <c r="G103" t="n">
-        <v>16.9</v>
+        <v>0.4</v>
       </c>
       <c r="H103" t="n">
-        <v>8.200000000000001</v>
+        <v>1.55</v>
       </c>
       <c r="I103" t="n">
-        <v>9.1</v>
+        <v>1.95</v>
       </c>
       <c r="J103" t="n">
-        <v>8.449999999999999</v>
+        <v>0.6000000000000001</v>
       </c>
       <c r="K103" t="n">
-        <v>-8.449999999999999</v>
+        <v>0.2</v>
       </c>
       <c r="M103" t="n">
-        <v>0</v>
+        <v>-0.3</v>
       </c>
       <c r="N103" t="n">
-        <v>0</v>
+        <v>-0.767</v>
       </c>
       <c r="O103" t="n">
-        <v>8.65</v>
+        <v>2.05</v>
       </c>
       <c r="P103" t="n">
-        <v>0</v>
+        <v>1.167</v>
       </c>
       <c r="T103" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="U103" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="V103" t="n">
-        <v>-49.95</v>
+        <v>-0</v>
       </c>
       <c r="W103" t="n">
-        <v>0</v>
+        <v>0.099</v>
       </c>
       <c r="X103" t="n">
-        <v>99.88</v>
+        <v>11</v>
       </c>
       <c r="Y103" t="n">
-        <v>38.9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="104" spans="1:25">
       <c r="A104" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C104" t="s">
         <v>111</v>
       </c>
       <c r="D104" t="n">
-        <v>1.75</v>
+        <v>6.45</v>
       </c>
       <c r="E104" t="n">
-        <v>0.4</v>
+        <v>-2.15</v>
       </c>
       <c r="F104" t="n">
-        <v>0.4</v>
+        <v>3.1</v>
       </c>
       <c r="G104" t="n">
-        <v>0.4</v>
+        <v>1.8</v>
       </c>
       <c r="H104" t="n">
-        <v>1.55</v>
+        <v>4.9</v>
       </c>
       <c r="I104" t="n">
-        <v>1.95</v>
+        <v>8</v>
       </c>
       <c r="J104" t="n">
-        <v>0.6000000000000001</v>
+        <v>-1.25</v>
       </c>
       <c r="K104" t="n">
-        <v>0.2</v>
+        <v>-3.05</v>
       </c>
       <c r="M104" t="n">
-        <v>-0.3</v>
+        <v>-0.5629999999999999</v>
       </c>
       <c r="N104" t="n">
-        <v>-0.767</v>
+        <v>0</v>
       </c>
       <c r="O104" t="n">
-        <v>2.05</v>
+        <v>7.013</v>
       </c>
       <c r="P104" t="n">
-        <v>1.167</v>
+        <v>-2.15</v>
       </c>
       <c r="T104" t="n">
         <v>8</v>
@@ -5220,64 +5223,64 @@
     </row>
     <row r="105" spans="1:25">
       <c r="A105" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="C105" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D105" t="n">
-        <v>6.45</v>
+        <v>3</v>
       </c>
       <c r="E105" t="n">
-        <v>-2.15</v>
+        <v>0.65</v>
       </c>
       <c r="F105" t="n">
-        <v>3.1</v>
+        <v>0.8</v>
       </c>
       <c r="G105" t="n">
-        <v>1.8</v>
+        <v>0.8</v>
       </c>
       <c r="H105" t="n">
-        <v>4.9</v>
+        <v>2.6</v>
       </c>
       <c r="I105" t="n">
-        <v>8</v>
+        <v>3.4</v>
       </c>
       <c r="J105" t="n">
-        <v>-1.25</v>
+        <v>1.05</v>
       </c>
       <c r="K105" t="n">
-        <v>-3.05</v>
+        <v>0.25</v>
       </c>
       <c r="M105" t="n">
-        <v>-0.5629999999999999</v>
+        <v>0</v>
       </c>
       <c r="N105" t="n">
         <v>0</v>
       </c>
       <c r="O105" t="n">
-        <v>7.013</v>
+        <v>3</v>
       </c>
       <c r="P105" t="n">
-        <v>-2.15</v>
+        <v>0.65</v>
       </c>
       <c r="T105" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="U105" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="V105" t="n">
-        <v>-0</v>
+        <v>2.996</v>
       </c>
       <c r="W105" t="n">
-        <v>0.099</v>
+        <v>0</v>
       </c>
       <c r="X105" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="Y105" t="n">
-        <v>11</v>
+        <v>32.604</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed bug in spreadsheet generator. Code now correctly produces the cell shift
</commit_message>
<xml_diff>
--- a/masks/code/ResonatorArray.xlsx
+++ b/masks/code/ResonatorArray.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -846,7 +846,7 @@
         <v>0.7</v>
       </c>
       <c r="W15" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="X15" t="n">
         <v>11</v>
@@ -887,13 +887,13 @@
         <v>-0.4</v>
       </c>
       <c r="M16" t="n">
-        <v>-2.655</v>
+        <v>-2.65</v>
       </c>
       <c r="N16" t="n">
         <v>0</v>
       </c>
       <c r="O16" t="n">
-        <v>3.755</v>
+        <v>3.75</v>
       </c>
       <c r="P16" t="n">
         <v>-0.15</v>
@@ -952,13 +952,13 @@
         <v>0</v>
       </c>
       <c r="N17" t="n">
-        <v>0</v>
+        <v>-0.959</v>
       </c>
       <c r="O17" t="n">
         <v>0</v>
       </c>
       <c r="P17" t="n">
-        <v>11.4</v>
+        <v>12.359</v>
       </c>
       <c r="T17" t="n">
         <v>8</v>
@@ -1011,16 +1011,16 @@
         <v>10</v>
       </c>
       <c r="M18" t="n">
-        <v>0</v>
+        <v>-47</v>
       </c>
       <c r="N18" t="n">
-        <v>-38.5</v>
+        <v>-39.459</v>
       </c>
       <c r="O18" t="n">
-        <v>0</v>
+        <v>47</v>
       </c>
       <c r="P18" t="n">
-        <v>48.7</v>
+        <v>49.65900000000001</v>
       </c>
       <c r="T18" t="n">
         <v>1</v>
@@ -1032,7 +1032,7 @@
         <v>-0</v>
       </c>
       <c r="W18" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="X18" t="n">
         <v>0</v>
@@ -1073,16 +1073,16 @@
         <v>-11.2</v>
       </c>
       <c r="M19" t="n">
-        <v>2.996</v>
+        <v>-44.004</v>
       </c>
       <c r="N19" t="n">
-        <v>-27.496</v>
+        <v>-28.455</v>
       </c>
       <c r="O19" t="n">
-        <v>-13.596</v>
+        <v>33.404</v>
       </c>
       <c r="P19" t="n">
-        <v>27.496</v>
+        <v>28.455</v>
       </c>
       <c r="T19" t="n">
         <v>1</v>
@@ -1094,7 +1094,7 @@
         <v>2.996</v>
       </c>
       <c r="W19" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="X19" t="n">
         <v>0</v>
@@ -1404,7 +1404,7 @@
         <v>-0.025</v>
       </c>
       <c r="W24" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="X24" t="n">
         <v>101</v>
@@ -4282,7 +4282,7 @@
         <v>0.7</v>
       </c>
       <c r="W89" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="X89" t="n">
         <v>11</v>
@@ -4344,7 +4344,7 @@
         <v>0.7</v>
       </c>
       <c r="W90" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="X90" t="n">
         <v>11</v>
@@ -4406,7 +4406,7 @@
         <v>-0</v>
       </c>
       <c r="W91" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="X91" t="n">
         <v>38.9</v>
@@ -4468,7 +4468,7 @@
         <v>-49.95</v>
       </c>
       <c r="W92" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="X92" t="n">
         <v>99.88</v>
@@ -4530,7 +4530,7 @@
         <v>2.996</v>
       </c>
       <c r="W93" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="X93" t="n">
         <v>0</v>
@@ -4698,13 +4698,13 @@
         <v>0</v>
       </c>
       <c r="N96" t="n">
-        <v>0</v>
+        <v>-0.959</v>
       </c>
       <c r="O96" t="n">
         <v>0</v>
       </c>
       <c r="P96" t="n">
-        <v>12</v>
+        <v>12.959</v>
       </c>
       <c r="T96" t="n">
         <v>8</v>
@@ -4757,16 +4757,16 @@
         <v>10.6</v>
       </c>
       <c r="M97" t="n">
-        <v>0</v>
+        <v>-47</v>
       </c>
       <c r="N97" t="n">
-        <v>-38.5</v>
+        <v>-39.459</v>
       </c>
       <c r="O97" t="n">
-        <v>0</v>
+        <v>47</v>
       </c>
       <c r="P97" t="n">
-        <v>49.3</v>
+        <v>50.259</v>
       </c>
       <c r="T97" t="n">
         <v>1</v>
@@ -4778,7 +4778,7 @@
         <v>-0</v>
       </c>
       <c r="W97" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="X97" t="n">
         <v>0</v>
@@ -4819,16 +4819,16 @@
         <v>-11.2</v>
       </c>
       <c r="M98" t="n">
-        <v>2.996</v>
+        <v>-44.004</v>
       </c>
       <c r="N98" t="n">
-        <v>-27.496</v>
+        <v>-28.455</v>
       </c>
       <c r="O98" t="n">
-        <v>7.603999999999999</v>
+        <v>54.604</v>
       </c>
       <c r="P98" t="n">
-        <v>27.496</v>
+        <v>28.455</v>
       </c>
       <c r="T98" t="n">
         <v>1</v>
@@ -4840,7 +4840,7 @@
         <v>2.996</v>
       </c>
       <c r="W98" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="X98" t="n">
         <v>0</v>
@@ -5026,7 +5026,7 @@
         <v>-0</v>
       </c>
       <c r="W101" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="X101" t="n">
         <v>38.9</v>
@@ -5088,7 +5088,7 @@
         <v>-49.95</v>
       </c>
       <c r="W102" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="X102" t="n">
         <v>99.88</v>
@@ -5274,7 +5274,7 @@
         <v>2.996</v>
       </c>
       <c r="W105" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="X105" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
unique shots now expressed as 1by1 arrays
</commit_message>
<xml_diff>
--- a/masks/code/ResonatorArray.xlsx
+++ b/masks/code/ResonatorArray.xlsx
@@ -825,13 +825,13 @@
         <v>0.15</v>
       </c>
       <c r="M15" t="n">
-        <v>0.821</v>
+        <v>0</v>
       </c>
       <c r="N15" t="n">
         <v>0</v>
       </c>
       <c r="O15" t="n">
-        <v>0.179</v>
+        <v>1</v>
       </c>
       <c r="P15" t="n">
         <v>0.4</v>
@@ -887,13 +887,13 @@
         <v>-0.4</v>
       </c>
       <c r="M16" t="n">
-        <v>-2.65</v>
+        <v>0</v>
       </c>
       <c r="N16" t="n">
         <v>0</v>
       </c>
       <c r="O16" t="n">
-        <v>3.75</v>
+        <v>1.1</v>
       </c>
       <c r="P16" t="n">
         <v>-0.15</v>
@@ -1011,16 +1011,16 @@
         <v>10</v>
       </c>
       <c r="M18" t="n">
-        <v>-47</v>
+        <v>0</v>
       </c>
       <c r="N18" t="n">
-        <v>-39.459</v>
+        <v>-38.5</v>
       </c>
       <c r="O18" t="n">
-        <v>47</v>
+        <v>0</v>
       </c>
       <c r="P18" t="n">
-        <v>49.65900000000001</v>
+        <v>48.7</v>
       </c>
       <c r="T18" t="n">
         <v>1</v>
@@ -1073,16 +1073,16 @@
         <v>-11.2</v>
       </c>
       <c r="M19" t="n">
-        <v>-44.004</v>
+        <v>2.996</v>
       </c>
       <c r="N19" t="n">
-        <v>-28.455</v>
+        <v>-27.496</v>
       </c>
       <c r="O19" t="n">
-        <v>33.404</v>
+        <v>-13.596</v>
       </c>
       <c r="P19" t="n">
-        <v>28.455</v>
+        <v>27.496</v>
       </c>
       <c r="T19" t="n">
         <v>1</v>
@@ -1445,16 +1445,34 @@
         <v>8.449999999999999</v>
       </c>
       <c r="M25" t="n">
+        <v>0</v>
+      </c>
+      <c r="N25" t="n">
+        <v>0</v>
+      </c>
+      <c r="O25" t="n">
+        <v>-3.7</v>
+      </c>
+      <c r="P25" t="n">
+        <v>9.199999999999999</v>
+      </c>
+      <c r="T25" t="n">
+        <v>1</v>
+      </c>
+      <c r="U25" t="n">
+        <v>1</v>
+      </c>
+      <c r="V25" t="n">
         <v>-39.483</v>
       </c>
-      <c r="N25" t="n">
+      <c r="W25" t="n">
         <v>-38.5</v>
       </c>
-      <c r="O25" t="n">
-        <v>35.78299999999999</v>
-      </c>
-      <c r="P25" t="n">
-        <v>47.7</v>
+      <c r="X25" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y25" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:25">
@@ -1489,16 +1507,34 @@
         <v>8.449999999999999</v>
       </c>
       <c r="M26" t="n">
+        <v>0</v>
+      </c>
+      <c r="N26" t="n">
+        <v>0</v>
+      </c>
+      <c r="O26" t="n">
+        <v>-1.85</v>
+      </c>
+      <c r="P26" t="n">
+        <v>9.199999999999999</v>
+      </c>
+      <c r="T26" t="n">
+        <v>1</v>
+      </c>
+      <c r="U26" t="n">
+        <v>1</v>
+      </c>
+      <c r="V26" t="n">
         <v>-39.483</v>
       </c>
-      <c r="N26" t="n">
+      <c r="W26" t="n">
         <v>-27.5</v>
       </c>
-      <c r="O26" t="n">
-        <v>37.633</v>
-      </c>
-      <c r="P26" t="n">
-        <v>36.7</v>
+      <c r="X26" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y26" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:25">
@@ -1533,16 +1569,34 @@
         <v>8.449999999999999</v>
       </c>
       <c r="M27" t="n">
+        <v>0</v>
+      </c>
+      <c r="N27" t="n">
+        <v>0</v>
+      </c>
+      <c r="O27" t="n">
+        <v>0</v>
+      </c>
+      <c r="P27" t="n">
+        <v>9.199999999999999</v>
+      </c>
+      <c r="T27" t="n">
+        <v>1</v>
+      </c>
+      <c r="U27" t="n">
+        <v>1</v>
+      </c>
+      <c r="V27" t="n">
         <v>-28.483</v>
       </c>
-      <c r="N27" t="n">
+      <c r="W27" t="n">
         <v>-27.5</v>
       </c>
-      <c r="O27" t="n">
-        <v>28.483</v>
-      </c>
-      <c r="P27" t="n">
-        <v>36.7</v>
+      <c r="X27" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y27" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:25">
@@ -1577,16 +1631,34 @@
         <v>8.449999999999999</v>
       </c>
       <c r="M28" t="n">
+        <v>0</v>
+      </c>
+      <c r="N28" t="n">
+        <v>0</v>
+      </c>
+      <c r="O28" t="n">
+        <v>1.85</v>
+      </c>
+      <c r="P28" t="n">
+        <v>9.199999999999999</v>
+      </c>
+      <c r="T28" t="n">
+        <v>1</v>
+      </c>
+      <c r="U28" t="n">
+        <v>1</v>
+      </c>
+      <c r="V28" t="n">
         <v>-28.483</v>
       </c>
-      <c r="N28" t="n">
+      <c r="W28" t="n">
         <v>-38.5</v>
       </c>
-      <c r="O28" t="n">
-        <v>30.333</v>
-      </c>
-      <c r="P28" t="n">
-        <v>47.7</v>
+      <c r="X28" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y28" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:25">
@@ -1621,16 +1693,34 @@
         <v>8.449999999999999</v>
       </c>
       <c r="M29" t="n">
+        <v>0</v>
+      </c>
+      <c r="N29" t="n">
+        <v>0</v>
+      </c>
+      <c r="O29" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="P29" t="n">
+        <v>9.199999999999999</v>
+      </c>
+      <c r="T29" t="n">
+        <v>1</v>
+      </c>
+      <c r="U29" t="n">
+        <v>1</v>
+      </c>
+      <c r="V29" t="n">
         <v>-17.483</v>
       </c>
-      <c r="N29" t="n">
+      <c r="W29" t="n">
         <v>-38.5</v>
       </c>
-      <c r="O29" t="n">
-        <v>21.183</v>
-      </c>
-      <c r="P29" t="n">
-        <v>47.7</v>
+      <c r="X29" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y29" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:25">
@@ -1665,16 +1755,34 @@
         <v>8.449999999999999</v>
       </c>
       <c r="M30" t="n">
+        <v>0</v>
+      </c>
+      <c r="N30" t="n">
+        <v>0</v>
+      </c>
+      <c r="O30" t="n">
+        <v>-3.7</v>
+      </c>
+      <c r="P30" t="n">
+        <v>9.199999999999999</v>
+      </c>
+      <c r="T30" t="n">
+        <v>1</v>
+      </c>
+      <c r="U30" t="n">
+        <v>1</v>
+      </c>
+      <c r="V30" t="n">
         <v>-6.483</v>
       </c>
-      <c r="N30" t="n">
+      <c r="W30" t="n">
         <v>-38.5</v>
       </c>
-      <c r="O30" t="n">
-        <v>2.782999999999999</v>
-      </c>
-      <c r="P30" t="n">
-        <v>47.7</v>
+      <c r="X30" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y30" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:25">
@@ -1709,16 +1817,34 @@
         <v>6.9</v>
       </c>
       <c r="M31" t="n">
+        <v>0</v>
+      </c>
+      <c r="N31" t="n">
+        <v>0</v>
+      </c>
+      <c r="O31" t="n">
+        <v>-1.85</v>
+      </c>
+      <c r="P31" t="n">
+        <v>7.65</v>
+      </c>
+      <c r="T31" t="n">
+        <v>1</v>
+      </c>
+      <c r="U31" t="n">
+        <v>1</v>
+      </c>
+      <c r="V31" t="n">
         <v>-6.483</v>
       </c>
-      <c r="N31" t="n">
+      <c r="W31" t="n">
         <v>-27.5</v>
       </c>
-      <c r="O31" t="n">
-        <v>4.632999999999999</v>
-      </c>
-      <c r="P31" t="n">
-        <v>35.15</v>
+      <c r="X31" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y31" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:25">
@@ -1753,16 +1879,34 @@
         <v>6.9</v>
       </c>
       <c r="M32" t="n">
+        <v>0</v>
+      </c>
+      <c r="N32" t="n">
+        <v>0</v>
+      </c>
+      <c r="O32" t="n">
+        <v>0</v>
+      </c>
+      <c r="P32" t="n">
+        <v>7.65</v>
+      </c>
+      <c r="T32" t="n">
+        <v>1</v>
+      </c>
+      <c r="U32" t="n">
+        <v>1</v>
+      </c>
+      <c r="V32" t="n">
         <v>-17.483</v>
       </c>
-      <c r="N32" t="n">
+      <c r="W32" t="n">
         <v>-27.5</v>
       </c>
-      <c r="O32" t="n">
-        <v>17.483</v>
-      </c>
-      <c r="P32" t="n">
-        <v>35.15</v>
+      <c r="X32" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y32" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:25">
@@ -1797,16 +1941,34 @@
         <v>6.9</v>
       </c>
       <c r="M33" t="n">
+        <v>0</v>
+      </c>
+      <c r="N33" t="n">
+        <v>0</v>
+      </c>
+      <c r="O33" t="n">
+        <v>1.85</v>
+      </c>
+      <c r="P33" t="n">
+        <v>7.65</v>
+      </c>
+      <c r="T33" t="n">
+        <v>1</v>
+      </c>
+      <c r="U33" t="n">
+        <v>1</v>
+      </c>
+      <c r="V33" t="n">
         <v>-17.483</v>
       </c>
-      <c r="N33" t="n">
+      <c r="W33" t="n">
         <v>-16.5</v>
       </c>
-      <c r="O33" t="n">
-        <v>19.333</v>
-      </c>
-      <c r="P33" t="n">
-        <v>24.15</v>
+      <c r="X33" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y33" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:25">
@@ -1841,16 +2003,34 @@
         <v>6.9</v>
       </c>
       <c r="M34" t="n">
+        <v>0</v>
+      </c>
+      <c r="N34" t="n">
+        <v>0</v>
+      </c>
+      <c r="O34" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="P34" t="n">
+        <v>7.65</v>
+      </c>
+      <c r="T34" t="n">
+        <v>1</v>
+      </c>
+      <c r="U34" t="n">
+        <v>1</v>
+      </c>
+      <c r="V34" t="n">
         <v>-6.483</v>
       </c>
-      <c r="N34" t="n">
+      <c r="W34" t="n">
         <v>-16.5</v>
       </c>
-      <c r="O34" t="n">
-        <v>10.183</v>
-      </c>
-      <c r="P34" t="n">
-        <v>24.15</v>
+      <c r="X34" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y34" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:25">
@@ -1885,16 +2065,34 @@
         <v>6.9</v>
       </c>
       <c r="M35" t="n">
+        <v>0</v>
+      </c>
+      <c r="N35" t="n">
+        <v>0</v>
+      </c>
+      <c r="O35" t="n">
+        <v>-3.7</v>
+      </c>
+      <c r="P35" t="n">
+        <v>7.65</v>
+      </c>
+      <c r="T35" t="n">
+        <v>1</v>
+      </c>
+      <c r="U35" t="n">
+        <v>1</v>
+      </c>
+      <c r="V35" t="n">
         <v>-6.483</v>
       </c>
-      <c r="N35" t="n">
+      <c r="W35" t="n">
         <v>-5.5</v>
       </c>
-      <c r="O35" t="n">
-        <v>2.782999999999999</v>
-      </c>
-      <c r="P35" t="n">
-        <v>13.15</v>
+      <c r="X35" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y35" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:25">
@@ -1929,16 +2127,34 @@
         <v>6.9</v>
       </c>
       <c r="M36" t="n">
+        <v>0</v>
+      </c>
+      <c r="N36" t="n">
+        <v>0</v>
+      </c>
+      <c r="O36" t="n">
+        <v>-1.85</v>
+      </c>
+      <c r="P36" t="n">
+        <v>7.65</v>
+      </c>
+      <c r="T36" t="n">
+        <v>1</v>
+      </c>
+      <c r="U36" t="n">
+        <v>1</v>
+      </c>
+      <c r="V36" t="n">
         <v>-17.483</v>
       </c>
-      <c r="N36" t="n">
+      <c r="W36" t="n">
         <v>-5.5</v>
       </c>
-      <c r="O36" t="n">
-        <v>15.633</v>
-      </c>
-      <c r="P36" t="n">
-        <v>13.15</v>
+      <c r="X36" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y36" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:25">
@@ -1973,16 +2189,34 @@
         <v>5.35</v>
       </c>
       <c r="M37" t="n">
+        <v>0</v>
+      </c>
+      <c r="N37" t="n">
+        <v>0</v>
+      </c>
+      <c r="O37" t="n">
+        <v>0</v>
+      </c>
+      <c r="P37" t="n">
+        <v>6.1</v>
+      </c>
+      <c r="T37" t="n">
+        <v>1</v>
+      </c>
+      <c r="U37" t="n">
+        <v>1</v>
+      </c>
+      <c r="V37" t="n">
         <v>-28.483</v>
       </c>
-      <c r="N37" t="n">
+      <c r="W37" t="n">
         <v>-5.5</v>
       </c>
-      <c r="O37" t="n">
-        <v>28.483</v>
-      </c>
-      <c r="P37" t="n">
-        <v>11.6</v>
+      <c r="X37" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y37" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:25">
@@ -2017,16 +2251,34 @@
         <v>5.35</v>
       </c>
       <c r="M38" t="n">
+        <v>0</v>
+      </c>
+      <c r="N38" t="n">
+        <v>0</v>
+      </c>
+      <c r="O38" t="n">
+        <v>1.85</v>
+      </c>
+      <c r="P38" t="n">
+        <v>6.1</v>
+      </c>
+      <c r="T38" t="n">
+        <v>1</v>
+      </c>
+      <c r="U38" t="n">
+        <v>1</v>
+      </c>
+      <c r="V38" t="n">
         <v>-28.483</v>
       </c>
-      <c r="N38" t="n">
+      <c r="W38" t="n">
         <v>-16.5</v>
       </c>
-      <c r="O38" t="n">
-        <v>30.333</v>
-      </c>
-      <c r="P38" t="n">
-        <v>22.6</v>
+      <c r="X38" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y38" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:25">
@@ -2061,16 +2313,34 @@
         <v>5.35</v>
       </c>
       <c r="M39" t="n">
+        <v>0</v>
+      </c>
+      <c r="N39" t="n">
+        <v>0</v>
+      </c>
+      <c r="O39" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="P39" t="n">
+        <v>6.1</v>
+      </c>
+      <c r="T39" t="n">
+        <v>1</v>
+      </c>
+      <c r="U39" t="n">
+        <v>1</v>
+      </c>
+      <c r="V39" t="n">
         <v>-39.483</v>
       </c>
-      <c r="N39" t="n">
+      <c r="W39" t="n">
         <v>-16.5</v>
       </c>
-      <c r="O39" t="n">
-        <v>43.183</v>
-      </c>
-      <c r="P39" t="n">
-        <v>22.6</v>
+      <c r="X39" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y39" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:25">
@@ -2105,16 +2375,34 @@
         <v>5.35</v>
       </c>
       <c r="M40" t="n">
+        <v>0</v>
+      </c>
+      <c r="N40" t="n">
+        <v>0</v>
+      </c>
+      <c r="O40" t="n">
+        <v>-3.7</v>
+      </c>
+      <c r="P40" t="n">
+        <v>6.1</v>
+      </c>
+      <c r="T40" t="n">
+        <v>1</v>
+      </c>
+      <c r="U40" t="n">
+        <v>1</v>
+      </c>
+      <c r="V40" t="n">
         <v>-39.483</v>
       </c>
-      <c r="N40" t="n">
+      <c r="W40" t="n">
         <v>-5.5</v>
       </c>
-      <c r="O40" t="n">
-        <v>35.78299999999999</v>
-      </c>
-      <c r="P40" t="n">
-        <v>11.6</v>
+      <c r="X40" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y40" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:25">
@@ -2149,16 +2437,34 @@
         <v>5.35</v>
       </c>
       <c r="M41" t="n">
+        <v>0</v>
+      </c>
+      <c r="N41" t="n">
+        <v>0</v>
+      </c>
+      <c r="O41" t="n">
+        <v>-1.85</v>
+      </c>
+      <c r="P41" t="n">
+        <v>6.1</v>
+      </c>
+      <c r="T41" t="n">
+        <v>1</v>
+      </c>
+      <c r="U41" t="n">
+        <v>1</v>
+      </c>
+      <c r="V41" t="n">
         <v>-39.483</v>
       </c>
-      <c r="N41" t="n">
+      <c r="W41" t="n">
         <v>5.5</v>
       </c>
-      <c r="O41" t="n">
-        <v>37.633</v>
-      </c>
-      <c r="P41" t="n">
-        <v>0.5999999999999996</v>
+      <c r="X41" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y41" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:25">
@@ -2193,16 +2499,34 @@
         <v>5.35</v>
       </c>
       <c r="M42" t="n">
+        <v>0</v>
+      </c>
+      <c r="N42" t="n">
+        <v>0</v>
+      </c>
+      <c r="O42" t="n">
+        <v>0</v>
+      </c>
+      <c r="P42" t="n">
+        <v>6.1</v>
+      </c>
+      <c r="T42" t="n">
+        <v>1</v>
+      </c>
+      <c r="U42" t="n">
+        <v>1</v>
+      </c>
+      <c r="V42" t="n">
         <v>-28.483</v>
       </c>
-      <c r="N42" t="n">
+      <c r="W42" t="n">
         <v>5.5</v>
       </c>
-      <c r="O42" t="n">
-        <v>28.483</v>
-      </c>
-      <c r="P42" t="n">
-        <v>0.5999999999999996</v>
+      <c r="X42" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y42" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:25">
@@ -2237,16 +2561,34 @@
         <v>3.8</v>
       </c>
       <c r="M43" t="n">
+        <v>0</v>
+      </c>
+      <c r="N43" t="n">
+        <v>0</v>
+      </c>
+      <c r="O43" t="n">
+        <v>1.85</v>
+      </c>
+      <c r="P43" t="n">
+        <v>4.55</v>
+      </c>
+      <c r="T43" t="n">
+        <v>1</v>
+      </c>
+      <c r="U43" t="n">
+        <v>1</v>
+      </c>
+      <c r="V43" t="n">
         <v>-28.483</v>
       </c>
-      <c r="N43" t="n">
+      <c r="W43" t="n">
         <v>16.5</v>
       </c>
-      <c r="O43" t="n">
-        <v>30.333</v>
-      </c>
-      <c r="P43" t="n">
-        <v>-11.95</v>
+      <c r="X43" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y43" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:25">
@@ -2281,16 +2623,34 @@
         <v>3.8</v>
       </c>
       <c r="M44" t="n">
+        <v>0</v>
+      </c>
+      <c r="N44" t="n">
+        <v>0</v>
+      </c>
+      <c r="O44" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="P44" t="n">
+        <v>4.55</v>
+      </c>
+      <c r="T44" t="n">
+        <v>1</v>
+      </c>
+      <c r="U44" t="n">
+        <v>1</v>
+      </c>
+      <c r="V44" t="n">
         <v>-39.483</v>
       </c>
-      <c r="N44" t="n">
+      <c r="W44" t="n">
         <v>16.5</v>
       </c>
-      <c r="O44" t="n">
-        <v>43.183</v>
-      </c>
-      <c r="P44" t="n">
-        <v>-11.95</v>
+      <c r="X44" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y44" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:25">
@@ -2325,16 +2685,34 @@
         <v>3.8</v>
       </c>
       <c r="M45" t="n">
+        <v>0</v>
+      </c>
+      <c r="N45" t="n">
+        <v>0</v>
+      </c>
+      <c r="O45" t="n">
+        <v>-3.7</v>
+      </c>
+      <c r="P45" t="n">
+        <v>4.55</v>
+      </c>
+      <c r="T45" t="n">
+        <v>1</v>
+      </c>
+      <c r="U45" t="n">
+        <v>1</v>
+      </c>
+      <c r="V45" t="n">
         <v>-39.483</v>
       </c>
-      <c r="N45" t="n">
+      <c r="W45" t="n">
         <v>27.5</v>
       </c>
-      <c r="O45" t="n">
-        <v>35.78299999999999</v>
-      </c>
-      <c r="P45" t="n">
-        <v>-22.95</v>
+      <c r="X45" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y45" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:25">
@@ -2369,16 +2747,34 @@
         <v>3.8</v>
       </c>
       <c r="M46" t="n">
+        <v>0</v>
+      </c>
+      <c r="N46" t="n">
+        <v>0</v>
+      </c>
+      <c r="O46" t="n">
+        <v>-1.85</v>
+      </c>
+      <c r="P46" t="n">
+        <v>4.55</v>
+      </c>
+      <c r="T46" t="n">
+        <v>1</v>
+      </c>
+      <c r="U46" t="n">
+        <v>1</v>
+      </c>
+      <c r="V46" t="n">
         <v>-39.483</v>
       </c>
-      <c r="N46" t="n">
+      <c r="W46" t="n">
         <v>38.5</v>
       </c>
-      <c r="O46" t="n">
-        <v>37.633</v>
-      </c>
-      <c r="P46" t="n">
-        <v>-33.95</v>
+      <c r="X46" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y46" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:25">
@@ -2413,16 +2809,34 @@
         <v>3.8</v>
       </c>
       <c r="M47" t="n">
+        <v>0</v>
+      </c>
+      <c r="N47" t="n">
+        <v>0</v>
+      </c>
+      <c r="O47" t="n">
+        <v>0</v>
+      </c>
+      <c r="P47" t="n">
+        <v>4.55</v>
+      </c>
+      <c r="T47" t="n">
+        <v>1</v>
+      </c>
+      <c r="U47" t="n">
+        <v>1</v>
+      </c>
+      <c r="V47" t="n">
         <v>-28.483</v>
       </c>
-      <c r="N47" t="n">
+      <c r="W47" t="n">
         <v>38.5</v>
       </c>
-      <c r="O47" t="n">
-        <v>28.483</v>
-      </c>
-      <c r="P47" t="n">
-        <v>-33.95</v>
+      <c r="X47" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y47" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:25">
@@ -2457,16 +2871,34 @@
         <v>3.8</v>
       </c>
       <c r="M48" t="n">
+        <v>0</v>
+      </c>
+      <c r="N48" t="n">
+        <v>0</v>
+      </c>
+      <c r="O48" t="n">
+        <v>1.85</v>
+      </c>
+      <c r="P48" t="n">
+        <v>4.55</v>
+      </c>
+      <c r="T48" t="n">
+        <v>1</v>
+      </c>
+      <c r="U48" t="n">
+        <v>1</v>
+      </c>
+      <c r="V48" t="n">
         <v>-28.483</v>
       </c>
-      <c r="N48" t="n">
+      <c r="W48" t="n">
         <v>27.5</v>
       </c>
-      <c r="O48" t="n">
-        <v>30.333</v>
-      </c>
-      <c r="P48" t="n">
-        <v>-22.95</v>
+      <c r="X48" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y48" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:25">
@@ -2501,16 +2933,34 @@
         <v>2.25</v>
       </c>
       <c r="M49" t="n">
+        <v>0</v>
+      </c>
+      <c r="N49" t="n">
+        <v>0</v>
+      </c>
+      <c r="O49" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="P49" t="n">
+        <v>3</v>
+      </c>
+      <c r="T49" t="n">
+        <v>1</v>
+      </c>
+      <c r="U49" t="n">
+        <v>1</v>
+      </c>
+      <c r="V49" t="n">
         <v>-17.483</v>
       </c>
-      <c r="N49" t="n">
+      <c r="W49" t="n">
         <v>27.5</v>
       </c>
-      <c r="O49" t="n">
-        <v>21.183</v>
-      </c>
-      <c r="P49" t="n">
-        <v>-24.5</v>
+      <c r="X49" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y49" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:25">
@@ -2545,16 +2995,34 @@
         <v>2.25</v>
       </c>
       <c r="M50" t="n">
+        <v>0</v>
+      </c>
+      <c r="N50" t="n">
+        <v>0</v>
+      </c>
+      <c r="O50" t="n">
+        <v>-3.7</v>
+      </c>
+      <c r="P50" t="n">
+        <v>3</v>
+      </c>
+      <c r="T50" t="n">
+        <v>1</v>
+      </c>
+      <c r="U50" t="n">
+        <v>1</v>
+      </c>
+      <c r="V50" t="n">
         <v>-17.483</v>
       </c>
-      <c r="N50" t="n">
+      <c r="W50" t="n">
         <v>38.5</v>
       </c>
-      <c r="O50" t="n">
-        <v>13.783</v>
-      </c>
-      <c r="P50" t="n">
-        <v>-35.5</v>
+      <c r="X50" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y50" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:25">
@@ -2589,16 +3057,34 @@
         <v>2.25</v>
       </c>
       <c r="M51" t="n">
+        <v>0</v>
+      </c>
+      <c r="N51" t="n">
+        <v>0</v>
+      </c>
+      <c r="O51" t="n">
+        <v>-1.85</v>
+      </c>
+      <c r="P51" t="n">
+        <v>3</v>
+      </c>
+      <c r="T51" t="n">
+        <v>1</v>
+      </c>
+      <c r="U51" t="n">
+        <v>1</v>
+      </c>
+      <c r="V51" t="n">
         <v>-6.483</v>
       </c>
-      <c r="N51" t="n">
+      <c r="W51" t="n">
         <v>38.5</v>
       </c>
-      <c r="O51" t="n">
-        <v>4.632999999999999</v>
-      </c>
-      <c r="P51" t="n">
-        <v>-35.5</v>
+      <c r="X51" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y51" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:25">
@@ -2633,16 +3119,34 @@
         <v>2.25</v>
       </c>
       <c r="M52" t="n">
+        <v>0</v>
+      </c>
+      <c r="N52" t="n">
+        <v>0</v>
+      </c>
+      <c r="O52" t="n">
+        <v>0</v>
+      </c>
+      <c r="P52" t="n">
+        <v>3</v>
+      </c>
+      <c r="T52" t="n">
+        <v>1</v>
+      </c>
+      <c r="U52" t="n">
+        <v>1</v>
+      </c>
+      <c r="V52" t="n">
         <v>-6.483</v>
       </c>
-      <c r="N52" t="n">
+      <c r="W52" t="n">
         <v>27.5</v>
       </c>
-      <c r="O52" t="n">
-        <v>6.483</v>
-      </c>
-      <c r="P52" t="n">
-        <v>-24.5</v>
+      <c r="X52" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y52" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:25">
@@ -2677,16 +3181,34 @@
         <v>2.25</v>
       </c>
       <c r="M53" t="n">
+        <v>0</v>
+      </c>
+      <c r="N53" t="n">
+        <v>0</v>
+      </c>
+      <c r="O53" t="n">
+        <v>1.85</v>
+      </c>
+      <c r="P53" t="n">
+        <v>3</v>
+      </c>
+      <c r="T53" t="n">
+        <v>1</v>
+      </c>
+      <c r="U53" t="n">
+        <v>1</v>
+      </c>
+      <c r="V53" t="n">
         <v>-6.483</v>
       </c>
-      <c r="N53" t="n">
+      <c r="W53" t="n">
         <v>16.5</v>
       </c>
-      <c r="O53" t="n">
-        <v>8.333</v>
-      </c>
-      <c r="P53" t="n">
-        <v>-13.5</v>
+      <c r="X53" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y53" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:25">
@@ -2721,16 +3243,34 @@
         <v>2.25</v>
       </c>
       <c r="M54" t="n">
+        <v>0</v>
+      </c>
+      <c r="N54" t="n">
+        <v>0</v>
+      </c>
+      <c r="O54" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="P54" t="n">
+        <v>3</v>
+      </c>
+      <c r="T54" t="n">
+        <v>1</v>
+      </c>
+      <c r="U54" t="n">
+        <v>1</v>
+      </c>
+      <c r="V54" t="n">
         <v>-17.483</v>
       </c>
-      <c r="N54" t="n">
+      <c r="W54" t="n">
         <v>16.5</v>
       </c>
-      <c r="O54" t="n">
-        <v>21.183</v>
-      </c>
-      <c r="P54" t="n">
-        <v>-13.5</v>
+      <c r="X54" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y54" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:25">
@@ -2765,16 +3305,34 @@
         <v>-2.2</v>
       </c>
       <c r="M55" t="n">
+        <v>0</v>
+      </c>
+      <c r="N55" t="n">
+        <v>0</v>
+      </c>
+      <c r="O55" t="n">
+        <v>-0.9</v>
+      </c>
+      <c r="P55" t="n">
+        <v>-1.45</v>
+      </c>
+      <c r="T55" t="n">
+        <v>1</v>
+      </c>
+      <c r="U55" t="n">
+        <v>1</v>
+      </c>
+      <c r="V55" t="n">
         <v>-17.483</v>
       </c>
-      <c r="N55" t="n">
+      <c r="W55" t="n">
         <v>5.5</v>
       </c>
-      <c r="O55" t="n">
-        <v>16.583</v>
-      </c>
-      <c r="P55" t="n">
-        <v>-6.95</v>
+      <c r="X55" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y55" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:25">
@@ -2809,16 +3367,34 @@
         <v>-2.2</v>
       </c>
       <c r="M56" t="n">
+        <v>0</v>
+      </c>
+      <c r="N56" t="n">
+        <v>0</v>
+      </c>
+      <c r="O56" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="P56" t="n">
+        <v>-1.45</v>
+      </c>
+      <c r="T56" t="n">
+        <v>1</v>
+      </c>
+      <c r="U56" t="n">
+        <v>1</v>
+      </c>
+      <c r="V56" t="n">
         <v>-6.483</v>
       </c>
-      <c r="N56" t="n">
+      <c r="W56" t="n">
         <v>5.5</v>
       </c>
-      <c r="O56" t="n">
-        <v>7.383</v>
-      </c>
-      <c r="P56" t="n">
-        <v>-6.95</v>
+      <c r="X56" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y56" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:25">
@@ -2853,16 +3429,34 @@
         <v>0.7</v>
       </c>
       <c r="M57" t="n">
+        <v>0</v>
+      </c>
+      <c r="N57" t="n">
+        <v>0</v>
+      </c>
+      <c r="O57" t="n">
+        <v>-0.9</v>
+      </c>
+      <c r="P57" t="n">
+        <v>1.45</v>
+      </c>
+      <c r="T57" t="n">
+        <v>1</v>
+      </c>
+      <c r="U57" t="n">
+        <v>1</v>
+      </c>
+      <c r="V57" t="n">
         <v>4.517</v>
       </c>
-      <c r="N57" t="n">
+      <c r="W57" t="n">
         <v>5.5</v>
       </c>
-      <c r="O57" t="n">
-        <v>-5.417000000000001</v>
-      </c>
-      <c r="P57" t="n">
-        <v>-4.05</v>
+      <c r="X57" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y57" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="58" spans="1:25">
@@ -2897,16 +3491,34 @@
         <v>0.7</v>
       </c>
       <c r="M58" t="n">
+        <v>0</v>
+      </c>
+      <c r="N58" t="n">
+        <v>0</v>
+      </c>
+      <c r="O58" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="P58" t="n">
+        <v>1.45</v>
+      </c>
+      <c r="T58" t="n">
+        <v>1</v>
+      </c>
+      <c r="U58" t="n">
+        <v>1</v>
+      </c>
+      <c r="V58" t="n">
         <v>15.517</v>
       </c>
-      <c r="N58" t="n">
+      <c r="W58" t="n">
         <v>5.5</v>
       </c>
-      <c r="O58" t="n">
-        <v>-14.617</v>
-      </c>
-      <c r="P58" t="n">
-        <v>-4.05</v>
+      <c r="X58" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y58" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:25">
@@ -2941,16 +3553,34 @@
         <v>-9.949999999999999</v>
       </c>
       <c r="M59" t="n">
+        <v>0</v>
+      </c>
+      <c r="N59" t="n">
+        <v>0</v>
+      </c>
+      <c r="O59" t="n">
+        <v>-3.7</v>
+      </c>
+      <c r="P59" t="n">
+        <v>-9.199999999999999</v>
+      </c>
+      <c r="T59" t="n">
+        <v>1</v>
+      </c>
+      <c r="U59" t="n">
+        <v>1</v>
+      </c>
+      <c r="V59" t="n">
         <v>15.517</v>
       </c>
-      <c r="N59" t="n">
+      <c r="W59" t="n">
         <v>16.5</v>
       </c>
-      <c r="O59" t="n">
-        <v>-19.217</v>
-      </c>
-      <c r="P59" t="n">
-        <v>-25.7</v>
+      <c r="X59" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y59" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="60" spans="1:25">
@@ -2985,16 +3615,34 @@
         <v>-9.949999999999999</v>
       </c>
       <c r="M60" t="n">
+        <v>0</v>
+      </c>
+      <c r="N60" t="n">
+        <v>0</v>
+      </c>
+      <c r="O60" t="n">
+        <v>-1.85</v>
+      </c>
+      <c r="P60" t="n">
+        <v>-9.199999999999999</v>
+      </c>
+      <c r="T60" t="n">
+        <v>1</v>
+      </c>
+      <c r="U60" t="n">
+        <v>1</v>
+      </c>
+      <c r="V60" t="n">
         <v>4.517</v>
       </c>
-      <c r="N60" t="n">
+      <c r="W60" t="n">
         <v>16.5</v>
       </c>
-      <c r="O60" t="n">
-        <v>-6.367000000000001</v>
-      </c>
-      <c r="P60" t="n">
-        <v>-25.7</v>
+      <c r="X60" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y60" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:25">
@@ -3029,16 +3677,34 @@
         <v>-9.949999999999999</v>
       </c>
       <c r="M61" t="n">
+        <v>0</v>
+      </c>
+      <c r="N61" t="n">
+        <v>0</v>
+      </c>
+      <c r="O61" t="n">
+        <v>0</v>
+      </c>
+      <c r="P61" t="n">
+        <v>-9.199999999999999</v>
+      </c>
+      <c r="T61" t="n">
+        <v>1</v>
+      </c>
+      <c r="U61" t="n">
+        <v>1</v>
+      </c>
+      <c r="V61" t="n">
         <v>4.517</v>
       </c>
-      <c r="N61" t="n">
+      <c r="W61" t="n">
         <v>27.5</v>
       </c>
-      <c r="O61" t="n">
-        <v>-4.517</v>
-      </c>
-      <c r="P61" t="n">
-        <v>-36.7</v>
+      <c r="X61" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y61" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="62" spans="1:25">
@@ -3073,16 +3739,34 @@
         <v>-9.949999999999999</v>
       </c>
       <c r="M62" t="n">
+        <v>0</v>
+      </c>
+      <c r="N62" t="n">
+        <v>0</v>
+      </c>
+      <c r="O62" t="n">
+        <v>1.85</v>
+      </c>
+      <c r="P62" t="n">
+        <v>-9.199999999999999</v>
+      </c>
+      <c r="T62" t="n">
+        <v>1</v>
+      </c>
+      <c r="U62" t="n">
+        <v>1</v>
+      </c>
+      <c r="V62" t="n">
         <v>4.517</v>
       </c>
-      <c r="N62" t="n">
+      <c r="W62" t="n">
         <v>38.5</v>
       </c>
-      <c r="O62" t="n">
-        <v>-2.667</v>
-      </c>
-      <c r="P62" t="n">
-        <v>-47.7</v>
+      <c r="X62" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y62" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="63" spans="1:25">
@@ -3117,16 +3801,34 @@
         <v>-9.949999999999999</v>
       </c>
       <c r="M63" t="n">
+        <v>0</v>
+      </c>
+      <c r="N63" t="n">
+        <v>0</v>
+      </c>
+      <c r="O63" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="P63" t="n">
+        <v>-9.199999999999999</v>
+      </c>
+      <c r="T63" t="n">
+        <v>1</v>
+      </c>
+      <c r="U63" t="n">
+        <v>1</v>
+      </c>
+      <c r="V63" t="n">
         <v>15.517</v>
       </c>
-      <c r="N63" t="n">
+      <c r="W63" t="n">
         <v>38.5</v>
       </c>
-      <c r="O63" t="n">
-        <v>-11.817</v>
-      </c>
-      <c r="P63" t="n">
-        <v>-47.7</v>
+      <c r="X63" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y63" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="64" spans="1:25">
@@ -3161,16 +3863,34 @@
         <v>-9.949999999999999</v>
       </c>
       <c r="M64" t="n">
+        <v>0</v>
+      </c>
+      <c r="N64" t="n">
+        <v>0</v>
+      </c>
+      <c r="O64" t="n">
+        <v>-3.7</v>
+      </c>
+      <c r="P64" t="n">
+        <v>-9.199999999999999</v>
+      </c>
+      <c r="T64" t="n">
+        <v>1</v>
+      </c>
+      <c r="U64" t="n">
+        <v>1</v>
+      </c>
+      <c r="V64" t="n">
         <v>15.517</v>
       </c>
-      <c r="N64" t="n">
+      <c r="W64" t="n">
         <v>27.5</v>
       </c>
-      <c r="O64" t="n">
-        <v>-19.217</v>
-      </c>
-      <c r="P64" t="n">
-        <v>-36.7</v>
+      <c r="X64" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y64" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="65" spans="1:25">
@@ -3205,16 +3925,34 @@
         <v>-8.4</v>
       </c>
       <c r="M65" t="n">
+        <v>0</v>
+      </c>
+      <c r="N65" t="n">
+        <v>0</v>
+      </c>
+      <c r="O65" t="n">
+        <v>-1.85</v>
+      </c>
+      <c r="P65" t="n">
+        <v>-7.65</v>
+      </c>
+      <c r="T65" t="n">
+        <v>1</v>
+      </c>
+      <c r="U65" t="n">
+        <v>1</v>
+      </c>
+      <c r="V65" t="n">
         <v>26.517</v>
       </c>
-      <c r="N65" t="n">
+      <c r="W65" t="n">
         <v>27.5</v>
       </c>
-      <c r="O65" t="n">
-        <v>-28.367</v>
-      </c>
-      <c r="P65" t="n">
-        <v>-35.15</v>
+      <c r="X65" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y65" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="66" spans="1:25">
@@ -3249,16 +3987,34 @@
         <v>-8.4</v>
       </c>
       <c r="M66" t="n">
+        <v>0</v>
+      </c>
+      <c r="N66" t="n">
+        <v>0</v>
+      </c>
+      <c r="O66" t="n">
+        <v>0</v>
+      </c>
+      <c r="P66" t="n">
+        <v>-7.65</v>
+      </c>
+      <c r="T66" t="n">
+        <v>1</v>
+      </c>
+      <c r="U66" t="n">
+        <v>1</v>
+      </c>
+      <c r="V66" t="n">
         <v>26.517</v>
       </c>
-      <c r="N66" t="n">
+      <c r="W66" t="n">
         <v>38.5</v>
       </c>
-      <c r="O66" t="n">
-        <v>-26.517</v>
-      </c>
-      <c r="P66" t="n">
-        <v>-46.15</v>
+      <c r="X66" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y66" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="67" spans="1:25">
@@ -3293,16 +4049,34 @@
         <v>-8.4</v>
       </c>
       <c r="M67" t="n">
+        <v>0</v>
+      </c>
+      <c r="N67" t="n">
+        <v>0</v>
+      </c>
+      <c r="O67" t="n">
+        <v>1.85</v>
+      </c>
+      <c r="P67" t="n">
+        <v>-7.65</v>
+      </c>
+      <c r="T67" t="n">
+        <v>1</v>
+      </c>
+      <c r="U67" t="n">
+        <v>1</v>
+      </c>
+      <c r="V67" t="n">
         <v>37.517</v>
       </c>
-      <c r="N67" t="n">
+      <c r="W67" t="n">
         <v>38.5</v>
       </c>
-      <c r="O67" t="n">
-        <v>-35.667</v>
-      </c>
-      <c r="P67" t="n">
-        <v>-46.15</v>
+      <c r="X67" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y67" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="68" spans="1:25">
@@ -3337,16 +4111,34 @@
         <v>-8.4</v>
       </c>
       <c r="M68" t="n">
+        <v>0</v>
+      </c>
+      <c r="N68" t="n">
+        <v>0</v>
+      </c>
+      <c r="O68" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="P68" t="n">
+        <v>-7.65</v>
+      </c>
+      <c r="T68" t="n">
+        <v>1</v>
+      </c>
+      <c r="U68" t="n">
+        <v>1</v>
+      </c>
+      <c r="V68" t="n">
         <v>37.517</v>
       </c>
-      <c r="N68" t="n">
+      <c r="W68" t="n">
         <v>27.5</v>
       </c>
-      <c r="O68" t="n">
-        <v>-33.817</v>
-      </c>
-      <c r="P68" t="n">
-        <v>-35.15</v>
+      <c r="X68" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y68" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="69" spans="1:25">
@@ -3381,16 +4173,34 @@
         <v>-8.4</v>
       </c>
       <c r="M69" t="n">
+        <v>0</v>
+      </c>
+      <c r="N69" t="n">
+        <v>0</v>
+      </c>
+      <c r="O69" t="n">
+        <v>-3.7</v>
+      </c>
+      <c r="P69" t="n">
+        <v>-7.65</v>
+      </c>
+      <c r="T69" t="n">
+        <v>1</v>
+      </c>
+      <c r="U69" t="n">
+        <v>1</v>
+      </c>
+      <c r="V69" t="n">
         <v>37.517</v>
       </c>
-      <c r="N69" t="n">
+      <c r="W69" t="n">
         <v>16.5</v>
       </c>
-      <c r="O69" t="n">
-        <v>-41.21700000000001</v>
-      </c>
-      <c r="P69" t="n">
-        <v>-24.15</v>
+      <c r="X69" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y69" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="70" spans="1:25">
@@ -3425,16 +4235,34 @@
         <v>-8.4</v>
       </c>
       <c r="M70" t="n">
+        <v>0</v>
+      </c>
+      <c r="N70" t="n">
+        <v>0</v>
+      </c>
+      <c r="O70" t="n">
+        <v>-1.85</v>
+      </c>
+      <c r="P70" t="n">
+        <v>-7.65</v>
+      </c>
+      <c r="T70" t="n">
+        <v>1</v>
+      </c>
+      <c r="U70" t="n">
+        <v>1</v>
+      </c>
+      <c r="V70" t="n">
         <v>26.517</v>
       </c>
-      <c r="N70" t="n">
+      <c r="W70" t="n">
         <v>16.5</v>
       </c>
-      <c r="O70" t="n">
-        <v>-28.367</v>
-      </c>
-      <c r="P70" t="n">
-        <v>-24.15</v>
+      <c r="X70" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y70" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="71" spans="1:25">
@@ -3469,16 +4297,34 @@
         <v>-6.85</v>
       </c>
       <c r="M71" t="n">
+        <v>0</v>
+      </c>
+      <c r="N71" t="n">
+        <v>0</v>
+      </c>
+      <c r="O71" t="n">
+        <v>0</v>
+      </c>
+      <c r="P71" t="n">
+        <v>-6.1</v>
+      </c>
+      <c r="T71" t="n">
+        <v>1</v>
+      </c>
+      <c r="U71" t="n">
+        <v>1</v>
+      </c>
+      <c r="V71" t="n">
         <v>26.517</v>
       </c>
-      <c r="N71" t="n">
+      <c r="W71" t="n">
         <v>5.5</v>
       </c>
-      <c r="O71" t="n">
-        <v>-26.517</v>
-      </c>
-      <c r="P71" t="n">
-        <v>-11.6</v>
+      <c r="X71" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y71" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="72" spans="1:25">
@@ -3513,16 +4359,34 @@
         <v>-6.85</v>
       </c>
       <c r="M72" t="n">
+        <v>0</v>
+      </c>
+      <c r="N72" t="n">
+        <v>0</v>
+      </c>
+      <c r="O72" t="n">
+        <v>1.85</v>
+      </c>
+      <c r="P72" t="n">
+        <v>-6.1</v>
+      </c>
+      <c r="T72" t="n">
+        <v>1</v>
+      </c>
+      <c r="U72" t="n">
+        <v>1</v>
+      </c>
+      <c r="V72" t="n">
         <v>37.517</v>
       </c>
-      <c r="N72" t="n">
+      <c r="W72" t="n">
         <v>5.5</v>
       </c>
-      <c r="O72" t="n">
-        <v>-35.667</v>
-      </c>
-      <c r="P72" t="n">
-        <v>-11.6</v>
+      <c r="X72" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y72" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="73" spans="1:25">
@@ -3557,16 +4421,34 @@
         <v>-6.85</v>
       </c>
       <c r="M73" t="n">
+        <v>0</v>
+      </c>
+      <c r="N73" t="n">
+        <v>0</v>
+      </c>
+      <c r="O73" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="P73" t="n">
+        <v>-6.1</v>
+      </c>
+      <c r="T73" t="n">
+        <v>1</v>
+      </c>
+      <c r="U73" t="n">
+        <v>1</v>
+      </c>
+      <c r="V73" t="n">
         <v>37.517</v>
       </c>
-      <c r="N73" t="n">
+      <c r="W73" t="n">
         <v>-5.5</v>
       </c>
-      <c r="O73" t="n">
-        <v>-33.817</v>
-      </c>
-      <c r="P73" t="n">
-        <v>-0.5999999999999996</v>
+      <c r="X73" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y73" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="74" spans="1:25">
@@ -3601,16 +4483,34 @@
         <v>-6.85</v>
       </c>
       <c r="M74" t="n">
+        <v>0</v>
+      </c>
+      <c r="N74" t="n">
+        <v>0</v>
+      </c>
+      <c r="O74" t="n">
+        <v>-3.7</v>
+      </c>
+      <c r="P74" t="n">
+        <v>-6.1</v>
+      </c>
+      <c r="T74" t="n">
+        <v>1</v>
+      </c>
+      <c r="U74" t="n">
+        <v>1</v>
+      </c>
+      <c r="V74" t="n">
         <v>37.517</v>
       </c>
-      <c r="N74" t="n">
+      <c r="W74" t="n">
         <v>-16.5</v>
       </c>
-      <c r="O74" t="n">
-        <v>-41.21700000000001</v>
-      </c>
-      <c r="P74" t="n">
-        <v>10.4</v>
+      <c r="X74" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y74" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="75" spans="1:25">
@@ -3645,16 +4545,34 @@
         <v>-6.85</v>
       </c>
       <c r="M75" t="n">
+        <v>0</v>
+      </c>
+      <c r="N75" t="n">
+        <v>0</v>
+      </c>
+      <c r="O75" t="n">
+        <v>-1.85</v>
+      </c>
+      <c r="P75" t="n">
+        <v>-6.1</v>
+      </c>
+      <c r="T75" t="n">
+        <v>1</v>
+      </c>
+      <c r="U75" t="n">
+        <v>1</v>
+      </c>
+      <c r="V75" t="n">
         <v>26.517</v>
       </c>
-      <c r="N75" t="n">
+      <c r="W75" t="n">
         <v>-16.5</v>
       </c>
-      <c r="O75" t="n">
-        <v>-28.367</v>
-      </c>
-      <c r="P75" t="n">
-        <v>10.4</v>
+      <c r="X75" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y75" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="76" spans="1:25">
@@ -3689,16 +4607,34 @@
         <v>-6.85</v>
       </c>
       <c r="M76" t="n">
+        <v>0</v>
+      </c>
+      <c r="N76" t="n">
+        <v>0</v>
+      </c>
+      <c r="O76" t="n">
+        <v>0</v>
+      </c>
+      <c r="P76" t="n">
+        <v>-6.1</v>
+      </c>
+      <c r="T76" t="n">
+        <v>1</v>
+      </c>
+      <c r="U76" t="n">
+        <v>1</v>
+      </c>
+      <c r="V76" t="n">
         <v>26.517</v>
       </c>
-      <c r="N76" t="n">
+      <c r="W76" t="n">
         <v>-5.5</v>
       </c>
-      <c r="O76" t="n">
-        <v>-26.517</v>
-      </c>
-      <c r="P76" t="n">
-        <v>-0.5999999999999996</v>
+      <c r="X76" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y76" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="77" spans="1:25">
@@ -3733,16 +4669,34 @@
         <v>-5.3</v>
       </c>
       <c r="M77" t="n">
+        <v>0</v>
+      </c>
+      <c r="N77" t="n">
+        <v>0</v>
+      </c>
+      <c r="O77" t="n">
+        <v>1.85</v>
+      </c>
+      <c r="P77" t="n">
+        <v>-4.55</v>
+      </c>
+      <c r="T77" t="n">
+        <v>1</v>
+      </c>
+      <c r="U77" t="n">
+        <v>1</v>
+      </c>
+      <c r="V77" t="n">
         <v>15.517</v>
       </c>
-      <c r="N77" t="n">
+      <c r="W77" t="n">
         <v>-5.5</v>
       </c>
-      <c r="O77" t="n">
-        <v>-13.667</v>
-      </c>
-      <c r="P77" t="n">
-        <v>0.9500000000000002</v>
+      <c r="X77" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y77" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="78" spans="1:25">
@@ -3777,16 +4731,34 @@
         <v>-5.3</v>
       </c>
       <c r="M78" t="n">
+        <v>0</v>
+      </c>
+      <c r="N78" t="n">
+        <v>0</v>
+      </c>
+      <c r="O78" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="P78" t="n">
+        <v>-4.55</v>
+      </c>
+      <c r="T78" t="n">
+        <v>1</v>
+      </c>
+      <c r="U78" t="n">
+        <v>1</v>
+      </c>
+      <c r="V78" t="n">
         <v>4.517</v>
       </c>
-      <c r="N78" t="n">
+      <c r="W78" t="n">
         <v>-5.5</v>
       </c>
-      <c r="O78" t="n">
-        <v>-0.8170000000000002</v>
-      </c>
-      <c r="P78" t="n">
-        <v>0.9500000000000002</v>
+      <c r="X78" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y78" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="79" spans="1:25">
@@ -3821,16 +4793,34 @@
         <v>-5.3</v>
       </c>
       <c r="M79" t="n">
+        <v>0</v>
+      </c>
+      <c r="N79" t="n">
+        <v>0</v>
+      </c>
+      <c r="O79" t="n">
+        <v>-3.7</v>
+      </c>
+      <c r="P79" t="n">
+        <v>-4.55</v>
+      </c>
+      <c r="T79" t="n">
+        <v>1</v>
+      </c>
+      <c r="U79" t="n">
+        <v>1</v>
+      </c>
+      <c r="V79" t="n">
         <v>4.517</v>
       </c>
-      <c r="N79" t="n">
+      <c r="W79" t="n">
         <v>-16.5</v>
       </c>
-      <c r="O79" t="n">
-        <v>-8.217000000000001</v>
-      </c>
-      <c r="P79" t="n">
-        <v>11.95</v>
+      <c r="X79" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y79" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="80" spans="1:25">
@@ -3865,16 +4855,34 @@
         <v>-5.3</v>
       </c>
       <c r="M80" t="n">
+        <v>0</v>
+      </c>
+      <c r="N80" t="n">
+        <v>0</v>
+      </c>
+      <c r="O80" t="n">
+        <v>-1.85</v>
+      </c>
+      <c r="P80" t="n">
+        <v>-4.55</v>
+      </c>
+      <c r="T80" t="n">
+        <v>1</v>
+      </c>
+      <c r="U80" t="n">
+        <v>1</v>
+      </c>
+      <c r="V80" t="n">
         <v>15.517</v>
       </c>
-      <c r="N80" t="n">
+      <c r="W80" t="n">
         <v>-16.5</v>
       </c>
-      <c r="O80" t="n">
-        <v>-17.367</v>
-      </c>
-      <c r="P80" t="n">
-        <v>11.95</v>
+      <c r="X80" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y80" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="81" spans="1:25">
@@ -3909,16 +4917,34 @@
         <v>-5.3</v>
       </c>
       <c r="M81" t="n">
+        <v>0</v>
+      </c>
+      <c r="N81" t="n">
+        <v>0</v>
+      </c>
+      <c r="O81" t="n">
+        <v>0</v>
+      </c>
+      <c r="P81" t="n">
+        <v>-4.55</v>
+      </c>
+      <c r="T81" t="n">
+        <v>1</v>
+      </c>
+      <c r="U81" t="n">
+        <v>1</v>
+      </c>
+      <c r="V81" t="n">
         <v>15.517</v>
       </c>
-      <c r="N81" t="n">
+      <c r="W81" t="n">
         <v>-27.5</v>
       </c>
-      <c r="O81" t="n">
-        <v>-15.517</v>
-      </c>
-      <c r="P81" t="n">
-        <v>22.95</v>
+      <c r="X81" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y81" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="82" spans="1:25">
@@ -3953,16 +4979,34 @@
         <v>-5.3</v>
       </c>
       <c r="M82" t="n">
+        <v>0</v>
+      </c>
+      <c r="N82" t="n">
+        <v>0</v>
+      </c>
+      <c r="O82" t="n">
+        <v>1.85</v>
+      </c>
+      <c r="P82" t="n">
+        <v>-4.55</v>
+      </c>
+      <c r="T82" t="n">
+        <v>1</v>
+      </c>
+      <c r="U82" t="n">
+        <v>1</v>
+      </c>
+      <c r="V82" t="n">
         <v>4.517</v>
       </c>
-      <c r="N82" t="n">
+      <c r="W82" t="n">
         <v>-27.5</v>
       </c>
-      <c r="O82" t="n">
-        <v>-2.667</v>
-      </c>
-      <c r="P82" t="n">
-        <v>22.95</v>
+      <c r="X82" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y82" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="83" spans="1:25">
@@ -3997,16 +5041,34 @@
         <v>-3.75</v>
       </c>
       <c r="M83" t="n">
+        <v>0</v>
+      </c>
+      <c r="N83" t="n">
+        <v>0</v>
+      </c>
+      <c r="O83" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="P83" t="n">
+        <v>-3</v>
+      </c>
+      <c r="T83" t="n">
+        <v>1</v>
+      </c>
+      <c r="U83" t="n">
+        <v>1</v>
+      </c>
+      <c r="V83" t="n">
         <v>4.517</v>
       </c>
-      <c r="N83" t="n">
+      <c r="W83" t="n">
         <v>-38.5</v>
       </c>
-      <c r="O83" t="n">
-        <v>-0.8170000000000002</v>
-      </c>
-      <c r="P83" t="n">
-        <v>35.5</v>
+      <c r="X83" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y83" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="84" spans="1:25">
@@ -4041,16 +5103,34 @@
         <v>-3.75</v>
       </c>
       <c r="M84" t="n">
+        <v>0</v>
+      </c>
+      <c r="N84" t="n">
+        <v>0</v>
+      </c>
+      <c r="O84" t="n">
+        <v>-3.7</v>
+      </c>
+      <c r="P84" t="n">
+        <v>-3</v>
+      </c>
+      <c r="T84" t="n">
+        <v>1</v>
+      </c>
+      <c r="U84" t="n">
+        <v>1</v>
+      </c>
+      <c r="V84" t="n">
         <v>15.517</v>
       </c>
-      <c r="N84" t="n">
+      <c r="W84" t="n">
         <v>-38.5</v>
       </c>
-      <c r="O84" t="n">
-        <v>-19.217</v>
-      </c>
-      <c r="P84" t="n">
-        <v>35.5</v>
+      <c r="X84" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y84" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="85" spans="1:25">
@@ -4085,16 +5165,34 @@
         <v>-3.75</v>
       </c>
       <c r="M85" t="n">
+        <v>0</v>
+      </c>
+      <c r="N85" t="n">
+        <v>0</v>
+      </c>
+      <c r="O85" t="n">
+        <v>-1.85</v>
+      </c>
+      <c r="P85" t="n">
+        <v>-3</v>
+      </c>
+      <c r="T85" t="n">
+        <v>1</v>
+      </c>
+      <c r="U85" t="n">
+        <v>1</v>
+      </c>
+      <c r="V85" t="n">
         <v>26.517</v>
       </c>
-      <c r="N85" t="n">
+      <c r="W85" t="n">
         <v>-38.5</v>
       </c>
-      <c r="O85" t="n">
-        <v>-28.367</v>
-      </c>
-      <c r="P85" t="n">
-        <v>35.5</v>
+      <c r="X85" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y85" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="86" spans="1:25">
@@ -4129,16 +5227,34 @@
         <v>-3.75</v>
       </c>
       <c r="M86" t="n">
+        <v>0</v>
+      </c>
+      <c r="N86" t="n">
+        <v>0</v>
+      </c>
+      <c r="O86" t="n">
+        <v>0</v>
+      </c>
+      <c r="P86" t="n">
+        <v>-3</v>
+      </c>
+      <c r="T86" t="n">
+        <v>1</v>
+      </c>
+      <c r="U86" t="n">
+        <v>1</v>
+      </c>
+      <c r="V86" t="n">
         <v>26.517</v>
       </c>
-      <c r="N86" t="n">
+      <c r="W86" t="n">
         <v>-27.5</v>
       </c>
-      <c r="O86" t="n">
-        <v>-26.517</v>
-      </c>
-      <c r="P86" t="n">
-        <v>24.5</v>
+      <c r="X86" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y86" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="87" spans="1:25">
@@ -4173,16 +5289,34 @@
         <v>-3.75</v>
       </c>
       <c r="M87" t="n">
+        <v>0</v>
+      </c>
+      <c r="N87" t="n">
+        <v>0</v>
+      </c>
+      <c r="O87" t="n">
+        <v>1.85</v>
+      </c>
+      <c r="P87" t="n">
+        <v>-3</v>
+      </c>
+      <c r="T87" t="n">
+        <v>1</v>
+      </c>
+      <c r="U87" t="n">
+        <v>1</v>
+      </c>
+      <c r="V87" t="n">
         <v>37.517</v>
       </c>
-      <c r="N87" t="n">
+      <c r="W87" t="n">
         <v>-27.5</v>
       </c>
-      <c r="O87" t="n">
-        <v>-35.667</v>
-      </c>
-      <c r="P87" t="n">
-        <v>24.5</v>
+      <c r="X87" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y87" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="88" spans="1:25">
@@ -4217,16 +5351,34 @@
         <v>-3.75</v>
       </c>
       <c r="M88" t="n">
+        <v>0</v>
+      </c>
+      <c r="N88" t="n">
+        <v>0</v>
+      </c>
+      <c r="O88" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="P88" t="n">
+        <v>-3</v>
+      </c>
+      <c r="T88" t="n">
+        <v>1</v>
+      </c>
+      <c r="U88" t="n">
+        <v>1</v>
+      </c>
+      <c r="V88" t="n">
         <v>37.517</v>
       </c>
-      <c r="N88" t="n">
+      <c r="W88" t="n">
         <v>-38.5</v>
       </c>
-      <c r="O88" t="n">
-        <v>-33.817</v>
-      </c>
-      <c r="P88" t="n">
-        <v>35.5</v>
+      <c r="X88" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y88" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="89" spans="1:25">
@@ -4261,13 +5413,13 @@
         <v>-0.6</v>
       </c>
       <c r="M89" t="n">
-        <v>-0.5629999999999999</v>
+        <v>0</v>
       </c>
       <c r="N89" t="n">
         <v>0</v>
       </c>
       <c r="O89" t="n">
-        <v>-0.7370000000000001</v>
+        <v>-1.3</v>
       </c>
       <c r="P89" t="n">
         <v>0</v>
@@ -4323,13 +5475,13 @@
         <v>-0.65</v>
       </c>
       <c r="M90" t="n">
-        <v>0.2585</v>
+        <v>0</v>
       </c>
       <c r="N90" t="n">
         <v>0</v>
       </c>
       <c r="O90" t="n">
-        <v>-0.2585</v>
+        <v>0</v>
       </c>
       <c r="P90" t="n">
         <v>0</v>
@@ -4509,16 +5661,16 @@
         <v>-0.75</v>
       </c>
       <c r="M93" t="n">
-        <v>0</v>
+        <v>-2.996000000000001</v>
       </c>
       <c r="N93" t="n">
-        <v>0</v>
+        <v>16.302</v>
       </c>
       <c r="O93" t="n">
-        <v>3</v>
+        <v>5.996</v>
       </c>
       <c r="P93" t="n">
-        <v>-0.35</v>
+        <v>-16.652</v>
       </c>
       <c r="T93" t="n">
         <v>1</v>
@@ -4571,16 +5723,16 @@
         <v>0.25</v>
       </c>
       <c r="M94" t="n">
-        <v>-0.3</v>
+        <v>0</v>
       </c>
       <c r="N94" t="n">
-        <v>0.756</v>
+        <v>0</v>
       </c>
       <c r="O94" t="n">
-        <v>2.5</v>
+        <v>2.2</v>
       </c>
       <c r="P94" t="n">
-        <v>-0.106</v>
+        <v>0.65</v>
       </c>
       <c r="T94" t="n">
         <v>8</v>
@@ -4633,16 +5785,16 @@
         <v>-0.55</v>
       </c>
       <c r="M95" t="n">
-        <v>-0.3</v>
+        <v>0</v>
       </c>
       <c r="N95" t="n">
-        <v>-0.662</v>
+        <v>0</v>
       </c>
       <c r="O95" t="n">
-        <v>2.5</v>
+        <v>2.2</v>
       </c>
       <c r="P95" t="n">
-        <v>0.412</v>
+        <v>-0.25</v>
       </c>
       <c r="T95" t="n">
         <v>8</v>
@@ -4757,16 +5909,16 @@
         <v>10.6</v>
       </c>
       <c r="M97" t="n">
-        <v>-47</v>
+        <v>0</v>
       </c>
       <c r="N97" t="n">
-        <v>-39.459</v>
+        <v>-38.5</v>
       </c>
       <c r="O97" t="n">
-        <v>47</v>
+        <v>0</v>
       </c>
       <c r="P97" t="n">
-        <v>50.259</v>
+        <v>49.3</v>
       </c>
       <c r="T97" t="n">
         <v>1</v>
@@ -4819,16 +5971,16 @@
         <v>-11.2</v>
       </c>
       <c r="M98" t="n">
-        <v>-44.004</v>
+        <v>2.996</v>
       </c>
       <c r="N98" t="n">
-        <v>-28.455</v>
+        <v>-27.496</v>
       </c>
       <c r="O98" t="n">
-        <v>54.604</v>
+        <v>7.603999999999999</v>
       </c>
       <c r="P98" t="n">
-        <v>28.455</v>
+        <v>27.496</v>
       </c>
       <c r="T98" t="n">
         <v>1</v>
@@ -5129,16 +6281,16 @@
         <v>0.2</v>
       </c>
       <c r="M103" t="n">
-        <v>-0.3</v>
+        <v>0</v>
       </c>
       <c r="N103" t="n">
-        <v>-0.767</v>
+        <v>0</v>
       </c>
       <c r="O103" t="n">
-        <v>2.05</v>
+        <v>1.75</v>
       </c>
       <c r="P103" t="n">
-        <v>1.167</v>
+        <v>0.4</v>
       </c>
       <c r="T103" t="n">
         <v>8</v>
@@ -5191,13 +6343,13 @@
         <v>-3.05</v>
       </c>
       <c r="M104" t="n">
-        <v>-0.5629999999999999</v>
+        <v>0</v>
       </c>
       <c r="N104" t="n">
         <v>0</v>
       </c>
       <c r="O104" t="n">
-        <v>7.013</v>
+        <v>6.45</v>
       </c>
       <c r="P104" t="n">
         <v>-2.15</v>
@@ -5253,16 +6405,16 @@
         <v>0.25</v>
       </c>
       <c r="M105" t="n">
-        <v>0</v>
+        <v>-2.996000000000001</v>
       </c>
       <c r="N105" t="n">
-        <v>0</v>
+        <v>16.302</v>
       </c>
       <c r="O105" t="n">
-        <v>3</v>
+        <v>5.996</v>
       </c>
       <c r="P105" t="n">
-        <v>0.65</v>
+        <v>-15.652</v>
       </c>
       <c r="T105" t="n">
         <v>1</v>

</xml_diff>

<commit_message>
fixed a long standing bug in rotating the capacitors before inverting
</commit_message>
<xml_diff>
--- a/masks/code/ResonatorArray.xlsx
+++ b/masks/code/ResonatorArray.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -5639,13 +5639,13 @@
         <v>49.996</v>
       </c>
       <c r="N84" s="1" t="n">
-        <v>-15.323</v>
+        <v>-15.337</v>
       </c>
       <c r="O84" s="1" t="n">
         <v>-46.996</v>
       </c>
       <c r="P84" s="1" t="n">
-        <v>14.973</v>
+        <v>14.987</v>
       </c>
       <c r="Q84" s="1" t="n"/>
       <c r="R84" s="1" t="n"/>
@@ -5668,7 +5668,7 @@
         <v>0</v>
       </c>
       <c r="Y84" s="1" t="n">
-        <v>32.564</v>
+        <v>32.592</v>
       </c>
     </row>
     <row r="85" spans="1:25">

</xml_diff>

<commit_message>
fixed array positioning on spreadsheet. Added more formatting to spreadsheet with cell width adjustment
</commit_message>
<xml_diff>
--- a/masks/code/ResonatorArray.xlsx
+++ b/masks/code/ResonatorArray.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -735,14 +735,51 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A11:Y106"/>
+  <dimension ref="A1:Y106"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <cols>
+    <col customWidth="1" max="1" min="1" width="16"/>
+    <col customWidth="1" max="2" min="2" width="6"/>
+    <col customWidth="1" max="3" min="3" width="29"/>
+    <col customWidth="1" max="4" min="4" width="7"/>
+    <col customWidth="1" max="5" min="5" width="8"/>
+    <col customWidth="1" max="6" min="6" width="6"/>
+    <col customWidth="1" max="7" min="7" width="6"/>
+    <col customWidth="1" max="8" min="8" width="21"/>
+    <col customWidth="1" max="9" min="9" width="21"/>
+    <col customWidth="1" max="10" min="10" width="22"/>
+    <col customWidth="1" max="11" min="11" width="21"/>
+    <col customWidth="1" max="12" min="12" width="6"/>
+    <col customWidth="1" max="13" min="13" width="19"/>
+    <col customWidth="1" max="14" min="14" width="9"/>
+    <col customWidth="1" max="15" min="15" width="20"/>
+    <col customWidth="1" max="16" min="16" width="20"/>
+    <col customWidth="1" max="17" min="17" width="6"/>
+    <col customWidth="1" max="18" min="18" width="6"/>
+    <col customWidth="1" max="19" min="19" width="24"/>
+    <col customWidth="1" max="20" min="20" width="6"/>
+    <col customWidth="1" max="21" min="21" width="6"/>
+    <col customWidth="1" max="22" min="22" width="9"/>
+    <col customWidth="1" max="23" min="23" width="8"/>
+    <col customWidth="1" max="24" min="24" width="7"/>
+    <col customWidth="1" max="25" min="25" width="8"/>
+  </cols>
   <sheetData>
+    <row r="1" spans="1:25"/>
+    <row r="2" spans="1:25"/>
+    <row r="3" spans="1:25"/>
+    <row r="4" spans="1:25"/>
+    <row r="5" spans="1:25"/>
+    <row r="6" spans="1:25"/>
+    <row r="7" spans="1:25"/>
+    <row r="8" spans="1:25"/>
+    <row r="9" spans="1:25"/>
+    <row r="10" spans="1:25"/>
     <row r="11" spans="1:25">
       <c r="A11" s="1" t="n"/>
       <c r="B11" s="1" t="n"/>
@@ -939,13 +976,13 @@
         <v>-41.15</v>
       </c>
       <c r="N15" s="1" t="n">
-        <v>-38.5</v>
+        <v>-38.401</v>
       </c>
       <c r="O15" s="1" t="n">
         <v>42.25</v>
       </c>
       <c r="P15" s="1" t="n">
-        <v>38.35</v>
+        <v>38.251</v>
       </c>
       <c r="Q15" s="1" t="s">
         <v>25</v>
@@ -1010,13 +1047,13 @@
         <v>-38.5</v>
       </c>
       <c r="N16" s="1" t="n">
-        <v>-37.541</v>
+        <v>-37.442</v>
       </c>
       <c r="O16" s="1" t="n">
         <v>38.5</v>
       </c>
       <c r="P16" s="1" t="n">
-        <v>48.941</v>
+        <v>48.842</v>
       </c>
       <c r="Q16" s="1" t="n"/>
       <c r="R16" s="1" t="n"/>
@@ -1076,16 +1113,16 @@
       </c>
       <c r="L17" s="1" t="n"/>
       <c r="M17" s="1" t="n">
-        <v>49.996</v>
+        <v>5.992000000000001</v>
       </c>
       <c r="N17" s="1" t="n">
-        <v>-15.337</v>
+        <v>-16.296</v>
       </c>
       <c r="O17" s="1" t="n">
-        <v>-46.996</v>
+        <v>-2.992000000000001</v>
       </c>
       <c r="P17" s="1" t="n">
-        <v>15.987</v>
+        <v>16.946</v>
       </c>
       <c r="Q17" s="1" t="n"/>
       <c r="R17" s="1" t="n"/>
@@ -1145,16 +1182,16 @@
       </c>
       <c r="L18" s="1" t="n"/>
       <c r="M18" s="1" t="n">
-        <v>47</v>
+        <v>0</v>
       </c>
       <c r="N18" s="1" t="n">
-        <v>-37.541</v>
+        <v>-38.5</v>
       </c>
       <c r="O18" s="1" t="n">
-        <v>-47</v>
+        <v>0</v>
       </c>
       <c r="P18" s="1" t="n">
-        <v>47.741</v>
+        <v>48.7</v>
       </c>
       <c r="Q18" s="1" t="n"/>
       <c r="R18" s="1" t="n"/>
@@ -1214,16 +1251,16 @@
       </c>
       <c r="L19" s="1" t="n"/>
       <c r="M19" s="1" t="n">
-        <v>49.996</v>
+        <v>5.992</v>
       </c>
       <c r="N19" s="1" t="n">
-        <v>-26.537</v>
+        <v>-27.496</v>
       </c>
       <c r="O19" s="1" t="n">
-        <v>-60.596</v>
+        <v>-16.592</v>
       </c>
       <c r="P19" s="1" t="n">
-        <v>26.537</v>
+        <v>27.496</v>
       </c>
       <c r="Q19" s="1" t="n"/>
       <c r="R19" s="1" t="n"/>
@@ -1286,13 +1323,13 @@
         <v>-38.5</v>
       </c>
       <c r="N20" s="1" t="n">
-        <v>-38.5</v>
+        <v>-38.401</v>
       </c>
       <c r="O20" s="1" t="n">
         <v>44.3</v>
       </c>
       <c r="P20" s="1" t="n">
-        <v>38.5</v>
+        <v>38.401</v>
       </c>
       <c r="Q20" s="1" t="n"/>
       <c r="R20" s="1" t="n"/>
@@ -1352,16 +1389,16 @@
       </c>
       <c r="L21" s="1" t="n"/>
       <c r="M21" s="1" t="n">
-        <v>-44</v>
+        <v>-88</v>
       </c>
       <c r="N21" s="1" t="n">
-        <v>-32.041</v>
+        <v>-31.082</v>
       </c>
       <c r="O21" s="1" t="n">
-        <v>35.2</v>
+        <v>79.2</v>
       </c>
       <c r="P21" s="1" t="n">
-        <v>32.041</v>
+        <v>31.082</v>
       </c>
       <c r="Q21" s="1" t="n"/>
       <c r="R21" s="1" t="n"/>
@@ -1421,16 +1458,16 @@
       </c>
       <c r="L22" s="1" t="n"/>
       <c r="M22" s="1" t="n">
-        <v>44</v>
+        <v>88</v>
       </c>
       <c r="N22" s="1" t="n">
-        <v>-21.041</v>
+        <v>-20.082</v>
       </c>
       <c r="O22" s="1" t="n">
-        <v>-52.8</v>
+        <v>-96.8</v>
       </c>
       <c r="P22" s="1" t="n">
-        <v>21.041</v>
+        <v>20.082</v>
       </c>
       <c r="Q22" s="1" t="n"/>
       <c r="R22" s="1" t="n"/>
@@ -1559,13 +1596,13 @@
       </c>
       <c r="L24" s="1" t="n"/>
       <c r="M24" s="1" t="n">
-        <v>-49.95</v>
+        <v>-99.90000000000001</v>
       </c>
       <c r="N24" s="1" t="n">
         <v>-38.9</v>
       </c>
       <c r="O24" s="1" t="n">
-        <v>58.6</v>
+        <v>108.55</v>
       </c>
       <c r="P24" s="1" t="n">
         <v>38.9</v>
@@ -1631,13 +1668,13 @@
         <v>-38.8</v>
       </c>
       <c r="N25" s="1" t="n">
-        <v>-39.267</v>
+        <v>-39.168</v>
       </c>
       <c r="O25" s="1" t="n">
         <v>40.55</v>
       </c>
       <c r="P25" s="1" t="n">
-        <v>39.667</v>
+        <v>39.568</v>
       </c>
       <c r="Q25" s="1" t="n"/>
       <c r="R25" s="1" t="n"/>
@@ -1700,13 +1737,13 @@
         <v>-39.063</v>
       </c>
       <c r="N26" s="1" t="n">
-        <v>-38.5</v>
+        <v>-38.401</v>
       </c>
       <c r="O26" s="1" t="n">
         <v>45.51300000000001</v>
       </c>
       <c r="P26" s="1" t="n">
-        <v>36.35</v>
+        <v>36.251</v>
       </c>
       <c r="Q26" s="1" t="n"/>
       <c r="R26" s="1" t="n"/>
@@ -1769,13 +1806,13 @@
         <v>-52.5</v>
       </c>
       <c r="N27" s="1" t="n">
-        <v>-50.525</v>
+        <v>-50.55</v>
       </c>
       <c r="O27" s="1" t="n">
         <v>52.5</v>
       </c>
       <c r="P27" s="1" t="n">
-        <v>63.125</v>
+        <v>63.15</v>
       </c>
       <c r="Q27" s="1" t="n"/>
       <c r="R27" s="1" t="n"/>
@@ -1835,13 +1872,13 @@
       </c>
       <c r="L28" s="1" t="n"/>
       <c r="M28" s="1" t="n">
-        <v>-50.525</v>
+        <v>-50.55</v>
       </c>
       <c r="N28" s="1" t="n">
         <v>-52.5</v>
       </c>
       <c r="O28" s="1" t="n">
-        <v>40.525</v>
+        <v>40.55</v>
       </c>
       <c r="P28" s="1" t="n">
         <v>52.5</v>
@@ -6323,13 +6360,13 @@
         <v>-38.363</v>
       </c>
       <c r="N93" s="1" t="n">
-        <v>-38.5</v>
+        <v>-38.401</v>
       </c>
       <c r="O93" s="1" t="n">
         <v>37.113</v>
       </c>
       <c r="P93" s="1" t="n">
-        <v>38.5</v>
+        <v>38.401</v>
       </c>
       <c r="Q93" s="1" t="n"/>
       <c r="R93" s="1" t="n"/>
@@ -6392,13 +6429,13 @@
         <v>-36.98</v>
       </c>
       <c r="N94" s="1" t="n">
-        <v>-38.5</v>
+        <v>-38.401</v>
       </c>
       <c r="O94" s="1" t="n">
         <v>37.98</v>
       </c>
       <c r="P94" s="1" t="n">
-        <v>38.9</v>
+        <v>38.801</v>
       </c>
       <c r="Q94" s="1" t="n"/>
       <c r="R94" s="1" t="n"/>
@@ -6461,13 +6498,13 @@
         <v>-37.542</v>
       </c>
       <c r="N95" s="1" t="n">
-        <v>-38.5</v>
+        <v>-38.401</v>
       </c>
       <c r="O95" s="1" t="n">
         <v>37.542</v>
       </c>
       <c r="P95" s="1" t="n">
-        <v>38.5</v>
+        <v>38.401</v>
       </c>
       <c r="Q95" s="1" t="n"/>
       <c r="R95" s="1" t="n"/>
@@ -6596,13 +6633,13 @@
       </c>
       <c r="L97" s="1" t="n"/>
       <c r="M97" s="1" t="n">
-        <v>-49.95</v>
+        <v>-99.90000000000001</v>
       </c>
       <c r="N97" s="1" t="n">
         <v>-38.9</v>
       </c>
       <c r="O97" s="1" t="n">
-        <v>59.7</v>
+        <v>109.65</v>
       </c>
       <c r="P97" s="1" t="n">
         <v>38.9</v>
@@ -6665,16 +6702,16 @@
       </c>
       <c r="L98" s="1" t="n"/>
       <c r="M98" s="1" t="n">
-        <v>49.996</v>
+        <v>5.992000000000001</v>
       </c>
       <c r="N98" s="1" t="n">
-        <v>-15.337</v>
+        <v>-16.296</v>
       </c>
       <c r="O98" s="1" t="n">
-        <v>-46.996</v>
+        <v>-2.992000000000001</v>
       </c>
       <c r="P98" s="1" t="n">
-        <v>14.987</v>
+        <v>15.946</v>
       </c>
       <c r="Q98" s="1" t="n"/>
       <c r="R98" s="1" t="n"/>
@@ -6737,13 +6774,13 @@
         <v>-38.8</v>
       </c>
       <c r="N99" s="1" t="n">
-        <v>-37.744</v>
+        <v>-37.645</v>
       </c>
       <c r="O99" s="1" t="n">
         <v>41</v>
       </c>
       <c r="P99" s="1" t="n">
-        <v>38.394</v>
+        <v>38.295</v>
       </c>
       <c r="Q99" s="1" t="n"/>
       <c r="R99" s="1" t="n"/>
@@ -6806,13 +6843,13 @@
         <v>-38.8</v>
       </c>
       <c r="N100" s="1" t="n">
-        <v>-39.162</v>
+        <v>-39.063</v>
       </c>
       <c r="O100" s="1" t="n">
         <v>41</v>
       </c>
       <c r="P100" s="1" t="n">
-        <v>38.912</v>
+        <v>38.813</v>
       </c>
       <c r="Q100" s="1" t="n"/>
       <c r="R100" s="1" t="n"/>
@@ -6875,13 +6912,13 @@
         <v>-38.5</v>
       </c>
       <c r="N101" s="1" t="n">
-        <v>-37.541</v>
+        <v>-37.442</v>
       </c>
       <c r="O101" s="1" t="n">
         <v>38.5</v>
       </c>
       <c r="P101" s="1" t="n">
-        <v>49.541</v>
+        <v>49.442</v>
       </c>
       <c r="Q101" s="1" t="n"/>
       <c r="R101" s="1" t="n"/>
@@ -6941,16 +6978,16 @@
       </c>
       <c r="L102" s="1" t="n"/>
       <c r="M102" s="1" t="n">
-        <v>47</v>
+        <v>0</v>
       </c>
       <c r="N102" s="1" t="n">
-        <v>-37.541</v>
+        <v>-38.5</v>
       </c>
       <c r="O102" s="1" t="n">
-        <v>-47</v>
+        <v>0</v>
       </c>
       <c r="P102" s="1" t="n">
-        <v>48.34099999999999</v>
+        <v>49.3</v>
       </c>
       <c r="Q102" s="1" t="n"/>
       <c r="R102" s="1" t="n"/>
@@ -7010,16 +7047,16 @@
       </c>
       <c r="L103" s="1" t="n"/>
       <c r="M103" s="1" t="n">
-        <v>49.996</v>
+        <v>5.992</v>
       </c>
       <c r="N103" s="1" t="n">
-        <v>-26.537</v>
+        <v>-27.496</v>
       </c>
       <c r="O103" s="1" t="n">
-        <v>-39.396</v>
+        <v>4.608</v>
       </c>
       <c r="P103" s="1" t="n">
-        <v>26.537</v>
+        <v>27.496</v>
       </c>
       <c r="Q103" s="1" t="n"/>
       <c r="R103" s="1" t="n"/>
@@ -7079,16 +7116,16 @@
       </c>
       <c r="L104" s="1" t="n"/>
       <c r="M104" s="1" t="n">
-        <v>-44</v>
+        <v>-88</v>
       </c>
       <c r="N104" s="1" t="n">
-        <v>-32.041</v>
+        <v>-31.082</v>
       </c>
       <c r="O104" s="1" t="n">
-        <v>34.6</v>
+        <v>78.59999999999999</v>
       </c>
       <c r="P104" s="1" t="n">
-        <v>32.041</v>
+        <v>31.082</v>
       </c>
       <c r="Q104" s="1" t="n"/>
       <c r="R104" s="1" t="n"/>
@@ -7148,16 +7185,16 @@
       </c>
       <c r="L105" s="1" t="n"/>
       <c r="M105" s="1" t="n">
-        <v>44</v>
+        <v>88</v>
       </c>
       <c r="N105" s="1" t="n">
-        <v>-21.041</v>
+        <v>-20.082</v>
       </c>
       <c r="O105" s="1" t="n">
-        <v>-53.4</v>
+        <v>-97.40000000000001</v>
       </c>
       <c r="P105" s="1" t="n">
-        <v>21.041</v>
+        <v>20.082</v>
       </c>
       <c r="Q105" s="1" t="n"/>
       <c r="R105" s="1" t="n"/>

</xml_diff>

<commit_message>
fixed major bug in capacitor placement. Added pro padding to empty areas of the reticle cell
</commit_message>
<xml_diff>
--- a/masks/code/ResonatorArray.xlsx
+++ b/masks/code/ResonatorArray.xlsx
@@ -1916,7 +1916,7 @@
         <v>41</v>
       </c>
       <c r="D29" s="1" t="n">
-        <v>-3.7</v>
+        <v>-5.55</v>
       </c>
       <c r="E29" s="1" t="n">
         <v>9.199999999999999</v>
@@ -1928,10 +1928,10 @@
         <v>1.5</v>
       </c>
       <c r="H29" s="1" t="n">
-        <v>-4.600000000000001</v>
+        <v>-6.45</v>
       </c>
       <c r="I29" s="1" t="n">
-        <v>-2.8</v>
+        <v>-4.649999999999999</v>
       </c>
       <c r="J29" s="1" t="n">
         <v>9.949999999999999</v>
@@ -1947,7 +1947,7 @@
         <v>0</v>
       </c>
       <c r="O29" s="1" t="n">
-        <v>-3.7</v>
+        <v>-5.55</v>
       </c>
       <c r="P29" s="1" t="n">
         <v>9.199999999999999</v>
@@ -1985,7 +1985,7 @@
         <v>42</v>
       </c>
       <c r="D30" s="1" t="n">
-        <v>-1.85</v>
+        <v>-3.7</v>
       </c>
       <c r="E30" s="1" t="n">
         <v>9.199999999999999</v>
@@ -1997,10 +1997,10 @@
         <v>1.5</v>
       </c>
       <c r="H30" s="1" t="n">
-        <v>-2.75</v>
+        <v>-4.600000000000001</v>
       </c>
       <c r="I30" s="1" t="n">
-        <v>-0.9500000000000001</v>
+        <v>-2.8</v>
       </c>
       <c r="J30" s="1" t="n">
         <v>9.949999999999999</v>
@@ -2016,7 +2016,7 @@
         <v>0</v>
       </c>
       <c r="O30" s="1" t="n">
-        <v>-1.85</v>
+        <v>-3.7</v>
       </c>
       <c r="P30" s="1" t="n">
         <v>9.199999999999999</v>
@@ -2054,7 +2054,7 @@
         <v>43</v>
       </c>
       <c r="D31" s="1" t="n">
-        <v>0</v>
+        <v>-1.85</v>
       </c>
       <c r="E31" s="1" t="n">
         <v>9.199999999999999</v>
@@ -2066,10 +2066,10 @@
         <v>1.5</v>
       </c>
       <c r="H31" s="1" t="n">
-        <v>-0.9</v>
+        <v>-2.75</v>
       </c>
       <c r="I31" s="1" t="n">
-        <v>0.9</v>
+        <v>-0.9500000000000001</v>
       </c>
       <c r="J31" s="1" t="n">
         <v>9.949999999999999</v>
@@ -2085,7 +2085,7 @@
         <v>0</v>
       </c>
       <c r="O31" s="1" t="n">
-        <v>0</v>
+        <v>-1.85</v>
       </c>
       <c r="P31" s="1" t="n">
         <v>9.199999999999999</v>
@@ -2123,7 +2123,7 @@
         <v>44</v>
       </c>
       <c r="D32" s="1" t="n">
-        <v>1.85</v>
+        <v>0</v>
       </c>
       <c r="E32" s="1" t="n">
         <v>9.199999999999999</v>
@@ -2135,10 +2135,10 @@
         <v>1.5</v>
       </c>
       <c r="H32" s="1" t="n">
-        <v>0.9500000000000001</v>
+        <v>-0.9</v>
       </c>
       <c r="I32" s="1" t="n">
-        <v>2.75</v>
+        <v>0.9</v>
       </c>
       <c r="J32" s="1" t="n">
         <v>9.949999999999999</v>
@@ -2154,7 +2154,7 @@
         <v>0</v>
       </c>
       <c r="O32" s="1" t="n">
-        <v>1.85</v>
+        <v>0</v>
       </c>
       <c r="P32" s="1" t="n">
         <v>9.199999999999999</v>
@@ -2192,7 +2192,7 @@
         <v>45</v>
       </c>
       <c r="D33" s="1" t="n">
-        <v>3.7</v>
+        <v>1.85</v>
       </c>
       <c r="E33" s="1" t="n">
         <v>9.199999999999999</v>
@@ -2204,10 +2204,10 @@
         <v>1.5</v>
       </c>
       <c r="H33" s="1" t="n">
-        <v>2.8</v>
+        <v>0.9500000000000001</v>
       </c>
       <c r="I33" s="1" t="n">
-        <v>4.600000000000001</v>
+        <v>2.75</v>
       </c>
       <c r="J33" s="1" t="n">
         <v>9.949999999999999</v>
@@ -2223,7 +2223,7 @@
         <v>0</v>
       </c>
       <c r="O33" s="1" t="n">
-        <v>3.7</v>
+        <v>1.85</v>
       </c>
       <c r="P33" s="1" t="n">
         <v>9.199999999999999</v>
@@ -2261,7 +2261,7 @@
         <v>46</v>
       </c>
       <c r="D34" s="1" t="n">
-        <v>-3.7</v>
+        <v>3.7</v>
       </c>
       <c r="E34" s="1" t="n">
         <v>9.199999999999999</v>
@@ -2273,10 +2273,10 @@
         <v>1.5</v>
       </c>
       <c r="H34" s="1" t="n">
-        <v>-4.600000000000001</v>
+        <v>2.8</v>
       </c>
       <c r="I34" s="1" t="n">
-        <v>-2.8</v>
+        <v>4.600000000000001</v>
       </c>
       <c r="J34" s="1" t="n">
         <v>9.949999999999999</v>
@@ -2292,7 +2292,7 @@
         <v>0</v>
       </c>
       <c r="O34" s="1" t="n">
-        <v>-3.7</v>
+        <v>3.7</v>
       </c>
       <c r="P34" s="1" t="n">
         <v>9.199999999999999</v>
@@ -2330,7 +2330,7 @@
         <v>47</v>
       </c>
       <c r="D35" s="1" t="n">
-        <v>-1.85</v>
+        <v>-5.55</v>
       </c>
       <c r="E35" s="1" t="n">
         <v>7.65</v>
@@ -2342,10 +2342,10 @@
         <v>1.5</v>
       </c>
       <c r="H35" s="1" t="n">
-        <v>-2.75</v>
+        <v>-6.45</v>
       </c>
       <c r="I35" s="1" t="n">
-        <v>-0.9500000000000001</v>
+        <v>-4.649999999999999</v>
       </c>
       <c r="J35" s="1" t="n">
         <v>8.4</v>
@@ -2361,7 +2361,7 @@
         <v>0</v>
       </c>
       <c r="O35" s="1" t="n">
-        <v>-1.85</v>
+        <v>-5.55</v>
       </c>
       <c r="P35" s="1" t="n">
         <v>7.65</v>
@@ -2399,7 +2399,7 @@
         <v>48</v>
       </c>
       <c r="D36" s="1" t="n">
-        <v>0</v>
+        <v>-3.7</v>
       </c>
       <c r="E36" s="1" t="n">
         <v>7.65</v>
@@ -2411,10 +2411,10 @@
         <v>1.5</v>
       </c>
       <c r="H36" s="1" t="n">
-        <v>-0.9</v>
+        <v>-4.600000000000001</v>
       </c>
       <c r="I36" s="1" t="n">
-        <v>0.9</v>
+        <v>-2.8</v>
       </c>
       <c r="J36" s="1" t="n">
         <v>8.4</v>
@@ -2430,7 +2430,7 @@
         <v>0</v>
       </c>
       <c r="O36" s="1" t="n">
-        <v>0</v>
+        <v>-3.7</v>
       </c>
       <c r="P36" s="1" t="n">
         <v>7.65</v>
@@ -2468,7 +2468,7 @@
         <v>49</v>
       </c>
       <c r="D37" s="1" t="n">
-        <v>1.85</v>
+        <v>-1.85</v>
       </c>
       <c r="E37" s="1" t="n">
         <v>7.65</v>
@@ -2480,10 +2480,10 @@
         <v>1.5</v>
       </c>
       <c r="H37" s="1" t="n">
-        <v>0.9500000000000001</v>
+        <v>-2.75</v>
       </c>
       <c r="I37" s="1" t="n">
-        <v>2.75</v>
+        <v>-0.9500000000000001</v>
       </c>
       <c r="J37" s="1" t="n">
         <v>8.4</v>
@@ -2499,7 +2499,7 @@
         <v>0</v>
       </c>
       <c r="O37" s="1" t="n">
-        <v>1.85</v>
+        <v>-1.85</v>
       </c>
       <c r="P37" s="1" t="n">
         <v>7.65</v>
@@ -2537,7 +2537,7 @@
         <v>50</v>
       </c>
       <c r="D38" s="1" t="n">
-        <v>3.7</v>
+        <v>0</v>
       </c>
       <c r="E38" s="1" t="n">
         <v>7.65</v>
@@ -2549,10 +2549,10 @@
         <v>1.5</v>
       </c>
       <c r="H38" s="1" t="n">
-        <v>2.8</v>
+        <v>-0.9</v>
       </c>
       <c r="I38" s="1" t="n">
-        <v>4.600000000000001</v>
+        <v>0.9</v>
       </c>
       <c r="J38" s="1" t="n">
         <v>8.4</v>
@@ -2568,7 +2568,7 @@
         <v>0</v>
       </c>
       <c r="O38" s="1" t="n">
-        <v>3.7</v>
+        <v>0</v>
       </c>
       <c r="P38" s="1" t="n">
         <v>7.65</v>
@@ -2606,7 +2606,7 @@
         <v>51</v>
       </c>
       <c r="D39" s="1" t="n">
-        <v>-3.7</v>
+        <v>1.85</v>
       </c>
       <c r="E39" s="1" t="n">
         <v>7.65</v>
@@ -2618,10 +2618,10 @@
         <v>1.5</v>
       </c>
       <c r="H39" s="1" t="n">
-        <v>-4.600000000000001</v>
+        <v>0.9500000000000001</v>
       </c>
       <c r="I39" s="1" t="n">
-        <v>-2.8</v>
+        <v>2.75</v>
       </c>
       <c r="J39" s="1" t="n">
         <v>8.4</v>
@@ -2637,7 +2637,7 @@
         <v>0</v>
       </c>
       <c r="O39" s="1" t="n">
-        <v>-3.7</v>
+        <v>1.85</v>
       </c>
       <c r="P39" s="1" t="n">
         <v>7.65</v>
@@ -2675,7 +2675,7 @@
         <v>52</v>
       </c>
       <c r="D40" s="1" t="n">
-        <v>-1.85</v>
+        <v>3.7</v>
       </c>
       <c r="E40" s="1" t="n">
         <v>7.65</v>
@@ -2687,10 +2687,10 @@
         <v>1.5</v>
       </c>
       <c r="H40" s="1" t="n">
-        <v>-2.75</v>
+        <v>2.8</v>
       </c>
       <c r="I40" s="1" t="n">
-        <v>-0.9500000000000001</v>
+        <v>4.600000000000001</v>
       </c>
       <c r="J40" s="1" t="n">
         <v>8.4</v>
@@ -2706,7 +2706,7 @@
         <v>0</v>
       </c>
       <c r="O40" s="1" t="n">
-        <v>-1.85</v>
+        <v>3.7</v>
       </c>
       <c r="P40" s="1" t="n">
         <v>7.65</v>
@@ -2744,7 +2744,7 @@
         <v>53</v>
       </c>
       <c r="D41" s="1" t="n">
-        <v>0</v>
+        <v>-5.55</v>
       </c>
       <c r="E41" s="1" t="n">
         <v>6.1</v>
@@ -2756,10 +2756,10 @@
         <v>1.5</v>
       </c>
       <c r="H41" s="1" t="n">
-        <v>-0.9</v>
+        <v>-6.45</v>
       </c>
       <c r="I41" s="1" t="n">
-        <v>0.9</v>
+        <v>-4.649999999999999</v>
       </c>
       <c r="J41" s="1" t="n">
         <v>6.85</v>
@@ -2775,7 +2775,7 @@
         <v>0</v>
       </c>
       <c r="O41" s="1" t="n">
-        <v>0</v>
+        <v>-5.55</v>
       </c>
       <c r="P41" s="1" t="n">
         <v>6.1</v>
@@ -2813,7 +2813,7 @@
         <v>54</v>
       </c>
       <c r="D42" s="1" t="n">
-        <v>1.85</v>
+        <v>-3.7</v>
       </c>
       <c r="E42" s="1" t="n">
         <v>6.1</v>
@@ -2825,10 +2825,10 @@
         <v>1.5</v>
       </c>
       <c r="H42" s="1" t="n">
-        <v>0.9500000000000001</v>
+        <v>-4.600000000000001</v>
       </c>
       <c r="I42" s="1" t="n">
-        <v>2.75</v>
+        <v>-2.8</v>
       </c>
       <c r="J42" s="1" t="n">
         <v>6.85</v>
@@ -2844,7 +2844,7 @@
         <v>0</v>
       </c>
       <c r="O42" s="1" t="n">
-        <v>1.85</v>
+        <v>-3.7</v>
       </c>
       <c r="P42" s="1" t="n">
         <v>6.1</v>
@@ -2882,7 +2882,7 @@
         <v>55</v>
       </c>
       <c r="D43" s="1" t="n">
-        <v>3.7</v>
+        <v>-1.85</v>
       </c>
       <c r="E43" s="1" t="n">
         <v>6.1</v>
@@ -2894,10 +2894,10 @@
         <v>1.5</v>
       </c>
       <c r="H43" s="1" t="n">
-        <v>2.8</v>
+        <v>-2.75</v>
       </c>
       <c r="I43" s="1" t="n">
-        <v>4.600000000000001</v>
+        <v>-0.9500000000000001</v>
       </c>
       <c r="J43" s="1" t="n">
         <v>6.85</v>
@@ -2913,7 +2913,7 @@
         <v>0</v>
       </c>
       <c r="O43" s="1" t="n">
-        <v>3.7</v>
+        <v>-1.85</v>
       </c>
       <c r="P43" s="1" t="n">
         <v>6.1</v>
@@ -2951,7 +2951,7 @@
         <v>56</v>
       </c>
       <c r="D44" s="1" t="n">
-        <v>-3.7</v>
+        <v>0</v>
       </c>
       <c r="E44" s="1" t="n">
         <v>6.1</v>
@@ -2963,10 +2963,10 @@
         <v>1.5</v>
       </c>
       <c r="H44" s="1" t="n">
-        <v>-4.600000000000001</v>
+        <v>-0.9</v>
       </c>
       <c r="I44" s="1" t="n">
-        <v>-2.8</v>
+        <v>0.9</v>
       </c>
       <c r="J44" s="1" t="n">
         <v>6.85</v>
@@ -2982,7 +2982,7 @@
         <v>0</v>
       </c>
       <c r="O44" s="1" t="n">
-        <v>-3.7</v>
+        <v>0</v>
       </c>
       <c r="P44" s="1" t="n">
         <v>6.1</v>
@@ -3020,7 +3020,7 @@
         <v>57</v>
       </c>
       <c r="D45" s="1" t="n">
-        <v>-1.85</v>
+        <v>1.85</v>
       </c>
       <c r="E45" s="1" t="n">
         <v>6.1</v>
@@ -3032,10 +3032,10 @@
         <v>1.5</v>
       </c>
       <c r="H45" s="1" t="n">
-        <v>-2.75</v>
+        <v>0.9500000000000001</v>
       </c>
       <c r="I45" s="1" t="n">
-        <v>-0.9500000000000001</v>
+        <v>2.75</v>
       </c>
       <c r="J45" s="1" t="n">
         <v>6.85</v>
@@ -3051,7 +3051,7 @@
         <v>0</v>
       </c>
       <c r="O45" s="1" t="n">
-        <v>-1.85</v>
+        <v>1.85</v>
       </c>
       <c r="P45" s="1" t="n">
         <v>6.1</v>
@@ -3089,7 +3089,7 @@
         <v>58</v>
       </c>
       <c r="D46" s="1" t="n">
-        <v>0</v>
+        <v>3.7</v>
       </c>
       <c r="E46" s="1" t="n">
         <v>6.1</v>
@@ -3101,10 +3101,10 @@
         <v>1.5</v>
       </c>
       <c r="H46" s="1" t="n">
-        <v>-0.9</v>
+        <v>2.8</v>
       </c>
       <c r="I46" s="1" t="n">
-        <v>0.9</v>
+        <v>4.600000000000001</v>
       </c>
       <c r="J46" s="1" t="n">
         <v>6.85</v>
@@ -3120,7 +3120,7 @@
         <v>0</v>
       </c>
       <c r="O46" s="1" t="n">
-        <v>0</v>
+        <v>3.7</v>
       </c>
       <c r="P46" s="1" t="n">
         <v>6.1</v>
@@ -3158,7 +3158,7 @@
         <v>59</v>
       </c>
       <c r="D47" s="1" t="n">
-        <v>1.85</v>
+        <v>-5.55</v>
       </c>
       <c r="E47" s="1" t="n">
         <v>4.55</v>
@@ -3170,10 +3170,10 @@
         <v>1.5</v>
       </c>
       <c r="H47" s="1" t="n">
-        <v>0.9500000000000001</v>
+        <v>-6.45</v>
       </c>
       <c r="I47" s="1" t="n">
-        <v>2.75</v>
+        <v>-4.649999999999999</v>
       </c>
       <c r="J47" s="1" t="n">
         <v>5.3</v>
@@ -3189,7 +3189,7 @@
         <v>0</v>
       </c>
       <c r="O47" s="1" t="n">
-        <v>1.85</v>
+        <v>-5.55</v>
       </c>
       <c r="P47" s="1" t="n">
         <v>4.55</v>
@@ -3227,7 +3227,7 @@
         <v>60</v>
       </c>
       <c r="D48" s="1" t="n">
-        <v>3.7</v>
+        <v>-3.7</v>
       </c>
       <c r="E48" s="1" t="n">
         <v>4.55</v>
@@ -3239,10 +3239,10 @@
         <v>1.5</v>
       </c>
       <c r="H48" s="1" t="n">
-        <v>2.8</v>
+        <v>-4.600000000000001</v>
       </c>
       <c r="I48" s="1" t="n">
-        <v>4.600000000000001</v>
+        <v>-2.8</v>
       </c>
       <c r="J48" s="1" t="n">
         <v>5.3</v>
@@ -3258,7 +3258,7 @@
         <v>0</v>
       </c>
       <c r="O48" s="1" t="n">
-        <v>3.7</v>
+        <v>-3.7</v>
       </c>
       <c r="P48" s="1" t="n">
         <v>4.55</v>
@@ -3296,7 +3296,7 @@
         <v>61</v>
       </c>
       <c r="D49" s="1" t="n">
-        <v>-3.7</v>
+        <v>-1.85</v>
       </c>
       <c r="E49" s="1" t="n">
         <v>4.55</v>
@@ -3308,10 +3308,10 @@
         <v>1.5</v>
       </c>
       <c r="H49" s="1" t="n">
-        <v>-4.600000000000001</v>
+        <v>-2.75</v>
       </c>
       <c r="I49" s="1" t="n">
-        <v>-2.8</v>
+        <v>-0.9500000000000001</v>
       </c>
       <c r="J49" s="1" t="n">
         <v>5.3</v>
@@ -3327,7 +3327,7 @@
         <v>0</v>
       </c>
       <c r="O49" s="1" t="n">
-        <v>-3.7</v>
+        <v>-1.85</v>
       </c>
       <c r="P49" s="1" t="n">
         <v>4.55</v>
@@ -3365,7 +3365,7 @@
         <v>62</v>
       </c>
       <c r="D50" s="1" t="n">
-        <v>-1.85</v>
+        <v>0</v>
       </c>
       <c r="E50" s="1" t="n">
         <v>4.55</v>
@@ -3377,10 +3377,10 @@
         <v>1.5</v>
       </c>
       <c r="H50" s="1" t="n">
-        <v>-2.75</v>
+        <v>-0.9</v>
       </c>
       <c r="I50" s="1" t="n">
-        <v>-0.9500000000000001</v>
+        <v>0.9</v>
       </c>
       <c r="J50" s="1" t="n">
         <v>5.3</v>
@@ -3396,7 +3396,7 @@
         <v>0</v>
       </c>
       <c r="O50" s="1" t="n">
-        <v>-1.85</v>
+        <v>0</v>
       </c>
       <c r="P50" s="1" t="n">
         <v>4.55</v>
@@ -3434,7 +3434,7 @@
         <v>63</v>
       </c>
       <c r="D51" s="1" t="n">
-        <v>0</v>
+        <v>1.85</v>
       </c>
       <c r="E51" s="1" t="n">
         <v>4.55</v>
@@ -3446,10 +3446,10 @@
         <v>1.5</v>
       </c>
       <c r="H51" s="1" t="n">
-        <v>-0.9</v>
+        <v>0.9500000000000001</v>
       </c>
       <c r="I51" s="1" t="n">
-        <v>0.9</v>
+        <v>2.75</v>
       </c>
       <c r="J51" s="1" t="n">
         <v>5.3</v>
@@ -3465,7 +3465,7 @@
         <v>0</v>
       </c>
       <c r="O51" s="1" t="n">
-        <v>0</v>
+        <v>1.85</v>
       </c>
       <c r="P51" s="1" t="n">
         <v>4.55</v>
@@ -3503,7 +3503,7 @@
         <v>64</v>
       </c>
       <c r="D52" s="1" t="n">
-        <v>1.85</v>
+        <v>3.7</v>
       </c>
       <c r="E52" s="1" t="n">
         <v>4.55</v>
@@ -3515,10 +3515,10 @@
         <v>1.5</v>
       </c>
       <c r="H52" s="1" t="n">
-        <v>0.9500000000000001</v>
+        <v>2.8</v>
       </c>
       <c r="I52" s="1" t="n">
-        <v>2.75</v>
+        <v>4.600000000000001</v>
       </c>
       <c r="J52" s="1" t="n">
         <v>5.3</v>
@@ -3534,7 +3534,7 @@
         <v>0</v>
       </c>
       <c r="O52" s="1" t="n">
-        <v>1.85</v>
+        <v>3.7</v>
       </c>
       <c r="P52" s="1" t="n">
         <v>4.55</v>
@@ -3572,7 +3572,7 @@
         <v>65</v>
       </c>
       <c r="D53" s="1" t="n">
-        <v>3.7</v>
+        <v>-5.55</v>
       </c>
       <c r="E53" s="1" t="n">
         <v>3</v>
@@ -3584,10 +3584,10 @@
         <v>1.5</v>
       </c>
       <c r="H53" s="1" t="n">
-        <v>2.8</v>
+        <v>-6.45</v>
       </c>
       <c r="I53" s="1" t="n">
-        <v>4.600000000000001</v>
+        <v>-4.649999999999999</v>
       </c>
       <c r="J53" s="1" t="n">
         <v>3.75</v>
@@ -3603,7 +3603,7 @@
         <v>0</v>
       </c>
       <c r="O53" s="1" t="n">
-        <v>3.7</v>
+        <v>-5.55</v>
       </c>
       <c r="P53" s="1" t="n">
         <v>3</v>
@@ -4262,7 +4262,7 @@
         <v>75</v>
       </c>
       <c r="D63" s="1" t="n">
-        <v>-3.7</v>
+        <v>-5.55</v>
       </c>
       <c r="E63" s="1" t="n">
         <v>-9.199999999999999</v>
@@ -4274,10 +4274,10 @@
         <v>1.5</v>
       </c>
       <c r="H63" s="1" t="n">
-        <v>-4.600000000000001</v>
+        <v>-6.45</v>
       </c>
       <c r="I63" s="1" t="n">
-        <v>-2.8</v>
+        <v>-4.649999999999999</v>
       </c>
       <c r="J63" s="1" t="n">
         <v>-8.449999999999999</v>
@@ -4293,7 +4293,7 @@
         <v>0</v>
       </c>
       <c r="O63" s="1" t="n">
-        <v>-3.7</v>
+        <v>-5.55</v>
       </c>
       <c r="P63" s="1" t="n">
         <v>-9.199999999999999</v>
@@ -4331,7 +4331,7 @@
         <v>76</v>
       </c>
       <c r="D64" s="1" t="n">
-        <v>-1.85</v>
+        <v>-3.7</v>
       </c>
       <c r="E64" s="1" t="n">
         <v>-9.199999999999999</v>
@@ -4343,10 +4343,10 @@
         <v>1.5</v>
       </c>
       <c r="H64" s="1" t="n">
-        <v>-2.75</v>
+        <v>-4.600000000000001</v>
       </c>
       <c r="I64" s="1" t="n">
-        <v>-0.9500000000000001</v>
+        <v>-2.8</v>
       </c>
       <c r="J64" s="1" t="n">
         <v>-8.449999999999999</v>
@@ -4362,7 +4362,7 @@
         <v>0</v>
       </c>
       <c r="O64" s="1" t="n">
-        <v>-1.85</v>
+        <v>-3.7</v>
       </c>
       <c r="P64" s="1" t="n">
         <v>-9.199999999999999</v>
@@ -4400,7 +4400,7 @@
         <v>77</v>
       </c>
       <c r="D65" s="1" t="n">
-        <v>0</v>
+        <v>-1.85</v>
       </c>
       <c r="E65" s="1" t="n">
         <v>-9.199999999999999</v>
@@ -4412,10 +4412,10 @@
         <v>1.5</v>
       </c>
       <c r="H65" s="1" t="n">
-        <v>-0.9</v>
+        <v>-2.75</v>
       </c>
       <c r="I65" s="1" t="n">
-        <v>0.9</v>
+        <v>-0.9500000000000001</v>
       </c>
       <c r="J65" s="1" t="n">
         <v>-8.449999999999999</v>
@@ -4431,7 +4431,7 @@
         <v>0</v>
       </c>
       <c r="O65" s="1" t="n">
-        <v>0</v>
+        <v>-1.85</v>
       </c>
       <c r="P65" s="1" t="n">
         <v>-9.199999999999999</v>
@@ -4469,7 +4469,7 @@
         <v>78</v>
       </c>
       <c r="D66" s="1" t="n">
-        <v>1.85</v>
+        <v>0</v>
       </c>
       <c r="E66" s="1" t="n">
         <v>-9.199999999999999</v>
@@ -4481,10 +4481,10 @@
         <v>1.5</v>
       </c>
       <c r="H66" s="1" t="n">
-        <v>0.9500000000000001</v>
+        <v>-0.9</v>
       </c>
       <c r="I66" s="1" t="n">
-        <v>2.75</v>
+        <v>0.9</v>
       </c>
       <c r="J66" s="1" t="n">
         <v>-8.449999999999999</v>
@@ -4500,7 +4500,7 @@
         <v>0</v>
       </c>
       <c r="O66" s="1" t="n">
-        <v>1.85</v>
+        <v>0</v>
       </c>
       <c r="P66" s="1" t="n">
         <v>-9.199999999999999</v>
@@ -4538,7 +4538,7 @@
         <v>79</v>
       </c>
       <c r="D67" s="1" t="n">
-        <v>3.7</v>
+        <v>1.85</v>
       </c>
       <c r="E67" s="1" t="n">
         <v>-9.199999999999999</v>
@@ -4550,10 +4550,10 @@
         <v>1.5</v>
       </c>
       <c r="H67" s="1" t="n">
-        <v>2.8</v>
+        <v>0.9500000000000001</v>
       </c>
       <c r="I67" s="1" t="n">
-        <v>4.600000000000001</v>
+        <v>2.75</v>
       </c>
       <c r="J67" s="1" t="n">
         <v>-8.449999999999999</v>
@@ -4569,7 +4569,7 @@
         <v>0</v>
       </c>
       <c r="O67" s="1" t="n">
-        <v>3.7</v>
+        <v>1.85</v>
       </c>
       <c r="P67" s="1" t="n">
         <v>-9.199999999999999</v>
@@ -4607,7 +4607,7 @@
         <v>80</v>
       </c>
       <c r="D68" s="1" t="n">
-        <v>-3.7</v>
+        <v>3.7</v>
       </c>
       <c r="E68" s="1" t="n">
         <v>-9.199999999999999</v>
@@ -4619,10 +4619,10 @@
         <v>1.5</v>
       </c>
       <c r="H68" s="1" t="n">
-        <v>-4.600000000000001</v>
+        <v>2.8</v>
       </c>
       <c r="I68" s="1" t="n">
-        <v>-2.8</v>
+        <v>4.600000000000001</v>
       </c>
       <c r="J68" s="1" t="n">
         <v>-8.449999999999999</v>
@@ -4638,7 +4638,7 @@
         <v>0</v>
       </c>
       <c r="O68" s="1" t="n">
-        <v>-3.7</v>
+        <v>3.7</v>
       </c>
       <c r="P68" s="1" t="n">
         <v>-9.199999999999999</v>
@@ -4676,7 +4676,7 @@
         <v>81</v>
       </c>
       <c r="D69" s="1" t="n">
-        <v>-1.85</v>
+        <v>-5.55</v>
       </c>
       <c r="E69" s="1" t="n">
         <v>-7.65</v>
@@ -4688,10 +4688,10 @@
         <v>1.5</v>
       </c>
       <c r="H69" s="1" t="n">
-        <v>-2.75</v>
+        <v>-6.45</v>
       </c>
       <c r="I69" s="1" t="n">
-        <v>-0.9500000000000001</v>
+        <v>-4.649999999999999</v>
       </c>
       <c r="J69" s="1" t="n">
         <v>-6.9</v>
@@ -4707,7 +4707,7 @@
         <v>0</v>
       </c>
       <c r="O69" s="1" t="n">
-        <v>-1.85</v>
+        <v>-5.55</v>
       </c>
       <c r="P69" s="1" t="n">
         <v>-7.65</v>
@@ -4745,7 +4745,7 @@
         <v>82</v>
       </c>
       <c r="D70" s="1" t="n">
-        <v>0</v>
+        <v>-3.7</v>
       </c>
       <c r="E70" s="1" t="n">
         <v>-7.65</v>
@@ -4757,10 +4757,10 @@
         <v>1.5</v>
       </c>
       <c r="H70" s="1" t="n">
-        <v>-0.9</v>
+        <v>-4.600000000000001</v>
       </c>
       <c r="I70" s="1" t="n">
-        <v>0.9</v>
+        <v>-2.8</v>
       </c>
       <c r="J70" s="1" t="n">
         <v>-6.9</v>
@@ -4776,7 +4776,7 @@
         <v>0</v>
       </c>
       <c r="O70" s="1" t="n">
-        <v>0</v>
+        <v>-3.7</v>
       </c>
       <c r="P70" s="1" t="n">
         <v>-7.65</v>
@@ -4814,7 +4814,7 @@
         <v>83</v>
       </c>
       <c r="D71" s="1" t="n">
-        <v>1.85</v>
+        <v>-1.85</v>
       </c>
       <c r="E71" s="1" t="n">
         <v>-7.65</v>
@@ -4826,10 +4826,10 @@
         <v>1.5</v>
       </c>
       <c r="H71" s="1" t="n">
-        <v>0.9500000000000001</v>
+        <v>-2.75</v>
       </c>
       <c r="I71" s="1" t="n">
-        <v>2.75</v>
+        <v>-0.9500000000000001</v>
       </c>
       <c r="J71" s="1" t="n">
         <v>-6.9</v>
@@ -4845,7 +4845,7 @@
         <v>0</v>
       </c>
       <c r="O71" s="1" t="n">
-        <v>1.85</v>
+        <v>-1.85</v>
       </c>
       <c r="P71" s="1" t="n">
         <v>-7.65</v>
@@ -4883,7 +4883,7 @@
         <v>84</v>
       </c>
       <c r="D72" s="1" t="n">
-        <v>3.7</v>
+        <v>0</v>
       </c>
       <c r="E72" s="1" t="n">
         <v>-7.65</v>
@@ -4895,10 +4895,10 @@
         <v>1.5</v>
       </c>
       <c r="H72" s="1" t="n">
-        <v>2.8</v>
+        <v>-0.9</v>
       </c>
       <c r="I72" s="1" t="n">
-        <v>4.600000000000001</v>
+        <v>0.9</v>
       </c>
       <c r="J72" s="1" t="n">
         <v>-6.9</v>
@@ -4914,7 +4914,7 @@
         <v>0</v>
       </c>
       <c r="O72" s="1" t="n">
-        <v>3.7</v>
+        <v>0</v>
       </c>
       <c r="P72" s="1" t="n">
         <v>-7.65</v>
@@ -4952,7 +4952,7 @@
         <v>85</v>
       </c>
       <c r="D73" s="1" t="n">
-        <v>-3.7</v>
+        <v>1.85</v>
       </c>
       <c r="E73" s="1" t="n">
         <v>-7.65</v>
@@ -4964,10 +4964,10 @@
         <v>1.5</v>
       </c>
       <c r="H73" s="1" t="n">
-        <v>-4.600000000000001</v>
+        <v>0.9500000000000001</v>
       </c>
       <c r="I73" s="1" t="n">
-        <v>-2.8</v>
+        <v>2.75</v>
       </c>
       <c r="J73" s="1" t="n">
         <v>-6.9</v>
@@ -4983,7 +4983,7 @@
         <v>0</v>
       </c>
       <c r="O73" s="1" t="n">
-        <v>-3.7</v>
+        <v>1.85</v>
       </c>
       <c r="P73" s="1" t="n">
         <v>-7.65</v>
@@ -5021,7 +5021,7 @@
         <v>86</v>
       </c>
       <c r="D74" s="1" t="n">
-        <v>-1.85</v>
+        <v>3.7</v>
       </c>
       <c r="E74" s="1" t="n">
         <v>-7.65</v>
@@ -5033,10 +5033,10 @@
         <v>1.5</v>
       </c>
       <c r="H74" s="1" t="n">
-        <v>-2.75</v>
+        <v>2.8</v>
       </c>
       <c r="I74" s="1" t="n">
-        <v>-0.9500000000000001</v>
+        <v>4.600000000000001</v>
       </c>
       <c r="J74" s="1" t="n">
         <v>-6.9</v>
@@ -5052,7 +5052,7 @@
         <v>0</v>
       </c>
       <c r="O74" s="1" t="n">
-        <v>-1.85</v>
+        <v>3.7</v>
       </c>
       <c r="P74" s="1" t="n">
         <v>-7.65</v>
@@ -5090,7 +5090,7 @@
         <v>87</v>
       </c>
       <c r="D75" s="1" t="n">
-        <v>0</v>
+        <v>-5.55</v>
       </c>
       <c r="E75" s="1" t="n">
         <v>-6.1</v>
@@ -5102,10 +5102,10 @@
         <v>1.5</v>
       </c>
       <c r="H75" s="1" t="n">
-        <v>-0.9</v>
+        <v>-6.45</v>
       </c>
       <c r="I75" s="1" t="n">
-        <v>0.9</v>
+        <v>-4.649999999999999</v>
       </c>
       <c r="J75" s="1" t="n">
         <v>-5.35</v>
@@ -5121,7 +5121,7 @@
         <v>0</v>
       </c>
       <c r="O75" s="1" t="n">
-        <v>0</v>
+        <v>-5.55</v>
       </c>
       <c r="P75" s="1" t="n">
         <v>-6.1</v>
@@ -5159,7 +5159,7 @@
         <v>88</v>
       </c>
       <c r="D76" s="1" t="n">
-        <v>1.85</v>
+        <v>-3.7</v>
       </c>
       <c r="E76" s="1" t="n">
         <v>-6.1</v>
@@ -5171,10 +5171,10 @@
         <v>1.5</v>
       </c>
       <c r="H76" s="1" t="n">
-        <v>0.9500000000000001</v>
+        <v>-4.600000000000001</v>
       </c>
       <c r="I76" s="1" t="n">
-        <v>2.75</v>
+        <v>-2.8</v>
       </c>
       <c r="J76" s="1" t="n">
         <v>-5.35</v>
@@ -5190,7 +5190,7 @@
         <v>0</v>
       </c>
       <c r="O76" s="1" t="n">
-        <v>1.85</v>
+        <v>-3.7</v>
       </c>
       <c r="P76" s="1" t="n">
         <v>-6.1</v>
@@ -5228,7 +5228,7 @@
         <v>89</v>
       </c>
       <c r="D77" s="1" t="n">
-        <v>3.7</v>
+        <v>-1.85</v>
       </c>
       <c r="E77" s="1" t="n">
         <v>-6.1</v>
@@ -5240,10 +5240,10 @@
         <v>1.5</v>
       </c>
       <c r="H77" s="1" t="n">
-        <v>2.8</v>
+        <v>-2.75</v>
       </c>
       <c r="I77" s="1" t="n">
-        <v>4.600000000000001</v>
+        <v>-0.9500000000000001</v>
       </c>
       <c r="J77" s="1" t="n">
         <v>-5.35</v>
@@ -5259,7 +5259,7 @@
         <v>0</v>
       </c>
       <c r="O77" s="1" t="n">
-        <v>3.7</v>
+        <v>-1.85</v>
       </c>
       <c r="P77" s="1" t="n">
         <v>-6.1</v>
@@ -5297,7 +5297,7 @@
         <v>90</v>
       </c>
       <c r="D78" s="1" t="n">
-        <v>-3.7</v>
+        <v>0</v>
       </c>
       <c r="E78" s="1" t="n">
         <v>-6.1</v>
@@ -5309,10 +5309,10 @@
         <v>1.5</v>
       </c>
       <c r="H78" s="1" t="n">
-        <v>-4.600000000000001</v>
+        <v>-0.9</v>
       </c>
       <c r="I78" s="1" t="n">
-        <v>-2.8</v>
+        <v>0.9</v>
       </c>
       <c r="J78" s="1" t="n">
         <v>-5.35</v>
@@ -5328,7 +5328,7 @@
         <v>0</v>
       </c>
       <c r="O78" s="1" t="n">
-        <v>-3.7</v>
+        <v>0</v>
       </c>
       <c r="P78" s="1" t="n">
         <v>-6.1</v>
@@ -5366,7 +5366,7 @@
         <v>91</v>
       </c>
       <c r="D79" s="1" t="n">
-        <v>-1.85</v>
+        <v>1.85</v>
       </c>
       <c r="E79" s="1" t="n">
         <v>-6.1</v>
@@ -5378,10 +5378,10 @@
         <v>1.5</v>
       </c>
       <c r="H79" s="1" t="n">
-        <v>-2.75</v>
+        <v>0.9500000000000001</v>
       </c>
       <c r="I79" s="1" t="n">
-        <v>-0.9500000000000001</v>
+        <v>2.75</v>
       </c>
       <c r="J79" s="1" t="n">
         <v>-5.35</v>
@@ -5397,7 +5397,7 @@
         <v>0</v>
       </c>
       <c r="O79" s="1" t="n">
-        <v>-1.85</v>
+        <v>1.85</v>
       </c>
       <c r="P79" s="1" t="n">
         <v>-6.1</v>
@@ -5435,7 +5435,7 @@
         <v>92</v>
       </c>
       <c r="D80" s="1" t="n">
-        <v>0</v>
+        <v>3.7</v>
       </c>
       <c r="E80" s="1" t="n">
         <v>-6.1</v>
@@ -5447,10 +5447,10 @@
         <v>1.5</v>
       </c>
       <c r="H80" s="1" t="n">
-        <v>-0.9</v>
+        <v>2.8</v>
       </c>
       <c r="I80" s="1" t="n">
-        <v>0.9</v>
+        <v>4.600000000000001</v>
       </c>
       <c r="J80" s="1" t="n">
         <v>-5.35</v>
@@ -5466,7 +5466,7 @@
         <v>0</v>
       </c>
       <c r="O80" s="1" t="n">
-        <v>0</v>
+        <v>3.7</v>
       </c>
       <c r="P80" s="1" t="n">
         <v>-6.1</v>
@@ -5504,7 +5504,7 @@
         <v>93</v>
       </c>
       <c r="D81" s="1" t="n">
-        <v>1.85</v>
+        <v>-5.55</v>
       </c>
       <c r="E81" s="1" t="n">
         <v>-4.55</v>
@@ -5516,10 +5516,10 @@
         <v>1.5</v>
       </c>
       <c r="H81" s="1" t="n">
-        <v>0.9500000000000001</v>
+        <v>-6.45</v>
       </c>
       <c r="I81" s="1" t="n">
-        <v>2.75</v>
+        <v>-4.649999999999999</v>
       </c>
       <c r="J81" s="1" t="n">
         <v>-3.8</v>
@@ -5535,7 +5535,7 @@
         <v>0</v>
       </c>
       <c r="O81" s="1" t="n">
-        <v>1.85</v>
+        <v>-5.55</v>
       </c>
       <c r="P81" s="1" t="n">
         <v>-4.55</v>
@@ -5573,7 +5573,7 @@
         <v>94</v>
       </c>
       <c r="D82" s="1" t="n">
-        <v>3.7</v>
+        <v>-3.7</v>
       </c>
       <c r="E82" s="1" t="n">
         <v>-4.55</v>
@@ -5585,10 +5585,10 @@
         <v>1.5</v>
       </c>
       <c r="H82" s="1" t="n">
-        <v>2.8</v>
+        <v>-4.600000000000001</v>
       </c>
       <c r="I82" s="1" t="n">
-        <v>4.600000000000001</v>
+        <v>-2.8</v>
       </c>
       <c r="J82" s="1" t="n">
         <v>-3.8</v>
@@ -5604,7 +5604,7 @@
         <v>0</v>
       </c>
       <c r="O82" s="1" t="n">
-        <v>3.7</v>
+        <v>-3.7</v>
       </c>
       <c r="P82" s="1" t="n">
         <v>-4.55</v>
@@ -5642,7 +5642,7 @@
         <v>95</v>
       </c>
       <c r="D83" s="1" t="n">
-        <v>-3.7</v>
+        <v>-1.85</v>
       </c>
       <c r="E83" s="1" t="n">
         <v>-4.55</v>
@@ -5654,10 +5654,10 @@
         <v>1.5</v>
       </c>
       <c r="H83" s="1" t="n">
-        <v>-4.600000000000001</v>
+        <v>-2.75</v>
       </c>
       <c r="I83" s="1" t="n">
-        <v>-2.8</v>
+        <v>-0.9500000000000001</v>
       </c>
       <c r="J83" s="1" t="n">
         <v>-3.8</v>
@@ -5673,7 +5673,7 @@
         <v>0</v>
       </c>
       <c r="O83" s="1" t="n">
-        <v>-3.7</v>
+        <v>-1.85</v>
       </c>
       <c r="P83" s="1" t="n">
         <v>-4.55</v>
@@ -5711,7 +5711,7 @@
         <v>96</v>
       </c>
       <c r="D84" s="1" t="n">
-        <v>-1.85</v>
+        <v>0</v>
       </c>
       <c r="E84" s="1" t="n">
         <v>-4.55</v>
@@ -5723,10 +5723,10 @@
         <v>1.5</v>
       </c>
       <c r="H84" s="1" t="n">
-        <v>-2.75</v>
+        <v>-0.9</v>
       </c>
       <c r="I84" s="1" t="n">
-        <v>-0.9500000000000001</v>
+        <v>0.9</v>
       </c>
       <c r="J84" s="1" t="n">
         <v>-3.8</v>
@@ -5742,7 +5742,7 @@
         <v>0</v>
       </c>
       <c r="O84" s="1" t="n">
-        <v>-1.85</v>
+        <v>0</v>
       </c>
       <c r="P84" s="1" t="n">
         <v>-4.55</v>
@@ -5780,7 +5780,7 @@
         <v>97</v>
       </c>
       <c r="D85" s="1" t="n">
-        <v>0</v>
+        <v>1.85</v>
       </c>
       <c r="E85" s="1" t="n">
         <v>-4.55</v>
@@ -5792,10 +5792,10 @@
         <v>1.5</v>
       </c>
       <c r="H85" s="1" t="n">
-        <v>-0.9</v>
+        <v>0.9500000000000001</v>
       </c>
       <c r="I85" s="1" t="n">
-        <v>0.9</v>
+        <v>2.75</v>
       </c>
       <c r="J85" s="1" t="n">
         <v>-3.8</v>
@@ -5811,7 +5811,7 @@
         <v>0</v>
       </c>
       <c r="O85" s="1" t="n">
-        <v>0</v>
+        <v>1.85</v>
       </c>
       <c r="P85" s="1" t="n">
         <v>-4.55</v>
@@ -5849,7 +5849,7 @@
         <v>98</v>
       </c>
       <c r="D86" s="1" t="n">
-        <v>1.85</v>
+        <v>3.7</v>
       </c>
       <c r="E86" s="1" t="n">
         <v>-4.55</v>
@@ -5861,10 +5861,10 @@
         <v>1.5</v>
       </c>
       <c r="H86" s="1" t="n">
-        <v>0.9500000000000001</v>
+        <v>2.8</v>
       </c>
       <c r="I86" s="1" t="n">
-        <v>2.75</v>
+        <v>4.600000000000001</v>
       </c>
       <c r="J86" s="1" t="n">
         <v>-3.8</v>
@@ -5880,7 +5880,7 @@
         <v>0</v>
       </c>
       <c r="O86" s="1" t="n">
-        <v>1.85</v>
+        <v>3.7</v>
       </c>
       <c r="P86" s="1" t="n">
         <v>-4.55</v>
@@ -5918,7 +5918,7 @@
         <v>99</v>
       </c>
       <c r="D87" s="1" t="n">
-        <v>3.7</v>
+        <v>-5.55</v>
       </c>
       <c r="E87" s="1" t="n">
         <v>-3</v>
@@ -5930,10 +5930,10 @@
         <v>1.5</v>
       </c>
       <c r="H87" s="1" t="n">
-        <v>2.8</v>
+        <v>-6.45</v>
       </c>
       <c r="I87" s="1" t="n">
-        <v>4.600000000000001</v>
+        <v>-4.649999999999999</v>
       </c>
       <c r="J87" s="1" t="n">
         <v>-2.25</v>
@@ -5949,7 +5949,7 @@
         <v>0</v>
       </c>
       <c r="O87" s="1" t="n">
-        <v>3.7</v>
+        <v>-5.55</v>
       </c>
       <c r="P87" s="1" t="n">
         <v>-3</v>

</xml_diff>

<commit_message>
initial code framework for testing on already generated masks
</commit_message>
<xml_diff>
--- a/masks/code/ResonatorArray.xlsx
+++ b/masks/code/ResonatorArray.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -750,15 +750,15 @@
     <col customWidth="1" max="5" min="5" width="8"/>
     <col customWidth="1" max="6" min="6" width="6"/>
     <col customWidth="1" max="7" min="7" width="6"/>
-    <col customWidth="1" max="8" min="8" width="21"/>
-    <col customWidth="1" max="9" min="9" width="21"/>
-    <col customWidth="1" max="10" min="10" width="22"/>
-    <col customWidth="1" max="11" min="11" width="21"/>
+    <col customWidth="1" max="8" min="8" width="7"/>
+    <col customWidth="1" max="9" min="9" width="7"/>
+    <col customWidth="1" max="10" min="10" width="7"/>
+    <col customWidth="1" max="11" min="11" width="7"/>
     <col customWidth="1" max="12" min="12" width="6"/>
-    <col customWidth="1" max="13" min="13" width="19"/>
+    <col customWidth="1" max="13" min="13" width="9"/>
     <col customWidth="1" max="14" min="14" width="9"/>
-    <col customWidth="1" max="15" min="15" width="20"/>
-    <col customWidth="1" max="16" min="16" width="20"/>
+    <col customWidth="1" max="15" min="15" width="9"/>
+    <col customWidth="1" max="16" min="16" width="8"/>
     <col customWidth="1" max="17" min="17" width="6"/>
     <col customWidth="1" max="18" min="18" width="6"/>
     <col customWidth="1" max="19" min="19" width="24"/>

</xml_diff>

<commit_message>
finalized Dark resonator array
</commit_message>
<xml_diff>
--- a/masks/code/ResonatorArray.xlsx
+++ b/masks/code/ResonatorArray.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -750,15 +750,15 @@
     <col customWidth="1" max="5" min="5" width="8"/>
     <col customWidth="1" max="6" min="6" width="6"/>
     <col customWidth="1" max="7" min="7" width="6"/>
-    <col customWidth="1" max="8" min="8" width="7"/>
-    <col customWidth="1" max="9" min="9" width="7"/>
-    <col customWidth="1" max="10" min="10" width="7"/>
-    <col customWidth="1" max="11" min="11" width="7"/>
+    <col customWidth="1" max="8" min="8" width="21"/>
+    <col customWidth="1" max="9" min="9" width="21"/>
+    <col customWidth="1" max="10" min="10" width="22"/>
+    <col customWidth="1" max="11" min="11" width="21"/>
     <col customWidth="1" max="12" min="12" width="6"/>
-    <col customWidth="1" max="13" min="13" width="9"/>
+    <col customWidth="1" max="13" min="13" width="19"/>
     <col customWidth="1" max="14" min="14" width="9"/>
-    <col customWidth="1" max="15" min="15" width="9"/>
-    <col customWidth="1" max="16" min="16" width="8"/>
+    <col customWidth="1" max="15" min="15" width="20"/>
+    <col customWidth="1" max="16" min="16" width="20"/>
     <col customWidth="1" max="17" min="17" width="6"/>
     <col customWidth="1" max="18" min="18" width="6"/>
     <col customWidth="1" max="19" min="19" width="24"/>
@@ -1088,7 +1088,7 @@
         <v>28</v>
       </c>
       <c r="D17" s="1" t="n">
-        <v>3</v>
+        <v>3.6</v>
       </c>
       <c r="E17" s="1" t="n">
         <v>0.65</v>
@@ -1100,10 +1100,10 @@
         <v>0.8</v>
       </c>
       <c r="H17" s="1" t="n">
-        <v>2.6</v>
+        <v>3.2</v>
       </c>
       <c r="I17" s="1" t="n">
-        <v>3.4</v>
+        <v>4</v>
       </c>
       <c r="J17" s="1" t="n">
         <v>1.05</v>
@@ -1119,7 +1119,7 @@
         <v>-16.296</v>
       </c>
       <c r="O17" s="1" t="n">
-        <v>-2.992000000000001</v>
+        <v>-2.392000000000001</v>
       </c>
       <c r="P17" s="1" t="n">
         <v>16.946</v>
@@ -1160,7 +1160,7 @@
         <v>0</v>
       </c>
       <c r="E18" s="1" t="n">
-        <v>10.2</v>
+        <v>10.3</v>
       </c>
       <c r="F18" s="1" t="n">
         <v>6.4</v>
@@ -1175,10 +1175,10 @@
         <v>3.2</v>
       </c>
       <c r="J18" s="1" t="n">
-        <v>10.4</v>
+        <v>10.5</v>
       </c>
       <c r="K18" s="1" t="n">
-        <v>10</v>
+        <v>10.1</v>
       </c>
       <c r="L18" s="1" t="n"/>
       <c r="M18" s="1" t="n">
@@ -1191,7 +1191,7 @@
         <v>0</v>
       </c>
       <c r="P18" s="1" t="n">
-        <v>48.7</v>
+        <v>48.8</v>
       </c>
       <c r="Q18" s="1" t="n"/>
       <c r="R18" s="1" t="n"/>
@@ -1226,7 +1226,7 @@
         <v>30</v>
       </c>
       <c r="D19" s="1" t="n">
-        <v>-10.6</v>
+        <v>-8.75</v>
       </c>
       <c r="E19" s="1" t="n">
         <v>0</v>
@@ -1238,10 +1238,10 @@
         <v>22.4</v>
       </c>
       <c r="H19" s="1" t="n">
-        <v>-10.8</v>
+        <v>-8.949999999999999</v>
       </c>
       <c r="I19" s="1" t="n">
-        <v>-10.4</v>
+        <v>-8.550000000000001</v>
       </c>
       <c r="J19" s="1" t="n">
         <v>11.2</v>
@@ -1257,7 +1257,7 @@
         <v>-27.496</v>
       </c>
       <c r="O19" s="1" t="n">
-        <v>-16.592</v>
+        <v>-14.742</v>
       </c>
       <c r="P19" s="1" t="n">
         <v>27.496</v>
@@ -1295,7 +1295,7 @@
         <v>31</v>
       </c>
       <c r="D20" s="1" t="n">
-        <v>5.8</v>
+        <v>6.4</v>
       </c>
       <c r="E20" s="1" t="n">
         <v>0</v>
@@ -1307,10 +1307,10 @@
         <v>2.1</v>
       </c>
       <c r="H20" s="1" t="n">
-        <v>3.6</v>
+        <v>4.2</v>
       </c>
       <c r="I20" s="1" t="n">
-        <v>8</v>
+        <v>8.600000000000001</v>
       </c>
       <c r="J20" s="1" t="n">
         <v>1.05</v>
@@ -1326,7 +1326,7 @@
         <v>-38.401</v>
       </c>
       <c r="O20" s="1" t="n">
-        <v>44.3</v>
+        <v>44.9</v>
       </c>
       <c r="P20" s="1" t="n">
         <v>38.401</v>
@@ -1364,7 +1364,7 @@
         <v>32</v>
       </c>
       <c r="D21" s="1" t="n">
-        <v>-8.800000000000001</v>
+        <v>-9.35</v>
       </c>
       <c r="E21" s="1" t="n">
         <v>0</v>
@@ -1376,10 +1376,10 @@
         <v>11.4</v>
       </c>
       <c r="H21" s="1" t="n">
-        <v>-9</v>
+        <v>-9.549999999999999</v>
       </c>
       <c r="I21" s="1" t="n">
-        <v>-8.600000000000001</v>
+        <v>-9.15</v>
       </c>
       <c r="J21" s="1" t="n">
         <v>5.7</v>
@@ -1395,7 +1395,7 @@
         <v>-31.082</v>
       </c>
       <c r="O21" s="1" t="n">
-        <v>79.2</v>
+        <v>78.65000000000001</v>
       </c>
       <c r="P21" s="1" t="n">
         <v>31.082</v>
@@ -1433,7 +1433,7 @@
         <v>32</v>
       </c>
       <c r="D22" s="1" t="n">
-        <v>-8.800000000000001</v>
+        <v>-9.35</v>
       </c>
       <c r="E22" s="1" t="n">
         <v>0</v>
@@ -1445,10 +1445,10 @@
         <v>11.4</v>
       </c>
       <c r="H22" s="1" t="n">
-        <v>-9</v>
+        <v>-9.549999999999999</v>
       </c>
       <c r="I22" s="1" t="n">
-        <v>-8.600000000000001</v>
+        <v>-9.15</v>
       </c>
       <c r="J22" s="1" t="n">
         <v>5.7</v>
@@ -1464,7 +1464,7 @@
         <v>-20.082</v>
       </c>
       <c r="O22" s="1" t="n">
-        <v>-96.8</v>
+        <v>-97.34999999999999</v>
       </c>
       <c r="P22" s="1" t="n">
         <v>20.082</v>
@@ -1571,7 +1571,7 @@
         <v>35</v>
       </c>
       <c r="D24" s="1" t="n">
-        <v>8.65</v>
+        <v>9.25</v>
       </c>
       <c r="E24" s="1" t="n">
         <v>0</v>
@@ -1583,10 +1583,10 @@
         <v>16.9</v>
       </c>
       <c r="H24" s="1" t="n">
-        <v>8.200000000000001</v>
+        <v>8.800000000000001</v>
       </c>
       <c r="I24" s="1" t="n">
-        <v>9.1</v>
+        <v>9.699999999999999</v>
       </c>
       <c r="J24" s="1" t="n">
         <v>8.449999999999999</v>
@@ -1602,7 +1602,7 @@
         <v>-38.9</v>
       </c>
       <c r="O24" s="1" t="n">
-        <v>108.55</v>
+        <v>109.15</v>
       </c>
       <c r="P24" s="1" t="n">
         <v>38.9</v>
@@ -1709,7 +1709,7 @@
         <v>37</v>
       </c>
       <c r="D26" s="1" t="n">
-        <v>6.45</v>
+        <v>7.05</v>
       </c>
       <c r="E26" s="1" t="n">
         <v>-2.15</v>
@@ -1721,10 +1721,10 @@
         <v>1.8</v>
       </c>
       <c r="H26" s="1" t="n">
-        <v>4.9</v>
+        <v>5.5</v>
       </c>
       <c r="I26" s="1" t="n">
-        <v>8</v>
+        <v>8.6</v>
       </c>
       <c r="J26" s="1" t="n">
         <v>-1.25</v>
@@ -1740,7 +1740,7 @@
         <v>-38.401</v>
       </c>
       <c r="O26" s="1" t="n">
-        <v>45.51300000000001</v>
+        <v>46.113</v>
       </c>
       <c r="P26" s="1" t="n">
         <v>36.251</v>
@@ -1781,13 +1781,13 @@
         <v>0</v>
       </c>
       <c r="E27" s="1" t="n">
-        <v>12.6</v>
+        <v>12.55</v>
       </c>
       <c r="F27" s="1" t="n">
         <v>15.4</v>
       </c>
       <c r="G27" s="1" t="n">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="H27" s="1" t="n">
         <v>-7.7</v>
@@ -1799,20 +1799,20 @@
         <v>12.8</v>
       </c>
       <c r="K27" s="1" t="n">
-        <v>12.4</v>
+        <v>12.3</v>
       </c>
       <c r="L27" s="1" t="n"/>
       <c r="M27" s="1" t="n">
         <v>-52.5</v>
       </c>
       <c r="N27" s="1" t="n">
-        <v>-50.55</v>
+        <v>-50.624</v>
       </c>
       <c r="O27" s="1" t="n">
         <v>52.5</v>
       </c>
       <c r="P27" s="1" t="n">
-        <v>63.15</v>
+        <v>63.17400000000001</v>
       </c>
       <c r="Q27" s="1" t="n"/>
       <c r="R27" s="1" t="n"/>
@@ -1829,7 +1829,7 @@
         <v>-0</v>
       </c>
       <c r="W27" s="1" t="n">
-        <v>-0.025</v>
+        <v>-0.062</v>
       </c>
       <c r="X27" s="1" t="n">
         <v>15</v>
@@ -1847,22 +1847,22 @@
         <v>40</v>
       </c>
       <c r="D28" s="1" t="n">
-        <v>-10</v>
+        <v>-10.6</v>
       </c>
       <c r="E28" s="1" t="n">
         <v>0</v>
       </c>
       <c r="F28" s="1" t="n">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="G28" s="1" t="n">
         <v>15.4</v>
       </c>
       <c r="H28" s="1" t="n">
-        <v>-10.2</v>
+        <v>-10.85</v>
       </c>
       <c r="I28" s="1" t="n">
-        <v>-9.800000000000001</v>
+        <v>-10.35</v>
       </c>
       <c r="J28" s="1" t="n">
         <v>7.7</v>
@@ -1872,13 +1872,13 @@
       </c>
       <c r="L28" s="1" t="n"/>
       <c r="M28" s="1" t="n">
-        <v>-50.55</v>
+        <v>-50.624</v>
       </c>
       <c r="N28" s="1" t="n">
         <v>-52.5</v>
       </c>
       <c r="O28" s="1" t="n">
-        <v>40.55</v>
+        <v>40.024</v>
       </c>
       <c r="P28" s="1" t="n">
         <v>52.5</v>
@@ -1895,7 +1895,7 @@
         <v>8</v>
       </c>
       <c r="V28" s="1" t="n">
-        <v>-0.025</v>
+        <v>-0.062</v>
       </c>
       <c r="W28" s="1" t="n">
         <v>-0</v>
@@ -6608,7 +6608,7 @@
         <v>111</v>
       </c>
       <c r="D97" s="1" t="n">
-        <v>9.75</v>
+        <v>10.35</v>
       </c>
       <c r="E97" s="1" t="n">
         <v>0</v>
@@ -6620,10 +6620,10 @@
         <v>16.9</v>
       </c>
       <c r="H97" s="1" t="n">
-        <v>9.300000000000001</v>
+        <v>9.9</v>
       </c>
       <c r="I97" s="1" t="n">
-        <v>10.2</v>
+        <v>10.8</v>
       </c>
       <c r="J97" s="1" t="n">
         <v>8.449999999999999</v>
@@ -6639,7 +6639,7 @@
         <v>-38.9</v>
       </c>
       <c r="O97" s="1" t="n">
-        <v>109.65</v>
+        <v>110.25</v>
       </c>
       <c r="P97" s="1" t="n">
         <v>38.9</v>
@@ -6677,7 +6677,7 @@
         <v>112</v>
       </c>
       <c r="D98" s="1" t="n">
-        <v>3</v>
+        <v>3.6</v>
       </c>
       <c r="E98" s="1" t="n">
         <v>-0.35</v>
@@ -6689,10 +6689,10 @@
         <v>0.8</v>
       </c>
       <c r="H98" s="1" t="n">
-        <v>2.6</v>
+        <v>3.2</v>
       </c>
       <c r="I98" s="1" t="n">
-        <v>3.4</v>
+        <v>4</v>
       </c>
       <c r="J98" s="1" t="n">
         <v>0.05000000000000004</v>
@@ -6708,7 +6708,7 @@
         <v>-16.296</v>
       </c>
       <c r="O98" s="1" t="n">
-        <v>-2.992000000000001</v>
+        <v>-2.392000000000001</v>
       </c>
       <c r="P98" s="1" t="n">
         <v>15.946</v>
@@ -6746,7 +6746,7 @@
         <v>113</v>
       </c>
       <c r="D99" s="1" t="n">
-        <v>2.2</v>
+        <v>2.8</v>
       </c>
       <c r="E99" s="1" t="n">
         <v>0.65</v>
@@ -6758,10 +6758,10 @@
         <v>0.8</v>
       </c>
       <c r="H99" s="1" t="n">
-        <v>2</v>
+        <v>2.6</v>
       </c>
       <c r="I99" s="1" t="n">
-        <v>2.4</v>
+        <v>3</v>
       </c>
       <c r="J99" s="1" t="n">
         <v>1.05</v>
@@ -6777,7 +6777,7 @@
         <v>-37.645</v>
       </c>
       <c r="O99" s="1" t="n">
-        <v>41</v>
+        <v>41.59999999999999</v>
       </c>
       <c r="P99" s="1" t="n">
         <v>38.295</v>
@@ -6815,7 +6815,7 @@
         <v>114</v>
       </c>
       <c r="D100" s="1" t="n">
-        <v>2.2</v>
+        <v>2.8</v>
       </c>
       <c r="E100" s="1" t="n">
         <v>-0.25</v>
@@ -6827,10 +6827,10 @@
         <v>0.6</v>
       </c>
       <c r="H100" s="1" t="n">
-        <v>2</v>
+        <v>2.6</v>
       </c>
       <c r="I100" s="1" t="n">
-        <v>2.4</v>
+        <v>3</v>
       </c>
       <c r="J100" s="1" t="n">
         <v>0.04999999999999999</v>
@@ -6846,7 +6846,7 @@
         <v>-39.063</v>
       </c>
       <c r="O100" s="1" t="n">
-        <v>41</v>
+        <v>41.59999999999999</v>
       </c>
       <c r="P100" s="1" t="n">
         <v>38.813</v>
@@ -7022,10 +7022,10 @@
         <v>117</v>
       </c>
       <c r="D103" s="1" t="n">
-        <v>10.6</v>
+        <v>-8.15</v>
       </c>
       <c r="E103" s="1" t="n">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="F103" s="1" t="n">
         <v>0.4</v>
@@ -7034,16 +7034,16 @@
         <v>22.4</v>
       </c>
       <c r="H103" s="1" t="n">
-        <v>10.4</v>
+        <v>-8.35</v>
       </c>
       <c r="I103" s="1" t="n">
-        <v>10.8</v>
+        <v>-7.95</v>
       </c>
       <c r="J103" s="1" t="n">
-        <v>11.2</v>
+        <v>12</v>
       </c>
       <c r="K103" s="1" t="n">
-        <v>-11.2</v>
+        <v>-10.4</v>
       </c>
       <c r="L103" s="1" t="n"/>
       <c r="M103" s="1" t="n">
@@ -7053,10 +7053,10 @@
         <v>-27.496</v>
       </c>
       <c r="O103" s="1" t="n">
-        <v>4.608</v>
+        <v>-14.142</v>
       </c>
       <c r="P103" s="1" t="n">
-        <v>27.496</v>
+        <v>28.296</v>
       </c>
       <c r="Q103" s="1" t="n"/>
       <c r="R103" s="1" t="n"/>
@@ -7091,7 +7091,7 @@
         <v>118</v>
       </c>
       <c r="D104" s="1" t="n">
-        <v>-9.4</v>
+        <v>-9.949999999999999</v>
       </c>
       <c r="E104" s="1" t="n">
         <v>0</v>
@@ -7103,10 +7103,10 @@
         <v>11.4</v>
       </c>
       <c r="H104" s="1" t="n">
-        <v>-9.6</v>
+        <v>-10.15</v>
       </c>
       <c r="I104" s="1" t="n">
-        <v>-9.200000000000001</v>
+        <v>-9.75</v>
       </c>
       <c r="J104" s="1" t="n">
         <v>5.7</v>
@@ -7122,7 +7122,7 @@
         <v>-31.082</v>
       </c>
       <c r="O104" s="1" t="n">
-        <v>78.59999999999999</v>
+        <v>78.05</v>
       </c>
       <c r="P104" s="1" t="n">
         <v>31.082</v>
@@ -7160,7 +7160,7 @@
         <v>118</v>
       </c>
       <c r="D105" s="1" t="n">
-        <v>-9.4</v>
+        <v>-9.949999999999999</v>
       </c>
       <c r="E105" s="1" t="n">
         <v>0</v>
@@ -7172,10 +7172,10 @@
         <v>11.4</v>
       </c>
       <c r="H105" s="1" t="n">
-        <v>-9.6</v>
+        <v>-10.15</v>
       </c>
       <c r="I105" s="1" t="n">
-        <v>-9.200000000000001</v>
+        <v>-9.75</v>
       </c>
       <c r="J105" s="1" t="n">
         <v>5.7</v>
@@ -7191,7 +7191,7 @@
         <v>-20.082</v>
       </c>
       <c r="O105" s="1" t="n">
-        <v>-97.40000000000001</v>
+        <v>-97.95</v>
       </c>
       <c r="P105" s="1" t="n">
         <v>20.082</v>

</xml_diff>

<commit_message>
fixes to cell shift calculations
</commit_message>
<xml_diff>
--- a/masks/code/ResonatorArray.xlsx
+++ b/masks/code/ResonatorArray.xlsx
@@ -755,16 +755,16 @@
     <col customWidth="1" max="10" min="10" width="22"/>
     <col customWidth="1" max="11" min="11" width="21"/>
     <col customWidth="1" max="12" min="12" width="6"/>
-    <col customWidth="1" max="13" min="13" width="19"/>
+    <col customWidth="1" max="13" min="13" width="20"/>
     <col customWidth="1" max="14" min="14" width="9"/>
     <col customWidth="1" max="15" min="15" width="20"/>
-    <col customWidth="1" max="16" min="16" width="20"/>
+    <col customWidth="1" max="16" min="16" width="22"/>
     <col customWidth="1" max="17" min="17" width="6"/>
     <col customWidth="1" max="18" min="18" width="6"/>
     <col customWidth="1" max="19" min="19" width="24"/>
     <col customWidth="1" max="20" min="20" width="6"/>
     <col customWidth="1" max="21" min="21" width="6"/>
-    <col customWidth="1" max="22" min="22" width="9"/>
+    <col customWidth="1" max="22" min="22" width="20"/>
     <col customWidth="1" max="23" min="23" width="8"/>
     <col customWidth="1" max="24" min="24" width="7"/>
     <col customWidth="1" max="25" min="25" width="8"/>
@@ -973,16 +973,16 @@
       </c>
       <c r="L15" s="1" t="n"/>
       <c r="M15" s="1" t="n">
-        <v>-41.15</v>
+        <v>-2.65</v>
       </c>
       <c r="N15" s="1" t="n">
-        <v>-38.401</v>
+        <v>0</v>
       </c>
       <c r="O15" s="1" t="n">
-        <v>42.25</v>
+        <v>3.75</v>
       </c>
       <c r="P15" s="1" t="n">
-        <v>38.251</v>
+        <v>-0.15</v>
       </c>
       <c r="Q15" s="1" t="s">
         <v>25</v>
@@ -1001,7 +1001,7 @@
         <v>-0</v>
       </c>
       <c r="W15" s="1" t="n">
-        <v>0.099</v>
+        <v>0</v>
       </c>
       <c r="X15" s="1" t="n">
         <v>11</v>
@@ -1044,16 +1044,16 @@
       </c>
       <c r="L16" s="1" t="n"/>
       <c r="M16" s="1" t="n">
-        <v>-38.5</v>
+        <v>0</v>
       </c>
       <c r="N16" s="1" t="n">
-        <v>-37.442</v>
+        <v>0.959</v>
       </c>
       <c r="O16" s="1" t="n">
-        <v>38.5</v>
+        <v>0</v>
       </c>
       <c r="P16" s="1" t="n">
-        <v>48.842</v>
+        <v>10.441</v>
       </c>
       <c r="Q16" s="1" t="n"/>
       <c r="R16" s="1" t="n"/>
@@ -1070,7 +1070,7 @@
         <v>-0</v>
       </c>
       <c r="W16" s="1" t="n">
-        <v>0.099</v>
+        <v>0</v>
       </c>
       <c r="X16" s="1" t="n">
         <v>11</v>
@@ -1113,16 +1113,16 @@
       </c>
       <c r="L17" s="1" t="n"/>
       <c r="M17" s="1" t="n">
-        <v>5.992000000000001</v>
+        <v>49.996</v>
       </c>
       <c r="N17" s="1" t="n">
-        <v>-16.296</v>
+        <v>0.959</v>
       </c>
       <c r="O17" s="1" t="n">
-        <v>-2.392000000000001</v>
+        <v>-46.396</v>
       </c>
       <c r="P17" s="1" t="n">
-        <v>16.946</v>
+        <v>-0.3089999999999999</v>
       </c>
       <c r="Q17" s="1" t="n"/>
       <c r="R17" s="1" t="n"/>
@@ -1182,16 +1182,16 @@
       </c>
       <c r="L18" s="1" t="n"/>
       <c r="M18" s="1" t="n">
-        <v>0</v>
+        <v>47</v>
       </c>
       <c r="N18" s="1" t="n">
-        <v>-38.5</v>
+        <v>-37.541</v>
       </c>
       <c r="O18" s="1" t="n">
-        <v>0</v>
+        <v>-47</v>
       </c>
       <c r="P18" s="1" t="n">
-        <v>48.8</v>
+        <v>47.84099999999999</v>
       </c>
       <c r="Q18" s="1" t="n"/>
       <c r="R18" s="1" t="n"/>
@@ -1251,16 +1251,16 @@
       </c>
       <c r="L19" s="1" t="n"/>
       <c r="M19" s="1" t="n">
-        <v>5.992</v>
+        <v>49.996</v>
       </c>
       <c r="N19" s="1" t="n">
-        <v>-27.496</v>
+        <v>-26.537</v>
       </c>
       <c r="O19" s="1" t="n">
-        <v>-14.742</v>
+        <v>-58.746</v>
       </c>
       <c r="P19" s="1" t="n">
-        <v>27.496</v>
+        <v>26.537</v>
       </c>
       <c r="Q19" s="1" t="n"/>
       <c r="R19" s="1" t="n"/>
@@ -1320,16 +1320,16 @@
       </c>
       <c r="L20" s="1" t="n"/>
       <c r="M20" s="1" t="n">
-        <v>-38.5</v>
+        <v>0</v>
       </c>
       <c r="N20" s="1" t="n">
-        <v>-38.401</v>
+        <v>0</v>
       </c>
       <c r="O20" s="1" t="n">
-        <v>44.9</v>
+        <v>6.4</v>
       </c>
       <c r="P20" s="1" t="n">
-        <v>38.401</v>
+        <v>0</v>
       </c>
       <c r="Q20" s="1" t="n"/>
       <c r="R20" s="1" t="n"/>
@@ -1346,7 +1346,7 @@
         <v>-0</v>
       </c>
       <c r="W20" s="1" t="n">
-        <v>0.099</v>
+        <v>0</v>
       </c>
       <c r="X20" s="1" t="n">
         <v>11</v>
@@ -1389,16 +1389,16 @@
       </c>
       <c r="L21" s="1" t="n"/>
       <c r="M21" s="1" t="n">
-        <v>-88</v>
+        <v>-44</v>
       </c>
       <c r="N21" s="1" t="n">
-        <v>-31.082</v>
+        <v>0.959</v>
       </c>
       <c r="O21" s="1" t="n">
-        <v>78.65000000000001</v>
+        <v>34.65</v>
       </c>
       <c r="P21" s="1" t="n">
-        <v>31.082</v>
+        <v>-0.959</v>
       </c>
       <c r="Q21" s="1" t="n"/>
       <c r="R21" s="1" t="n"/>
@@ -1458,16 +1458,16 @@
       </c>
       <c r="L22" s="1" t="n"/>
       <c r="M22" s="1" t="n">
-        <v>88</v>
+        <v>44</v>
       </c>
       <c r="N22" s="1" t="n">
-        <v>-20.082</v>
+        <v>0.959</v>
       </c>
       <c r="O22" s="1" t="n">
-        <v>-97.34999999999999</v>
+        <v>-53.35</v>
       </c>
       <c r="P22" s="1" t="n">
-        <v>20.082</v>
+        <v>-0.959</v>
       </c>
       <c r="Q22" s="1" t="n"/>
       <c r="R22" s="1" t="n"/>
@@ -1527,16 +1527,16 @@
       </c>
       <c r="L23" s="1" t="n"/>
       <c r="M23" s="1" t="n">
-        <v>-38.9</v>
+        <v>0</v>
       </c>
       <c r="N23" s="1" t="n">
-        <v>-49.94</v>
+        <v>0</v>
       </c>
       <c r="O23" s="1" t="n">
-        <v>38.9</v>
+        <v>0</v>
       </c>
       <c r="P23" s="1" t="n">
-        <v>37.59</v>
+        <v>-12.35</v>
       </c>
       <c r="Q23" s="1" t="n"/>
       <c r="R23" s="1" t="n"/>
@@ -1596,16 +1596,16 @@
       </c>
       <c r="L24" s="1" t="n"/>
       <c r="M24" s="1" t="n">
-        <v>-99.90000000000001</v>
+        <v>-49.95</v>
       </c>
       <c r="N24" s="1" t="n">
-        <v>-38.9</v>
+        <v>0</v>
       </c>
       <c r="O24" s="1" t="n">
-        <v>109.15</v>
+        <v>59.2</v>
       </c>
       <c r="P24" s="1" t="n">
-        <v>38.9</v>
+        <v>0</v>
       </c>
       <c r="Q24" s="1" t="n"/>
       <c r="R24" s="1" t="n"/>
@@ -1665,16 +1665,16 @@
       </c>
       <c r="L25" s="1" t="n"/>
       <c r="M25" s="1" t="n">
-        <v>-38.8</v>
+        <v>-0.3</v>
       </c>
       <c r="N25" s="1" t="n">
-        <v>-39.168</v>
+        <v>-0.767</v>
       </c>
       <c r="O25" s="1" t="n">
-        <v>40.55</v>
+        <v>2.05</v>
       </c>
       <c r="P25" s="1" t="n">
-        <v>39.568</v>
+        <v>1.167</v>
       </c>
       <c r="Q25" s="1" t="n"/>
       <c r="R25" s="1" t="n"/>
@@ -1691,7 +1691,7 @@
         <v>-0</v>
       </c>
       <c r="W25" s="1" t="n">
-        <v>0.099</v>
+        <v>0</v>
       </c>
       <c r="X25" s="1" t="n">
         <v>11</v>
@@ -1734,16 +1734,16 @@
       </c>
       <c r="L26" s="1" t="n"/>
       <c r="M26" s="1" t="n">
-        <v>-39.063</v>
+        <v>-0.5629999999999999</v>
       </c>
       <c r="N26" s="1" t="n">
-        <v>-38.401</v>
+        <v>0</v>
       </c>
       <c r="O26" s="1" t="n">
-        <v>46.113</v>
+        <v>7.613</v>
       </c>
       <c r="P26" s="1" t="n">
-        <v>36.251</v>
+        <v>-2.15</v>
       </c>
       <c r="Q26" s="1" t="n"/>
       <c r="R26" s="1" t="n"/>
@@ -1760,7 +1760,7 @@
         <v>-0</v>
       </c>
       <c r="W26" s="1" t="n">
-        <v>0.099</v>
+        <v>0</v>
       </c>
       <c r="X26" s="1" t="n">
         <v>11</v>
@@ -1806,13 +1806,13 @@
         <v>-52.5</v>
       </c>
       <c r="N27" s="1" t="n">
-        <v>-50.624</v>
+        <v>-50.562</v>
       </c>
       <c r="O27" s="1" t="n">
         <v>52.5</v>
       </c>
       <c r="P27" s="1" t="n">
-        <v>63.17400000000001</v>
+        <v>63.11199999999999</v>
       </c>
       <c r="Q27" s="1" t="n"/>
       <c r="R27" s="1" t="n"/>
@@ -1872,13 +1872,13 @@
       </c>
       <c r="L28" s="1" t="n"/>
       <c r="M28" s="1" t="n">
-        <v>-50.624</v>
+        <v>-50.562</v>
       </c>
       <c r="N28" s="1" t="n">
         <v>-52.5</v>
       </c>
       <c r="O28" s="1" t="n">
-        <v>40.024</v>
+        <v>39.962</v>
       </c>
       <c r="P28" s="1" t="n">
         <v>52.5</v>
@@ -6357,16 +6357,16 @@
       </c>
       <c r="L93" s="1" t="n"/>
       <c r="M93" s="1" t="n">
-        <v>-38.363</v>
+        <v>0.1369999999999999</v>
       </c>
       <c r="N93" s="1" t="n">
-        <v>-38.401</v>
+        <v>0</v>
       </c>
       <c r="O93" s="1" t="n">
-        <v>37.113</v>
+        <v>-1.387</v>
       </c>
       <c r="P93" s="1" t="n">
-        <v>38.401</v>
+        <v>0</v>
       </c>
       <c r="Q93" s="1" t="n"/>
       <c r="R93" s="1" t="n"/>
@@ -6383,7 +6383,7 @@
         <v>-0</v>
       </c>
       <c r="W93" s="1" t="n">
-        <v>0.099</v>
+        <v>0</v>
       </c>
       <c r="X93" s="1" t="n">
         <v>11</v>
@@ -6426,16 +6426,16 @@
       </c>
       <c r="L94" s="1" t="n"/>
       <c r="M94" s="1" t="n">
-        <v>-36.98</v>
+        <v>1.52</v>
       </c>
       <c r="N94" s="1" t="n">
-        <v>-38.401</v>
+        <v>0</v>
       </c>
       <c r="O94" s="1" t="n">
-        <v>37.98</v>
+        <v>-0.52</v>
       </c>
       <c r="P94" s="1" t="n">
-        <v>38.801</v>
+        <v>0.4</v>
       </c>
       <c r="Q94" s="1" t="n"/>
       <c r="R94" s="1" t="n"/>
@@ -6452,7 +6452,7 @@
         <v>-0</v>
       </c>
       <c r="W94" s="1" t="n">
-        <v>0.099</v>
+        <v>0</v>
       </c>
       <c r="X94" s="1" t="n">
         <v>11</v>
@@ -6495,16 +6495,16 @@
       </c>
       <c r="L95" s="1" t="n"/>
       <c r="M95" s="1" t="n">
-        <v>-37.542</v>
+        <v>0.958</v>
       </c>
       <c r="N95" s="1" t="n">
-        <v>-38.401</v>
+        <v>0</v>
       </c>
       <c r="O95" s="1" t="n">
-        <v>37.542</v>
+        <v>-0.958</v>
       </c>
       <c r="P95" s="1" t="n">
-        <v>38.401</v>
+        <v>0</v>
       </c>
       <c r="Q95" s="1" t="n"/>
       <c r="R95" s="1" t="n"/>
@@ -6521,7 +6521,7 @@
         <v>-0</v>
       </c>
       <c r="W95" s="1" t="n">
-        <v>0.099</v>
+        <v>0</v>
       </c>
       <c r="X95" s="1" t="n">
         <v>11</v>
@@ -6564,16 +6564,16 @@
       </c>
       <c r="L96" s="1" t="n"/>
       <c r="M96" s="1" t="n">
-        <v>-38.9</v>
+        <v>0</v>
       </c>
       <c r="N96" s="1" t="n">
-        <v>-49.94</v>
+        <v>0</v>
       </c>
       <c r="O96" s="1" t="n">
-        <v>38.9</v>
+        <v>0</v>
       </c>
       <c r="P96" s="1" t="n">
-        <v>38.69</v>
+        <v>-11.25</v>
       </c>
       <c r="Q96" s="1" t="n"/>
       <c r="R96" s="1" t="n"/>
@@ -6633,16 +6633,16 @@
       </c>
       <c r="L97" s="1" t="n"/>
       <c r="M97" s="1" t="n">
-        <v>-99.90000000000001</v>
+        <v>-49.95</v>
       </c>
       <c r="N97" s="1" t="n">
-        <v>-38.9</v>
+        <v>0</v>
       </c>
       <c r="O97" s="1" t="n">
-        <v>110.25</v>
+        <v>60.3</v>
       </c>
       <c r="P97" s="1" t="n">
-        <v>38.9</v>
+        <v>0</v>
       </c>
       <c r="Q97" s="1" t="n"/>
       <c r="R97" s="1" t="n"/>
@@ -6702,16 +6702,16 @@
       </c>
       <c r="L98" s="1" t="n"/>
       <c r="M98" s="1" t="n">
-        <v>5.992000000000001</v>
+        <v>49.996</v>
       </c>
       <c r="N98" s="1" t="n">
-        <v>-16.296</v>
+        <v>0.959</v>
       </c>
       <c r="O98" s="1" t="n">
-        <v>-2.392000000000001</v>
+        <v>-46.396</v>
       </c>
       <c r="P98" s="1" t="n">
-        <v>15.946</v>
+        <v>-1.309</v>
       </c>
       <c r="Q98" s="1" t="n"/>
       <c r="R98" s="1" t="n"/>
@@ -6771,16 +6771,16 @@
       </c>
       <c r="L99" s="1" t="n"/>
       <c r="M99" s="1" t="n">
-        <v>-38.8</v>
+        <v>-0.3</v>
       </c>
       <c r="N99" s="1" t="n">
-        <v>-37.645</v>
+        <v>0.756</v>
       </c>
       <c r="O99" s="1" t="n">
-        <v>41.59999999999999</v>
+        <v>3.1</v>
       </c>
       <c r="P99" s="1" t="n">
-        <v>38.295</v>
+        <v>-0.106</v>
       </c>
       <c r="Q99" s="1" t="n"/>
       <c r="R99" s="1" t="n"/>
@@ -6797,7 +6797,7 @@
         <v>-0</v>
       </c>
       <c r="W99" s="1" t="n">
-        <v>0.099</v>
+        <v>0</v>
       </c>
       <c r="X99" s="1" t="n">
         <v>11</v>
@@ -6840,16 +6840,16 @@
       </c>
       <c r="L100" s="1" t="n"/>
       <c r="M100" s="1" t="n">
-        <v>-38.8</v>
+        <v>-0.3</v>
       </c>
       <c r="N100" s="1" t="n">
-        <v>-39.063</v>
+        <v>-0.662</v>
       </c>
       <c r="O100" s="1" t="n">
-        <v>41.59999999999999</v>
+        <v>3.1</v>
       </c>
       <c r="P100" s="1" t="n">
-        <v>38.813</v>
+        <v>0.412</v>
       </c>
       <c r="Q100" s="1" t="n"/>
       <c r="R100" s="1" t="n"/>
@@ -6866,7 +6866,7 @@
         <v>-0</v>
       </c>
       <c r="W100" s="1" t="n">
-        <v>0.099</v>
+        <v>0</v>
       </c>
       <c r="X100" s="1" t="n">
         <v>11</v>
@@ -6909,16 +6909,16 @@
       </c>
       <c r="L101" s="1" t="n"/>
       <c r="M101" s="1" t="n">
-        <v>-38.5</v>
+        <v>0</v>
       </c>
       <c r="N101" s="1" t="n">
-        <v>-37.442</v>
+        <v>0.959</v>
       </c>
       <c r="O101" s="1" t="n">
-        <v>38.5</v>
+        <v>0</v>
       </c>
       <c r="P101" s="1" t="n">
-        <v>49.442</v>
+        <v>11.041</v>
       </c>
       <c r="Q101" s="1" t="n"/>
       <c r="R101" s="1" t="n"/>
@@ -6935,7 +6935,7 @@
         <v>-0</v>
       </c>
       <c r="W101" s="1" t="n">
-        <v>0.099</v>
+        <v>0</v>
       </c>
       <c r="X101" s="1" t="n">
         <v>11</v>
@@ -6978,16 +6978,16 @@
       </c>
       <c r="L102" s="1" t="n"/>
       <c r="M102" s="1" t="n">
-        <v>0</v>
+        <v>47</v>
       </c>
       <c r="N102" s="1" t="n">
-        <v>-38.5</v>
+        <v>-37.541</v>
       </c>
       <c r="O102" s="1" t="n">
-        <v>0</v>
+        <v>-47</v>
       </c>
       <c r="P102" s="1" t="n">
-        <v>49.3</v>
+        <v>48.34099999999999</v>
       </c>
       <c r="Q102" s="1" t="n"/>
       <c r="R102" s="1" t="n"/>
@@ -7047,16 +7047,16 @@
       </c>
       <c r="L103" s="1" t="n"/>
       <c r="M103" s="1" t="n">
-        <v>5.992</v>
+        <v>49.996</v>
       </c>
       <c r="N103" s="1" t="n">
-        <v>-27.496</v>
+        <v>-26.537</v>
       </c>
       <c r="O103" s="1" t="n">
-        <v>-14.142</v>
+        <v>-58.146</v>
       </c>
       <c r="P103" s="1" t="n">
-        <v>28.296</v>
+        <v>27.337</v>
       </c>
       <c r="Q103" s="1" t="n"/>
       <c r="R103" s="1" t="n"/>
@@ -7116,16 +7116,16 @@
       </c>
       <c r="L104" s="1" t="n"/>
       <c r="M104" s="1" t="n">
-        <v>-88</v>
+        <v>-44</v>
       </c>
       <c r="N104" s="1" t="n">
-        <v>-31.082</v>
+        <v>0.959</v>
       </c>
       <c r="O104" s="1" t="n">
-        <v>78.05</v>
+        <v>34.05</v>
       </c>
       <c r="P104" s="1" t="n">
-        <v>31.082</v>
+        <v>-0.959</v>
       </c>
       <c r="Q104" s="1" t="n"/>
       <c r="R104" s="1" t="n"/>
@@ -7185,16 +7185,16 @@
       </c>
       <c r="L105" s="1" t="n"/>
       <c r="M105" s="1" t="n">
-        <v>88</v>
+        <v>44</v>
       </c>
       <c r="N105" s="1" t="n">
-        <v>-20.082</v>
+        <v>0.959</v>
       </c>
       <c r="O105" s="1" t="n">
-        <v>-97.95</v>
+        <v>-53.95</v>
       </c>
       <c r="P105" s="1" t="n">
-        <v>20.082</v>
+        <v>-0.959</v>
       </c>
       <c r="Q105" s="1" t="n"/>
       <c r="R105" s="1" t="n"/>

</xml_diff>

<commit_message>
fixing some bugs in patches.py
</commit_message>
<xml_diff>
--- a/masks/code/ResonatorArray.xlsx
+++ b/masks/code/ResonatorArray.xlsx
@@ -765,7 +765,7 @@
     <col customWidth="1" max="20" min="20" width="6"/>
     <col customWidth="1" max="21" min="21" width="6"/>
     <col customWidth="1" max="22" min="22" width="20"/>
-    <col customWidth="1" max="23" min="23" width="8"/>
+    <col customWidth="1" max="23" min="23" width="9"/>
     <col customWidth="1" max="24" min="24" width="7"/>
     <col customWidth="1" max="25" min="25" width="8"/>
   </cols>
@@ -976,13 +976,13 @@
         <v>-2.65</v>
       </c>
       <c r="N15" s="1" t="n">
-        <v>0</v>
+        <v>-0.864</v>
       </c>
       <c r="O15" s="1" t="n">
         <v>3.75</v>
       </c>
       <c r="P15" s="1" t="n">
-        <v>-0.15</v>
+        <v>0.714</v>
       </c>
       <c r="Q15" s="1" t="s">
         <v>25</v>
@@ -1047,13 +1047,13 @@
         <v>0</v>
       </c>
       <c r="N16" s="1" t="n">
-        <v>0.959</v>
+        <v>0.095</v>
       </c>
       <c r="O16" s="1" t="n">
         <v>0</v>
       </c>
       <c r="P16" s="1" t="n">
-        <v>10.441</v>
+        <v>11.305</v>
       </c>
       <c r="Q16" s="1" t="n"/>
       <c r="R16" s="1" t="n"/>
@@ -1116,13 +1116,13 @@
         <v>49.996</v>
       </c>
       <c r="N17" s="1" t="n">
-        <v>0.959</v>
+        <v>0.095</v>
       </c>
       <c r="O17" s="1" t="n">
         <v>-46.396</v>
       </c>
       <c r="P17" s="1" t="n">
-        <v>-0.3089999999999999</v>
+        <v>0.555</v>
       </c>
       <c r="Q17" s="1" t="n"/>
       <c r="R17" s="1" t="n"/>
@@ -1185,13 +1185,13 @@
         <v>47</v>
       </c>
       <c r="N18" s="1" t="n">
-        <v>-37.541</v>
+        <v>-38.405</v>
       </c>
       <c r="O18" s="1" t="n">
         <v>-47</v>
       </c>
       <c r="P18" s="1" t="n">
-        <v>47.84099999999999</v>
+        <v>48.705</v>
       </c>
       <c r="Q18" s="1" t="n"/>
       <c r="R18" s="1" t="n"/>
@@ -1254,13 +1254,13 @@
         <v>49.996</v>
       </c>
       <c r="N19" s="1" t="n">
-        <v>-26.537</v>
+        <v>-27.401</v>
       </c>
       <c r="O19" s="1" t="n">
         <v>-58.746</v>
       </c>
       <c r="P19" s="1" t="n">
-        <v>26.537</v>
+        <v>27.401</v>
       </c>
       <c r="Q19" s="1" t="n"/>
       <c r="R19" s="1" t="n"/>
@@ -1323,13 +1323,13 @@
         <v>0</v>
       </c>
       <c r="N20" s="1" t="n">
-        <v>0</v>
+        <v>-0.864</v>
       </c>
       <c r="O20" s="1" t="n">
         <v>6.4</v>
       </c>
       <c r="P20" s="1" t="n">
-        <v>0</v>
+        <v>0.864</v>
       </c>
       <c r="Q20" s="1" t="n"/>
       <c r="R20" s="1" t="n"/>
@@ -1392,13 +1392,13 @@
         <v>-44</v>
       </c>
       <c r="N21" s="1" t="n">
-        <v>0.959</v>
+        <v>0.095</v>
       </c>
       <c r="O21" s="1" t="n">
         <v>34.65</v>
       </c>
       <c r="P21" s="1" t="n">
-        <v>-0.959</v>
+        <v>-0.095</v>
       </c>
       <c r="Q21" s="1" t="n"/>
       <c r="R21" s="1" t="n"/>
@@ -1415,7 +1415,7 @@
         <v>-44</v>
       </c>
       <c r="W21" s="1" t="n">
-        <v>0.959</v>
+        <v>0.095</v>
       </c>
       <c r="X21" s="1" t="n">
         <v>0</v>
@@ -1461,13 +1461,13 @@
         <v>44</v>
       </c>
       <c r="N22" s="1" t="n">
-        <v>0.959</v>
+        <v>0.095</v>
       </c>
       <c r="O22" s="1" t="n">
         <v>-53.35</v>
       </c>
       <c r="P22" s="1" t="n">
-        <v>-0.959</v>
+        <v>-0.095</v>
       </c>
       <c r="Q22" s="1" t="n"/>
       <c r="R22" s="1" t="n"/>
@@ -1484,7 +1484,7 @@
         <v>44</v>
       </c>
       <c r="W22" s="1" t="n">
-        <v>0.959</v>
+        <v>0.095</v>
       </c>
       <c r="X22" s="1" t="n">
         <v>0</v>
@@ -1668,13 +1668,13 @@
         <v>-0.3</v>
       </c>
       <c r="N25" s="1" t="n">
-        <v>-0.767</v>
+        <v>-1.631</v>
       </c>
       <c r="O25" s="1" t="n">
         <v>2.05</v>
       </c>
       <c r="P25" s="1" t="n">
-        <v>1.167</v>
+        <v>2.031</v>
       </c>
       <c r="Q25" s="1" t="n"/>
       <c r="R25" s="1" t="n"/>
@@ -1737,13 +1737,13 @@
         <v>-0.5629999999999999</v>
       </c>
       <c r="N26" s="1" t="n">
-        <v>0</v>
+        <v>-0.864</v>
       </c>
       <c r="O26" s="1" t="n">
         <v>7.613</v>
       </c>
       <c r="P26" s="1" t="n">
-        <v>-2.15</v>
+        <v>-1.286</v>
       </c>
       <c r="Q26" s="1" t="n"/>
       <c r="R26" s="1" t="n"/>
@@ -1967,7 +1967,7 @@
         <v>-39.483</v>
       </c>
       <c r="W29" s="1" t="n">
-        <v>-38.5</v>
+        <v>-39.364</v>
       </c>
       <c r="X29" s="1" t="n">
         <v>0</v>
@@ -2036,7 +2036,7 @@
         <v>-39.483</v>
       </c>
       <c r="W30" s="1" t="n">
-        <v>-27.5</v>
+        <v>-28.364</v>
       </c>
       <c r="X30" s="1" t="n">
         <v>0</v>
@@ -2105,7 +2105,7 @@
         <v>-28.483</v>
       </c>
       <c r="W31" s="1" t="n">
-        <v>-27.5</v>
+        <v>-28.364</v>
       </c>
       <c r="X31" s="1" t="n">
         <v>0</v>
@@ -2174,7 +2174,7 @@
         <v>-28.483</v>
       </c>
       <c r="W32" s="1" t="n">
-        <v>-38.5</v>
+        <v>-39.364</v>
       </c>
       <c r="X32" s="1" t="n">
         <v>0</v>
@@ -2243,7 +2243,7 @@
         <v>-17.483</v>
       </c>
       <c r="W33" s="1" t="n">
-        <v>-38.5</v>
+        <v>-39.364</v>
       </c>
       <c r="X33" s="1" t="n">
         <v>0</v>
@@ -2312,7 +2312,7 @@
         <v>-6.483</v>
       </c>
       <c r="W34" s="1" t="n">
-        <v>-38.5</v>
+        <v>-39.364</v>
       </c>
       <c r="X34" s="1" t="n">
         <v>0</v>
@@ -2381,7 +2381,7 @@
         <v>-6.483</v>
       </c>
       <c r="W35" s="1" t="n">
-        <v>-27.5</v>
+        <v>-28.364</v>
       </c>
       <c r="X35" s="1" t="n">
         <v>0</v>
@@ -2450,7 +2450,7 @@
         <v>-17.483</v>
       </c>
       <c r="W36" s="1" t="n">
-        <v>-27.5</v>
+        <v>-28.364</v>
       </c>
       <c r="X36" s="1" t="n">
         <v>0</v>
@@ -2519,7 +2519,7 @@
         <v>-17.483</v>
       </c>
       <c r="W37" s="1" t="n">
-        <v>-16.5</v>
+        <v>-17.364</v>
       </c>
       <c r="X37" s="1" t="n">
         <v>0</v>
@@ -2588,7 +2588,7 @@
         <v>-6.483</v>
       </c>
       <c r="W38" s="1" t="n">
-        <v>-16.5</v>
+        <v>-17.364</v>
       </c>
       <c r="X38" s="1" t="n">
         <v>0</v>
@@ -2657,7 +2657,7 @@
         <v>-6.483</v>
       </c>
       <c r="W39" s="1" t="n">
-        <v>-5.5</v>
+        <v>-6.364</v>
       </c>
       <c r="X39" s="1" t="n">
         <v>0</v>
@@ -2726,7 +2726,7 @@
         <v>-17.483</v>
       </c>
       <c r="W40" s="1" t="n">
-        <v>-5.5</v>
+        <v>-6.364</v>
       </c>
       <c r="X40" s="1" t="n">
         <v>0</v>
@@ -2795,7 +2795,7 @@
         <v>-28.483</v>
       </c>
       <c r="W41" s="1" t="n">
-        <v>-5.5</v>
+        <v>-6.364</v>
       </c>
       <c r="X41" s="1" t="n">
         <v>0</v>
@@ -2864,7 +2864,7 @@
         <v>-28.483</v>
       </c>
       <c r="W42" s="1" t="n">
-        <v>-16.5</v>
+        <v>-17.364</v>
       </c>
       <c r="X42" s="1" t="n">
         <v>0</v>
@@ -2933,7 +2933,7 @@
         <v>-39.483</v>
       </c>
       <c r="W43" s="1" t="n">
-        <v>-16.5</v>
+        <v>-17.364</v>
       </c>
       <c r="X43" s="1" t="n">
         <v>0</v>
@@ -3002,7 +3002,7 @@
         <v>-39.483</v>
       </c>
       <c r="W44" s="1" t="n">
-        <v>-5.5</v>
+        <v>-6.364</v>
       </c>
       <c r="X44" s="1" t="n">
         <v>0</v>
@@ -3071,7 +3071,7 @@
         <v>-39.483</v>
       </c>
       <c r="W45" s="1" t="n">
-        <v>5.5</v>
+        <v>4.636</v>
       </c>
       <c r="X45" s="1" t="n">
         <v>0</v>
@@ -3140,7 +3140,7 @@
         <v>-28.483</v>
       </c>
       <c r="W46" s="1" t="n">
-        <v>5.5</v>
+        <v>4.636</v>
       </c>
       <c r="X46" s="1" t="n">
         <v>0</v>
@@ -3209,7 +3209,7 @@
         <v>-28.483</v>
       </c>
       <c r="W47" s="1" t="n">
-        <v>16.5</v>
+        <v>15.636</v>
       </c>
       <c r="X47" s="1" t="n">
         <v>0</v>
@@ -3278,7 +3278,7 @@
         <v>-39.483</v>
       </c>
       <c r="W48" s="1" t="n">
-        <v>16.5</v>
+        <v>15.636</v>
       </c>
       <c r="X48" s="1" t="n">
         <v>0</v>
@@ -3347,7 +3347,7 @@
         <v>-39.483</v>
       </c>
       <c r="W49" s="1" t="n">
-        <v>27.5</v>
+        <v>26.636</v>
       </c>
       <c r="X49" s="1" t="n">
         <v>0</v>
@@ -3416,7 +3416,7 @@
         <v>-39.483</v>
       </c>
       <c r="W50" s="1" t="n">
-        <v>38.5</v>
+        <v>37.636</v>
       </c>
       <c r="X50" s="1" t="n">
         <v>0</v>
@@ -3485,7 +3485,7 @@
         <v>-28.483</v>
       </c>
       <c r="W51" s="1" t="n">
-        <v>38.5</v>
+        <v>37.636</v>
       </c>
       <c r="X51" s="1" t="n">
         <v>0</v>
@@ -3554,7 +3554,7 @@
         <v>-28.483</v>
       </c>
       <c r="W52" s="1" t="n">
-        <v>27.5</v>
+        <v>26.636</v>
       </c>
       <c r="X52" s="1" t="n">
         <v>0</v>
@@ -3623,7 +3623,7 @@
         <v>-17.483</v>
       </c>
       <c r="W53" s="1" t="n">
-        <v>27.5</v>
+        <v>26.636</v>
       </c>
       <c r="X53" s="1" t="n">
         <v>0</v>
@@ -3692,7 +3692,7 @@
         <v>-17.483</v>
       </c>
       <c r="W54" s="1" t="n">
-        <v>38.5</v>
+        <v>37.636</v>
       </c>
       <c r="X54" s="1" t="n">
         <v>0</v>
@@ -3761,7 +3761,7 @@
         <v>-6.483</v>
       </c>
       <c r="W55" s="1" t="n">
-        <v>38.5</v>
+        <v>37.636</v>
       </c>
       <c r="X55" s="1" t="n">
         <v>0</v>
@@ -3830,7 +3830,7 @@
         <v>-6.483</v>
       </c>
       <c r="W56" s="1" t="n">
-        <v>27.5</v>
+        <v>26.636</v>
       </c>
       <c r="X56" s="1" t="n">
         <v>0</v>
@@ -3899,7 +3899,7 @@
         <v>-6.483</v>
       </c>
       <c r="W57" s="1" t="n">
-        <v>16.5</v>
+        <v>15.636</v>
       </c>
       <c r="X57" s="1" t="n">
         <v>0</v>
@@ -3968,7 +3968,7 @@
         <v>-17.483</v>
       </c>
       <c r="W58" s="1" t="n">
-        <v>16.5</v>
+        <v>15.636</v>
       </c>
       <c r="X58" s="1" t="n">
         <v>0</v>
@@ -4037,7 +4037,7 @@
         <v>-17.483</v>
       </c>
       <c r="W59" s="1" t="n">
-        <v>5.5</v>
+        <v>4.636</v>
       </c>
       <c r="X59" s="1" t="n">
         <v>0</v>
@@ -4106,7 +4106,7 @@
         <v>-6.483</v>
       </c>
       <c r="W60" s="1" t="n">
-        <v>5.5</v>
+        <v>4.636</v>
       </c>
       <c r="X60" s="1" t="n">
         <v>0</v>
@@ -4175,7 +4175,7 @@
         <v>4.517</v>
       </c>
       <c r="W61" s="1" t="n">
-        <v>5.5</v>
+        <v>4.636</v>
       </c>
       <c r="X61" s="1" t="n">
         <v>0</v>
@@ -4244,7 +4244,7 @@
         <v>15.517</v>
       </c>
       <c r="W62" s="1" t="n">
-        <v>5.5</v>
+        <v>4.636</v>
       </c>
       <c r="X62" s="1" t="n">
         <v>0</v>
@@ -4313,7 +4313,7 @@
         <v>15.517</v>
       </c>
       <c r="W63" s="1" t="n">
-        <v>16.5</v>
+        <v>15.636</v>
       </c>
       <c r="X63" s="1" t="n">
         <v>0</v>
@@ -4382,7 +4382,7 @@
         <v>4.517</v>
       </c>
       <c r="W64" s="1" t="n">
-        <v>16.5</v>
+        <v>15.636</v>
       </c>
       <c r="X64" s="1" t="n">
         <v>0</v>
@@ -4451,7 +4451,7 @@
         <v>4.517</v>
       </c>
       <c r="W65" s="1" t="n">
-        <v>27.5</v>
+        <v>26.636</v>
       </c>
       <c r="X65" s="1" t="n">
         <v>0</v>
@@ -4520,7 +4520,7 @@
         <v>4.517</v>
       </c>
       <c r="W66" s="1" t="n">
-        <v>38.5</v>
+        <v>37.636</v>
       </c>
       <c r="X66" s="1" t="n">
         <v>0</v>
@@ -4589,7 +4589,7 @@
         <v>15.517</v>
       </c>
       <c r="W67" s="1" t="n">
-        <v>38.5</v>
+        <v>37.636</v>
       </c>
       <c r="X67" s="1" t="n">
         <v>0</v>
@@ -4658,7 +4658,7 @@
         <v>15.517</v>
       </c>
       <c r="W68" s="1" t="n">
-        <v>27.5</v>
+        <v>26.636</v>
       </c>
       <c r="X68" s="1" t="n">
         <v>0</v>
@@ -4727,7 +4727,7 @@
         <v>26.517</v>
       </c>
       <c r="W69" s="1" t="n">
-        <v>27.5</v>
+        <v>26.636</v>
       </c>
       <c r="X69" s="1" t="n">
         <v>0</v>
@@ -4796,7 +4796,7 @@
         <v>26.517</v>
       </c>
       <c r="W70" s="1" t="n">
-        <v>38.5</v>
+        <v>37.636</v>
       </c>
       <c r="X70" s="1" t="n">
         <v>0</v>
@@ -4865,7 +4865,7 @@
         <v>37.517</v>
       </c>
       <c r="W71" s="1" t="n">
-        <v>38.5</v>
+        <v>37.636</v>
       </c>
       <c r="X71" s="1" t="n">
         <v>0</v>
@@ -4934,7 +4934,7 @@
         <v>37.517</v>
       </c>
       <c r="W72" s="1" t="n">
-        <v>27.5</v>
+        <v>26.636</v>
       </c>
       <c r="X72" s="1" t="n">
         <v>0</v>
@@ -5003,7 +5003,7 @@
         <v>37.517</v>
       </c>
       <c r="W73" s="1" t="n">
-        <v>16.5</v>
+        <v>15.636</v>
       </c>
       <c r="X73" s="1" t="n">
         <v>0</v>
@@ -5072,7 +5072,7 @@
         <v>26.517</v>
       </c>
       <c r="W74" s="1" t="n">
-        <v>16.5</v>
+        <v>15.636</v>
       </c>
       <c r="X74" s="1" t="n">
         <v>0</v>
@@ -5141,7 +5141,7 @@
         <v>26.517</v>
       </c>
       <c r="W75" s="1" t="n">
-        <v>5.5</v>
+        <v>4.636</v>
       </c>
       <c r="X75" s="1" t="n">
         <v>0</v>
@@ -5210,7 +5210,7 @@
         <v>37.517</v>
       </c>
       <c r="W76" s="1" t="n">
-        <v>5.5</v>
+        <v>4.636</v>
       </c>
       <c r="X76" s="1" t="n">
         <v>0</v>
@@ -5279,7 +5279,7 @@
         <v>37.517</v>
       </c>
       <c r="W77" s="1" t="n">
-        <v>-5.5</v>
+        <v>-6.364</v>
       </c>
       <c r="X77" s="1" t="n">
         <v>0</v>
@@ -5348,7 +5348,7 @@
         <v>37.517</v>
       </c>
       <c r="W78" s="1" t="n">
-        <v>-16.5</v>
+        <v>-17.364</v>
       </c>
       <c r="X78" s="1" t="n">
         <v>0</v>
@@ -5417,7 +5417,7 @@
         <v>26.517</v>
       </c>
       <c r="W79" s="1" t="n">
-        <v>-16.5</v>
+        <v>-17.364</v>
       </c>
       <c r="X79" s="1" t="n">
         <v>0</v>
@@ -5486,7 +5486,7 @@
         <v>26.517</v>
       </c>
       <c r="W80" s="1" t="n">
-        <v>-5.5</v>
+        <v>-6.364</v>
       </c>
       <c r="X80" s="1" t="n">
         <v>0</v>
@@ -5555,7 +5555,7 @@
         <v>15.517</v>
       </c>
       <c r="W81" s="1" t="n">
-        <v>-5.5</v>
+        <v>-6.364</v>
       </c>
       <c r="X81" s="1" t="n">
         <v>0</v>
@@ -5624,7 +5624,7 @@
         <v>4.517</v>
       </c>
       <c r="W82" s="1" t="n">
-        <v>-5.5</v>
+        <v>-6.364</v>
       </c>
       <c r="X82" s="1" t="n">
         <v>0</v>
@@ -5693,7 +5693,7 @@
         <v>4.517</v>
       </c>
       <c r="W83" s="1" t="n">
-        <v>-16.5</v>
+        <v>-17.364</v>
       </c>
       <c r="X83" s="1" t="n">
         <v>0</v>
@@ -5762,7 +5762,7 @@
         <v>15.517</v>
       </c>
       <c r="W84" s="1" t="n">
-        <v>-16.5</v>
+        <v>-17.364</v>
       </c>
       <c r="X84" s="1" t="n">
         <v>0</v>
@@ -5831,7 +5831,7 @@
         <v>15.517</v>
       </c>
       <c r="W85" s="1" t="n">
-        <v>-27.5</v>
+        <v>-28.364</v>
       </c>
       <c r="X85" s="1" t="n">
         <v>0</v>
@@ -5900,7 +5900,7 @@
         <v>4.517</v>
       </c>
       <c r="W86" s="1" t="n">
-        <v>-27.5</v>
+        <v>-28.364</v>
       </c>
       <c r="X86" s="1" t="n">
         <v>0</v>
@@ -5969,7 +5969,7 @@
         <v>4.517</v>
       </c>
       <c r="W87" s="1" t="n">
-        <v>-38.5</v>
+        <v>-39.364</v>
       </c>
       <c r="X87" s="1" t="n">
         <v>0</v>
@@ -6038,7 +6038,7 @@
         <v>15.517</v>
       </c>
       <c r="W88" s="1" t="n">
-        <v>-38.5</v>
+        <v>-39.364</v>
       </c>
       <c r="X88" s="1" t="n">
         <v>0</v>
@@ -6107,7 +6107,7 @@
         <v>26.517</v>
       </c>
       <c r="W89" s="1" t="n">
-        <v>-38.5</v>
+        <v>-39.364</v>
       </c>
       <c r="X89" s="1" t="n">
         <v>0</v>
@@ -6176,7 +6176,7 @@
         <v>26.517</v>
       </c>
       <c r="W90" s="1" t="n">
-        <v>-27.5</v>
+        <v>-28.364</v>
       </c>
       <c r="X90" s="1" t="n">
         <v>0</v>
@@ -6245,7 +6245,7 @@
         <v>37.517</v>
       </c>
       <c r="W91" s="1" t="n">
-        <v>-27.5</v>
+        <v>-28.364</v>
       </c>
       <c r="X91" s="1" t="n">
         <v>0</v>
@@ -6314,7 +6314,7 @@
         <v>37.517</v>
       </c>
       <c r="W92" s="1" t="n">
-        <v>-38.5</v>
+        <v>-39.364</v>
       </c>
       <c r="X92" s="1" t="n">
         <v>0</v>
@@ -6360,13 +6360,13 @@
         <v>0.1369999999999999</v>
       </c>
       <c r="N93" s="1" t="n">
-        <v>0</v>
+        <v>-0.864</v>
       </c>
       <c r="O93" s="1" t="n">
         <v>-1.387</v>
       </c>
       <c r="P93" s="1" t="n">
-        <v>0</v>
+        <v>0.864</v>
       </c>
       <c r="Q93" s="1" t="n"/>
       <c r="R93" s="1" t="n"/>
@@ -6429,13 +6429,13 @@
         <v>1.52</v>
       </c>
       <c r="N94" s="1" t="n">
-        <v>0</v>
+        <v>-0.864</v>
       </c>
       <c r="O94" s="1" t="n">
         <v>-0.52</v>
       </c>
       <c r="P94" s="1" t="n">
-        <v>0.4</v>
+        <v>1.264</v>
       </c>
       <c r="Q94" s="1" t="n"/>
       <c r="R94" s="1" t="n"/>
@@ -6498,13 +6498,13 @@
         <v>0.958</v>
       </c>
       <c r="N95" s="1" t="n">
-        <v>0</v>
+        <v>-0.864</v>
       </c>
       <c r="O95" s="1" t="n">
         <v>-0.958</v>
       </c>
       <c r="P95" s="1" t="n">
-        <v>0</v>
+        <v>0.864</v>
       </c>
       <c r="Q95" s="1" t="n"/>
       <c r="R95" s="1" t="n"/>
@@ -6705,13 +6705,13 @@
         <v>49.996</v>
       </c>
       <c r="N98" s="1" t="n">
-        <v>0.959</v>
+        <v>0.095</v>
       </c>
       <c r="O98" s="1" t="n">
         <v>-46.396</v>
       </c>
       <c r="P98" s="1" t="n">
-        <v>-1.309</v>
+        <v>-0.445</v>
       </c>
       <c r="Q98" s="1" t="n"/>
       <c r="R98" s="1" t="n"/>
@@ -6774,13 +6774,13 @@
         <v>-0.3</v>
       </c>
       <c r="N99" s="1" t="n">
-        <v>0.756</v>
+        <v>-0.108</v>
       </c>
       <c r="O99" s="1" t="n">
         <v>3.1</v>
       </c>
       <c r="P99" s="1" t="n">
-        <v>-0.106</v>
+        <v>0.758</v>
       </c>
       <c r="Q99" s="1" t="n"/>
       <c r="R99" s="1" t="n"/>
@@ -6843,13 +6843,13 @@
         <v>-0.3</v>
       </c>
       <c r="N100" s="1" t="n">
-        <v>-0.662</v>
+        <v>-1.526</v>
       </c>
       <c r="O100" s="1" t="n">
         <v>3.1</v>
       </c>
       <c r="P100" s="1" t="n">
-        <v>0.412</v>
+        <v>1.276</v>
       </c>
       <c r="Q100" s="1" t="n"/>
       <c r="R100" s="1" t="n"/>
@@ -6912,13 +6912,13 @@
         <v>0</v>
       </c>
       <c r="N101" s="1" t="n">
-        <v>0.959</v>
+        <v>0.095</v>
       </c>
       <c r="O101" s="1" t="n">
         <v>0</v>
       </c>
       <c r="P101" s="1" t="n">
-        <v>11.041</v>
+        <v>11.905</v>
       </c>
       <c r="Q101" s="1" t="n"/>
       <c r="R101" s="1" t="n"/>
@@ -6981,13 +6981,13 @@
         <v>47</v>
       </c>
       <c r="N102" s="1" t="n">
-        <v>-37.541</v>
+        <v>-38.405</v>
       </c>
       <c r="O102" s="1" t="n">
         <v>-47</v>
       </c>
       <c r="P102" s="1" t="n">
-        <v>48.34099999999999</v>
+        <v>49.205</v>
       </c>
       <c r="Q102" s="1" t="n"/>
       <c r="R102" s="1" t="n"/>
@@ -7050,13 +7050,13 @@
         <v>49.996</v>
       </c>
       <c r="N103" s="1" t="n">
-        <v>-26.537</v>
+        <v>-27.401</v>
       </c>
       <c r="O103" s="1" t="n">
         <v>-58.146</v>
       </c>
       <c r="P103" s="1" t="n">
-        <v>27.337</v>
+        <v>28.201</v>
       </c>
       <c r="Q103" s="1" t="n"/>
       <c r="R103" s="1" t="n"/>
@@ -7119,13 +7119,13 @@
         <v>-44</v>
       </c>
       <c r="N104" s="1" t="n">
-        <v>0.959</v>
+        <v>0.095</v>
       </c>
       <c r="O104" s="1" t="n">
         <v>34.05</v>
       </c>
       <c r="P104" s="1" t="n">
-        <v>-0.959</v>
+        <v>-0.095</v>
       </c>
       <c r="Q104" s="1" t="n"/>
       <c r="R104" s="1" t="n"/>
@@ -7142,7 +7142,7 @@
         <v>-44</v>
       </c>
       <c r="W104" s="1" t="n">
-        <v>0.959</v>
+        <v>0.095</v>
       </c>
       <c r="X104" s="1" t="n">
         <v>0</v>
@@ -7188,13 +7188,13 @@
         <v>44</v>
       </c>
       <c r="N105" s="1" t="n">
-        <v>0.959</v>
+        <v>0.095</v>
       </c>
       <c r="O105" s="1" t="n">
         <v>-53.95</v>
       </c>
       <c r="P105" s="1" t="n">
-        <v>-0.959</v>
+        <v>-0.095</v>
       </c>
       <c r="Q105" s="1" t="n"/>
       <c r="R105" s="1" t="n"/>
@@ -7211,7 +7211,7 @@
         <v>44</v>
       </c>
       <c r="W105" s="1" t="n">
-        <v>0.959</v>
+        <v>0.095</v>
       </c>
       <c r="X105" s="1" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
fixed the problem with cell shifts and array centers when generating patches
</commit_message>
<xml_diff>
--- a/masks/code/ResonatorArray.xlsx
+++ b/masks/code/ResonatorArray.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -750,22 +750,22 @@
     <col customWidth="1" max="5" min="5" width="8"/>
     <col customWidth="1" max="6" min="6" width="6"/>
     <col customWidth="1" max="7" min="7" width="6"/>
-    <col customWidth="1" max="8" min="8" width="21"/>
-    <col customWidth="1" max="9" min="9" width="21"/>
-    <col customWidth="1" max="10" min="10" width="22"/>
-    <col customWidth="1" max="11" min="11" width="21"/>
+    <col customWidth="1" max="8" min="8" width="8"/>
+    <col customWidth="1" max="9" min="9" width="8"/>
+    <col customWidth="1" max="10" min="10" width="7"/>
+    <col customWidth="1" max="11" min="11" width="7"/>
     <col customWidth="1" max="12" min="12" width="6"/>
-    <col customWidth="1" max="13" min="13" width="20"/>
-    <col customWidth="1" max="14" min="14" width="9"/>
-    <col customWidth="1" max="15" min="15" width="20"/>
-    <col customWidth="1" max="16" min="16" width="22"/>
+    <col customWidth="1" max="13" min="13" width="8"/>
+    <col customWidth="1" max="14" min="14" width="8"/>
+    <col customWidth="1" max="15" min="15" width="8"/>
+    <col customWidth="1" max="16" min="16" width="8"/>
     <col customWidth="1" max="17" min="17" width="6"/>
     <col customWidth="1" max="18" min="18" width="6"/>
     <col customWidth="1" max="19" min="19" width="24"/>
     <col customWidth="1" max="20" min="20" width="6"/>
     <col customWidth="1" max="21" min="21" width="6"/>
-    <col customWidth="1" max="22" min="22" width="20"/>
-    <col customWidth="1" max="23" min="23" width="9"/>
+    <col customWidth="1" max="22" min="22" width="9"/>
+    <col customWidth="1" max="23" min="23" width="7"/>
     <col customWidth="1" max="24" min="24" width="7"/>
     <col customWidth="1" max="25" min="25" width="8"/>
   </cols>
@@ -976,13 +976,13 @@
         <v>-2.65</v>
       </c>
       <c r="N15" s="1" t="n">
-        <v>-0.864</v>
+        <v>0</v>
       </c>
       <c r="O15" s="1" t="n">
         <v>3.75</v>
       </c>
       <c r="P15" s="1" t="n">
-        <v>0.714</v>
+        <v>-0.15</v>
       </c>
       <c r="Q15" s="1" t="s">
         <v>25</v>
@@ -998,7 +998,7 @@
         <v>8</v>
       </c>
       <c r="V15" s="1" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="W15" s="1" t="n">
         <v>0</v>
@@ -1047,13 +1047,13 @@
         <v>0</v>
       </c>
       <c r="N16" s="1" t="n">
-        <v>0.095</v>
+        <v>0.959</v>
       </c>
       <c r="O16" s="1" t="n">
         <v>0</v>
       </c>
       <c r="P16" s="1" t="n">
-        <v>11.305</v>
+        <v>10.441</v>
       </c>
       <c r="Q16" s="1" t="n"/>
       <c r="R16" s="1" t="n"/>
@@ -1067,7 +1067,7 @@
         <v>8</v>
       </c>
       <c r="V16" s="1" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="W16" s="1" t="n">
         <v>0</v>
@@ -1113,16 +1113,16 @@
       </c>
       <c r="L17" s="1" t="n"/>
       <c r="M17" s="1" t="n">
-        <v>49.996</v>
+        <v>0</v>
       </c>
       <c r="N17" s="1" t="n">
-        <v>0.095</v>
+        <v>0</v>
       </c>
       <c r="O17" s="1" t="n">
-        <v>-46.396</v>
+        <v>3.6</v>
       </c>
       <c r="P17" s="1" t="n">
-        <v>0.555</v>
+        <v>0.65</v>
       </c>
       <c r="Q17" s="1" t="n"/>
       <c r="R17" s="1" t="n"/>
@@ -1136,10 +1136,10 @@
         <v>2</v>
       </c>
       <c r="V17" s="1" t="n">
-        <v>2.996</v>
+        <v>49.996</v>
       </c>
       <c r="W17" s="1" t="n">
-        <v>-0</v>
+        <v>0.959</v>
       </c>
       <c r="X17" s="1" t="n">
         <v>0</v>
@@ -1182,16 +1182,16 @@
       </c>
       <c r="L18" s="1" t="n"/>
       <c r="M18" s="1" t="n">
-        <v>47</v>
+        <v>0</v>
       </c>
       <c r="N18" s="1" t="n">
-        <v>-38.405</v>
+        <v>0</v>
       </c>
       <c r="O18" s="1" t="n">
-        <v>-47</v>
+        <v>0</v>
       </c>
       <c r="P18" s="1" t="n">
-        <v>48.705</v>
+        <v>10.3</v>
       </c>
       <c r="Q18" s="1" t="n"/>
       <c r="R18" s="1" t="n"/>
@@ -1205,10 +1205,10 @@
         <v>2</v>
       </c>
       <c r="V18" s="1" t="n">
-        <v>-0</v>
+        <v>47</v>
       </c>
       <c r="W18" s="1" t="n">
-        <v>-0</v>
+        <v>0.959</v>
       </c>
       <c r="X18" s="1" t="n">
         <v>0</v>
@@ -1251,16 +1251,16 @@
       </c>
       <c r="L19" s="1" t="n"/>
       <c r="M19" s="1" t="n">
-        <v>49.996</v>
+        <v>0</v>
       </c>
       <c r="N19" s="1" t="n">
-        <v>-27.401</v>
+        <v>0</v>
       </c>
       <c r="O19" s="1" t="n">
-        <v>-58.746</v>
+        <v>-8.75</v>
       </c>
       <c r="P19" s="1" t="n">
-        <v>27.401</v>
+        <v>0</v>
       </c>
       <c r="Q19" s="1" t="n"/>
       <c r="R19" s="1" t="n"/>
@@ -1274,10 +1274,10 @@
         <v>2</v>
       </c>
       <c r="V19" s="1" t="n">
-        <v>2.996</v>
+        <v>49.996</v>
       </c>
       <c r="W19" s="1" t="n">
-        <v>-0</v>
+        <v>0.959</v>
       </c>
       <c r="X19" s="1" t="n">
         <v>0</v>
@@ -1323,13 +1323,13 @@
         <v>0</v>
       </c>
       <c r="N20" s="1" t="n">
-        <v>-0.864</v>
+        <v>0</v>
       </c>
       <c r="O20" s="1" t="n">
         <v>6.4</v>
       </c>
       <c r="P20" s="1" t="n">
-        <v>0.864</v>
+        <v>0</v>
       </c>
       <c r="Q20" s="1" t="n"/>
       <c r="R20" s="1" t="n"/>
@@ -1343,7 +1343,7 @@
         <v>8</v>
       </c>
       <c r="V20" s="1" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="W20" s="1" t="n">
         <v>0</v>
@@ -1389,16 +1389,16 @@
       </c>
       <c r="L21" s="1" t="n"/>
       <c r="M21" s="1" t="n">
-        <v>-44</v>
+        <v>0</v>
       </c>
       <c r="N21" s="1" t="n">
-        <v>0.095</v>
+        <v>0</v>
       </c>
       <c r="O21" s="1" t="n">
-        <v>34.65</v>
+        <v>-9.35</v>
       </c>
       <c r="P21" s="1" t="n">
-        <v>-0.095</v>
+        <v>0</v>
       </c>
       <c r="Q21" s="1" t="n"/>
       <c r="R21" s="1" t="n"/>
@@ -1415,7 +1415,7 @@
         <v>-44</v>
       </c>
       <c r="W21" s="1" t="n">
-        <v>0.095</v>
+        <v>0.959</v>
       </c>
       <c r="X21" s="1" t="n">
         <v>0</v>
@@ -1458,16 +1458,16 @@
       </c>
       <c r="L22" s="1" t="n"/>
       <c r="M22" s="1" t="n">
-        <v>44</v>
+        <v>0</v>
       </c>
       <c r="N22" s="1" t="n">
-        <v>0.095</v>
+        <v>0</v>
       </c>
       <c r="O22" s="1" t="n">
-        <v>-53.35</v>
+        <v>-9.35</v>
       </c>
       <c r="P22" s="1" t="n">
-        <v>-0.095</v>
+        <v>0</v>
       </c>
       <c r="Q22" s="1" t="n"/>
       <c r="R22" s="1" t="n"/>
@@ -1484,7 +1484,7 @@
         <v>44</v>
       </c>
       <c r="W22" s="1" t="n">
-        <v>0.095</v>
+        <v>0.959</v>
       </c>
       <c r="X22" s="1" t="n">
         <v>0</v>
@@ -1550,10 +1550,10 @@
         <v>2</v>
       </c>
       <c r="V23" s="1" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="W23" s="1" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="X23" s="1" t="n">
         <v>38.9</v>
@@ -1596,13 +1596,13 @@
       </c>
       <c r="L24" s="1" t="n"/>
       <c r="M24" s="1" t="n">
-        <v>-49.95</v>
+        <v>0</v>
       </c>
       <c r="N24" s="1" t="n">
         <v>0</v>
       </c>
       <c r="O24" s="1" t="n">
-        <v>59.2</v>
+        <v>9.25</v>
       </c>
       <c r="P24" s="1" t="n">
         <v>0</v>
@@ -1622,7 +1622,7 @@
         <v>-49.95</v>
       </c>
       <c r="W24" s="1" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="X24" s="1" t="n">
         <v>99.88</v>
@@ -1668,13 +1668,13 @@
         <v>-0.3</v>
       </c>
       <c r="N25" s="1" t="n">
-        <v>-1.631</v>
+        <v>-0.767</v>
       </c>
       <c r="O25" s="1" t="n">
         <v>2.05</v>
       </c>
       <c r="P25" s="1" t="n">
-        <v>2.031</v>
+        <v>1.167</v>
       </c>
       <c r="Q25" s="1" t="n"/>
       <c r="R25" s="1" t="n"/>
@@ -1688,7 +1688,7 @@
         <v>8</v>
       </c>
       <c r="V25" s="1" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="W25" s="1" t="n">
         <v>0</v>
@@ -1737,13 +1737,13 @@
         <v>-0.5629999999999999</v>
       </c>
       <c r="N26" s="1" t="n">
-        <v>-0.864</v>
+        <v>0</v>
       </c>
       <c r="O26" s="1" t="n">
         <v>7.613</v>
       </c>
       <c r="P26" s="1" t="n">
-        <v>-1.286</v>
+        <v>-2.15</v>
       </c>
       <c r="Q26" s="1" t="n"/>
       <c r="R26" s="1" t="n"/>
@@ -1757,7 +1757,7 @@
         <v>8</v>
       </c>
       <c r="V26" s="1" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="W26" s="1" t="n">
         <v>0</v>
@@ -1803,16 +1803,16 @@
       </c>
       <c r="L27" s="1" t="n"/>
       <c r="M27" s="1" t="n">
-        <v>-52.5</v>
+        <v>0</v>
       </c>
       <c r="N27" s="1" t="n">
-        <v>-50.562</v>
+        <v>0</v>
       </c>
       <c r="O27" s="1" t="n">
-        <v>52.5</v>
+        <v>0</v>
       </c>
       <c r="P27" s="1" t="n">
-        <v>63.11199999999999</v>
+        <v>12.55</v>
       </c>
       <c r="Q27" s="1" t="n"/>
       <c r="R27" s="1" t="n"/>
@@ -1826,10 +1826,10 @@
         <v>2</v>
       </c>
       <c r="V27" s="1" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="W27" s="1" t="n">
-        <v>-0.062</v>
+        <v>0</v>
       </c>
       <c r="X27" s="1" t="n">
         <v>15</v>
@@ -1872,16 +1872,16 @@
       </c>
       <c r="L28" s="1" t="n"/>
       <c r="M28" s="1" t="n">
-        <v>-50.562</v>
+        <v>0</v>
       </c>
       <c r="N28" s="1" t="n">
-        <v>-52.5</v>
+        <v>0</v>
       </c>
       <c r="O28" s="1" t="n">
-        <v>39.962</v>
+        <v>-10.6</v>
       </c>
       <c r="P28" s="1" t="n">
-        <v>52.5</v>
+        <v>0</v>
       </c>
       <c r="Q28" s="1" t="n"/>
       <c r="R28" s="1" t="n"/>
@@ -1895,10 +1895,10 @@
         <v>8</v>
       </c>
       <c r="V28" s="1" t="n">
-        <v>-0.062</v>
+        <v>0</v>
       </c>
       <c r="W28" s="1" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="X28" s="1" t="n">
         <v>101</v>
@@ -1967,7 +1967,7 @@
         <v>-39.483</v>
       </c>
       <c r="W29" s="1" t="n">
-        <v>-39.364</v>
+        <v>-38.5</v>
       </c>
       <c r="X29" s="1" t="n">
         <v>0</v>
@@ -2036,7 +2036,7 @@
         <v>-39.483</v>
       </c>
       <c r="W30" s="1" t="n">
-        <v>-28.364</v>
+        <v>-27.5</v>
       </c>
       <c r="X30" s="1" t="n">
         <v>0</v>
@@ -2105,7 +2105,7 @@
         <v>-28.483</v>
       </c>
       <c r="W31" s="1" t="n">
-        <v>-28.364</v>
+        <v>-27.5</v>
       </c>
       <c r="X31" s="1" t="n">
         <v>0</v>
@@ -2174,7 +2174,7 @@
         <v>-28.483</v>
       </c>
       <c r="W32" s="1" t="n">
-        <v>-39.364</v>
+        <v>-38.5</v>
       </c>
       <c r="X32" s="1" t="n">
         <v>0</v>
@@ -2243,7 +2243,7 @@
         <v>-17.483</v>
       </c>
       <c r="W33" s="1" t="n">
-        <v>-39.364</v>
+        <v>-38.5</v>
       </c>
       <c r="X33" s="1" t="n">
         <v>0</v>
@@ -2312,7 +2312,7 @@
         <v>-6.483</v>
       </c>
       <c r="W34" s="1" t="n">
-        <v>-39.364</v>
+        <v>-38.5</v>
       </c>
       <c r="X34" s="1" t="n">
         <v>0</v>
@@ -2381,7 +2381,7 @@
         <v>-6.483</v>
       </c>
       <c r="W35" s="1" t="n">
-        <v>-28.364</v>
+        <v>-27.5</v>
       </c>
       <c r="X35" s="1" t="n">
         <v>0</v>
@@ -2450,7 +2450,7 @@
         <v>-17.483</v>
       </c>
       <c r="W36" s="1" t="n">
-        <v>-28.364</v>
+        <v>-27.5</v>
       </c>
       <c r="X36" s="1" t="n">
         <v>0</v>
@@ -2519,7 +2519,7 @@
         <v>-17.483</v>
       </c>
       <c r="W37" s="1" t="n">
-        <v>-17.364</v>
+        <v>-16.5</v>
       </c>
       <c r="X37" s="1" t="n">
         <v>0</v>
@@ -2588,7 +2588,7 @@
         <v>-6.483</v>
       </c>
       <c r="W38" s="1" t="n">
-        <v>-17.364</v>
+        <v>-16.5</v>
       </c>
       <c r="X38" s="1" t="n">
         <v>0</v>
@@ -2657,7 +2657,7 @@
         <v>-6.483</v>
       </c>
       <c r="W39" s="1" t="n">
-        <v>-6.364</v>
+        <v>-5.5</v>
       </c>
       <c r="X39" s="1" t="n">
         <v>0</v>
@@ -2726,7 +2726,7 @@
         <v>-17.483</v>
       </c>
       <c r="W40" s="1" t="n">
-        <v>-6.364</v>
+        <v>-5.5</v>
       </c>
       <c r="X40" s="1" t="n">
         <v>0</v>
@@ -2795,7 +2795,7 @@
         <v>-28.483</v>
       </c>
       <c r="W41" s="1" t="n">
-        <v>-6.364</v>
+        <v>-5.5</v>
       </c>
       <c r="X41" s="1" t="n">
         <v>0</v>
@@ -2864,7 +2864,7 @@
         <v>-28.483</v>
       </c>
       <c r="W42" s="1" t="n">
-        <v>-17.364</v>
+        <v>-16.5</v>
       </c>
       <c r="X42" s="1" t="n">
         <v>0</v>
@@ -2933,7 +2933,7 @@
         <v>-39.483</v>
       </c>
       <c r="W43" s="1" t="n">
-        <v>-17.364</v>
+        <v>-16.5</v>
       </c>
       <c r="X43" s="1" t="n">
         <v>0</v>
@@ -3002,7 +3002,7 @@
         <v>-39.483</v>
       </c>
       <c r="W44" s="1" t="n">
-        <v>-6.364</v>
+        <v>-5.5</v>
       </c>
       <c r="X44" s="1" t="n">
         <v>0</v>
@@ -3071,7 +3071,7 @@
         <v>-39.483</v>
       </c>
       <c r="W45" s="1" t="n">
-        <v>4.636</v>
+        <v>5.5</v>
       </c>
       <c r="X45" s="1" t="n">
         <v>0</v>
@@ -3140,7 +3140,7 @@
         <v>-28.483</v>
       </c>
       <c r="W46" s="1" t="n">
-        <v>4.636</v>
+        <v>5.5</v>
       </c>
       <c r="X46" s="1" t="n">
         <v>0</v>
@@ -3209,7 +3209,7 @@
         <v>-28.483</v>
       </c>
       <c r="W47" s="1" t="n">
-        <v>15.636</v>
+        <v>16.5</v>
       </c>
       <c r="X47" s="1" t="n">
         <v>0</v>
@@ -3278,7 +3278,7 @@
         <v>-39.483</v>
       </c>
       <c r="W48" s="1" t="n">
-        <v>15.636</v>
+        <v>16.5</v>
       </c>
       <c r="X48" s="1" t="n">
         <v>0</v>
@@ -3347,7 +3347,7 @@
         <v>-39.483</v>
       </c>
       <c r="W49" s="1" t="n">
-        <v>26.636</v>
+        <v>27.5</v>
       </c>
       <c r="X49" s="1" t="n">
         <v>0</v>
@@ -3416,7 +3416,7 @@
         <v>-39.483</v>
       </c>
       <c r="W50" s="1" t="n">
-        <v>37.636</v>
+        <v>38.5</v>
       </c>
       <c r="X50" s="1" t="n">
         <v>0</v>
@@ -3485,7 +3485,7 @@
         <v>-28.483</v>
       </c>
       <c r="W51" s="1" t="n">
-        <v>37.636</v>
+        <v>38.5</v>
       </c>
       <c r="X51" s="1" t="n">
         <v>0</v>
@@ -3554,7 +3554,7 @@
         <v>-28.483</v>
       </c>
       <c r="W52" s="1" t="n">
-        <v>26.636</v>
+        <v>27.5</v>
       </c>
       <c r="X52" s="1" t="n">
         <v>0</v>
@@ -3623,7 +3623,7 @@
         <v>-17.483</v>
       </c>
       <c r="W53" s="1" t="n">
-        <v>26.636</v>
+        <v>27.5</v>
       </c>
       <c r="X53" s="1" t="n">
         <v>0</v>
@@ -3692,7 +3692,7 @@
         <v>-17.483</v>
       </c>
       <c r="W54" s="1" t="n">
-        <v>37.636</v>
+        <v>38.5</v>
       </c>
       <c r="X54" s="1" t="n">
         <v>0</v>
@@ -3761,7 +3761,7 @@
         <v>-6.483</v>
       </c>
       <c r="W55" s="1" t="n">
-        <v>37.636</v>
+        <v>38.5</v>
       </c>
       <c r="X55" s="1" t="n">
         <v>0</v>
@@ -3830,7 +3830,7 @@
         <v>-6.483</v>
       </c>
       <c r="W56" s="1" t="n">
-        <v>26.636</v>
+        <v>27.5</v>
       </c>
       <c r="X56" s="1" t="n">
         <v>0</v>
@@ -3899,7 +3899,7 @@
         <v>-6.483</v>
       </c>
       <c r="W57" s="1" t="n">
-        <v>15.636</v>
+        <v>16.5</v>
       </c>
       <c r="X57" s="1" t="n">
         <v>0</v>
@@ -3968,7 +3968,7 @@
         <v>-17.483</v>
       </c>
       <c r="W58" s="1" t="n">
-        <v>15.636</v>
+        <v>16.5</v>
       </c>
       <c r="X58" s="1" t="n">
         <v>0</v>
@@ -4037,7 +4037,7 @@
         <v>-17.483</v>
       </c>
       <c r="W59" s="1" t="n">
-        <v>4.636</v>
+        <v>5.5</v>
       </c>
       <c r="X59" s="1" t="n">
         <v>0</v>
@@ -4106,7 +4106,7 @@
         <v>-6.483</v>
       </c>
       <c r="W60" s="1" t="n">
-        <v>4.636</v>
+        <v>5.5</v>
       </c>
       <c r="X60" s="1" t="n">
         <v>0</v>
@@ -4175,7 +4175,7 @@
         <v>4.517</v>
       </c>
       <c r="W61" s="1" t="n">
-        <v>4.636</v>
+        <v>5.5</v>
       </c>
       <c r="X61" s="1" t="n">
         <v>0</v>
@@ -4244,7 +4244,7 @@
         <v>15.517</v>
       </c>
       <c r="W62" s="1" t="n">
-        <v>4.636</v>
+        <v>5.5</v>
       </c>
       <c r="X62" s="1" t="n">
         <v>0</v>
@@ -4313,7 +4313,7 @@
         <v>15.517</v>
       </c>
       <c r="W63" s="1" t="n">
-        <v>15.636</v>
+        <v>16.5</v>
       </c>
       <c r="X63" s="1" t="n">
         <v>0</v>
@@ -4382,7 +4382,7 @@
         <v>4.517</v>
       </c>
       <c r="W64" s="1" t="n">
-        <v>15.636</v>
+        <v>16.5</v>
       </c>
       <c r="X64" s="1" t="n">
         <v>0</v>
@@ -4451,7 +4451,7 @@
         <v>4.517</v>
       </c>
       <c r="W65" s="1" t="n">
-        <v>26.636</v>
+        <v>27.5</v>
       </c>
       <c r="X65" s="1" t="n">
         <v>0</v>
@@ -4520,7 +4520,7 @@
         <v>4.517</v>
       </c>
       <c r="W66" s="1" t="n">
-        <v>37.636</v>
+        <v>38.5</v>
       </c>
       <c r="X66" s="1" t="n">
         <v>0</v>
@@ -4589,7 +4589,7 @@
         <v>15.517</v>
       </c>
       <c r="W67" s="1" t="n">
-        <v>37.636</v>
+        <v>38.5</v>
       </c>
       <c r="X67" s="1" t="n">
         <v>0</v>
@@ -4658,7 +4658,7 @@
         <v>15.517</v>
       </c>
       <c r="W68" s="1" t="n">
-        <v>26.636</v>
+        <v>27.5</v>
       </c>
       <c r="X68" s="1" t="n">
         <v>0</v>
@@ -4727,7 +4727,7 @@
         <v>26.517</v>
       </c>
       <c r="W69" s="1" t="n">
-        <v>26.636</v>
+        <v>27.5</v>
       </c>
       <c r="X69" s="1" t="n">
         <v>0</v>
@@ -4796,7 +4796,7 @@
         <v>26.517</v>
       </c>
       <c r="W70" s="1" t="n">
-        <v>37.636</v>
+        <v>38.5</v>
       </c>
       <c r="X70" s="1" t="n">
         <v>0</v>
@@ -4865,7 +4865,7 @@
         <v>37.517</v>
       </c>
       <c r="W71" s="1" t="n">
-        <v>37.636</v>
+        <v>38.5</v>
       </c>
       <c r="X71" s="1" t="n">
         <v>0</v>
@@ -4934,7 +4934,7 @@
         <v>37.517</v>
       </c>
       <c r="W72" s="1" t="n">
-        <v>26.636</v>
+        <v>27.5</v>
       </c>
       <c r="X72" s="1" t="n">
         <v>0</v>
@@ -5003,7 +5003,7 @@
         <v>37.517</v>
       </c>
       <c r="W73" s="1" t="n">
-        <v>15.636</v>
+        <v>16.5</v>
       </c>
       <c r="X73" s="1" t="n">
         <v>0</v>
@@ -5072,7 +5072,7 @@
         <v>26.517</v>
       </c>
       <c r="W74" s="1" t="n">
-        <v>15.636</v>
+        <v>16.5</v>
       </c>
       <c r="X74" s="1" t="n">
         <v>0</v>
@@ -5141,7 +5141,7 @@
         <v>26.517</v>
       </c>
       <c r="W75" s="1" t="n">
-        <v>4.636</v>
+        <v>5.5</v>
       </c>
       <c r="X75" s="1" t="n">
         <v>0</v>
@@ -5210,7 +5210,7 @@
         <v>37.517</v>
       </c>
       <c r="W76" s="1" t="n">
-        <v>4.636</v>
+        <v>5.5</v>
       </c>
       <c r="X76" s="1" t="n">
         <v>0</v>
@@ -5279,7 +5279,7 @@
         <v>37.517</v>
       </c>
       <c r="W77" s="1" t="n">
-        <v>-6.364</v>
+        <v>-5.5</v>
       </c>
       <c r="X77" s="1" t="n">
         <v>0</v>
@@ -5348,7 +5348,7 @@
         <v>37.517</v>
       </c>
       <c r="W78" s="1" t="n">
-        <v>-17.364</v>
+        <v>-16.5</v>
       </c>
       <c r="X78" s="1" t="n">
         <v>0</v>
@@ -5417,7 +5417,7 @@
         <v>26.517</v>
       </c>
       <c r="W79" s="1" t="n">
-        <v>-17.364</v>
+        <v>-16.5</v>
       </c>
       <c r="X79" s="1" t="n">
         <v>0</v>
@@ -5486,7 +5486,7 @@
         <v>26.517</v>
       </c>
       <c r="W80" s="1" t="n">
-        <v>-6.364</v>
+        <v>-5.5</v>
       </c>
       <c r="X80" s="1" t="n">
         <v>0</v>
@@ -5555,7 +5555,7 @@
         <v>15.517</v>
       </c>
       <c r="W81" s="1" t="n">
-        <v>-6.364</v>
+        <v>-5.5</v>
       </c>
       <c r="X81" s="1" t="n">
         <v>0</v>
@@ -5624,7 +5624,7 @@
         <v>4.517</v>
       </c>
       <c r="W82" s="1" t="n">
-        <v>-6.364</v>
+        <v>-5.5</v>
       </c>
       <c r="X82" s="1" t="n">
         <v>0</v>
@@ -5693,7 +5693,7 @@
         <v>4.517</v>
       </c>
       <c r="W83" s="1" t="n">
-        <v>-17.364</v>
+        <v>-16.5</v>
       </c>
       <c r="X83" s="1" t="n">
         <v>0</v>
@@ -5762,7 +5762,7 @@
         <v>15.517</v>
       </c>
       <c r="W84" s="1" t="n">
-        <v>-17.364</v>
+        <v>-16.5</v>
       </c>
       <c r="X84" s="1" t="n">
         <v>0</v>
@@ -5831,7 +5831,7 @@
         <v>15.517</v>
       </c>
       <c r="W85" s="1" t="n">
-        <v>-28.364</v>
+        <v>-27.5</v>
       </c>
       <c r="X85" s="1" t="n">
         <v>0</v>
@@ -5900,7 +5900,7 @@
         <v>4.517</v>
       </c>
       <c r="W86" s="1" t="n">
-        <v>-28.364</v>
+        <v>-27.5</v>
       </c>
       <c r="X86" s="1" t="n">
         <v>0</v>
@@ -5969,7 +5969,7 @@
         <v>4.517</v>
       </c>
       <c r="W87" s="1" t="n">
-        <v>-39.364</v>
+        <v>-38.5</v>
       </c>
       <c r="X87" s="1" t="n">
         <v>0</v>
@@ -6038,7 +6038,7 @@
         <v>15.517</v>
       </c>
       <c r="W88" s="1" t="n">
-        <v>-39.364</v>
+        <v>-38.5</v>
       </c>
       <c r="X88" s="1" t="n">
         <v>0</v>
@@ -6107,7 +6107,7 @@
         <v>26.517</v>
       </c>
       <c r="W89" s="1" t="n">
-        <v>-39.364</v>
+        <v>-38.5</v>
       </c>
       <c r="X89" s="1" t="n">
         <v>0</v>
@@ -6176,7 +6176,7 @@
         <v>26.517</v>
       </c>
       <c r="W90" s="1" t="n">
-        <v>-28.364</v>
+        <v>-27.5</v>
       </c>
       <c r="X90" s="1" t="n">
         <v>0</v>
@@ -6245,7 +6245,7 @@
         <v>37.517</v>
       </c>
       <c r="W91" s="1" t="n">
-        <v>-28.364</v>
+        <v>-27.5</v>
       </c>
       <c r="X91" s="1" t="n">
         <v>0</v>
@@ -6314,7 +6314,7 @@
         <v>37.517</v>
       </c>
       <c r="W92" s="1" t="n">
-        <v>-39.364</v>
+        <v>-38.5</v>
       </c>
       <c r="X92" s="1" t="n">
         <v>0</v>
@@ -6360,13 +6360,13 @@
         <v>0.1369999999999999</v>
       </c>
       <c r="N93" s="1" t="n">
-        <v>-0.864</v>
+        <v>0</v>
       </c>
       <c r="O93" s="1" t="n">
         <v>-1.387</v>
       </c>
       <c r="P93" s="1" t="n">
-        <v>0.864</v>
+        <v>0</v>
       </c>
       <c r="Q93" s="1" t="n"/>
       <c r="R93" s="1" t="n"/>
@@ -6380,7 +6380,7 @@
         <v>8</v>
       </c>
       <c r="V93" s="1" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="W93" s="1" t="n">
         <v>0</v>
@@ -6429,13 +6429,13 @@
         <v>1.52</v>
       </c>
       <c r="N94" s="1" t="n">
-        <v>-0.864</v>
+        <v>0</v>
       </c>
       <c r="O94" s="1" t="n">
         <v>-0.52</v>
       </c>
       <c r="P94" s="1" t="n">
-        <v>1.264</v>
+        <v>0.4</v>
       </c>
       <c r="Q94" s="1" t="n"/>
       <c r="R94" s="1" t="n"/>
@@ -6449,7 +6449,7 @@
         <v>8</v>
       </c>
       <c r="V94" s="1" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="W94" s="1" t="n">
         <v>0</v>
@@ -6498,13 +6498,13 @@
         <v>0.958</v>
       </c>
       <c r="N95" s="1" t="n">
-        <v>-0.864</v>
+        <v>0</v>
       </c>
       <c r="O95" s="1" t="n">
         <v>-0.958</v>
       </c>
       <c r="P95" s="1" t="n">
-        <v>0.864</v>
+        <v>0</v>
       </c>
       <c r="Q95" s="1" t="n"/>
       <c r="R95" s="1" t="n"/>
@@ -6518,7 +6518,7 @@
         <v>8</v>
       </c>
       <c r="V95" s="1" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="W95" s="1" t="n">
         <v>0</v>
@@ -6587,10 +6587,10 @@
         <v>2</v>
       </c>
       <c r="V96" s="1" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="W96" s="1" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="X96" s="1" t="n">
         <v>38.9</v>
@@ -6633,13 +6633,13 @@
       </c>
       <c r="L97" s="1" t="n"/>
       <c r="M97" s="1" t="n">
-        <v>-49.95</v>
+        <v>0</v>
       </c>
       <c r="N97" s="1" t="n">
         <v>0</v>
       </c>
       <c r="O97" s="1" t="n">
-        <v>60.3</v>
+        <v>10.35</v>
       </c>
       <c r="P97" s="1" t="n">
         <v>0</v>
@@ -6659,7 +6659,7 @@
         <v>-49.95</v>
       </c>
       <c r="W97" s="1" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="X97" s="1" t="n">
         <v>99.88</v>
@@ -6702,16 +6702,16 @@
       </c>
       <c r="L98" s="1" t="n"/>
       <c r="M98" s="1" t="n">
-        <v>49.996</v>
+        <v>0</v>
       </c>
       <c r="N98" s="1" t="n">
-        <v>0.095</v>
+        <v>0</v>
       </c>
       <c r="O98" s="1" t="n">
-        <v>-46.396</v>
+        <v>3.6</v>
       </c>
       <c r="P98" s="1" t="n">
-        <v>-0.445</v>
+        <v>-0.35</v>
       </c>
       <c r="Q98" s="1" t="n"/>
       <c r="R98" s="1" t="n"/>
@@ -6725,10 +6725,10 @@
         <v>2</v>
       </c>
       <c r="V98" s="1" t="n">
-        <v>2.996</v>
+        <v>49.996</v>
       </c>
       <c r="W98" s="1" t="n">
-        <v>-0</v>
+        <v>0.959</v>
       </c>
       <c r="X98" s="1" t="n">
         <v>0</v>
@@ -6774,13 +6774,13 @@
         <v>-0.3</v>
       </c>
       <c r="N99" s="1" t="n">
-        <v>-0.108</v>
+        <v>0.756</v>
       </c>
       <c r="O99" s="1" t="n">
         <v>3.1</v>
       </c>
       <c r="P99" s="1" t="n">
-        <v>0.758</v>
+        <v>-0.106</v>
       </c>
       <c r="Q99" s="1" t="n"/>
       <c r="R99" s="1" t="n"/>
@@ -6794,7 +6794,7 @@
         <v>8</v>
       </c>
       <c r="V99" s="1" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="W99" s="1" t="n">
         <v>0</v>
@@ -6843,13 +6843,13 @@
         <v>-0.3</v>
       </c>
       <c r="N100" s="1" t="n">
-        <v>-1.526</v>
+        <v>-0.662</v>
       </c>
       <c r="O100" s="1" t="n">
         <v>3.1</v>
       </c>
       <c r="P100" s="1" t="n">
-        <v>1.276</v>
+        <v>0.412</v>
       </c>
       <c r="Q100" s="1" t="n"/>
       <c r="R100" s="1" t="n"/>
@@ -6863,7 +6863,7 @@
         <v>8</v>
       </c>
       <c r="V100" s="1" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="W100" s="1" t="n">
         <v>0</v>
@@ -6912,13 +6912,13 @@
         <v>0</v>
       </c>
       <c r="N101" s="1" t="n">
-        <v>0.095</v>
+        <v>0.959</v>
       </c>
       <c r="O101" s="1" t="n">
         <v>0</v>
       </c>
       <c r="P101" s="1" t="n">
-        <v>11.905</v>
+        <v>11.041</v>
       </c>
       <c r="Q101" s="1" t="n"/>
       <c r="R101" s="1" t="n"/>
@@ -6932,7 +6932,7 @@
         <v>8</v>
       </c>
       <c r="V101" s="1" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="W101" s="1" t="n">
         <v>0</v>
@@ -6978,16 +6978,16 @@
       </c>
       <c r="L102" s="1" t="n"/>
       <c r="M102" s="1" t="n">
-        <v>47</v>
+        <v>0</v>
       </c>
       <c r="N102" s="1" t="n">
-        <v>-38.405</v>
+        <v>0</v>
       </c>
       <c r="O102" s="1" t="n">
-        <v>-47</v>
+        <v>0</v>
       </c>
       <c r="P102" s="1" t="n">
-        <v>49.205</v>
+        <v>10.8</v>
       </c>
       <c r="Q102" s="1" t="n"/>
       <c r="R102" s="1" t="n"/>
@@ -7001,10 +7001,10 @@
         <v>2</v>
       </c>
       <c r="V102" s="1" t="n">
-        <v>-0</v>
+        <v>47</v>
       </c>
       <c r="W102" s="1" t="n">
-        <v>-0</v>
+        <v>0.959</v>
       </c>
       <c r="X102" s="1" t="n">
         <v>0</v>
@@ -7047,16 +7047,16 @@
       </c>
       <c r="L103" s="1" t="n"/>
       <c r="M103" s="1" t="n">
-        <v>49.996</v>
+        <v>0</v>
       </c>
       <c r="N103" s="1" t="n">
-        <v>-27.401</v>
+        <v>0</v>
       </c>
       <c r="O103" s="1" t="n">
-        <v>-58.146</v>
+        <v>-8.15</v>
       </c>
       <c r="P103" s="1" t="n">
-        <v>28.201</v>
+        <v>0.8</v>
       </c>
       <c r="Q103" s="1" t="n"/>
       <c r="R103" s="1" t="n"/>
@@ -7070,10 +7070,10 @@
         <v>2</v>
       </c>
       <c r="V103" s="1" t="n">
-        <v>2.996</v>
+        <v>49.996</v>
       </c>
       <c r="W103" s="1" t="n">
-        <v>-0</v>
+        <v>0.959</v>
       </c>
       <c r="X103" s="1" t="n">
         <v>0</v>
@@ -7116,16 +7116,16 @@
       </c>
       <c r="L104" s="1" t="n"/>
       <c r="M104" s="1" t="n">
-        <v>-44</v>
+        <v>0</v>
       </c>
       <c r="N104" s="1" t="n">
-        <v>0.095</v>
+        <v>0</v>
       </c>
       <c r="O104" s="1" t="n">
-        <v>34.05</v>
+        <v>-9.949999999999999</v>
       </c>
       <c r="P104" s="1" t="n">
-        <v>-0.095</v>
+        <v>0</v>
       </c>
       <c r="Q104" s="1" t="n"/>
       <c r="R104" s="1" t="n"/>
@@ -7142,7 +7142,7 @@
         <v>-44</v>
       </c>
       <c r="W104" s="1" t="n">
-        <v>0.095</v>
+        <v>0.959</v>
       </c>
       <c r="X104" s="1" t="n">
         <v>0</v>
@@ -7185,16 +7185,16 @@
       </c>
       <c r="L105" s="1" t="n"/>
       <c r="M105" s="1" t="n">
-        <v>44</v>
+        <v>0</v>
       </c>
       <c r="N105" s="1" t="n">
-        <v>0.095</v>
+        <v>0</v>
       </c>
       <c r="O105" s="1" t="n">
-        <v>-53.95</v>
+        <v>-9.949999999999999</v>
       </c>
       <c r="P105" s="1" t="n">
-        <v>-0.095</v>
+        <v>0</v>
       </c>
       <c r="Q105" s="1" t="n"/>
       <c r="R105" s="1" t="n"/>
@@ -7211,7 +7211,7 @@
         <v>44</v>
       </c>
       <c r="W105" s="1" t="n">
-        <v>0.095</v>
+        <v>0.959</v>
       </c>
       <c r="X105" s="1" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
code for adding the TVPA and AGA marks. Plus more miscellaneous stuff
</commit_message>
<xml_diff>
--- a/masks/code/ResonatorArray.xlsx
+++ b/masks/code/ResonatorArray.xlsx
@@ -15,7 +15,28 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="123">
+  <si>
+    <t>AGA Marks</t>
+  </si>
+  <si>
+    <t>TVPA</t>
+  </si>
+  <si>
+    <t>direction</t>
+  </si>
+  <si>
+    <t>layer</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>GP</t>
+  </si>
   <si>
     <t>Alternate Array Layout</t>
   </si>
@@ -53,12 +74,6 @@
     <t>Cell name</t>
   </si>
   <si>
-    <t>x</t>
-  </si>
-  <si>
-    <t>y</t>
-  </si>
-  <si>
     <t>xl</t>
   </si>
   <si>
@@ -84,9 +99,6 @@
   </si>
   <si>
     <t>R</t>
-  </si>
-  <si>
-    <t>GP</t>
   </si>
   <si>
     <t>alignment_marks_patch_new</t>
@@ -744,12 +756,12 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col customWidth="1" max="1" min="1" width="16"/>
-    <col customWidth="1" max="2" min="2" width="6"/>
+    <col customWidth="1" max="2" min="2" width="11"/>
     <col customWidth="1" max="3" min="3" width="29"/>
-    <col customWidth="1" max="4" min="4" width="7"/>
+    <col customWidth="1" max="4" min="4" width="8"/>
     <col customWidth="1" max="5" min="5" width="8"/>
     <col customWidth="1" max="6" min="6" width="6"/>
-    <col customWidth="1" max="7" min="7" width="6"/>
+    <col customWidth="1" max="7" min="7" width="7"/>
     <col customWidth="1" max="8" min="8" width="8"/>
     <col customWidth="1" max="9" min="9" width="8"/>
     <col customWidth="1" max="10" min="10" width="7"/>
@@ -773,13 +785,235 @@
     <row r="1" spans="1:25"/>
     <row r="2" spans="1:25"/>
     <row r="3" spans="1:25"/>
-    <row r="4" spans="1:25"/>
-    <row r="5" spans="1:25"/>
-    <row r="6" spans="1:25"/>
-    <row r="7" spans="1:25"/>
-    <row r="8" spans="1:25"/>
-    <row r="9" spans="1:25"/>
-    <row r="10" spans="1:25"/>
+    <row r="4" spans="1:25">
+      <c r="A4" s="1" t="n"/>
+      <c r="B4" s="1" t="n"/>
+      <c r="C4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="1" t="n"/>
+      <c r="E4" s="1" t="n"/>
+      <c r="F4" s="1" t="n"/>
+      <c r="G4" s="1" t="n"/>
+      <c r="H4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I4" s="1" t="n"/>
+      <c r="J4" s="1" t="n"/>
+      <c r="K4" s="1" t="n"/>
+      <c r="L4" s="1" t="n"/>
+      <c r="M4" s="1" t="n"/>
+      <c r="N4" s="1" t="n"/>
+      <c r="O4" s="1" t="n"/>
+      <c r="P4" s="1" t="n"/>
+      <c r="Q4" s="1" t="n"/>
+      <c r="R4" s="1" t="n"/>
+      <c r="S4" s="1" t="n"/>
+      <c r="T4" s="1" t="n"/>
+      <c r="U4" s="1" t="n"/>
+      <c r="V4" s="1" t="n"/>
+      <c r="W4" s="1" t="n"/>
+      <c r="X4" s="1" t="n"/>
+      <c r="Y4" s="1" t="n"/>
+    </row>
+    <row r="5" spans="1:25">
+      <c r="A5" s="1" t="n"/>
+      <c r="B5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="1" t="n"/>
+      <c r="G5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J5" s="1" t="n"/>
+      <c r="K5" s="1" t="n"/>
+      <c r="L5" s="1" t="n"/>
+      <c r="M5" s="1" t="n"/>
+      <c r="N5" s="1" t="n"/>
+      <c r="O5" s="1" t="n"/>
+      <c r="P5" s="1" t="n"/>
+      <c r="Q5" s="1" t="n"/>
+      <c r="R5" s="1" t="n"/>
+      <c r="S5" s="1" t="n"/>
+      <c r="T5" s="1" t="n"/>
+      <c r="U5" s="1" t="n"/>
+      <c r="V5" s="1" t="n"/>
+      <c r="W5" s="1" t="n"/>
+      <c r="X5" s="1" t="n"/>
+      <c r="Y5" s="1" t="n"/>
+    </row>
+    <row r="6" spans="1:25">
+      <c r="A6" s="1" t="n"/>
+      <c r="B6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="1" t="n">
+        <v>-2.875</v>
+      </c>
+      <c r="E6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" s="1" t="n"/>
+      <c r="G6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H6" s="1" t="n">
+        <v>-2.525</v>
+      </c>
+      <c r="I6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" s="1" t="n"/>
+      <c r="K6" s="1" t="n"/>
+      <c r="L6" s="1" t="n"/>
+      <c r="M6" s="1" t="n"/>
+      <c r="N6" s="1" t="n"/>
+      <c r="O6" s="1" t="n"/>
+      <c r="P6" s="1" t="n"/>
+      <c r="Q6" s="1" t="n"/>
+      <c r="R6" s="1" t="n"/>
+      <c r="S6" s="1" t="n"/>
+      <c r="T6" s="1" t="n"/>
+      <c r="U6" s="1" t="n"/>
+      <c r="V6" s="1" t="n"/>
+      <c r="W6" s="1" t="n"/>
+      <c r="X6" s="1" t="n"/>
+      <c r="Y6" s="1" t="n"/>
+    </row>
+    <row r="7" spans="1:25">
+      <c r="A7" s="1" t="n"/>
+      <c r="B7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="1" t="n">
+        <v>-2.775</v>
+      </c>
+      <c r="E7" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" s="1" t="n"/>
+      <c r="G7" s="1" t="n"/>
+      <c r="H7" s="1" t="n"/>
+      <c r="I7" s="1" t="n"/>
+      <c r="J7" s="1" t="n"/>
+      <c r="K7" s="1" t="n"/>
+      <c r="L7" s="1" t="n"/>
+      <c r="M7" s="1" t="n"/>
+      <c r="N7" s="1" t="n"/>
+      <c r="O7" s="1" t="n"/>
+      <c r="P7" s="1" t="n"/>
+      <c r="Q7" s="1" t="n"/>
+      <c r="R7" s="1" t="n"/>
+      <c r="S7" s="1" t="n"/>
+      <c r="T7" s="1" t="n"/>
+      <c r="U7" s="1" t="n"/>
+      <c r="V7" s="1" t="n"/>
+      <c r="W7" s="1" t="n"/>
+      <c r="X7" s="1" t="n"/>
+      <c r="Y7" s="1" t="n"/>
+    </row>
+    <row r="8" spans="1:25">
+      <c r="A8" s="1" t="n"/>
+      <c r="B8" s="1" t="n"/>
+      <c r="C8" s="1" t="n"/>
+      <c r="D8" s="1" t="n"/>
+      <c r="E8" s="1" t="n"/>
+      <c r="F8" s="1" t="n"/>
+      <c r="G8" s="1" t="n"/>
+      <c r="H8" s="1" t="n"/>
+      <c r="I8" s="1" t="n"/>
+      <c r="J8" s="1" t="n"/>
+      <c r="K8" s="1" t="n"/>
+      <c r="L8" s="1" t="n"/>
+      <c r="M8" s="1" t="n"/>
+      <c r="N8" s="1" t="n"/>
+      <c r="O8" s="1" t="n"/>
+      <c r="P8" s="1" t="n"/>
+      <c r="Q8" s="1" t="n"/>
+      <c r="R8" s="1" t="n"/>
+      <c r="S8" s="1" t="n"/>
+      <c r="T8" s="1" t="n"/>
+      <c r="U8" s="1" t="n"/>
+      <c r="V8" s="1" t="n"/>
+      <c r="W8" s="1" t="n"/>
+      <c r="X8" s="1" t="n"/>
+      <c r="Y8" s="1" t="n"/>
+    </row>
+    <row r="9" spans="1:25">
+      <c r="A9" s="1" t="n"/>
+      <c r="B9" s="1" t="n"/>
+      <c r="C9" s="1" t="n"/>
+      <c r="D9" s="1" t="n"/>
+      <c r="E9" s="1" t="n"/>
+      <c r="F9" s="1" t="n"/>
+      <c r="G9" s="1" t="n"/>
+      <c r="H9" s="1" t="n"/>
+      <c r="I9" s="1" t="n"/>
+      <c r="J9" s="1" t="n"/>
+      <c r="K9" s="1" t="n"/>
+      <c r="L9" s="1" t="n"/>
+      <c r="M9" s="1" t="n"/>
+      <c r="N9" s="1" t="n"/>
+      <c r="O9" s="1" t="n"/>
+      <c r="P9" s="1" t="n"/>
+      <c r="Q9" s="1" t="n"/>
+      <c r="R9" s="1" t="n"/>
+      <c r="S9" s="1" t="n"/>
+      <c r="T9" s="1" t="n"/>
+      <c r="U9" s="1" t="n"/>
+      <c r="V9" s="1" t="n"/>
+      <c r="W9" s="1" t="n"/>
+      <c r="X9" s="1" t="n"/>
+      <c r="Y9" s="1" t="n"/>
+    </row>
+    <row r="10" spans="1:25">
+      <c r="A10" s="1" t="n"/>
+      <c r="B10" s="1" t="n"/>
+      <c r="C10" s="1" t="n"/>
+      <c r="D10" s="1" t="n"/>
+      <c r="E10" s="1" t="n"/>
+      <c r="F10" s="1" t="n"/>
+      <c r="G10" s="1" t="n"/>
+      <c r="H10" s="1" t="n"/>
+      <c r="I10" s="1" t="n"/>
+      <c r="J10" s="1" t="n"/>
+      <c r="K10" s="1" t="n"/>
+      <c r="L10" s="1" t="n"/>
+      <c r="M10" s="1" t="n"/>
+      <c r="N10" s="1" t="n"/>
+      <c r="O10" s="1" t="n"/>
+      <c r="P10" s="1" t="n"/>
+      <c r="Q10" s="1" t="n"/>
+      <c r="R10" s="1" t="n"/>
+      <c r="S10" s="1" t="n"/>
+      <c r="T10" s="1" t="n"/>
+      <c r="U10" s="1" t="n"/>
+      <c r="V10" s="1" t="n"/>
+      <c r="W10" s="1" t="n"/>
+      <c r="X10" s="1" t="n"/>
+      <c r="Y10" s="1" t="n"/>
+    </row>
     <row r="11" spans="1:25">
       <c r="A11" s="1" t="n"/>
       <c r="B11" s="1" t="n"/>
@@ -828,7 +1062,7 @@
       <c r="R12" s="1" t="n"/>
       <c r="S12" s="1" t="n"/>
       <c r="T12" s="1" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:25">
@@ -836,116 +1070,116 @@
       <c r="B13" s="1" t="n"/>
       <c r="C13" s="1" t="n"/>
       <c r="D13" s="1" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="L13" s="1" t="n"/>
       <c r="M13" s="1" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="O13" s="1" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="Q13" s="1" t="n"/>
       <c r="R13" s="1" t="n"/>
       <c r="S13" s="1" t="n"/>
       <c r="T13" s="1" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="V13" s="1" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="X13" s="1" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:25">
       <c r="A14" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="L14" s="1" t="n"/>
       <c r="M14" s="1" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="N14" s="1" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="O14" s="1" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="P14" s="1" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="Q14" s="1" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="R14" s="1" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="S14" s="1" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="T14" s="1" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="U14" s="1" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="V14" s="1" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="W14" s="1" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="X14" s="1" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="Y14" s="1" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:25">
       <c r="A15" s="1" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="B15" s="1" t="n"/>
       <c r="C15" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="D15" s="1" t="n">
         <v>1.1</v>
@@ -985,11 +1219,11 @@
         <v>-0.15</v>
       </c>
       <c r="Q15" s="1" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="R15" s="1" t="n"/>
       <c r="S15" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T15" s="1" t="n">
         <v>8</v>
@@ -1012,11 +1246,11 @@
     </row>
     <row r="16" spans="1:25">
       <c r="A16" s="1" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="B16" s="1" t="n"/>
       <c r="C16" s="1" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="D16" s="1" t="n">
         <v>0</v>
@@ -1058,7 +1292,7 @@
       <c r="Q16" s="1" t="n"/>
       <c r="R16" s="1" t="n"/>
       <c r="S16" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T16" s="1" t="n">
         <v>8</v>
@@ -1081,11 +1315,11 @@
     </row>
     <row r="17" spans="1:25">
       <c r="A17" s="1" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="B17" s="1" t="n"/>
       <c r="C17" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="D17" s="1" t="n">
         <v>3.6</v>
@@ -1127,7 +1361,7 @@
       <c r="Q17" s="1" t="n"/>
       <c r="R17" s="1" t="n"/>
       <c r="S17" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T17" s="1" t="n">
         <v>1</v>
@@ -1150,11 +1384,11 @@
     </row>
     <row r="18" spans="1:25">
       <c r="A18" s="1" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="B18" s="1" t="n"/>
       <c r="C18" s="1" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D18" s="1" t="n">
         <v>0</v>
@@ -1196,7 +1430,7 @@
       <c r="Q18" s="1" t="n"/>
       <c r="R18" s="1" t="n"/>
       <c r="S18" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T18" s="1" t="n">
         <v>1</v>
@@ -1219,11 +1453,11 @@
     </row>
     <row r="19" spans="1:25">
       <c r="A19" s="1" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="B19" s="1" t="n"/>
       <c r="C19" s="1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D19" s="1" t="n">
         <v>-8.75</v>
@@ -1265,7 +1499,7 @@
       <c r="Q19" s="1" t="n"/>
       <c r="R19" s="1" t="n"/>
       <c r="S19" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T19" s="1" t="n">
         <v>1</v>
@@ -1288,11 +1522,11 @@
     </row>
     <row r="20" spans="1:25">
       <c r="A20" s="1" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="B20" s="1" t="n"/>
       <c r="C20" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D20" s="1" t="n">
         <v>6.4</v>
@@ -1334,7 +1568,7 @@
       <c r="Q20" s="1" t="n"/>
       <c r="R20" s="1" t="n"/>
       <c r="S20" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T20" s="1" t="n">
         <v>8</v>
@@ -1357,11 +1591,11 @@
     </row>
     <row r="21" spans="1:25">
       <c r="A21" s="1" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="B21" s="1" t="n"/>
       <c r="C21" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D21" s="1" t="n">
         <v>-9.35</v>
@@ -1403,7 +1637,7 @@
       <c r="Q21" s="1" t="n"/>
       <c r="R21" s="1" t="n"/>
       <c r="S21" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T21" s="1" t="n">
         <v>1</v>
@@ -1426,11 +1660,11 @@
     </row>
     <row r="22" spans="1:25">
       <c r="A22" s="1" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="B22" s="1" t="n"/>
       <c r="C22" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D22" s="1" t="n">
         <v>-9.35</v>
@@ -1472,7 +1706,7 @@
       <c r="Q22" s="1" t="n"/>
       <c r="R22" s="1" t="n"/>
       <c r="S22" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T22" s="1" t="n">
         <v>1</v>
@@ -1495,11 +1729,11 @@
     </row>
     <row r="23" spans="1:25">
       <c r="A23" s="1" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="B23" s="1" t="n"/>
       <c r="C23" s="1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D23" s="1" t="n">
         <v>0</v>
@@ -1541,7 +1775,7 @@
       <c r="Q23" s="1" t="n"/>
       <c r="R23" s="1" t="n"/>
       <c r="S23" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T23" s="1" t="n">
         <v>3</v>
@@ -1564,11 +1798,11 @@
     </row>
     <row r="24" spans="1:25">
       <c r="A24" s="1" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="B24" s="1" t="n"/>
       <c r="C24" s="1" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="D24" s="1" t="n">
         <v>9.25</v>
@@ -1610,7 +1844,7 @@
       <c r="Q24" s="1" t="n"/>
       <c r="R24" s="1" t="n"/>
       <c r="S24" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T24" s="1" t="n">
         <v>1</v>
@@ -1633,11 +1867,11 @@
     </row>
     <row r="25" spans="1:25">
       <c r="A25" s="1" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="B25" s="1" t="n"/>
       <c r="C25" s="1" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="D25" s="1" t="n">
         <v>1.75</v>
@@ -1679,7 +1913,7 @@
       <c r="Q25" s="1" t="n"/>
       <c r="R25" s="1" t="n"/>
       <c r="S25" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T25" s="1" t="n">
         <v>8</v>
@@ -1702,11 +1936,11 @@
     </row>
     <row r="26" spans="1:25">
       <c r="A26" s="1" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="B26" s="1" t="n"/>
       <c r="C26" s="1" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="D26" s="1" t="n">
         <v>7.05</v>
@@ -1748,7 +1982,7 @@
       <c r="Q26" s="1" t="n"/>
       <c r="R26" s="1" t="n"/>
       <c r="S26" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T26" s="1" t="n">
         <v>8</v>
@@ -1771,11 +2005,11 @@
     </row>
     <row r="27" spans="1:25">
       <c r="A27" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B27" s="1" t="n"/>
       <c r="C27" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="D27" s="1" t="n">
         <v>0</v>
@@ -1817,7 +2051,7 @@
       <c r="Q27" s="1" t="n"/>
       <c r="R27" s="1" t="n"/>
       <c r="S27" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T27" s="1" t="n">
         <v>8</v>
@@ -1840,11 +2074,11 @@
     </row>
     <row r="28" spans="1:25">
       <c r="A28" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B28" s="1" t="n"/>
       <c r="C28" s="1" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="D28" s="1" t="n">
         <v>-10.6</v>
@@ -1886,7 +2120,7 @@
       <c r="Q28" s="1" t="n"/>
       <c r="R28" s="1" t="n"/>
       <c r="S28" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T28" s="1" t="n">
         <v>2</v>
@@ -1909,11 +2143,11 @@
     </row>
     <row r="29" spans="1:25">
       <c r="A29" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B29" s="1" t="n"/>
       <c r="C29" s="1" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="D29" s="1" t="n">
         <v>-5.55</v>
@@ -1955,7 +2189,7 @@
       <c r="Q29" s="1" t="n"/>
       <c r="R29" s="1" t="n"/>
       <c r="S29" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T29" s="1" t="n">
         <v>1</v>
@@ -1978,11 +2212,11 @@
     </row>
     <row r="30" spans="1:25">
       <c r="A30" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B30" s="1" t="n"/>
       <c r="C30" s="1" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="D30" s="1" t="n">
         <v>-3.7</v>
@@ -2024,7 +2258,7 @@
       <c r="Q30" s="1" t="n"/>
       <c r="R30" s="1" t="n"/>
       <c r="S30" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T30" s="1" t="n">
         <v>1</v>
@@ -2047,11 +2281,11 @@
     </row>
     <row r="31" spans="1:25">
       <c r="A31" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B31" s="1" t="n"/>
       <c r="C31" s="1" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="D31" s="1" t="n">
         <v>-1.85</v>
@@ -2093,7 +2327,7 @@
       <c r="Q31" s="1" t="n"/>
       <c r="R31" s="1" t="n"/>
       <c r="S31" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T31" s="1" t="n">
         <v>1</v>
@@ -2116,11 +2350,11 @@
     </row>
     <row r="32" spans="1:25">
       <c r="A32" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B32" s="1" t="n"/>
       <c r="C32" s="1" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="D32" s="1" t="n">
         <v>0</v>
@@ -2162,7 +2396,7 @@
       <c r="Q32" s="1" t="n"/>
       <c r="R32" s="1" t="n"/>
       <c r="S32" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T32" s="1" t="n">
         <v>1</v>
@@ -2185,11 +2419,11 @@
     </row>
     <row r="33" spans="1:25">
       <c r="A33" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B33" s="1" t="n"/>
       <c r="C33" s="1" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="D33" s="1" t="n">
         <v>1.85</v>
@@ -2231,7 +2465,7 @@
       <c r="Q33" s="1" t="n"/>
       <c r="R33" s="1" t="n"/>
       <c r="S33" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T33" s="1" t="n">
         <v>1</v>
@@ -2254,11 +2488,11 @@
     </row>
     <row r="34" spans="1:25">
       <c r="A34" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B34" s="1" t="n"/>
       <c r="C34" s="1" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="D34" s="1" t="n">
         <v>3.7</v>
@@ -2300,7 +2534,7 @@
       <c r="Q34" s="1" t="n"/>
       <c r="R34" s="1" t="n"/>
       <c r="S34" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T34" s="1" t="n">
         <v>1</v>
@@ -2323,11 +2557,11 @@
     </row>
     <row r="35" spans="1:25">
       <c r="A35" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B35" s="1" t="n"/>
       <c r="C35" s="1" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="D35" s="1" t="n">
         <v>-5.55</v>
@@ -2369,7 +2603,7 @@
       <c r="Q35" s="1" t="n"/>
       <c r="R35" s="1" t="n"/>
       <c r="S35" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T35" s="1" t="n">
         <v>1</v>
@@ -2392,11 +2626,11 @@
     </row>
     <row r="36" spans="1:25">
       <c r="A36" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B36" s="1" t="n"/>
       <c r="C36" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="D36" s="1" t="n">
         <v>-3.7</v>
@@ -2438,7 +2672,7 @@
       <c r="Q36" s="1" t="n"/>
       <c r="R36" s="1" t="n"/>
       <c r="S36" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T36" s="1" t="n">
         <v>1</v>
@@ -2461,11 +2695,11 @@
     </row>
     <row r="37" spans="1:25">
       <c r="A37" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B37" s="1" t="n"/>
       <c r="C37" s="1" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="D37" s="1" t="n">
         <v>-1.85</v>
@@ -2507,7 +2741,7 @@
       <c r="Q37" s="1" t="n"/>
       <c r="R37" s="1" t="n"/>
       <c r="S37" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T37" s="1" t="n">
         <v>1</v>
@@ -2530,11 +2764,11 @@
     </row>
     <row r="38" spans="1:25">
       <c r="A38" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B38" s="1" t="n"/>
       <c r="C38" s="1" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="D38" s="1" t="n">
         <v>0</v>
@@ -2576,7 +2810,7 @@
       <c r="Q38" s="1" t="n"/>
       <c r="R38" s="1" t="n"/>
       <c r="S38" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T38" s="1" t="n">
         <v>1</v>
@@ -2599,11 +2833,11 @@
     </row>
     <row r="39" spans="1:25">
       <c r="A39" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B39" s="1" t="n"/>
       <c r="C39" s="1" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="D39" s="1" t="n">
         <v>1.85</v>
@@ -2645,7 +2879,7 @@
       <c r="Q39" s="1" t="n"/>
       <c r="R39" s="1" t="n"/>
       <c r="S39" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T39" s="1" t="n">
         <v>1</v>
@@ -2668,11 +2902,11 @@
     </row>
     <row r="40" spans="1:25">
       <c r="A40" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B40" s="1" t="n"/>
       <c r="C40" s="1" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="D40" s="1" t="n">
         <v>3.7</v>
@@ -2714,7 +2948,7 @@
       <c r="Q40" s="1" t="n"/>
       <c r="R40" s="1" t="n"/>
       <c r="S40" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T40" s="1" t="n">
         <v>1</v>
@@ -2737,11 +2971,11 @@
     </row>
     <row r="41" spans="1:25">
       <c r="A41" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B41" s="1" t="n"/>
       <c r="C41" s="1" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="D41" s="1" t="n">
         <v>-5.55</v>
@@ -2783,7 +3017,7 @@
       <c r="Q41" s="1" t="n"/>
       <c r="R41" s="1" t="n"/>
       <c r="S41" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T41" s="1" t="n">
         <v>1</v>
@@ -2806,11 +3040,11 @@
     </row>
     <row r="42" spans="1:25">
       <c r="A42" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B42" s="1" t="n"/>
       <c r="C42" s="1" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="D42" s="1" t="n">
         <v>-3.7</v>
@@ -2852,7 +3086,7 @@
       <c r="Q42" s="1" t="n"/>
       <c r="R42" s="1" t="n"/>
       <c r="S42" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T42" s="1" t="n">
         <v>1</v>
@@ -2875,11 +3109,11 @@
     </row>
     <row r="43" spans="1:25">
       <c r="A43" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B43" s="1" t="n"/>
       <c r="C43" s="1" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="D43" s="1" t="n">
         <v>-1.85</v>
@@ -2921,7 +3155,7 @@
       <c r="Q43" s="1" t="n"/>
       <c r="R43" s="1" t="n"/>
       <c r="S43" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T43" s="1" t="n">
         <v>1</v>
@@ -2944,11 +3178,11 @@
     </row>
     <row r="44" spans="1:25">
       <c r="A44" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B44" s="1" t="n"/>
       <c r="C44" s="1" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="D44" s="1" t="n">
         <v>0</v>
@@ -2990,7 +3224,7 @@
       <c r="Q44" s="1" t="n"/>
       <c r="R44" s="1" t="n"/>
       <c r="S44" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T44" s="1" t="n">
         <v>1</v>
@@ -3013,11 +3247,11 @@
     </row>
     <row r="45" spans="1:25">
       <c r="A45" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B45" s="1" t="n"/>
       <c r="C45" s="1" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="D45" s="1" t="n">
         <v>1.85</v>
@@ -3059,7 +3293,7 @@
       <c r="Q45" s="1" t="n"/>
       <c r="R45" s="1" t="n"/>
       <c r="S45" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T45" s="1" t="n">
         <v>1</v>
@@ -3082,11 +3316,11 @@
     </row>
     <row r="46" spans="1:25">
       <c r="A46" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B46" s="1" t="n"/>
       <c r="C46" s="1" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="D46" s="1" t="n">
         <v>3.7</v>
@@ -3128,7 +3362,7 @@
       <c r="Q46" s="1" t="n"/>
       <c r="R46" s="1" t="n"/>
       <c r="S46" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T46" s="1" t="n">
         <v>1</v>
@@ -3151,11 +3385,11 @@
     </row>
     <row r="47" spans="1:25">
       <c r="A47" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B47" s="1" t="n"/>
       <c r="C47" s="1" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D47" s="1" t="n">
         <v>-5.55</v>
@@ -3197,7 +3431,7 @@
       <c r="Q47" s="1" t="n"/>
       <c r="R47" s="1" t="n"/>
       <c r="S47" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T47" s="1" t="n">
         <v>1</v>
@@ -3220,11 +3454,11 @@
     </row>
     <row r="48" spans="1:25">
       <c r="A48" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B48" s="1" t="n"/>
       <c r="C48" s="1" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="D48" s="1" t="n">
         <v>-3.7</v>
@@ -3266,7 +3500,7 @@
       <c r="Q48" s="1" t="n"/>
       <c r="R48" s="1" t="n"/>
       <c r="S48" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T48" s="1" t="n">
         <v>1</v>
@@ -3289,11 +3523,11 @@
     </row>
     <row r="49" spans="1:25">
       <c r="A49" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B49" s="1" t="n"/>
       <c r="C49" s="1" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="D49" s="1" t="n">
         <v>-1.85</v>
@@ -3335,7 +3569,7 @@
       <c r="Q49" s="1" t="n"/>
       <c r="R49" s="1" t="n"/>
       <c r="S49" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T49" s="1" t="n">
         <v>1</v>
@@ -3358,11 +3592,11 @@
     </row>
     <row r="50" spans="1:25">
       <c r="A50" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B50" s="1" t="n"/>
       <c r="C50" s="1" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="D50" s="1" t="n">
         <v>0</v>
@@ -3404,7 +3638,7 @@
       <c r="Q50" s="1" t="n"/>
       <c r="R50" s="1" t="n"/>
       <c r="S50" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T50" s="1" t="n">
         <v>1</v>
@@ -3427,11 +3661,11 @@
     </row>
     <row r="51" spans="1:25">
       <c r="A51" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B51" s="1" t="n"/>
       <c r="C51" s="1" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="D51" s="1" t="n">
         <v>1.85</v>
@@ -3473,7 +3707,7 @@
       <c r="Q51" s="1" t="n"/>
       <c r="R51" s="1" t="n"/>
       <c r="S51" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T51" s="1" t="n">
         <v>1</v>
@@ -3496,11 +3730,11 @@
     </row>
     <row r="52" spans="1:25">
       <c r="A52" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B52" s="1" t="n"/>
       <c r="C52" s="1" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="D52" s="1" t="n">
         <v>3.7</v>
@@ -3542,7 +3776,7 @@
       <c r="Q52" s="1" t="n"/>
       <c r="R52" s="1" t="n"/>
       <c r="S52" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T52" s="1" t="n">
         <v>1</v>
@@ -3565,11 +3799,11 @@
     </row>
     <row r="53" spans="1:25">
       <c r="A53" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B53" s="1" t="n"/>
       <c r="C53" s="1" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="D53" s="1" t="n">
         <v>-5.55</v>
@@ -3611,7 +3845,7 @@
       <c r="Q53" s="1" t="n"/>
       <c r="R53" s="1" t="n"/>
       <c r="S53" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T53" s="1" t="n">
         <v>1</v>
@@ -3634,11 +3868,11 @@
     </row>
     <row r="54" spans="1:25">
       <c r="A54" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B54" s="1" t="n"/>
       <c r="C54" s="1" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="D54" s="1" t="n">
         <v>-3.7</v>
@@ -3680,7 +3914,7 @@
       <c r="Q54" s="1" t="n"/>
       <c r="R54" s="1" t="n"/>
       <c r="S54" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T54" s="1" t="n">
         <v>1</v>
@@ -3703,11 +3937,11 @@
     </row>
     <row r="55" spans="1:25">
       <c r="A55" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B55" s="1" t="n"/>
       <c r="C55" s="1" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="D55" s="1" t="n">
         <v>-1.85</v>
@@ -3749,7 +3983,7 @@
       <c r="Q55" s="1" t="n"/>
       <c r="R55" s="1" t="n"/>
       <c r="S55" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T55" s="1" t="n">
         <v>1</v>
@@ -3772,11 +4006,11 @@
     </row>
     <row r="56" spans="1:25">
       <c r="A56" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B56" s="1" t="n"/>
       <c r="C56" s="1" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="D56" s="1" t="n">
         <v>0</v>
@@ -3818,7 +4052,7 @@
       <c r="Q56" s="1" t="n"/>
       <c r="R56" s="1" t="n"/>
       <c r="S56" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T56" s="1" t="n">
         <v>1</v>
@@ -3841,11 +4075,11 @@
     </row>
     <row r="57" spans="1:25">
       <c r="A57" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B57" s="1" t="n"/>
       <c r="C57" s="1" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="D57" s="1" t="n">
         <v>1.85</v>
@@ -3887,7 +4121,7 @@
       <c r="Q57" s="1" t="n"/>
       <c r="R57" s="1" t="n"/>
       <c r="S57" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T57" s="1" t="n">
         <v>1</v>
@@ -3910,11 +4144,11 @@
     </row>
     <row r="58" spans="1:25">
       <c r="A58" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B58" s="1" t="n"/>
       <c r="C58" s="1" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="D58" s="1" t="n">
         <v>3.7</v>
@@ -3956,7 +4190,7 @@
       <c r="Q58" s="1" t="n"/>
       <c r="R58" s="1" t="n"/>
       <c r="S58" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T58" s="1" t="n">
         <v>1</v>
@@ -3979,11 +4213,11 @@
     </row>
     <row r="59" spans="1:25">
       <c r="A59" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B59" s="1" t="n"/>
       <c r="C59" s="1" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="D59" s="1" t="n">
         <v>-0.9</v>
@@ -4025,7 +4259,7 @@
       <c r="Q59" s="1" t="n"/>
       <c r="R59" s="1" t="n"/>
       <c r="S59" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T59" s="1" t="n">
         <v>1</v>
@@ -4048,11 +4282,11 @@
     </row>
     <row r="60" spans="1:25">
       <c r="A60" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B60" s="1" t="n"/>
       <c r="C60" s="1" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="D60" s="1" t="n">
         <v>0.9</v>
@@ -4094,7 +4328,7 @@
       <c r="Q60" s="1" t="n"/>
       <c r="R60" s="1" t="n"/>
       <c r="S60" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T60" s="1" t="n">
         <v>1</v>
@@ -4117,11 +4351,11 @@
     </row>
     <row r="61" spans="1:25">
       <c r="A61" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B61" s="1" t="n"/>
       <c r="C61" s="1" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="D61" s="1" t="n">
         <v>-0.9</v>
@@ -4163,7 +4397,7 @@
       <c r="Q61" s="1" t="n"/>
       <c r="R61" s="1" t="n"/>
       <c r="S61" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T61" s="1" t="n">
         <v>1</v>
@@ -4186,11 +4420,11 @@
     </row>
     <row r="62" spans="1:25">
       <c r="A62" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B62" s="1" t="n"/>
       <c r="C62" s="1" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="D62" s="1" t="n">
         <v>0.9</v>
@@ -4232,7 +4466,7 @@
       <c r="Q62" s="1" t="n"/>
       <c r="R62" s="1" t="n"/>
       <c r="S62" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T62" s="1" t="n">
         <v>1</v>
@@ -4255,11 +4489,11 @@
     </row>
     <row r="63" spans="1:25">
       <c r="A63" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B63" s="1" t="n"/>
       <c r="C63" s="1" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="D63" s="1" t="n">
         <v>-5.55</v>
@@ -4301,7 +4535,7 @@
       <c r="Q63" s="1" t="n"/>
       <c r="R63" s="1" t="n"/>
       <c r="S63" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T63" s="1" t="n">
         <v>1</v>
@@ -4324,11 +4558,11 @@
     </row>
     <row r="64" spans="1:25">
       <c r="A64" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B64" s="1" t="n"/>
       <c r="C64" s="1" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="D64" s="1" t="n">
         <v>-3.7</v>
@@ -4370,7 +4604,7 @@
       <c r="Q64" s="1" t="n"/>
       <c r="R64" s="1" t="n"/>
       <c r="S64" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T64" s="1" t="n">
         <v>1</v>
@@ -4393,11 +4627,11 @@
     </row>
     <row r="65" spans="1:25">
       <c r="A65" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B65" s="1" t="n"/>
       <c r="C65" s="1" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="D65" s="1" t="n">
         <v>-1.85</v>
@@ -4439,7 +4673,7 @@
       <c r="Q65" s="1" t="n"/>
       <c r="R65" s="1" t="n"/>
       <c r="S65" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T65" s="1" t="n">
         <v>1</v>
@@ -4462,11 +4696,11 @@
     </row>
     <row r="66" spans="1:25">
       <c r="A66" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B66" s="1" t="n"/>
       <c r="C66" s="1" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="D66" s="1" t="n">
         <v>0</v>
@@ -4508,7 +4742,7 @@
       <c r="Q66" s="1" t="n"/>
       <c r="R66" s="1" t="n"/>
       <c r="S66" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T66" s="1" t="n">
         <v>1</v>
@@ -4531,11 +4765,11 @@
     </row>
     <row r="67" spans="1:25">
       <c r="A67" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B67" s="1" t="n"/>
       <c r="C67" s="1" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="D67" s="1" t="n">
         <v>1.85</v>
@@ -4577,7 +4811,7 @@
       <c r="Q67" s="1" t="n"/>
       <c r="R67" s="1" t="n"/>
       <c r="S67" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T67" s="1" t="n">
         <v>1</v>
@@ -4600,11 +4834,11 @@
     </row>
     <row r="68" spans="1:25">
       <c r="A68" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B68" s="1" t="n"/>
       <c r="C68" s="1" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="D68" s="1" t="n">
         <v>3.7</v>
@@ -4646,7 +4880,7 @@
       <c r="Q68" s="1" t="n"/>
       <c r="R68" s="1" t="n"/>
       <c r="S68" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T68" s="1" t="n">
         <v>1</v>
@@ -4669,11 +4903,11 @@
     </row>
     <row r="69" spans="1:25">
       <c r="A69" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B69" s="1" t="n"/>
       <c r="C69" s="1" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="D69" s="1" t="n">
         <v>-5.55</v>
@@ -4715,7 +4949,7 @@
       <c r="Q69" s="1" t="n"/>
       <c r="R69" s="1" t="n"/>
       <c r="S69" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T69" s="1" t="n">
         <v>1</v>
@@ -4738,11 +4972,11 @@
     </row>
     <row r="70" spans="1:25">
       <c r="A70" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B70" s="1" t="n"/>
       <c r="C70" s="1" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D70" s="1" t="n">
         <v>-3.7</v>
@@ -4784,7 +5018,7 @@
       <c r="Q70" s="1" t="n"/>
       <c r="R70" s="1" t="n"/>
       <c r="S70" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T70" s="1" t="n">
         <v>1</v>
@@ -4807,11 +5041,11 @@
     </row>
     <row r="71" spans="1:25">
       <c r="A71" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B71" s="1" t="n"/>
       <c r="C71" s="1" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="D71" s="1" t="n">
         <v>-1.85</v>
@@ -4853,7 +5087,7 @@
       <c r="Q71" s="1" t="n"/>
       <c r="R71" s="1" t="n"/>
       <c r="S71" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T71" s="1" t="n">
         <v>1</v>
@@ -4876,11 +5110,11 @@
     </row>
     <row r="72" spans="1:25">
       <c r="A72" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B72" s="1" t="n"/>
       <c r="C72" s="1" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="D72" s="1" t="n">
         <v>0</v>
@@ -4922,7 +5156,7 @@
       <c r="Q72" s="1" t="n"/>
       <c r="R72" s="1" t="n"/>
       <c r="S72" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T72" s="1" t="n">
         <v>1</v>
@@ -4945,11 +5179,11 @@
     </row>
     <row r="73" spans="1:25">
       <c r="A73" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B73" s="1" t="n"/>
       <c r="C73" s="1" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="D73" s="1" t="n">
         <v>1.85</v>
@@ -4991,7 +5225,7 @@
       <c r="Q73" s="1" t="n"/>
       <c r="R73" s="1" t="n"/>
       <c r="S73" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T73" s="1" t="n">
         <v>1</v>
@@ -5014,11 +5248,11 @@
     </row>
     <row r="74" spans="1:25">
       <c r="A74" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B74" s="1" t="n"/>
       <c r="C74" s="1" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="D74" s="1" t="n">
         <v>3.7</v>
@@ -5060,7 +5294,7 @@
       <c r="Q74" s="1" t="n"/>
       <c r="R74" s="1" t="n"/>
       <c r="S74" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T74" s="1" t="n">
         <v>1</v>
@@ -5083,11 +5317,11 @@
     </row>
     <row r="75" spans="1:25">
       <c r="A75" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B75" s="1" t="n"/>
       <c r="C75" s="1" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="D75" s="1" t="n">
         <v>-5.55</v>
@@ -5129,7 +5363,7 @@
       <c r="Q75" s="1" t="n"/>
       <c r="R75" s="1" t="n"/>
       <c r="S75" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T75" s="1" t="n">
         <v>1</v>
@@ -5152,11 +5386,11 @@
     </row>
     <row r="76" spans="1:25">
       <c r="A76" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B76" s="1" t="n"/>
       <c r="C76" s="1" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="D76" s="1" t="n">
         <v>-3.7</v>
@@ -5198,7 +5432,7 @@
       <c r="Q76" s="1" t="n"/>
       <c r="R76" s="1" t="n"/>
       <c r="S76" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T76" s="1" t="n">
         <v>1</v>
@@ -5221,11 +5455,11 @@
     </row>
     <row r="77" spans="1:25">
       <c r="A77" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B77" s="1" t="n"/>
       <c r="C77" s="1" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="D77" s="1" t="n">
         <v>-1.85</v>
@@ -5267,7 +5501,7 @@
       <c r="Q77" s="1" t="n"/>
       <c r="R77" s="1" t="n"/>
       <c r="S77" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T77" s="1" t="n">
         <v>1</v>
@@ -5290,11 +5524,11 @@
     </row>
     <row r="78" spans="1:25">
       <c r="A78" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B78" s="1" t="n"/>
       <c r="C78" s="1" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="D78" s="1" t="n">
         <v>0</v>
@@ -5336,7 +5570,7 @@
       <c r="Q78" s="1" t="n"/>
       <c r="R78" s="1" t="n"/>
       <c r="S78" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T78" s="1" t="n">
         <v>1</v>
@@ -5359,11 +5593,11 @@
     </row>
     <row r="79" spans="1:25">
       <c r="A79" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B79" s="1" t="n"/>
       <c r="C79" s="1" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="D79" s="1" t="n">
         <v>1.85</v>
@@ -5405,7 +5639,7 @@
       <c r="Q79" s="1" t="n"/>
       <c r="R79" s="1" t="n"/>
       <c r="S79" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T79" s="1" t="n">
         <v>1</v>
@@ -5428,11 +5662,11 @@
     </row>
     <row r="80" spans="1:25">
       <c r="A80" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B80" s="1" t="n"/>
       <c r="C80" s="1" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="D80" s="1" t="n">
         <v>3.7</v>
@@ -5474,7 +5708,7 @@
       <c r="Q80" s="1" t="n"/>
       <c r="R80" s="1" t="n"/>
       <c r="S80" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T80" s="1" t="n">
         <v>1</v>
@@ -5497,11 +5731,11 @@
     </row>
     <row r="81" spans="1:25">
       <c r="A81" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B81" s="1" t="n"/>
       <c r="C81" s="1" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="D81" s="1" t="n">
         <v>-5.55</v>
@@ -5543,7 +5777,7 @@
       <c r="Q81" s="1" t="n"/>
       <c r="R81" s="1" t="n"/>
       <c r="S81" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T81" s="1" t="n">
         <v>1</v>
@@ -5566,11 +5800,11 @@
     </row>
     <row r="82" spans="1:25">
       <c r="A82" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B82" s="1" t="n"/>
       <c r="C82" s="1" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="D82" s="1" t="n">
         <v>-3.7</v>
@@ -5612,7 +5846,7 @@
       <c r="Q82" s="1" t="n"/>
       <c r="R82" s="1" t="n"/>
       <c r="S82" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T82" s="1" t="n">
         <v>1</v>
@@ -5635,11 +5869,11 @@
     </row>
     <row r="83" spans="1:25">
       <c r="A83" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B83" s="1" t="n"/>
       <c r="C83" s="1" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="D83" s="1" t="n">
         <v>-1.85</v>
@@ -5681,7 +5915,7 @@
       <c r="Q83" s="1" t="n"/>
       <c r="R83" s="1" t="n"/>
       <c r="S83" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T83" s="1" t="n">
         <v>1</v>
@@ -5704,11 +5938,11 @@
     </row>
     <row r="84" spans="1:25">
       <c r="A84" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B84" s="1" t="n"/>
       <c r="C84" s="1" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="D84" s="1" t="n">
         <v>0</v>
@@ -5750,7 +5984,7 @@
       <c r="Q84" s="1" t="n"/>
       <c r="R84" s="1" t="n"/>
       <c r="S84" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T84" s="1" t="n">
         <v>1</v>
@@ -5773,11 +6007,11 @@
     </row>
     <row r="85" spans="1:25">
       <c r="A85" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B85" s="1" t="n"/>
       <c r="C85" s="1" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="D85" s="1" t="n">
         <v>1.85</v>
@@ -5819,7 +6053,7 @@
       <c r="Q85" s="1" t="n"/>
       <c r="R85" s="1" t="n"/>
       <c r="S85" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T85" s="1" t="n">
         <v>1</v>
@@ -5842,11 +6076,11 @@
     </row>
     <row r="86" spans="1:25">
       <c r="A86" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B86" s="1" t="n"/>
       <c r="C86" s="1" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="D86" s="1" t="n">
         <v>3.7</v>
@@ -5888,7 +6122,7 @@
       <c r="Q86" s="1" t="n"/>
       <c r="R86" s="1" t="n"/>
       <c r="S86" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T86" s="1" t="n">
         <v>1</v>
@@ -5911,11 +6145,11 @@
     </row>
     <row r="87" spans="1:25">
       <c r="A87" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B87" s="1" t="n"/>
       <c r="C87" s="1" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="D87" s="1" t="n">
         <v>-5.55</v>
@@ -5957,7 +6191,7 @@
       <c r="Q87" s="1" t="n"/>
       <c r="R87" s="1" t="n"/>
       <c r="S87" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T87" s="1" t="n">
         <v>1</v>
@@ -5980,11 +6214,11 @@
     </row>
     <row r="88" spans="1:25">
       <c r="A88" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B88" s="1" t="n"/>
       <c r="C88" s="1" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="D88" s="1" t="n">
         <v>-3.7</v>
@@ -6026,7 +6260,7 @@
       <c r="Q88" s="1" t="n"/>
       <c r="R88" s="1" t="n"/>
       <c r="S88" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T88" s="1" t="n">
         <v>1</v>
@@ -6049,11 +6283,11 @@
     </row>
     <row r="89" spans="1:25">
       <c r="A89" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B89" s="1" t="n"/>
       <c r="C89" s="1" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="D89" s="1" t="n">
         <v>-1.85</v>
@@ -6095,7 +6329,7 @@
       <c r="Q89" s="1" t="n"/>
       <c r="R89" s="1" t="n"/>
       <c r="S89" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T89" s="1" t="n">
         <v>1</v>
@@ -6118,11 +6352,11 @@
     </row>
     <row r="90" spans="1:25">
       <c r="A90" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B90" s="1" t="n"/>
       <c r="C90" s="1" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="D90" s="1" t="n">
         <v>0</v>
@@ -6164,7 +6398,7 @@
       <c r="Q90" s="1" t="n"/>
       <c r="R90" s="1" t="n"/>
       <c r="S90" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T90" s="1" t="n">
         <v>1</v>
@@ -6187,11 +6421,11 @@
     </row>
     <row r="91" spans="1:25">
       <c r="A91" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B91" s="1" t="n"/>
       <c r="C91" s="1" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="D91" s="1" t="n">
         <v>1.85</v>
@@ -6233,7 +6467,7 @@
       <c r="Q91" s="1" t="n"/>
       <c r="R91" s="1" t="n"/>
       <c r="S91" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T91" s="1" t="n">
         <v>1</v>
@@ -6256,11 +6490,11 @@
     </row>
     <row r="92" spans="1:25">
       <c r="A92" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B92" s="1" t="n"/>
       <c r="C92" s="1" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="D92" s="1" t="n">
         <v>3.7</v>
@@ -6302,7 +6536,7 @@
       <c r="Q92" s="1" t="n"/>
       <c r="R92" s="1" t="n"/>
       <c r="S92" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T92" s="1" t="n">
         <v>1</v>
@@ -6325,11 +6559,11 @@
     </row>
     <row r="93" spans="1:25">
       <c r="A93" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B93" s="1" t="n"/>
       <c r="C93" s="1" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="D93" s="1" t="n">
         <v>-1.25</v>
@@ -6371,7 +6605,7 @@
       <c r="Q93" s="1" t="n"/>
       <c r="R93" s="1" t="n"/>
       <c r="S93" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T93" s="1" t="n">
         <v>8</v>
@@ -6394,11 +6628,11 @@
     </row>
     <row r="94" spans="1:25">
       <c r="A94" s="1" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="B94" s="1" t="n"/>
       <c r="C94" s="1" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="D94" s="1" t="n">
         <v>1</v>
@@ -6440,7 +6674,7 @@
       <c r="Q94" s="1" t="n"/>
       <c r="R94" s="1" t="n"/>
       <c r="S94" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T94" s="1" t="n">
         <v>8</v>
@@ -6463,11 +6697,11 @@
     </row>
     <row r="95" spans="1:25">
       <c r="A95" s="1" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="B95" s="1" t="n"/>
       <c r="C95" s="1" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="D95" s="1" t="n">
         <v>0</v>
@@ -6509,7 +6743,7 @@
       <c r="Q95" s="1" t="n"/>
       <c r="R95" s="1" t="n"/>
       <c r="S95" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T95" s="1" t="n">
         <v>8</v>
@@ -6532,11 +6766,11 @@
     </row>
     <row r="96" spans="1:25">
       <c r="A96" s="1" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="B96" s="1" t="n"/>
       <c r="C96" s="1" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="D96" s="1" t="n">
         <v>0</v>
@@ -6578,7 +6812,7 @@
       <c r="Q96" s="1" t="n"/>
       <c r="R96" s="1" t="n"/>
       <c r="S96" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T96" s="1" t="n">
         <v>3</v>
@@ -6601,11 +6835,11 @@
     </row>
     <row r="97" spans="1:25">
       <c r="A97" s="1" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="B97" s="1" t="n"/>
       <c r="C97" s="1" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="D97" s="1" t="n">
         <v>10.35</v>
@@ -6647,7 +6881,7 @@
       <c r="Q97" s="1" t="n"/>
       <c r="R97" s="1" t="n"/>
       <c r="S97" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T97" s="1" t="n">
         <v>1</v>
@@ -6670,11 +6904,11 @@
     </row>
     <row r="98" spans="1:25">
       <c r="A98" s="1" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="B98" s="1" t="n"/>
       <c r="C98" s="1" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="D98" s="1" t="n">
         <v>3.6</v>
@@ -6716,7 +6950,7 @@
       <c r="Q98" s="1" t="n"/>
       <c r="R98" s="1" t="n"/>
       <c r="S98" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T98" s="1" t="n">
         <v>1</v>
@@ -6739,11 +6973,11 @@
     </row>
     <row r="99" spans="1:25">
       <c r="A99" s="1" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="B99" s="1" t="n"/>
       <c r="C99" s="1" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="D99" s="1" t="n">
         <v>2.8</v>
@@ -6785,7 +7019,7 @@
       <c r="Q99" s="1" t="n"/>
       <c r="R99" s="1" t="n"/>
       <c r="S99" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T99" s="1" t="n">
         <v>8</v>
@@ -6808,11 +7042,11 @@
     </row>
     <row r="100" spans="1:25">
       <c r="A100" s="1" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="B100" s="1" t="n"/>
       <c r="C100" s="1" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="D100" s="1" t="n">
         <v>2.8</v>
@@ -6854,7 +7088,7 @@
       <c r="Q100" s="1" t="n"/>
       <c r="R100" s="1" t="n"/>
       <c r="S100" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T100" s="1" t="n">
         <v>8</v>
@@ -6877,11 +7111,11 @@
     </row>
     <row r="101" spans="1:25">
       <c r="A101" s="1" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="B101" s="1" t="n"/>
       <c r="C101" s="1" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="D101" s="1" t="n">
         <v>0</v>
@@ -6923,7 +7157,7 @@
       <c r="Q101" s="1" t="n"/>
       <c r="R101" s="1" t="n"/>
       <c r="S101" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T101" s="1" t="n">
         <v>8</v>
@@ -6946,11 +7180,11 @@
     </row>
     <row r="102" spans="1:25">
       <c r="A102" s="1" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="B102" s="1" t="n"/>
       <c r="C102" s="1" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="D102" s="1" t="n">
         <v>0</v>
@@ -6992,7 +7226,7 @@
       <c r="Q102" s="1" t="n"/>
       <c r="R102" s="1" t="n"/>
       <c r="S102" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T102" s="1" t="n">
         <v>1</v>
@@ -7015,11 +7249,11 @@
     </row>
     <row r="103" spans="1:25">
       <c r="A103" s="1" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="B103" s="1" t="n"/>
       <c r="C103" s="1" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="D103" s="1" t="n">
         <v>-8.15</v>
@@ -7061,7 +7295,7 @@
       <c r="Q103" s="1" t="n"/>
       <c r="R103" s="1" t="n"/>
       <c r="S103" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T103" s="1" t="n">
         <v>1</v>
@@ -7084,11 +7318,11 @@
     </row>
     <row r="104" spans="1:25">
       <c r="A104" s="1" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="B104" s="1" t="n"/>
       <c r="C104" s="1" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="D104" s="1" t="n">
         <v>-9.949999999999999</v>
@@ -7130,7 +7364,7 @@
       <c r="Q104" s="1" t="n"/>
       <c r="R104" s="1" t="n"/>
       <c r="S104" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T104" s="1" t="n">
         <v>1</v>
@@ -7153,11 +7387,11 @@
     </row>
     <row r="105" spans="1:25">
       <c r="A105" s="1" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="B105" s="1" t="n"/>
       <c r="C105" s="1" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="D105" s="1" t="n">
         <v>-9.949999999999999</v>
@@ -7199,7 +7433,7 @@
       <c r="Q105" s="1" t="n"/>
       <c r="R105" s="1" t="n"/>
       <c r="S105" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T105" s="1" t="n">
         <v>1</v>

</xml_diff>